<commit_message>
All kinds of things. I tried to separate the cinemachine stuff, who knows if it worked?
</commit_message>
<xml_diff>
--- a/Other/RoStatProcessing.xlsx
+++ b/Other/RoStatProcessing.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25726"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26626"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\ProjectsSSD\RagnarokRebuildTcp\Other\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6C2DFE3F-823B-4E67-8F73-C46319708E85}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E695A9D7-A360-45A8-8D34-5B3DE2E77DD8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="6660" yWindow="2477" windowWidth="24129" windowHeight="14743" xr2:uid="{1C41742B-2950-4FF8-AA39-6557869B44EA}"/>
+    <workbookView xWindow="3763" yWindow="351" windowWidth="24094" windowHeight="17083" xr2:uid="{1C41742B-2950-4FF8-AA39-6557869B44EA}"/>
   </bookViews>
   <sheets>
     <sheet name="StatDef" sheetId="3" r:id="rId1"/>
@@ -48,7 +48,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2563" uniqueCount="958">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2653" uniqueCount="989">
   <si>
     <t>Level</t>
   </si>
@@ -2922,6 +2922,99 @@
   </si>
   <si>
     <t>Rank</t>
+  </si>
+  <si>
+    <t>COOKIE</t>
+  </si>
+  <si>
+    <t>Cookie</t>
+  </si>
+  <si>
+    <t>cookie.spr</t>
+  </si>
+  <si>
+    <t>COOKIE_XMAS</t>
+  </si>
+  <si>
+    <t>cookie_xmas.spr</t>
+  </si>
+  <si>
+    <t>CRUISER</t>
+  </si>
+  <si>
+    <t>Cruiser</t>
+  </si>
+  <si>
+    <t>cruiser.spr</t>
+  </si>
+  <si>
+    <t>CHEPET</t>
+  </si>
+  <si>
+    <t>Chepet</t>
+  </si>
+  <si>
+    <t>chepet.spr</t>
+  </si>
+  <si>
+    <t>GOBLINE_XMAS</t>
+  </si>
+  <si>
+    <t>Festive Goblin</t>
+  </si>
+  <si>
+    <t>gobline_xmas.spr</t>
+  </si>
+  <si>
+    <t>GARM</t>
+  </si>
+  <si>
+    <t>Garm</t>
+  </si>
+  <si>
+    <t>Normal,Elite</t>
+  </si>
+  <si>
+    <t>garm.spr</t>
+  </si>
+  <si>
+    <t>GARM_BABY</t>
+  </si>
+  <si>
+    <t>Baby Garm</t>
+  </si>
+  <si>
+    <t>garm_baby.spr</t>
+  </si>
+  <si>
+    <t>KNIGHT_OF_WINDSTORM</t>
+  </si>
+  <si>
+    <t>Stormy Knight</t>
+  </si>
+  <si>
+    <t>knight_of_windstorm.spr</t>
+  </si>
+  <si>
+    <t>MYSTCASE</t>
+  </si>
+  <si>
+    <t>Mystcase</t>
+  </si>
+  <si>
+    <t>mystcase.spr</t>
+  </si>
+  <si>
+    <t>WRAITH_DEAD</t>
+  </si>
+  <si>
+    <t>wraith_dead.spr</t>
+  </si>
+  <si>
+    <t>Wraith Dead</t>
+  </si>
+  <si>
+    <t>Elite,Undead</t>
   </si>
 </sst>
 </file>
@@ -3311,13 +3404,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{811A97A5-94A7-4FFA-A162-65D076B52481}">
-  <dimension ref="A1:AI258"/>
+  <dimension ref="A1:AI268"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <pane xSplit="2" ySplit="1" topLeftCell="C68" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="1" topLeftCell="C236" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="E94" sqref="E94"/>
+      <selection pane="bottomRight" activeCell="AC268" sqref="AC268"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
@@ -30962,6 +31055,1076 @@
         <v>1</v>
       </c>
     </row>
+    <row r="259" spans="1:35" x14ac:dyDescent="0.4">
+      <c r="A259">
+        <v>4256</v>
+      </c>
+      <c r="B259" t="s">
+        <v>958</v>
+      </c>
+      <c r="C259" t="s">
+        <v>959</v>
+      </c>
+      <c r="D259">
+        <v>25</v>
+      </c>
+      <c r="E259">
+        <v>100</v>
+      </c>
+      <c r="F259">
+        <v>100</v>
+      </c>
+      <c r="G259">
+        <v>100</v>
+      </c>
+      <c r="H259">
+        <v>100</v>
+      </c>
+      <c r="I259">
+        <v>100</v>
+      </c>
+      <c r="J259">
+        <v>100</v>
+      </c>
+      <c r="K259">
+        <v>100</v>
+      </c>
+      <c r="L259">
+        <v>100</v>
+      </c>
+      <c r="M259">
+        <v>10</v>
+      </c>
+      <c r="N259">
+        <v>1</v>
+      </c>
+      <c r="O259">
+        <v>100</v>
+      </c>
+      <c r="P259">
+        <v>100</v>
+      </c>
+      <c r="Q259">
+        <v>100</v>
+      </c>
+      <c r="R259">
+        <v>100</v>
+      </c>
+      <c r="S259">
+        <v>10</v>
+      </c>
+      <c r="T259">
+        <v>12</v>
+      </c>
+      <c r="U259" t="s">
+        <v>56</v>
+      </c>
+      <c r="V259" t="s">
+        <v>172</v>
+      </c>
+      <c r="W259" t="s">
+        <v>63</v>
+      </c>
+      <c r="X259">
+        <v>1036</v>
+      </c>
+      <c r="Y259">
+        <v>240</v>
+      </c>
+      <c r="Z259">
+        <v>936</v>
+      </c>
+      <c r="AA259">
+        <v>200</v>
+      </c>
+      <c r="AB259" t="s">
+        <v>42</v>
+      </c>
+      <c r="AC259" t="s">
+        <v>42</v>
+      </c>
+      <c r="AD259" t="s">
+        <v>43</v>
+      </c>
+      <c r="AE259">
+        <v>111</v>
+      </c>
+      <c r="AF259" t="s">
+        <v>960</v>
+      </c>
+      <c r="AG259">
+        <v>0</v>
+      </c>
+      <c r="AH259">
+        <v>0.5</v>
+      </c>
+      <c r="AI259">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="260" spans="1:35" x14ac:dyDescent="0.4">
+      <c r="A260">
+        <v>4257</v>
+      </c>
+      <c r="B260" t="s">
+        <v>961</v>
+      </c>
+      <c r="C260" t="s">
+        <v>959</v>
+      </c>
+      <c r="D260">
+        <v>28</v>
+      </c>
+      <c r="E260">
+        <v>100</v>
+      </c>
+      <c r="F260">
+        <v>100</v>
+      </c>
+      <c r="G260">
+        <v>100</v>
+      </c>
+      <c r="H260">
+        <v>100</v>
+      </c>
+      <c r="I260">
+        <v>100</v>
+      </c>
+      <c r="J260">
+        <v>100</v>
+      </c>
+      <c r="K260">
+        <v>100</v>
+      </c>
+      <c r="L260">
+        <v>100</v>
+      </c>
+      <c r="M260">
+        <v>10</v>
+      </c>
+      <c r="N260">
+        <v>1</v>
+      </c>
+      <c r="O260">
+        <v>100</v>
+      </c>
+      <c r="P260">
+        <v>100</v>
+      </c>
+      <c r="Q260">
+        <v>100</v>
+      </c>
+      <c r="R260">
+        <v>100</v>
+      </c>
+      <c r="S260">
+        <v>10</v>
+      </c>
+      <c r="T260">
+        <v>12</v>
+      </c>
+      <c r="U260" t="s">
+        <v>56</v>
+      </c>
+      <c r="V260" t="s">
+        <v>172</v>
+      </c>
+      <c r="W260" t="s">
+        <v>603</v>
+      </c>
+      <c r="X260">
+        <v>1248</v>
+      </c>
+      <c r="Y260">
+        <v>240</v>
+      </c>
+      <c r="Z260">
+        <v>1248</v>
+      </c>
+      <c r="AA260">
+        <v>400</v>
+      </c>
+      <c r="AB260" t="s">
+        <v>42</v>
+      </c>
+      <c r="AC260" t="s">
+        <v>42</v>
+      </c>
+      <c r="AD260" t="s">
+        <v>43</v>
+      </c>
+      <c r="AE260">
+        <v>350</v>
+      </c>
+      <c r="AF260" t="s">
+        <v>962</v>
+      </c>
+      <c r="AG260">
+        <v>0</v>
+      </c>
+      <c r="AH260">
+        <v>0.5</v>
+      </c>
+      <c r="AI260">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="261" spans="1:35" x14ac:dyDescent="0.4">
+      <c r="A261">
+        <v>4258</v>
+      </c>
+      <c r="B261" t="s">
+        <v>963</v>
+      </c>
+      <c r="C261" t="s">
+        <v>964</v>
+      </c>
+      <c r="D261">
+        <v>35</v>
+      </c>
+      <c r="E261">
+        <v>100</v>
+      </c>
+      <c r="F261">
+        <v>100</v>
+      </c>
+      <c r="G261">
+        <v>100</v>
+      </c>
+      <c r="H261">
+        <v>100</v>
+      </c>
+      <c r="I261">
+        <v>100</v>
+      </c>
+      <c r="J261">
+        <v>100</v>
+      </c>
+      <c r="K261">
+        <v>100</v>
+      </c>
+      <c r="L261">
+        <v>100</v>
+      </c>
+      <c r="M261">
+        <v>10</v>
+      </c>
+      <c r="N261">
+        <v>7</v>
+      </c>
+      <c r="O261">
+        <v>100</v>
+      </c>
+      <c r="P261">
+        <v>100</v>
+      </c>
+      <c r="Q261">
+        <v>100</v>
+      </c>
+      <c r="R261">
+        <v>100</v>
+      </c>
+      <c r="S261">
+        <v>10</v>
+      </c>
+      <c r="T261">
+        <v>12</v>
+      </c>
+      <c r="U261" t="s">
+        <v>39</v>
+      </c>
+      <c r="V261" t="s">
+        <v>50</v>
+      </c>
+      <c r="W261" t="s">
+        <v>63</v>
+      </c>
+      <c r="X261">
+        <v>1296</v>
+      </c>
+      <c r="Y261">
+        <v>432</v>
+      </c>
+      <c r="Z261">
+        <v>1296</v>
+      </c>
+      <c r="AA261">
+        <v>400</v>
+      </c>
+      <c r="AB261" t="s">
+        <v>42</v>
+      </c>
+      <c r="AC261" t="s">
+        <v>592</v>
+      </c>
+      <c r="AD261" t="s">
+        <v>72</v>
+      </c>
+      <c r="AE261">
+        <v>1000</v>
+      </c>
+      <c r="AF261" t="s">
+        <v>965</v>
+      </c>
+      <c r="AG261">
+        <v>0</v>
+      </c>
+      <c r="AH261">
+        <v>0.5</v>
+      </c>
+      <c r="AI261">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="262" spans="1:35" x14ac:dyDescent="0.4">
+      <c r="A262">
+        <v>4259</v>
+      </c>
+      <c r="B262" t="s">
+        <v>966</v>
+      </c>
+      <c r="C262" t="s">
+        <v>967</v>
+      </c>
+      <c r="D262">
+        <v>42</v>
+      </c>
+      <c r="E262">
+        <v>100</v>
+      </c>
+      <c r="F262">
+        <v>100</v>
+      </c>
+      <c r="G262">
+        <v>100</v>
+      </c>
+      <c r="H262">
+        <v>100</v>
+      </c>
+      <c r="I262">
+        <v>100</v>
+      </c>
+      <c r="J262">
+        <v>100</v>
+      </c>
+      <c r="K262">
+        <v>100</v>
+      </c>
+      <c r="L262">
+        <v>100</v>
+      </c>
+      <c r="M262">
+        <v>10</v>
+      </c>
+      <c r="N262">
+        <v>1</v>
+      </c>
+      <c r="O262">
+        <v>100</v>
+      </c>
+      <c r="P262">
+        <v>100</v>
+      </c>
+      <c r="Q262">
+        <v>100</v>
+      </c>
+      <c r="R262">
+        <v>100</v>
+      </c>
+      <c r="S262">
+        <v>10</v>
+      </c>
+      <c r="T262">
+        <v>12</v>
+      </c>
+      <c r="U262" t="s">
+        <v>39</v>
+      </c>
+      <c r="V262" t="s">
+        <v>172</v>
+      </c>
+      <c r="W262" t="s">
+        <v>111</v>
+      </c>
+      <c r="X262">
+        <v>672</v>
+      </c>
+      <c r="Y262">
+        <v>288</v>
+      </c>
+      <c r="Z262">
+        <v>672</v>
+      </c>
+      <c r="AA262">
+        <v>400</v>
+      </c>
+      <c r="AB262" t="s">
+        <v>42</v>
+      </c>
+      <c r="AC262" t="s">
+        <v>581</v>
+      </c>
+      <c r="AD262" t="s">
+        <v>72</v>
+      </c>
+      <c r="AE262">
+        <v>350</v>
+      </c>
+      <c r="AF262" t="s">
+        <v>968</v>
+      </c>
+      <c r="AG262">
+        <v>0</v>
+      </c>
+      <c r="AH262">
+        <v>0.5</v>
+      </c>
+      <c r="AI262">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="263" spans="1:35" x14ac:dyDescent="0.4">
+      <c r="A263">
+        <v>4260</v>
+      </c>
+      <c r="B263" t="s">
+        <v>969</v>
+      </c>
+      <c r="C263" t="s">
+        <v>970</v>
+      </c>
+      <c r="D263">
+        <v>25</v>
+      </c>
+      <c r="E263">
+        <v>100</v>
+      </c>
+      <c r="F263">
+        <v>100</v>
+      </c>
+      <c r="G263">
+        <v>100</v>
+      </c>
+      <c r="H263">
+        <v>100</v>
+      </c>
+      <c r="I263">
+        <v>100</v>
+      </c>
+      <c r="J263">
+        <v>100</v>
+      </c>
+      <c r="K263">
+        <v>100</v>
+      </c>
+      <c r="L263">
+        <v>100</v>
+      </c>
+      <c r="M263">
+        <v>10</v>
+      </c>
+      <c r="N263">
+        <v>1</v>
+      </c>
+      <c r="O263">
+        <v>100</v>
+      </c>
+      <c r="P263">
+        <v>100</v>
+      </c>
+      <c r="Q263">
+        <v>100</v>
+      </c>
+      <c r="R263">
+        <v>100</v>
+      </c>
+      <c r="S263">
+        <v>10</v>
+      </c>
+      <c r="T263">
+        <v>12</v>
+      </c>
+      <c r="U263" t="s">
+        <v>39</v>
+      </c>
+      <c r="V263" t="s">
+        <v>172</v>
+      </c>
+      <c r="W263" t="s">
+        <v>81</v>
+      </c>
+      <c r="X263">
+        <v>1120</v>
+      </c>
+      <c r="Y263">
+        <v>240</v>
+      </c>
+      <c r="Z263">
+        <v>620</v>
+      </c>
+      <c r="AA263">
+        <v>100</v>
+      </c>
+      <c r="AB263" t="s">
+        <v>42</v>
+      </c>
+      <c r="AC263" t="s">
+        <v>42</v>
+      </c>
+      <c r="AD263" t="s">
+        <v>72</v>
+      </c>
+      <c r="AE263">
+        <v>400</v>
+      </c>
+      <c r="AF263" t="s">
+        <v>971</v>
+      </c>
+      <c r="AG263">
+        <v>0</v>
+      </c>
+      <c r="AH263">
+        <v>0.5</v>
+      </c>
+      <c r="AI263">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="264" spans="1:35" x14ac:dyDescent="0.4">
+      <c r="A264">
+        <v>4261</v>
+      </c>
+      <c r="B264" t="s">
+        <v>972</v>
+      </c>
+      <c r="C264" t="s">
+        <v>973</v>
+      </c>
+      <c r="D264">
+        <v>73</v>
+      </c>
+      <c r="E264">
+        <v>100</v>
+      </c>
+      <c r="F264">
+        <v>100</v>
+      </c>
+      <c r="G264">
+        <v>100</v>
+      </c>
+      <c r="H264">
+        <v>100</v>
+      </c>
+      <c r="I264">
+        <v>100</v>
+      </c>
+      <c r="J264">
+        <v>100</v>
+      </c>
+      <c r="K264">
+        <v>100</v>
+      </c>
+      <c r="L264">
+        <v>100</v>
+      </c>
+      <c r="M264">
+        <v>10</v>
+      </c>
+      <c r="N264">
+        <v>3</v>
+      </c>
+      <c r="O264">
+        <v>100</v>
+      </c>
+      <c r="P264">
+        <v>100</v>
+      </c>
+      <c r="Q264">
+        <v>100</v>
+      </c>
+      <c r="R264">
+        <v>100</v>
+      </c>
+      <c r="S264">
+        <v>10</v>
+      </c>
+      <c r="T264">
+        <v>12</v>
+      </c>
+      <c r="U264" t="s">
+        <v>156</v>
+      </c>
+      <c r="V264" t="s">
+        <v>62</v>
+      </c>
+      <c r="W264" t="s">
+        <v>599</v>
+      </c>
+      <c r="X264">
+        <v>608</v>
+      </c>
+      <c r="Y264">
+        <v>336</v>
+      </c>
+      <c r="Z264">
+        <v>408</v>
+      </c>
+      <c r="AA264">
+        <v>400</v>
+      </c>
+      <c r="AB264" t="s">
+        <v>71</v>
+      </c>
+      <c r="AC264" t="s">
+        <v>974</v>
+      </c>
+      <c r="AD264" t="s">
+        <v>72</v>
+      </c>
+      <c r="AE264">
+        <v>325</v>
+      </c>
+      <c r="AF264" t="s">
+        <v>975</v>
+      </c>
+      <c r="AG264">
+        <v>0</v>
+      </c>
+      <c r="AH264">
+        <v>0.5</v>
+      </c>
+      <c r="AI264">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="265" spans="1:35" x14ac:dyDescent="0.4">
+      <c r="A265">
+        <v>4262</v>
+      </c>
+      <c r="B265" t="s">
+        <v>976</v>
+      </c>
+      <c r="C265" t="s">
+        <v>977</v>
+      </c>
+      <c r="D265">
+        <v>61</v>
+      </c>
+      <c r="E265">
+        <v>100</v>
+      </c>
+      <c r="F265">
+        <v>100</v>
+      </c>
+      <c r="G265">
+        <v>100</v>
+      </c>
+      <c r="H265">
+        <v>100</v>
+      </c>
+      <c r="I265">
+        <v>100</v>
+      </c>
+      <c r="J265">
+        <v>100</v>
+      </c>
+      <c r="K265">
+        <v>100</v>
+      </c>
+      <c r="L265">
+        <v>100</v>
+      </c>
+      <c r="M265">
+        <v>10</v>
+      </c>
+      <c r="N265">
+        <v>1</v>
+      </c>
+      <c r="O265">
+        <v>100</v>
+      </c>
+      <c r="P265">
+        <v>100</v>
+      </c>
+      <c r="Q265">
+        <v>100</v>
+      </c>
+      <c r="R265">
+        <v>100</v>
+      </c>
+      <c r="S265">
+        <v>10</v>
+      </c>
+      <c r="T265">
+        <v>12</v>
+      </c>
+      <c r="U265" t="s">
+        <v>39</v>
+      </c>
+      <c r="V265" t="s">
+        <v>62</v>
+      </c>
+      <c r="W265" t="s">
+        <v>220</v>
+      </c>
+      <c r="X265">
+        <v>879</v>
+      </c>
+      <c r="Y265">
+        <v>576</v>
+      </c>
+      <c r="Z265">
+        <v>672</v>
+      </c>
+      <c r="AA265">
+        <v>450</v>
+      </c>
+      <c r="AB265" t="s">
+        <v>42</v>
+      </c>
+      <c r="AC265" t="s">
+        <v>42</v>
+      </c>
+      <c r="AD265" t="s">
+        <v>72</v>
+      </c>
+      <c r="AE265">
+        <v>300</v>
+      </c>
+      <c r="AF265" t="s">
+        <v>978</v>
+      </c>
+      <c r="AG265">
+        <v>0</v>
+      </c>
+      <c r="AH265">
+        <v>0.5</v>
+      </c>
+      <c r="AI265">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="266" spans="1:35" x14ac:dyDescent="0.4">
+      <c r="A266">
+        <v>4263</v>
+      </c>
+      <c r="B266" t="s">
+        <v>979</v>
+      </c>
+      <c r="C266" t="s">
+        <v>980</v>
+      </c>
+      <c r="D266">
+        <v>77</v>
+      </c>
+      <c r="E266">
+        <v>100</v>
+      </c>
+      <c r="F266">
+        <v>100</v>
+      </c>
+      <c r="G266">
+        <v>100</v>
+      </c>
+      <c r="H266">
+        <v>100</v>
+      </c>
+      <c r="I266">
+        <v>100</v>
+      </c>
+      <c r="J266">
+        <v>100</v>
+      </c>
+      <c r="K266">
+        <v>100</v>
+      </c>
+      <c r="L266">
+        <v>100</v>
+      </c>
+      <c r="M266">
+        <v>10</v>
+      </c>
+      <c r="N266">
+        <v>2</v>
+      </c>
+      <c r="O266">
+        <v>100</v>
+      </c>
+      <c r="P266">
+        <v>100</v>
+      </c>
+      <c r="Q266">
+        <v>100</v>
+      </c>
+      <c r="R266">
+        <v>100</v>
+      </c>
+      <c r="S266">
+        <v>10</v>
+      </c>
+      <c r="T266">
+        <v>12</v>
+      </c>
+      <c r="U266" t="s">
+        <v>156</v>
+      </c>
+      <c r="V266" t="s">
+        <v>50</v>
+      </c>
+      <c r="W266" t="s">
+        <v>373</v>
+      </c>
+      <c r="X266">
+        <v>468</v>
+      </c>
+      <c r="Y266">
+        <v>288</v>
+      </c>
+      <c r="Z266">
+        <v>468</v>
+      </c>
+      <c r="AA266">
+        <v>200</v>
+      </c>
+      <c r="AB266" t="s">
+        <v>71</v>
+      </c>
+      <c r="AC266" t="s">
+        <v>584</v>
+      </c>
+      <c r="AD266" t="s">
+        <v>72</v>
+      </c>
+      <c r="AE266">
+        <v>259</v>
+      </c>
+      <c r="AF266" t="s">
+        <v>981</v>
+      </c>
+      <c r="AG266">
+        <v>0</v>
+      </c>
+      <c r="AH266">
+        <v>0.5</v>
+      </c>
+      <c r="AI266">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="267" spans="1:35" x14ac:dyDescent="0.4">
+      <c r="A267">
+        <v>4264</v>
+      </c>
+      <c r="B267" t="s">
+        <v>982</v>
+      </c>
+      <c r="C267" t="s">
+        <v>983</v>
+      </c>
+      <c r="D267">
+        <v>38</v>
+      </c>
+      <c r="E267">
+        <v>100</v>
+      </c>
+      <c r="F267">
+        <v>100</v>
+      </c>
+      <c r="G267">
+        <v>100</v>
+      </c>
+      <c r="H267">
+        <v>100</v>
+      </c>
+      <c r="I267">
+        <v>100</v>
+      </c>
+      <c r="J267">
+        <v>100</v>
+      </c>
+      <c r="K267">
+        <v>100</v>
+      </c>
+      <c r="L267">
+        <v>100</v>
+      </c>
+      <c r="M267">
+        <v>10</v>
+      </c>
+      <c r="N267">
+        <v>1</v>
+      </c>
+      <c r="O267">
+        <v>100</v>
+      </c>
+      <c r="P267">
+        <v>100</v>
+      </c>
+      <c r="Q267">
+        <v>100</v>
+      </c>
+      <c r="R267">
+        <v>100</v>
+      </c>
+      <c r="S267">
+        <v>10</v>
+      </c>
+      <c r="T267">
+        <v>12</v>
+      </c>
+      <c r="U267" t="s">
+        <v>39</v>
+      </c>
+      <c r="V267" t="s">
+        <v>50</v>
+      </c>
+      <c r="W267" t="s">
+        <v>63</v>
+      </c>
+      <c r="X267">
+        <v>1248</v>
+      </c>
+      <c r="Y267">
+        <v>432</v>
+      </c>
+      <c r="Z267">
+        <v>1248</v>
+      </c>
+      <c r="AA267">
+        <v>400</v>
+      </c>
+      <c r="AB267" t="s">
+        <v>42</v>
+      </c>
+      <c r="AC267" t="s">
+        <v>42</v>
+      </c>
+      <c r="AD267" t="s">
+        <v>43</v>
+      </c>
+      <c r="AE267">
+        <v>450</v>
+      </c>
+      <c r="AF267" t="s">
+        <v>984</v>
+      </c>
+      <c r="AG267">
+        <v>0</v>
+      </c>
+      <c r="AH267">
+        <v>0.5</v>
+      </c>
+      <c r="AI267">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="268" spans="1:35" x14ac:dyDescent="0.4">
+      <c r="A268">
+        <v>4265</v>
+      </c>
+      <c r="B268" t="s">
+        <v>985</v>
+      </c>
+      <c r="C268" t="s">
+        <v>987</v>
+      </c>
+      <c r="D268">
+        <v>74</v>
+      </c>
+      <c r="E268">
+        <v>100</v>
+      </c>
+      <c r="F268">
+        <v>100</v>
+      </c>
+      <c r="G268">
+        <v>100</v>
+      </c>
+      <c r="H268">
+        <v>100</v>
+      </c>
+      <c r="I268">
+        <v>100</v>
+      </c>
+      <c r="J268">
+        <v>100</v>
+      </c>
+      <c r="K268">
+        <v>100</v>
+      </c>
+      <c r="L268">
+        <v>100</v>
+      </c>
+      <c r="M268">
+        <v>10</v>
+      </c>
+      <c r="N268">
+        <v>2</v>
+      </c>
+      <c r="O268">
+        <v>100</v>
+      </c>
+      <c r="P268">
+        <v>100</v>
+      </c>
+      <c r="Q268">
+        <v>100</v>
+      </c>
+      <c r="R268">
+        <v>100</v>
+      </c>
+      <c r="S268">
+        <v>10</v>
+      </c>
+      <c r="T268">
+        <v>12</v>
+      </c>
+      <c r="U268" t="s">
+        <v>156</v>
+      </c>
+      <c r="V268" t="s">
+        <v>450</v>
+      </c>
+      <c r="W268" t="s">
+        <v>477</v>
+      </c>
+      <c r="X268">
+        <v>1816</v>
+      </c>
+      <c r="Y268">
+        <v>240</v>
+      </c>
+      <c r="Z268">
+        <v>576</v>
+      </c>
+      <c r="AA268">
+        <v>175</v>
+      </c>
+      <c r="AB268" t="s">
+        <v>42</v>
+      </c>
+      <c r="AC268" t="s">
+        <v>988</v>
+      </c>
+      <c r="AD268" t="s">
+        <v>72</v>
+      </c>
+      <c r="AE268">
+        <v>850</v>
+      </c>
+      <c r="AF268" t="s">
+        <v>986</v>
+      </c>
+      <c r="AG268">
+        <v>0</v>
+      </c>
+      <c r="AH268">
+        <v>0.5</v>
+      </c>
+      <c r="AI268">
+        <v>1</v>
+      </c>
+    </row>
   </sheetData>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:AI179">
     <sortCondition ref="D2:D179"/>

</xml_diff>

<commit_message>
Some other updated data.
</commit_message>
<xml_diff>
--- a/Other/RoStatProcessing.xlsx
+++ b/Other/RoStatProcessing.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\ProjectsSSD\RagnarokRebuildTcp\Other\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E695A9D7-A360-45A8-8D34-5B3DE2E77DD8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0F83316D-1843-41C7-87EF-CB415F337456}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3763" yWindow="351" windowWidth="24094" windowHeight="17083" xr2:uid="{1C41742B-2950-4FF8-AA39-6557869B44EA}"/>
+    <workbookView xWindow="2571" yWindow="2674" windowWidth="27798" windowHeight="14726" xr2:uid="{1C41742B-2950-4FF8-AA39-6557869B44EA}"/>
   </bookViews>
   <sheets>
     <sheet name="StatDef" sheetId="3" r:id="rId1"/>
@@ -48,7 +48,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2653" uniqueCount="989">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2816" uniqueCount="1045">
   <si>
     <t>Level</t>
   </si>
@@ -3015,6 +3015,174 @@
   </si>
   <si>
     <t>Elite,Undead</t>
+  </si>
+  <si>
+    <t>SHELLFISH</t>
+  </si>
+  <si>
+    <t>ALLIGATOR</t>
+  </si>
+  <si>
+    <t>ASTER</t>
+  </si>
+  <si>
+    <t>CRAB</t>
+  </si>
+  <si>
+    <t>RAGGLER</t>
+  </si>
+  <si>
+    <t>MOBSTER</t>
+  </si>
+  <si>
+    <t>FUR_SEAL</t>
+  </si>
+  <si>
+    <t>GALAPAGO</t>
+  </si>
+  <si>
+    <t>MUTANT_DRAGON</t>
+  </si>
+  <si>
+    <t>SEE_OTTER</t>
+  </si>
+  <si>
+    <t>GRYPHON</t>
+  </si>
+  <si>
+    <t>MEDUSA</t>
+  </si>
+  <si>
+    <t>NERAID</t>
+  </si>
+  <si>
+    <t>TRI_JOINT</t>
+  </si>
+  <si>
+    <t>STALACTIC_GOLEM</t>
+  </si>
+  <si>
+    <t>MEGALODON</t>
+  </si>
+  <si>
+    <t>MEGALITH</t>
+  </si>
+  <si>
+    <t>TAO_GUNKA</t>
+  </si>
+  <si>
+    <t>Shellfish</t>
+  </si>
+  <si>
+    <t>Alligator</t>
+  </si>
+  <si>
+    <t>Aster</t>
+  </si>
+  <si>
+    <t>Crab</t>
+  </si>
+  <si>
+    <t>Raggler</t>
+  </si>
+  <si>
+    <t>Mobster</t>
+  </si>
+  <si>
+    <t>Galapago</t>
+  </si>
+  <si>
+    <t>Gryphon</t>
+  </si>
+  <si>
+    <t>Medusa</t>
+  </si>
+  <si>
+    <t>Neraid</t>
+  </si>
+  <si>
+    <t>Megalodon</t>
+  </si>
+  <si>
+    <t>Megalith</t>
+  </si>
+  <si>
+    <t>Mutant Dragon</t>
+  </si>
+  <si>
+    <t>Fur Seal</t>
+  </si>
+  <si>
+    <t>See Otter</t>
+  </si>
+  <si>
+    <t>Tri Joint</t>
+  </si>
+  <si>
+    <t>Stalactic Golem</t>
+  </si>
+  <si>
+    <t>Tao Gunka</t>
+  </si>
+  <si>
+    <t>shellfish.spr</t>
+  </si>
+  <si>
+    <t>alligator.spr</t>
+  </si>
+  <si>
+    <t>aster.spr</t>
+  </si>
+  <si>
+    <t>crab.spr</t>
+  </si>
+  <si>
+    <t>raggler.spr</t>
+  </si>
+  <si>
+    <t>mobster.spr</t>
+  </si>
+  <si>
+    <t>fur_seal.spr</t>
+  </si>
+  <si>
+    <t>galapago.spr</t>
+  </si>
+  <si>
+    <t>mutant_dragon.spr</t>
+  </si>
+  <si>
+    <t>see_otter.spr</t>
+  </si>
+  <si>
+    <t>gryphon.spr</t>
+  </si>
+  <si>
+    <t>medusa.spr</t>
+  </si>
+  <si>
+    <t>Demon,Strong</t>
+  </si>
+  <si>
+    <t>neraid.spr</t>
+  </si>
+  <si>
+    <t>tri_joint.spr</t>
+  </si>
+  <si>
+    <t>stalactic_golem.spr</t>
+  </si>
+  <si>
+    <t>megalith.spr</t>
+  </si>
+  <si>
+    <t>megalodon.spr</t>
+  </si>
+  <si>
+    <t>tao_gunka.spr</t>
+  </si>
+  <si>
+    <t>Demon,Golem,WorldBoss</t>
   </si>
 </sst>
 </file>
@@ -3404,13 +3572,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{811A97A5-94A7-4FFA-A162-65D076B52481}">
-  <dimension ref="A1:AI268"/>
+  <dimension ref="A1:AI286"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <pane xSplit="2" ySplit="1" topLeftCell="C236" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="1" topLeftCell="C266" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="AC268" sqref="AC268"/>
+      <selection pane="bottomRight" activeCell="AC287" sqref="AC287"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
@@ -3440,7 +3608,7 @@
     <col min="26" max="26" width="10.4609375" bestFit="1" customWidth="1"/>
     <col min="27" max="27" width="10.84375" bestFit="1" customWidth="1"/>
     <col min="28" max="28" width="7.23046875" bestFit="1" customWidth="1"/>
-    <col min="29" max="29" width="18.3046875" customWidth="1"/>
+    <col min="29" max="29" width="22.4609375" bestFit="1" customWidth="1"/>
     <col min="30" max="30" width="18.765625" bestFit="1" customWidth="1"/>
     <col min="31" max="31" width="17.15234375" customWidth="1"/>
     <col min="32" max="32" width="22.84375" bestFit="1" customWidth="1"/>
@@ -32122,6 +32290,1932 @@
         <v>0.5</v>
       </c>
       <c r="AI268">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="269" spans="1:35" x14ac:dyDescent="0.4">
+      <c r="A269">
+        <v>4266</v>
+      </c>
+      <c r="B269" t="s">
+        <v>989</v>
+      </c>
+      <c r="C269" t="s">
+        <v>1007</v>
+      </c>
+      <c r="D269">
+        <v>15</v>
+      </c>
+      <c r="E269">
+        <v>100</v>
+      </c>
+      <c r="F269">
+        <v>100</v>
+      </c>
+      <c r="G269">
+        <v>100</v>
+      </c>
+      <c r="H269">
+        <v>100</v>
+      </c>
+      <c r="I269">
+        <v>100</v>
+      </c>
+      <c r="J269">
+        <v>100</v>
+      </c>
+      <c r="K269">
+        <v>100</v>
+      </c>
+      <c r="L269">
+        <v>100</v>
+      </c>
+      <c r="M269">
+        <v>10</v>
+      </c>
+      <c r="N269">
+        <v>1</v>
+      </c>
+      <c r="O269">
+        <v>100</v>
+      </c>
+      <c r="P269">
+        <v>100</v>
+      </c>
+      <c r="Q269">
+        <v>100</v>
+      </c>
+      <c r="R269">
+        <v>100</v>
+      </c>
+      <c r="S269">
+        <v>10</v>
+      </c>
+      <c r="T269">
+        <v>12</v>
+      </c>
+      <c r="U269" t="s">
+        <v>56</v>
+      </c>
+      <c r="V269" t="s">
+        <v>392</v>
+      </c>
+      <c r="W269" t="s">
+        <v>41</v>
+      </c>
+      <c r="X269">
+        <v>864</v>
+      </c>
+      <c r="Y269">
+        <v>384</v>
+      </c>
+      <c r="Z269">
+        <v>864</v>
+      </c>
+      <c r="AA269">
+        <v>200</v>
+      </c>
+      <c r="AB269" t="s">
+        <v>42</v>
+      </c>
+      <c r="AC269" t="s">
+        <v>42</v>
+      </c>
+      <c r="AD269" t="s">
+        <v>43</v>
+      </c>
+      <c r="AE269">
+        <v>481</v>
+      </c>
+      <c r="AF269" t="s">
+        <v>1025</v>
+      </c>
+      <c r="AG269">
+        <v>0</v>
+      </c>
+      <c r="AH269">
+        <v>0.5</v>
+      </c>
+      <c r="AI269">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="270" spans="1:35" x14ac:dyDescent="0.4">
+      <c r="A270">
+        <v>4267</v>
+      </c>
+      <c r="B270" t="s">
+        <v>990</v>
+      </c>
+      <c r="C270" t="s">
+        <v>1008</v>
+      </c>
+      <c r="D270">
+        <v>42</v>
+      </c>
+      <c r="E270">
+        <v>100</v>
+      </c>
+      <c r="F270">
+        <v>100</v>
+      </c>
+      <c r="G270">
+        <v>100</v>
+      </c>
+      <c r="H270">
+        <v>100</v>
+      </c>
+      <c r="I270">
+        <v>100</v>
+      </c>
+      <c r="J270">
+        <v>100</v>
+      </c>
+      <c r="K270">
+        <v>100</v>
+      </c>
+      <c r="L270">
+        <v>100</v>
+      </c>
+      <c r="M270">
+        <v>10</v>
+      </c>
+      <c r="N270">
+        <v>1</v>
+      </c>
+      <c r="O270">
+        <v>100</v>
+      </c>
+      <c r="P270">
+        <v>100</v>
+      </c>
+      <c r="Q270">
+        <v>100</v>
+      </c>
+      <c r="R270">
+        <v>100</v>
+      </c>
+      <c r="S270">
+        <v>10</v>
+      </c>
+      <c r="T270">
+        <v>12</v>
+      </c>
+      <c r="U270" t="s">
+        <v>39</v>
+      </c>
+      <c r="V270" t="s">
+        <v>62</v>
+      </c>
+      <c r="W270" t="s">
+        <v>41</v>
+      </c>
+      <c r="X270">
+        <v>1100</v>
+      </c>
+      <c r="Y270">
+        <v>480</v>
+      </c>
+      <c r="Z270">
+        <v>900</v>
+      </c>
+      <c r="AA270">
+        <v>200</v>
+      </c>
+      <c r="AB270" t="s">
+        <v>42</v>
+      </c>
+      <c r="AC270" t="s">
+        <v>42</v>
+      </c>
+      <c r="AD270" t="s">
+        <v>43</v>
+      </c>
+      <c r="AE270">
+        <v>558</v>
+      </c>
+      <c r="AF270" t="s">
+        <v>1026</v>
+      </c>
+      <c r="AG270">
+        <v>0</v>
+      </c>
+      <c r="AH270">
+        <v>0.5</v>
+      </c>
+      <c r="AI270">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="271" spans="1:35" x14ac:dyDescent="0.4">
+      <c r="A271">
+        <v>4268</v>
+      </c>
+      <c r="B271" t="s">
+        <v>991</v>
+      </c>
+      <c r="C271" t="s">
+        <v>1009</v>
+      </c>
+      <c r="D271">
+        <v>18</v>
+      </c>
+      <c r="E271">
+        <v>100</v>
+      </c>
+      <c r="F271">
+        <v>100</v>
+      </c>
+      <c r="G271">
+        <v>100</v>
+      </c>
+      <c r="H271">
+        <v>100</v>
+      </c>
+      <c r="I271">
+        <v>100</v>
+      </c>
+      <c r="J271">
+        <v>100</v>
+      </c>
+      <c r="K271">
+        <v>100</v>
+      </c>
+      <c r="L271">
+        <v>100</v>
+      </c>
+      <c r="M271">
+        <v>10</v>
+      </c>
+      <c r="N271">
+        <v>1</v>
+      </c>
+      <c r="O271">
+        <v>100</v>
+      </c>
+      <c r="P271">
+        <v>100</v>
+      </c>
+      <c r="Q271">
+        <v>100</v>
+      </c>
+      <c r="R271">
+        <v>100</v>
+      </c>
+      <c r="S271">
+        <v>10</v>
+      </c>
+      <c r="T271">
+        <v>12</v>
+      </c>
+      <c r="U271" t="s">
+        <v>56</v>
+      </c>
+      <c r="V271" t="s">
+        <v>392</v>
+      </c>
+      <c r="W271" t="s">
+        <v>58</v>
+      </c>
+      <c r="X271">
+        <v>1264</v>
+      </c>
+      <c r="Y271">
+        <v>216</v>
+      </c>
+      <c r="Z271">
+        <v>864</v>
+      </c>
+      <c r="AA271">
+        <v>400</v>
+      </c>
+      <c r="AB271" t="s">
+        <v>42</v>
+      </c>
+      <c r="AC271" t="s">
+        <v>42</v>
+      </c>
+      <c r="AD271" t="s">
+        <v>43</v>
+      </c>
+      <c r="AE271">
+        <v>350</v>
+      </c>
+      <c r="AF271" t="s">
+        <v>1027</v>
+      </c>
+      <c r="AG271">
+        <v>0</v>
+      </c>
+      <c r="AH271">
+        <v>0.5</v>
+      </c>
+      <c r="AI271">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="272" spans="1:35" x14ac:dyDescent="0.4">
+      <c r="A272">
+        <v>4269</v>
+      </c>
+      <c r="B272" t="s">
+        <v>992</v>
+      </c>
+      <c r="C272" t="s">
+        <v>1010</v>
+      </c>
+      <c r="D272">
+        <v>20</v>
+      </c>
+      <c r="E272">
+        <v>100</v>
+      </c>
+      <c r="F272">
+        <v>100</v>
+      </c>
+      <c r="G272">
+        <v>100</v>
+      </c>
+      <c r="H272">
+        <v>100</v>
+      </c>
+      <c r="I272">
+        <v>100</v>
+      </c>
+      <c r="J272">
+        <v>100</v>
+      </c>
+      <c r="K272">
+        <v>100</v>
+      </c>
+      <c r="L272">
+        <v>100</v>
+      </c>
+      <c r="M272">
+        <v>10</v>
+      </c>
+      <c r="N272">
+        <v>1</v>
+      </c>
+      <c r="O272">
+        <v>100</v>
+      </c>
+      <c r="P272">
+        <v>100</v>
+      </c>
+      <c r="Q272">
+        <v>100</v>
+      </c>
+      <c r="R272">
+        <v>100</v>
+      </c>
+      <c r="S272">
+        <v>7</v>
+      </c>
+      <c r="T272">
+        <v>12</v>
+      </c>
+      <c r="U272" t="s">
+        <v>56</v>
+      </c>
+      <c r="V272" t="s">
+        <v>392</v>
+      </c>
+      <c r="W272" t="s">
+        <v>41</v>
+      </c>
+      <c r="X272">
+        <v>992</v>
+      </c>
+      <c r="Y272">
+        <v>360</v>
+      </c>
+      <c r="Z272">
+        <v>792</v>
+      </c>
+      <c r="AA272">
+        <v>200</v>
+      </c>
+      <c r="AB272" t="s">
+        <v>42</v>
+      </c>
+      <c r="AC272" t="s">
+        <v>42</v>
+      </c>
+      <c r="AD272" t="s">
+        <v>43</v>
+      </c>
+      <c r="AE272">
+        <v>296</v>
+      </c>
+      <c r="AF272" t="s">
+        <v>1028</v>
+      </c>
+      <c r="AG272">
+        <v>0</v>
+      </c>
+      <c r="AH272">
+        <v>0.5</v>
+      </c>
+      <c r="AI272">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="273" spans="1:35" x14ac:dyDescent="0.4">
+      <c r="A273">
+        <v>4270</v>
+      </c>
+      <c r="B273" t="s">
+        <v>993</v>
+      </c>
+      <c r="C273" t="s">
+        <v>1011</v>
+      </c>
+      <c r="D273">
+        <v>21</v>
+      </c>
+      <c r="E273">
+        <v>100</v>
+      </c>
+      <c r="F273">
+        <v>100</v>
+      </c>
+      <c r="G273">
+        <v>100</v>
+      </c>
+      <c r="H273">
+        <v>100</v>
+      </c>
+      <c r="I273">
+        <v>100</v>
+      </c>
+      <c r="J273">
+        <v>100</v>
+      </c>
+      <c r="K273">
+        <v>100</v>
+      </c>
+      <c r="L273">
+        <v>100</v>
+      </c>
+      <c r="M273">
+        <v>10</v>
+      </c>
+      <c r="N273">
+        <v>1</v>
+      </c>
+      <c r="O273">
+        <v>100</v>
+      </c>
+      <c r="P273">
+        <v>100</v>
+      </c>
+      <c r="Q273">
+        <v>100</v>
+      </c>
+      <c r="R273">
+        <v>100</v>
+      </c>
+      <c r="S273">
+        <v>10</v>
+      </c>
+      <c r="T273">
+        <v>12</v>
+      </c>
+      <c r="U273" t="s">
+        <v>56</v>
+      </c>
+      <c r="V273" t="s">
+        <v>62</v>
+      </c>
+      <c r="W273" t="s">
+        <v>81</v>
+      </c>
+      <c r="X273">
+        <v>1000</v>
+      </c>
+      <c r="Y273">
+        <v>384</v>
+      </c>
+      <c r="Z273">
+        <v>900</v>
+      </c>
+      <c r="AA273">
+        <v>200</v>
+      </c>
+      <c r="AB273" t="s">
+        <v>42</v>
+      </c>
+      <c r="AC273" t="s">
+        <v>42</v>
+      </c>
+      <c r="AD273" t="s">
+        <v>72</v>
+      </c>
+      <c r="AE273">
+        <v>259</v>
+      </c>
+      <c r="AF273" t="s">
+        <v>1029</v>
+      </c>
+      <c r="AG273">
+        <v>0</v>
+      </c>
+      <c r="AH273">
+        <v>0.5</v>
+      </c>
+      <c r="AI273">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="274" spans="1:35" x14ac:dyDescent="0.4">
+      <c r="A274">
+        <v>4271</v>
+      </c>
+      <c r="B274" t="s">
+        <v>994</v>
+      </c>
+      <c r="C274" t="s">
+        <v>1012</v>
+      </c>
+      <c r="D274">
+        <v>61</v>
+      </c>
+      <c r="E274">
+        <v>100</v>
+      </c>
+      <c r="F274">
+        <v>100</v>
+      </c>
+      <c r="G274">
+        <v>100</v>
+      </c>
+      <c r="H274">
+        <v>100</v>
+      </c>
+      <c r="I274">
+        <v>100</v>
+      </c>
+      <c r="J274">
+        <v>100</v>
+      </c>
+      <c r="K274">
+        <v>100</v>
+      </c>
+      <c r="L274">
+        <v>100</v>
+      </c>
+      <c r="M274">
+        <v>10</v>
+      </c>
+      <c r="N274">
+        <v>1</v>
+      </c>
+      <c r="O274">
+        <v>100</v>
+      </c>
+      <c r="P274">
+        <v>100</v>
+      </c>
+      <c r="Q274">
+        <v>100</v>
+      </c>
+      <c r="R274">
+        <v>100</v>
+      </c>
+      <c r="S274">
+        <v>10</v>
+      </c>
+      <c r="T274">
+        <v>12</v>
+      </c>
+      <c r="U274" t="s">
+        <v>39</v>
+      </c>
+      <c r="V274" t="s">
+        <v>172</v>
+      </c>
+      <c r="W274" t="s">
+        <v>51</v>
+      </c>
+      <c r="X274">
+        <v>1100</v>
+      </c>
+      <c r="Y274">
+        <v>580</v>
+      </c>
+      <c r="Z274">
+        <v>560</v>
+      </c>
+      <c r="AA274">
+        <v>250</v>
+      </c>
+      <c r="AB274" t="s">
+        <v>42</v>
+      </c>
+      <c r="AC274" t="s">
+        <v>18</v>
+      </c>
+      <c r="AD274" t="s">
+        <v>72</v>
+      </c>
+      <c r="AE274">
+        <v>700</v>
+      </c>
+      <c r="AF274" t="s">
+        <v>1030</v>
+      </c>
+      <c r="AG274">
+        <v>0</v>
+      </c>
+      <c r="AH274">
+        <v>0.5</v>
+      </c>
+      <c r="AI274">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="275" spans="1:35" x14ac:dyDescent="0.4">
+      <c r="A275">
+        <v>4272</v>
+      </c>
+      <c r="B275" t="s">
+        <v>995</v>
+      </c>
+      <c r="C275" t="s">
+        <v>1020</v>
+      </c>
+      <c r="D275">
+        <v>63</v>
+      </c>
+      <c r="E275">
+        <v>100</v>
+      </c>
+      <c r="F275">
+        <v>100</v>
+      </c>
+      <c r="G275">
+        <v>100</v>
+      </c>
+      <c r="H275">
+        <v>100</v>
+      </c>
+      <c r="I275">
+        <v>100</v>
+      </c>
+      <c r="J275">
+        <v>100</v>
+      </c>
+      <c r="K275">
+        <v>100</v>
+      </c>
+      <c r="L275">
+        <v>100</v>
+      </c>
+      <c r="M275">
+        <v>10</v>
+      </c>
+      <c r="N275">
+        <v>1</v>
+      </c>
+      <c r="O275">
+        <v>100</v>
+      </c>
+      <c r="P275">
+        <v>100</v>
+      </c>
+      <c r="Q275">
+        <v>100</v>
+      </c>
+      <c r="R275">
+        <v>100</v>
+      </c>
+      <c r="S275">
+        <v>10</v>
+      </c>
+      <c r="T275">
+        <v>12</v>
+      </c>
+      <c r="U275" t="s">
+        <v>39</v>
+      </c>
+      <c r="V275" t="s">
+        <v>62</v>
+      </c>
+      <c r="W275" t="s">
+        <v>41</v>
+      </c>
+      <c r="X275">
+        <v>1612</v>
+      </c>
+      <c r="Y275">
+        <v>583</v>
+      </c>
+      <c r="Z275">
+        <v>622</v>
+      </c>
+      <c r="AA275">
+        <v>200</v>
+      </c>
+      <c r="AB275" t="s">
+        <v>42</v>
+      </c>
+      <c r="AC275" t="s">
+        <v>956</v>
+      </c>
+      <c r="AD275" t="s">
+        <v>72</v>
+      </c>
+      <c r="AE275">
+        <v>600</v>
+      </c>
+      <c r="AF275" t="s">
+        <v>1031</v>
+      </c>
+      <c r="AG275">
+        <v>0</v>
+      </c>
+      <c r="AH275">
+        <v>0.5</v>
+      </c>
+      <c r="AI275">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="276" spans="1:35" x14ac:dyDescent="0.4">
+      <c r="A276">
+        <v>4273</v>
+      </c>
+      <c r="B276" t="s">
+        <v>996</v>
+      </c>
+      <c r="C276" t="s">
+        <v>1013</v>
+      </c>
+      <c r="D276">
+        <v>61</v>
+      </c>
+      <c r="E276">
+        <v>100</v>
+      </c>
+      <c r="F276">
+        <v>100</v>
+      </c>
+      <c r="G276">
+        <v>100</v>
+      </c>
+      <c r="H276">
+        <v>100</v>
+      </c>
+      <c r="I276">
+        <v>100</v>
+      </c>
+      <c r="J276">
+        <v>100</v>
+      </c>
+      <c r="K276">
+        <v>100</v>
+      </c>
+      <c r="L276">
+        <v>100</v>
+      </c>
+      <c r="M276">
+        <v>10</v>
+      </c>
+      <c r="N276">
+        <v>1</v>
+      </c>
+      <c r="O276">
+        <v>100</v>
+      </c>
+      <c r="P276">
+        <v>100</v>
+      </c>
+      <c r="Q276">
+        <v>100</v>
+      </c>
+      <c r="R276">
+        <v>100</v>
+      </c>
+      <c r="S276">
+        <v>10</v>
+      </c>
+      <c r="T276">
+        <v>12</v>
+      </c>
+      <c r="U276" t="s">
+        <v>56</v>
+      </c>
+      <c r="V276" t="s">
+        <v>62</v>
+      </c>
+      <c r="W276" t="s">
+        <v>58</v>
+      </c>
+      <c r="X276">
+        <v>1430</v>
+      </c>
+      <c r="Y276">
+        <v>1080</v>
+      </c>
+      <c r="Z276">
+        <v>1080</v>
+      </c>
+      <c r="AA276">
+        <v>165</v>
+      </c>
+      <c r="AB276" t="s">
+        <v>42</v>
+      </c>
+      <c r="AC276" t="s">
+        <v>42</v>
+      </c>
+      <c r="AD276" t="s">
+        <v>43</v>
+      </c>
+      <c r="AE276">
+        <v>496</v>
+      </c>
+      <c r="AF276" t="s">
+        <v>1032</v>
+      </c>
+      <c r="AG276">
+        <v>0</v>
+      </c>
+      <c r="AH276">
+        <v>0.5</v>
+      </c>
+      <c r="AI276">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="277" spans="1:35" x14ac:dyDescent="0.4">
+      <c r="A277">
+        <v>4274</v>
+      </c>
+      <c r="B277" t="s">
+        <v>997</v>
+      </c>
+      <c r="C277" t="s">
+        <v>1019</v>
+      </c>
+      <c r="D277">
+        <v>65</v>
+      </c>
+      <c r="E277">
+        <v>100</v>
+      </c>
+      <c r="F277">
+        <v>100</v>
+      </c>
+      <c r="G277">
+        <v>100</v>
+      </c>
+      <c r="H277">
+        <v>100</v>
+      </c>
+      <c r="I277">
+        <v>100</v>
+      </c>
+      <c r="J277">
+        <v>100</v>
+      </c>
+      <c r="K277">
+        <v>100</v>
+      </c>
+      <c r="L277">
+        <v>100</v>
+      </c>
+      <c r="M277">
+        <v>10</v>
+      </c>
+      <c r="N277">
+        <v>4</v>
+      </c>
+      <c r="O277">
+        <v>100</v>
+      </c>
+      <c r="P277">
+        <v>100</v>
+      </c>
+      <c r="Q277">
+        <v>100</v>
+      </c>
+      <c r="R277">
+        <v>100</v>
+      </c>
+      <c r="S277">
+        <v>10</v>
+      </c>
+      <c r="T277">
+        <v>12</v>
+      </c>
+      <c r="U277" t="s">
+        <v>156</v>
+      </c>
+      <c r="V277" t="s">
+        <v>354</v>
+      </c>
+      <c r="W277" t="s">
+        <v>246</v>
+      </c>
+      <c r="X277">
+        <v>1280</v>
+      </c>
+      <c r="Y277">
+        <v>240</v>
+      </c>
+      <c r="Z277">
+        <v>1080</v>
+      </c>
+      <c r="AA277">
+        <v>250</v>
+      </c>
+      <c r="AB277" t="s">
+        <v>71</v>
+      </c>
+      <c r="AC277" t="s">
+        <v>753</v>
+      </c>
+      <c r="AD277" t="s">
+        <v>43</v>
+      </c>
+      <c r="AE277">
+        <v>925</v>
+      </c>
+      <c r="AF277" t="s">
+        <v>1033</v>
+      </c>
+      <c r="AG277">
+        <v>0</v>
+      </c>
+      <c r="AH277">
+        <v>0.5</v>
+      </c>
+      <c r="AI277">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="278" spans="1:35" x14ac:dyDescent="0.4">
+      <c r="A278">
+        <v>4275</v>
+      </c>
+      <c r="B278" t="s">
+        <v>998</v>
+      </c>
+      <c r="C278" t="s">
+        <v>1021</v>
+      </c>
+      <c r="D278">
+        <v>59</v>
+      </c>
+      <c r="E278">
+        <v>100</v>
+      </c>
+      <c r="F278">
+        <v>100</v>
+      </c>
+      <c r="G278">
+        <v>100</v>
+      </c>
+      <c r="H278">
+        <v>100</v>
+      </c>
+      <c r="I278">
+        <v>100</v>
+      </c>
+      <c r="J278">
+        <v>100</v>
+      </c>
+      <c r="K278">
+        <v>100</v>
+      </c>
+      <c r="L278">
+        <v>100</v>
+      </c>
+      <c r="M278">
+        <v>10</v>
+      </c>
+      <c r="N278">
+        <v>1</v>
+      </c>
+      <c r="O278">
+        <v>100</v>
+      </c>
+      <c r="P278">
+        <v>100</v>
+      </c>
+      <c r="Q278">
+        <v>100</v>
+      </c>
+      <c r="R278">
+        <v>100</v>
+      </c>
+      <c r="S278">
+        <v>10</v>
+      </c>
+      <c r="T278">
+        <v>12</v>
+      </c>
+      <c r="U278" t="s">
+        <v>39</v>
+      </c>
+      <c r="V278" t="s">
+        <v>62</v>
+      </c>
+      <c r="W278" t="s">
+        <v>496</v>
+      </c>
+      <c r="X278">
+        <v>1132</v>
+      </c>
+      <c r="Y278">
+        <v>532</v>
+      </c>
+      <c r="Z278">
+        <v>583</v>
+      </c>
+      <c r="AA278">
+        <v>190</v>
+      </c>
+      <c r="AB278" t="s">
+        <v>42</v>
+      </c>
+      <c r="AC278" t="s">
+        <v>956</v>
+      </c>
+      <c r="AD278" t="s">
+        <v>72</v>
+      </c>
+      <c r="AE278">
+        <v>450</v>
+      </c>
+      <c r="AF278" t="s">
+        <v>1034</v>
+      </c>
+      <c r="AG278">
+        <v>0</v>
+      </c>
+      <c r="AH278">
+        <v>0.5</v>
+      </c>
+      <c r="AI278">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="279" spans="1:35" x14ac:dyDescent="0.4">
+      <c r="A279">
+        <v>4276</v>
+      </c>
+      <c r="B279" t="s">
+        <v>999</v>
+      </c>
+      <c r="C279" t="s">
+        <v>1014</v>
+      </c>
+      <c r="D279">
+        <v>72</v>
+      </c>
+      <c r="E279">
+        <v>100</v>
+      </c>
+      <c r="F279">
+        <v>100</v>
+      </c>
+      <c r="G279">
+        <v>100</v>
+      </c>
+      <c r="H279">
+        <v>100</v>
+      </c>
+      <c r="I279">
+        <v>100</v>
+      </c>
+      <c r="J279">
+        <v>100</v>
+      </c>
+      <c r="K279">
+        <v>100</v>
+      </c>
+      <c r="L279">
+        <v>100</v>
+      </c>
+      <c r="M279">
+        <v>10</v>
+      </c>
+      <c r="N279">
+        <v>1</v>
+      </c>
+      <c r="O279">
+        <v>100</v>
+      </c>
+      <c r="P279">
+        <v>100</v>
+      </c>
+      <c r="Q279">
+        <v>100</v>
+      </c>
+      <c r="R279">
+        <v>100</v>
+      </c>
+      <c r="S279">
+        <v>10</v>
+      </c>
+      <c r="T279">
+        <v>12</v>
+      </c>
+      <c r="U279" t="s">
+        <v>156</v>
+      </c>
+      <c r="V279" t="s">
+        <v>62</v>
+      </c>
+      <c r="W279" t="s">
+        <v>373</v>
+      </c>
+      <c r="X279">
+        <v>704</v>
+      </c>
+      <c r="Y279">
+        <v>432</v>
+      </c>
+      <c r="Z279">
+        <v>504</v>
+      </c>
+      <c r="AA279">
+        <v>100</v>
+      </c>
+      <c r="AB279" t="s">
+        <v>71</v>
+      </c>
+      <c r="AC279" t="s">
+        <v>753</v>
+      </c>
+      <c r="AD279" t="s">
+        <v>72</v>
+      </c>
+      <c r="AE279">
+        <v>296</v>
+      </c>
+      <c r="AF279" t="s">
+        <v>1035</v>
+      </c>
+      <c r="AG279">
+        <v>0</v>
+      </c>
+      <c r="AH279">
+        <v>0.5</v>
+      </c>
+      <c r="AI279">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="280" spans="1:35" x14ac:dyDescent="0.4">
+      <c r="A280">
+        <v>4277</v>
+      </c>
+      <c r="B280" t="s">
+        <v>1000</v>
+      </c>
+      <c r="C280" t="s">
+        <v>1015</v>
+      </c>
+      <c r="D280">
+        <v>79</v>
+      </c>
+      <c r="E280">
+        <v>100</v>
+      </c>
+      <c r="F280">
+        <v>100</v>
+      </c>
+      <c r="G280">
+        <v>100</v>
+      </c>
+      <c r="H280">
+        <v>100</v>
+      </c>
+      <c r="I280">
+        <v>100</v>
+      </c>
+      <c r="J280">
+        <v>100</v>
+      </c>
+      <c r="K280">
+        <v>100</v>
+      </c>
+      <c r="L280">
+        <v>100</v>
+      </c>
+      <c r="M280">
+        <v>10</v>
+      </c>
+      <c r="N280">
+        <v>1</v>
+      </c>
+      <c r="O280">
+        <v>100</v>
+      </c>
+      <c r="P280">
+        <v>100</v>
+      </c>
+      <c r="Q280">
+        <v>100</v>
+      </c>
+      <c r="R280">
+        <v>100</v>
+      </c>
+      <c r="S280">
+        <v>10</v>
+      </c>
+      <c r="T280">
+        <v>12</v>
+      </c>
+      <c r="U280" t="s">
+        <v>39</v>
+      </c>
+      <c r="V280" t="s">
+        <v>76</v>
+      </c>
+      <c r="W280" t="s">
+        <v>598</v>
+      </c>
+      <c r="X280">
+        <v>1720</v>
+      </c>
+      <c r="Y280">
+        <v>360</v>
+      </c>
+      <c r="Z280">
+        <v>1320</v>
+      </c>
+      <c r="AA280">
+        <v>180</v>
+      </c>
+      <c r="AB280" t="s">
+        <v>42</v>
+      </c>
+      <c r="AC280" t="s">
+        <v>1037</v>
+      </c>
+      <c r="AD280" t="s">
+        <v>72</v>
+      </c>
+      <c r="AE280">
+        <v>1000</v>
+      </c>
+      <c r="AF280" t="s">
+        <v>1036</v>
+      </c>
+      <c r="AG280">
+        <v>0</v>
+      </c>
+      <c r="AH280">
+        <v>0.5</v>
+      </c>
+      <c r="AI280">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="281" spans="1:35" x14ac:dyDescent="0.4">
+      <c r="A281">
+        <v>4278</v>
+      </c>
+      <c r="B281" t="s">
+        <v>1001</v>
+      </c>
+      <c r="C281" t="s">
+        <v>1016</v>
+      </c>
+      <c r="D281">
+        <v>40</v>
+      </c>
+      <c r="E281">
+        <v>100</v>
+      </c>
+      <c r="F281">
+        <v>100</v>
+      </c>
+      <c r="G281">
+        <v>100</v>
+      </c>
+      <c r="H281">
+        <v>100</v>
+      </c>
+      <c r="I281">
+        <v>100</v>
+      </c>
+      <c r="J281">
+        <v>100</v>
+      </c>
+      <c r="K281">
+        <v>100</v>
+      </c>
+      <c r="L281">
+        <v>100</v>
+      </c>
+      <c r="M281">
+        <v>10</v>
+      </c>
+      <c r="N281">
+        <v>1</v>
+      </c>
+      <c r="O281">
+        <v>100</v>
+      </c>
+      <c r="P281">
+        <v>100</v>
+      </c>
+      <c r="Q281">
+        <v>100</v>
+      </c>
+      <c r="R281">
+        <v>100</v>
+      </c>
+      <c r="S281">
+        <v>10</v>
+      </c>
+      <c r="T281">
+        <v>12</v>
+      </c>
+      <c r="U281" t="s">
+        <v>56</v>
+      </c>
+      <c r="V281" t="s">
+        <v>62</v>
+      </c>
+      <c r="W281" t="s">
+        <v>58</v>
+      </c>
+      <c r="X281">
+        <v>776</v>
+      </c>
+      <c r="Y281">
+        <v>288</v>
+      </c>
+      <c r="Z281">
+        <v>576</v>
+      </c>
+      <c r="AA281">
+        <v>200</v>
+      </c>
+      <c r="AB281" t="s">
+        <v>42</v>
+      </c>
+      <c r="AC281" t="s">
+        <v>42</v>
+      </c>
+      <c r="AD281" t="s">
+        <v>72</v>
+      </c>
+      <c r="AE281">
+        <v>400</v>
+      </c>
+      <c r="AF281" t="s">
+        <v>1038</v>
+      </c>
+      <c r="AG281">
+        <v>0</v>
+      </c>
+      <c r="AH281">
+        <v>0.5</v>
+      </c>
+      <c r="AI281">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="282" spans="1:35" x14ac:dyDescent="0.4">
+      <c r="A282">
+        <v>4279</v>
+      </c>
+      <c r="B282" t="s">
+        <v>1002</v>
+      </c>
+      <c r="C282" t="s">
+        <v>1022</v>
+      </c>
+      <c r="D282">
+        <v>32</v>
+      </c>
+      <c r="E282">
+        <v>100</v>
+      </c>
+      <c r="F282">
+        <v>100</v>
+      </c>
+      <c r="G282">
+        <v>100</v>
+      </c>
+      <c r="H282">
+        <v>100</v>
+      </c>
+      <c r="I282">
+        <v>100</v>
+      </c>
+      <c r="J282">
+        <v>100</v>
+      </c>
+      <c r="K282">
+        <v>100</v>
+      </c>
+      <c r="L282">
+        <v>100</v>
+      </c>
+      <c r="M282">
+        <v>10</v>
+      </c>
+      <c r="N282">
+        <v>1</v>
+      </c>
+      <c r="O282">
+        <v>100</v>
+      </c>
+      <c r="P282">
+        <v>100</v>
+      </c>
+      <c r="Q282">
+        <v>100</v>
+      </c>
+      <c r="R282">
+        <v>100</v>
+      </c>
+      <c r="S282">
+        <v>10</v>
+      </c>
+      <c r="T282">
+        <v>12</v>
+      </c>
+      <c r="U282" t="s">
+        <v>56</v>
+      </c>
+      <c r="V282" t="s">
+        <v>57</v>
+      </c>
+      <c r="W282" t="s">
+        <v>58</v>
+      </c>
+      <c r="X282">
+        <v>860</v>
+      </c>
+      <c r="Y282">
+        <v>624</v>
+      </c>
+      <c r="Z282">
+        <v>660</v>
+      </c>
+      <c r="AA282">
+        <v>200</v>
+      </c>
+      <c r="AB282" t="s">
+        <v>42</v>
+      </c>
+      <c r="AC282" t="s">
+        <v>57</v>
+      </c>
+      <c r="AD282" t="s">
+        <v>43</v>
+      </c>
+      <c r="AE282">
+        <v>682</v>
+      </c>
+      <c r="AF282" t="s">
+        <v>1039</v>
+      </c>
+      <c r="AG282">
+        <v>0</v>
+      </c>
+      <c r="AH282">
+        <v>0.5</v>
+      </c>
+      <c r="AI282">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="283" spans="1:35" x14ac:dyDescent="0.4">
+      <c r="A283">
+        <v>4280</v>
+      </c>
+      <c r="B283" t="s">
+        <v>1003</v>
+      </c>
+      <c r="C283" t="s">
+        <v>1023</v>
+      </c>
+      <c r="D283">
+        <v>60</v>
+      </c>
+      <c r="E283">
+        <v>100</v>
+      </c>
+      <c r="F283">
+        <v>100</v>
+      </c>
+      <c r="G283">
+        <v>100</v>
+      </c>
+      <c r="H283">
+        <v>100</v>
+      </c>
+      <c r="I283">
+        <v>100</v>
+      </c>
+      <c r="J283">
+        <v>100</v>
+      </c>
+      <c r="K283">
+        <v>100</v>
+      </c>
+      <c r="L283">
+        <v>100</v>
+      </c>
+      <c r="M283">
+        <v>10</v>
+      </c>
+      <c r="N283">
+        <v>1</v>
+      </c>
+      <c r="O283">
+        <v>100</v>
+      </c>
+      <c r="P283">
+        <v>100</v>
+      </c>
+      <c r="Q283">
+        <v>100</v>
+      </c>
+      <c r="R283">
+        <v>100</v>
+      </c>
+      <c r="S283">
+        <v>10</v>
+      </c>
+      <c r="T283">
+        <v>12</v>
+      </c>
+      <c r="U283" t="s">
+        <v>156</v>
+      </c>
+      <c r="V283" t="s">
+        <v>50</v>
+      </c>
+      <c r="W283" t="s">
+        <v>541</v>
+      </c>
+      <c r="X283">
+        <v>1264</v>
+      </c>
+      <c r="Y283">
+        <v>288</v>
+      </c>
+      <c r="Z283">
+        <v>864</v>
+      </c>
+      <c r="AA283">
+        <v>200</v>
+      </c>
+      <c r="AB283" t="s">
+        <v>42</v>
+      </c>
+      <c r="AC283" t="s">
+        <v>302</v>
+      </c>
+      <c r="AD283" t="s">
+        <v>43</v>
+      </c>
+      <c r="AE283">
+        <v>900</v>
+      </c>
+      <c r="AF283" t="s">
+        <v>1040</v>
+      </c>
+      <c r="AG283">
+        <v>0</v>
+      </c>
+      <c r="AH283">
+        <v>0.5</v>
+      </c>
+      <c r="AI283">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="284" spans="1:35" x14ac:dyDescent="0.4">
+      <c r="A284">
+        <v>4281</v>
+      </c>
+      <c r="B284" t="s">
+        <v>1004</v>
+      </c>
+      <c r="C284" t="s">
+        <v>1017</v>
+      </c>
+      <c r="D284">
+        <v>24</v>
+      </c>
+      <c r="E284">
+        <v>100</v>
+      </c>
+      <c r="F284">
+        <v>100</v>
+      </c>
+      <c r="G284">
+        <v>100</v>
+      </c>
+      <c r="H284">
+        <v>100</v>
+      </c>
+      <c r="I284">
+        <v>100</v>
+      </c>
+      <c r="J284">
+        <v>100</v>
+      </c>
+      <c r="K284">
+        <v>100</v>
+      </c>
+      <c r="L284">
+        <v>100</v>
+      </c>
+      <c r="M284">
+        <v>10</v>
+      </c>
+      <c r="N284">
+        <v>1</v>
+      </c>
+      <c r="O284">
+        <v>100</v>
+      </c>
+      <c r="P284">
+        <v>100</v>
+      </c>
+      <c r="Q284">
+        <v>100</v>
+      </c>
+      <c r="R284">
+        <v>100</v>
+      </c>
+      <c r="S284">
+        <v>10</v>
+      </c>
+      <c r="T284">
+        <v>12</v>
+      </c>
+      <c r="U284" t="s">
+        <v>39</v>
+      </c>
+      <c r="V284" t="s">
+        <v>450</v>
+      </c>
+      <c r="W284" t="s">
+        <v>458</v>
+      </c>
+      <c r="X284">
+        <v>2492</v>
+      </c>
+      <c r="Y284">
+        <v>432</v>
+      </c>
+      <c r="Z284">
+        <v>792</v>
+      </c>
+      <c r="AA284">
+        <v>200</v>
+      </c>
+      <c r="AB284" t="s">
+        <v>42</v>
+      </c>
+      <c r="AC284" t="s">
+        <v>450</v>
+      </c>
+      <c r="AD284" t="s">
+        <v>43</v>
+      </c>
+      <c r="AE284">
+        <v>725</v>
+      </c>
+      <c r="AF284" t="s">
+        <v>1042</v>
+      </c>
+      <c r="AG284">
+        <v>0</v>
+      </c>
+      <c r="AH284">
+        <v>0.5</v>
+      </c>
+      <c r="AI284">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="285" spans="1:35" x14ac:dyDescent="0.4">
+      <c r="A285">
+        <v>4282</v>
+      </c>
+      <c r="B285" t="s">
+        <v>1005</v>
+      </c>
+      <c r="C285" t="s">
+        <v>1018</v>
+      </c>
+      <c r="D285">
+        <v>45</v>
+      </c>
+      <c r="E285">
+        <v>100</v>
+      </c>
+      <c r="F285">
+        <v>100</v>
+      </c>
+      <c r="G285">
+        <v>100</v>
+      </c>
+      <c r="H285">
+        <v>100</v>
+      </c>
+      <c r="I285">
+        <v>100</v>
+      </c>
+      <c r="J285">
+        <v>100</v>
+      </c>
+      <c r="K285">
+        <v>100</v>
+      </c>
+      <c r="L285">
+        <v>100</v>
+      </c>
+      <c r="M285">
+        <v>10</v>
+      </c>
+      <c r="N285">
+        <v>9</v>
+      </c>
+      <c r="O285">
+        <v>100</v>
+      </c>
+      <c r="P285">
+        <v>100</v>
+      </c>
+      <c r="Q285">
+        <v>100</v>
+      </c>
+      <c r="R285">
+        <v>100</v>
+      </c>
+      <c r="S285">
+        <v>10</v>
+      </c>
+      <c r="T285">
+        <v>12</v>
+      </c>
+      <c r="U285" t="s">
+        <v>156</v>
+      </c>
+      <c r="V285" t="s">
+        <v>50</v>
+      </c>
+      <c r="W285" t="s">
+        <v>541</v>
+      </c>
+      <c r="X285">
+        <v>1332</v>
+      </c>
+      <c r="Y285">
+        <v>672</v>
+      </c>
+      <c r="Z285">
+        <v>1332</v>
+      </c>
+      <c r="AA285">
+        <v>200</v>
+      </c>
+      <c r="AB285" t="s">
+        <v>42</v>
+      </c>
+      <c r="AC285" t="s">
+        <v>42</v>
+      </c>
+      <c r="AD285" t="s">
+        <v>131</v>
+      </c>
+      <c r="AE285">
+        <v>962</v>
+      </c>
+      <c r="AF285" t="s">
+        <v>1041</v>
+      </c>
+      <c r="AG285">
+        <v>0</v>
+      </c>
+      <c r="AH285">
+        <v>0.5</v>
+      </c>
+      <c r="AI285">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="286" spans="1:35" x14ac:dyDescent="0.4">
+      <c r="A286">
+        <v>4283</v>
+      </c>
+      <c r="B286" t="s">
+        <v>1006</v>
+      </c>
+      <c r="C286" t="s">
+        <v>1024</v>
+      </c>
+      <c r="D286">
+        <v>70</v>
+      </c>
+      <c r="E286">
+        <v>100</v>
+      </c>
+      <c r="F286">
+        <v>100</v>
+      </c>
+      <c r="G286">
+        <v>100</v>
+      </c>
+      <c r="H286">
+        <v>100</v>
+      </c>
+      <c r="I286">
+        <v>100</v>
+      </c>
+      <c r="J286">
+        <v>100</v>
+      </c>
+      <c r="K286">
+        <v>100</v>
+      </c>
+      <c r="L286">
+        <v>100</v>
+      </c>
+      <c r="M286">
+        <v>10</v>
+      </c>
+      <c r="N286">
+        <v>2</v>
+      </c>
+      <c r="O286">
+        <v>100</v>
+      </c>
+      <c r="P286">
+        <v>100</v>
+      </c>
+      <c r="Q286">
+        <v>100</v>
+      </c>
+      <c r="R286">
+        <v>100</v>
+      </c>
+      <c r="S286">
+        <v>10</v>
+      </c>
+      <c r="T286">
+        <v>12</v>
+      </c>
+      <c r="U286" t="s">
+        <v>156</v>
+      </c>
+      <c r="V286" t="s">
+        <v>76</v>
+      </c>
+      <c r="W286" t="s">
+        <v>63</v>
+      </c>
+      <c r="X286">
+        <v>1020</v>
+      </c>
+      <c r="Y286">
+        <v>144</v>
+      </c>
+      <c r="Z286">
+        <v>288</v>
+      </c>
+      <c r="AA286">
+        <v>150</v>
+      </c>
+      <c r="AB286" t="s">
+        <v>71</v>
+      </c>
+      <c r="AC286" t="s">
+        <v>1044</v>
+      </c>
+      <c r="AD286" t="s">
+        <v>72</v>
+      </c>
+      <c r="AE286">
+        <v>400</v>
+      </c>
+      <c r="AF286" t="s">
+        <v>1043</v>
+      </c>
+      <c r="AG286">
+        <v>0</v>
+      </c>
+      <c r="AH286">
+        <v>0.5</v>
+      </c>
+      <c r="AI286">
         <v>1</v>
       </c>
     </row>
@@ -33490,11 +35584,11 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0E19C42E-4D03-4797-B846-FB5E09BB39D3}">
-  <dimension ref="A1:N19"/>
+  <dimension ref="A1:N20"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="G21" sqref="G21"/>
+      <selection pane="bottomLeft" activeCell="K15" sqref="K15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
@@ -34120,87 +36214,87 @@
     </row>
     <row r="15" spans="1:14" x14ac:dyDescent="0.4">
       <c r="A15" t="s">
-        <v>826</v>
+        <v>302</v>
       </c>
       <c r="B15">
-        <v>250</v>
+        <v>130</v>
       </c>
       <c r="C15">
-        <v>130</v>
+        <v>110</v>
       </c>
       <c r="D15">
-        <v>110</v>
+        <v>120</v>
       </c>
       <c r="E15">
-        <v>110</v>
+        <v>60</v>
       </c>
       <c r="F15">
-        <v>110</v>
+        <v>150</v>
       </c>
       <c r="G15">
-        <v>110</v>
+        <v>80</v>
       </c>
       <c r="H15">
-        <v>110</v>
+        <v>90</v>
       </c>
       <c r="I15">
-        <v>110</v>
+        <v>90</v>
       </c>
       <c r="J15">
-        <v>110</v>
+        <v>150</v>
       </c>
       <c r="K15">
-        <v>110</v>
+        <v>105</v>
       </c>
       <c r="L15">
-        <v>180</v>
+        <v>125</v>
       </c>
       <c r="M15">
-        <v>180</v>
+        <v>135</v>
       </c>
       <c r="N15">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="16" spans="1:14" x14ac:dyDescent="0.4">
       <c r="A16" t="s">
-        <v>18</v>
+        <v>826</v>
       </c>
       <c r="B16">
-        <v>350</v>
+        <v>250</v>
       </c>
       <c r="C16">
-        <v>160</v>
+        <v>130</v>
       </c>
       <c r="D16">
-        <v>120</v>
+        <v>110</v>
       </c>
       <c r="E16">
-        <v>120</v>
+        <v>110</v>
       </c>
       <c r="F16">
-        <v>120</v>
+        <v>110</v>
       </c>
       <c r="G16">
-        <v>120</v>
+        <v>110</v>
       </c>
       <c r="H16">
-        <v>120</v>
+        <v>110</v>
       </c>
       <c r="I16">
-        <v>120</v>
+        <v>110</v>
       </c>
       <c r="J16">
-        <v>120</v>
+        <v>110</v>
       </c>
       <c r="K16">
-        <v>120</v>
+        <v>110</v>
       </c>
       <c r="L16">
-        <v>300</v>
+        <v>180</v>
       </c>
       <c r="M16">
-        <v>250</v>
+        <v>180</v>
       </c>
       <c r="N16">
         <v>2</v>
@@ -34208,75 +36302,75 @@
     </row>
     <row r="17" spans="1:14" x14ac:dyDescent="0.4">
       <c r="A17" t="s">
-        <v>689</v>
+        <v>18</v>
       </c>
       <c r="B17">
-        <v>1000</v>
+        <v>350</v>
       </c>
       <c r="C17">
-        <v>175</v>
+        <v>160</v>
       </c>
       <c r="D17">
-        <v>130</v>
+        <v>120</v>
       </c>
       <c r="E17">
-        <v>130</v>
+        <v>120</v>
       </c>
       <c r="F17">
-        <v>130</v>
+        <v>120</v>
       </c>
       <c r="G17">
-        <v>130</v>
+        <v>120</v>
       </c>
       <c r="H17">
-        <v>130</v>
+        <v>120</v>
       </c>
       <c r="I17">
-        <v>130</v>
+        <v>120</v>
       </c>
       <c r="J17">
-        <v>130</v>
+        <v>120</v>
       </c>
       <c r="K17">
-        <v>130</v>
+        <v>120</v>
       </c>
       <c r="L17">
-        <v>550</v>
+        <v>300</v>
       </c>
       <c r="M17">
-        <v>450</v>
+        <v>250</v>
       </c>
       <c r="N17">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="18" spans="1:14" x14ac:dyDescent="0.4">
       <c r="A18" t="s">
-        <v>20</v>
+        <v>689</v>
       </c>
       <c r="B18">
-        <v>2000</v>
+        <v>1000</v>
       </c>
       <c r="C18">
-        <v>200</v>
+        <v>175</v>
       </c>
       <c r="D18">
-        <v>140</v>
+        <v>130</v>
       </c>
       <c r="E18">
-        <v>140</v>
+        <v>130</v>
       </c>
       <c r="F18">
-        <v>140</v>
+        <v>130</v>
       </c>
       <c r="G18">
-        <v>140</v>
+        <v>130</v>
       </c>
       <c r="H18">
-        <v>140</v>
+        <v>130</v>
       </c>
       <c r="I18">
-        <v>140</v>
+        <v>130</v>
       </c>
       <c r="J18">
         <v>130</v>
@@ -34285,56 +36379,100 @@
         <v>130</v>
       </c>
       <c r="L18">
-        <v>1200</v>
+        <v>550</v>
       </c>
       <c r="M18">
-        <v>1000</v>
+        <v>450</v>
       </c>
       <c r="N18">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="19" spans="1:14" x14ac:dyDescent="0.4">
       <c r="A19" t="s">
+        <v>20</v>
+      </c>
+      <c r="B19">
+        <v>2000</v>
+      </c>
+      <c r="C19">
+        <v>200</v>
+      </c>
+      <c r="D19">
+        <v>140</v>
+      </c>
+      <c r="E19">
+        <v>140</v>
+      </c>
+      <c r="F19">
+        <v>140</v>
+      </c>
+      <c r="G19">
+        <v>140</v>
+      </c>
+      <c r="H19">
+        <v>140</v>
+      </c>
+      <c r="I19">
+        <v>140</v>
+      </c>
+      <c r="J19">
+        <v>130</v>
+      </c>
+      <c r="K19">
+        <v>130</v>
+      </c>
+      <c r="L19">
+        <v>1200</v>
+      </c>
+      <c r="M19">
+        <v>1000</v>
+      </c>
+      <c r="N19">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="20" spans="1:14" x14ac:dyDescent="0.4">
+      <c r="A20" t="s">
         <v>19</v>
       </c>
-      <c r="B19">
+      <c r="B20">
         <v>5000</v>
       </c>
-      <c r="C19">
+      <c r="C20">
         <v>230</v>
       </c>
-      <c r="D19">
+      <c r="D20">
         <v>180</v>
       </c>
-      <c r="E19">
+      <c r="E20">
         <v>180</v>
       </c>
-      <c r="F19">
+      <c r="F20">
         <v>180</v>
       </c>
-      <c r="G19">
+      <c r="G20">
         <v>180</v>
       </c>
-      <c r="H19">
+      <c r="H20">
         <v>180</v>
       </c>
-      <c r="I19">
+      <c r="I20">
         <v>180</v>
       </c>
-      <c r="J19">
+      <c r="J20">
         <v>140</v>
       </c>
-      <c r="K19">
+      <c r="K20">
         <v>140</v>
       </c>
-      <c r="L19">
+      <c r="L20">
         <v>5000</v>
       </c>
-      <c r="M19">
+      <c r="M20">
         <v>5000</v>
       </c>
-      <c r="N19">
+      <c r="N20">
         <v>5</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Damage indicator pooling and some cast effect stuff.
</commit_message>
<xml_diff>
--- a/Other/RoStatProcessing.xlsx
+++ b/Other/RoStatProcessing.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\ProjectsSSD\RagnarokRebuildTcp\Other\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0F83316D-1843-41C7-87EF-CB415F337456}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0DEFC7A2-F64C-4130-856F-8F90FBA85FC6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2571" yWindow="2674" windowWidth="27798" windowHeight="14726" xr2:uid="{1C41742B-2950-4FF8-AA39-6557869B44EA}"/>
+    <workbookView xWindow="377" yWindow="377" windowWidth="29494" windowHeight="16594" activeTab="1" xr2:uid="{1C41742B-2950-4FF8-AA39-6557869B44EA}"/>
   </bookViews>
   <sheets>
     <sheet name="StatDef" sheetId="3" r:id="rId1"/>
@@ -48,7 +48,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2816" uniqueCount="1045">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2817" uniqueCount="1045">
   <si>
     <t>Level</t>
   </si>
@@ -3574,11 +3574,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{811A97A5-94A7-4FFA-A162-65D076B52481}">
   <dimension ref="A1:AI286"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <pane xSplit="2" ySplit="1" topLeftCell="C266" activePane="bottomRight" state="frozen"/>
+    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <pane xSplit="2" ySplit="1" topLeftCell="C154" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="AC287" sqref="AC287"/>
+      <selection pane="bottomRight" activeCell="AC173" sqref="AC173"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
@@ -5554,7 +5554,7 @@
         <v>123</v>
       </c>
       <c r="D19">
-        <v>32</v>
+        <v>19</v>
       </c>
       <c r="E19">
         <v>100</v>
@@ -9085,7 +9085,7 @@
         <v>70</v>
       </c>
       <c r="D52">
-        <v>2</v>
+        <v>10</v>
       </c>
       <c r="E52">
         <v>100</v>
@@ -12263,7 +12263,7 @@
         <v>42</v>
       </c>
       <c r="AC81" t="s">
-        <v>42</v>
+        <v>302</v>
       </c>
       <c r="AD81" t="s">
         <v>43</v>
@@ -18484,7 +18484,7 @@
         <v>0</v>
       </c>
       <c r="AH139">
-        <v>0.5</v>
+        <v>1</v>
       </c>
       <c r="AI139">
         <v>1</v>
@@ -22107,7 +22107,7 @@
         <v>42</v>
       </c>
       <c r="AC173" t="s">
-        <v>42</v>
+        <v>56</v>
       </c>
       <c r="AD173" t="s">
         <v>43</v>
@@ -22214,7 +22214,7 @@
         <v>42</v>
       </c>
       <c r="AC174" t="s">
-        <v>42</v>
+        <v>588</v>
       </c>
       <c r="AD174" t="s">
         <v>72</v>
@@ -22321,7 +22321,7 @@
         <v>42</v>
       </c>
       <c r="AC175" t="s">
-        <v>18</v>
+        <v>828</v>
       </c>
       <c r="AD175" t="s">
         <v>72</v>
@@ -22749,7 +22749,7 @@
         <v>42</v>
       </c>
       <c r="AC179" t="s">
-        <v>42</v>
+        <v>76</v>
       </c>
       <c r="AD179" t="s">
         <v>72</v>
@@ -22856,7 +22856,7 @@
         <v>42</v>
       </c>
       <c r="AC180" t="s">
-        <v>42</v>
+        <v>450</v>
       </c>
       <c r="AD180" t="s">
         <v>72</v>
@@ -26295,7 +26295,7 @@
         <v>0</v>
       </c>
       <c r="AH212">
-        <v>0.5</v>
+        <v>1</v>
       </c>
       <c r="AI212">
         <v>1</v>
@@ -26509,7 +26509,7 @@
         <v>0</v>
       </c>
       <c r="AH214">
-        <v>0.5</v>
+        <v>1</v>
       </c>
       <c r="AI214">
         <v>1</v>
@@ -26830,7 +26830,7 @@
         <v>0</v>
       </c>
       <c r="AH217">
-        <v>0.5</v>
+        <v>1</v>
       </c>
       <c r="AI217">
         <v>1</v>
@@ -26937,7 +26937,7 @@
         <v>0</v>
       </c>
       <c r="AH218">
-        <v>0.5</v>
+        <v>1</v>
       </c>
       <c r="AI218">
         <v>1</v>
@@ -27365,7 +27365,7 @@
         <v>0</v>
       </c>
       <c r="AH222">
-        <v>0.5</v>
+        <v>1</v>
       </c>
       <c r="AI222">
         <v>1</v>
@@ -30283,7 +30283,7 @@
         <v>100</v>
       </c>
       <c r="H250">
-        <v>100</v>
+        <v>140</v>
       </c>
       <c r="I250">
         <v>100</v>
@@ -30304,13 +30304,13 @@
         <v>1</v>
       </c>
       <c r="O250">
-        <v>100</v>
+        <v>130</v>
       </c>
       <c r="P250">
         <v>100</v>
       </c>
       <c r="Q250">
-        <v>100</v>
+        <v>110</v>
       </c>
       <c r="R250">
         <v>100</v>
@@ -31859,7 +31859,7 @@
         <v>0</v>
       </c>
       <c r="AH264">
-        <v>0.5</v>
+        <v>1</v>
       </c>
       <c r="AI264">
         <v>1</v>
@@ -31951,7 +31951,7 @@
         <v>42</v>
       </c>
       <c r="AC265" t="s">
-        <v>42</v>
+        <v>826</v>
       </c>
       <c r="AD265" t="s">
         <v>72</v>
@@ -32394,7 +32394,7 @@
         <v>0</v>
       </c>
       <c r="AH269">
-        <v>0.5</v>
+        <v>-1</v>
       </c>
       <c r="AI269">
         <v>1</v>
@@ -32486,7 +32486,7 @@
         <v>42</v>
       </c>
       <c r="AC270" t="s">
-        <v>42</v>
+        <v>588</v>
       </c>
       <c r="AD270" t="s">
         <v>43</v>
@@ -33892,7 +33892,7 @@
         <v>0</v>
       </c>
       <c r="AH283">
-        <v>0.5</v>
+        <v>1</v>
       </c>
       <c r="AI283">
         <v>1</v>
@@ -34091,7 +34091,7 @@
         <v>42</v>
       </c>
       <c r="AC285" t="s">
-        <v>42</v>
+        <v>592</v>
       </c>
       <c r="AD285" t="s">
         <v>131</v>
@@ -34106,7 +34106,7 @@
         <v>0</v>
       </c>
       <c r="AH285">
-        <v>0.5</v>
+        <v>-1</v>
       </c>
       <c r="AI285">
         <v>1</v>
@@ -35584,11 +35584,11 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0E19C42E-4D03-4797-B846-FB5E09BB39D3}">
-  <dimension ref="A1:N20"/>
+  <dimension ref="A1:N21"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="K15" sqref="K15"/>
+      <selection pane="bottomLeft" activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
@@ -35818,43 +35818,43 @@
     </row>
     <row r="6" spans="1:14" x14ac:dyDescent="0.4">
       <c r="A6" t="s">
-        <v>591</v>
+        <v>56</v>
       </c>
       <c r="B6">
-        <v>85</v>
+        <v>70</v>
       </c>
       <c r="C6">
-        <v>80</v>
+        <v>70</v>
       </c>
       <c r="D6">
-        <v>95</v>
+        <v>70</v>
       </c>
       <c r="E6">
-        <v>80</v>
+        <v>70</v>
       </c>
       <c r="F6">
-        <v>100</v>
+        <v>70</v>
       </c>
       <c r="G6">
-        <v>100</v>
+        <v>70</v>
       </c>
       <c r="H6">
-        <v>120</v>
+        <v>70</v>
       </c>
       <c r="I6">
-        <v>100</v>
+        <v>70</v>
       </c>
       <c r="J6">
-        <v>90</v>
+        <v>70</v>
       </c>
       <c r="K6">
-        <v>90</v>
+        <v>70</v>
       </c>
       <c r="L6">
-        <v>85</v>
+        <v>70</v>
       </c>
       <c r="M6">
-        <v>85</v>
+        <v>70</v>
       </c>
       <c r="N6">
         <v>1</v>
@@ -35862,43 +35862,43 @@
     </row>
     <row r="7" spans="1:14" x14ac:dyDescent="0.4">
       <c r="A7" t="s">
-        <v>40</v>
+        <v>591</v>
       </c>
       <c r="B7">
-        <v>120</v>
+        <v>85</v>
       </c>
       <c r="C7">
-        <v>90</v>
+        <v>80</v>
       </c>
       <c r="D7">
-        <v>70</v>
+        <v>95</v>
       </c>
       <c r="E7">
         <v>80</v>
       </c>
       <c r="F7">
-        <v>112</v>
+        <v>100</v>
       </c>
       <c r="G7">
         <v>100</v>
       </c>
       <c r="H7">
-        <v>80</v>
+        <v>120</v>
       </c>
       <c r="I7">
         <v>100</v>
       </c>
       <c r="J7">
-        <v>120</v>
+        <v>90</v>
       </c>
       <c r="K7">
-        <v>120</v>
+        <v>90</v>
       </c>
       <c r="L7">
-        <v>90</v>
+        <v>85</v>
       </c>
       <c r="M7">
-        <v>90</v>
+        <v>85</v>
       </c>
       <c r="N7">
         <v>1</v>
@@ -35906,43 +35906,43 @@
     </row>
     <row r="8" spans="1:14" x14ac:dyDescent="0.4">
       <c r="A8" t="s">
-        <v>57</v>
+        <v>40</v>
       </c>
       <c r="B8">
+        <v>120</v>
+      </c>
+      <c r="C8">
+        <v>90</v>
+      </c>
+      <c r="D8">
+        <v>70</v>
+      </c>
+      <c r="E8">
         <v>80</v>
       </c>
-      <c r="C8">
-        <v>105</v>
-      </c>
-      <c r="D8">
+      <c r="F8">
+        <v>112</v>
+      </c>
+      <c r="G8">
+        <v>100</v>
+      </c>
+      <c r="H8">
         <v>80</v>
       </c>
-      <c r="E8">
-        <v>130</v>
-      </c>
-      <c r="F8">
-        <v>85</v>
-      </c>
-      <c r="G8">
-        <v>85</v>
-      </c>
-      <c r="H8">
+      <c r="I8">
+        <v>100</v>
+      </c>
+      <c r="J8">
         <v>120</v>
       </c>
-      <c r="I8">
-        <v>72</v>
-      </c>
-      <c r="J8">
-        <v>110</v>
-      </c>
       <c r="K8">
+        <v>120</v>
+      </c>
+      <c r="L8">
         <v>90</v>
       </c>
-      <c r="L8">
-        <v>94</v>
-      </c>
       <c r="M8">
-        <v>106</v>
+        <v>90</v>
       </c>
       <c r="N8">
         <v>1</v>
@@ -35950,43 +35950,43 @@
     </row>
     <row r="9" spans="1:14" x14ac:dyDescent="0.4">
       <c r="A9" t="s">
-        <v>76</v>
+        <v>57</v>
       </c>
       <c r="B9">
-        <v>92</v>
+        <v>80</v>
       </c>
       <c r="C9">
+        <v>105</v>
+      </c>
+      <c r="D9">
+        <v>80</v>
+      </c>
+      <c r="E9">
+        <v>130</v>
+      </c>
+      <c r="F9">
+        <v>85</v>
+      </c>
+      <c r="G9">
+        <v>85</v>
+      </c>
+      <c r="H9">
+        <v>120</v>
+      </c>
+      <c r="I9">
+        <v>72</v>
+      </c>
+      <c r="J9">
         <v>110</v>
       </c>
-      <c r="D9">
-        <v>110</v>
-      </c>
-      <c r="E9">
-        <v>98</v>
-      </c>
-      <c r="F9">
+      <c r="K9">
         <v>90</v>
       </c>
-      <c r="G9">
-        <v>120</v>
-      </c>
-      <c r="H9">
-        <v>102</v>
-      </c>
-      <c r="I9">
-        <v>95</v>
-      </c>
-      <c r="J9">
-        <v>95</v>
-      </c>
-      <c r="K9">
-        <v>95</v>
-      </c>
       <c r="L9">
-        <v>105</v>
+        <v>94</v>
       </c>
       <c r="M9">
-        <v>95</v>
+        <v>106</v>
       </c>
       <c r="N9">
         <v>1</v>
@@ -35994,43 +35994,43 @@
     </row>
     <row r="10" spans="1:14" x14ac:dyDescent="0.4">
       <c r="A10" t="s">
-        <v>596</v>
+        <v>76</v>
       </c>
       <c r="B10">
-        <v>60</v>
+        <v>92</v>
       </c>
       <c r="C10">
-        <v>100</v>
+        <v>110</v>
       </c>
       <c r="D10">
-        <v>60</v>
+        <v>110</v>
       </c>
       <c r="E10">
+        <v>98</v>
+      </c>
+      <c r="F10">
+        <v>90</v>
+      </c>
+      <c r="G10">
         <v>120</v>
       </c>
-      <c r="F10">
-        <v>50</v>
-      </c>
-      <c r="G10">
-        <v>150</v>
-      </c>
       <c r="H10">
-        <v>130</v>
+        <v>102</v>
       </c>
       <c r="I10">
-        <v>60</v>
+        <v>95</v>
       </c>
       <c r="J10">
-        <v>50</v>
+        <v>95</v>
       </c>
       <c r="K10">
-        <v>130</v>
+        <v>95</v>
       </c>
       <c r="L10">
-        <v>100</v>
+        <v>105</v>
       </c>
       <c r="M10">
-        <v>100</v>
+        <v>95</v>
       </c>
       <c r="N10">
         <v>1</v>
@@ -36038,43 +36038,43 @@
     </row>
     <row r="11" spans="1:14" x14ac:dyDescent="0.4">
       <c r="A11" t="s">
-        <v>450</v>
+        <v>596</v>
       </c>
       <c r="B11">
-        <v>140</v>
+        <v>60</v>
       </c>
       <c r="C11">
-        <v>90</v>
+        <v>100</v>
       </c>
       <c r="D11">
-        <v>70</v>
+        <v>60</v>
       </c>
       <c r="E11">
-        <v>90</v>
+        <v>120</v>
       </c>
       <c r="F11">
-        <v>70</v>
+        <v>50</v>
       </c>
       <c r="G11">
-        <v>90</v>
+        <v>150</v>
       </c>
       <c r="H11">
-        <v>100</v>
+        <v>130</v>
       </c>
       <c r="I11">
-        <v>0</v>
+        <v>60</v>
       </c>
       <c r="J11">
-        <v>70</v>
+        <v>50</v>
       </c>
       <c r="K11">
-        <v>70</v>
+        <v>130</v>
       </c>
       <c r="L11">
-        <v>82</v>
+        <v>100</v>
       </c>
       <c r="M11">
-        <v>85</v>
+        <v>100</v>
       </c>
       <c r="N11">
         <v>1</v>
@@ -36082,43 +36082,43 @@
     </row>
     <row r="12" spans="1:14" x14ac:dyDescent="0.4">
       <c r="A12" t="s">
-        <v>228</v>
+        <v>450</v>
       </c>
       <c r="B12">
-        <v>120</v>
+        <v>140</v>
       </c>
       <c r="C12">
-        <v>120</v>
+        <v>90</v>
       </c>
       <c r="D12">
+        <v>70</v>
+      </c>
+      <c r="E12">
         <v>90</v>
       </c>
-      <c r="E12">
-        <v>100</v>
-      </c>
       <c r="F12">
-        <v>110</v>
+        <v>70</v>
       </c>
       <c r="G12">
-        <v>130</v>
+        <v>90</v>
       </c>
       <c r="H12">
-        <v>110</v>
+        <v>100</v>
       </c>
       <c r="I12">
-        <v>130</v>
+        <v>0</v>
       </c>
       <c r="J12">
-        <v>90</v>
+        <v>70</v>
       </c>
       <c r="K12">
-        <v>110</v>
+        <v>70</v>
       </c>
       <c r="L12">
-        <v>105</v>
+        <v>82</v>
       </c>
       <c r="M12">
-        <v>110</v>
+        <v>85</v>
       </c>
       <c r="N12">
         <v>1</v>
@@ -36126,43 +36126,43 @@
     </row>
     <row r="13" spans="1:14" x14ac:dyDescent="0.4">
       <c r="A13" t="s">
-        <v>588</v>
+        <v>228</v>
       </c>
       <c r="B13">
+        <v>120</v>
+      </c>
+      <c r="C13">
+        <v>120</v>
+      </c>
+      <c r="D13">
+        <v>90</v>
+      </c>
+      <c r="E13">
+        <v>100</v>
+      </c>
+      <c r="F13">
+        <v>110</v>
+      </c>
+      <c r="G13">
         <v>130</v>
       </c>
-      <c r="C13">
+      <c r="H13">
         <v>110</v>
       </c>
-      <c r="D13">
+      <c r="I13">
         <v>130</v>
       </c>
-      <c r="E13">
-        <v>100</v>
-      </c>
-      <c r="F13">
-        <v>120</v>
-      </c>
-      <c r="G13">
-        <v>70</v>
-      </c>
-      <c r="H13">
+      <c r="J13">
         <v>90</v>
       </c>
-      <c r="I13">
-        <v>80</v>
-      </c>
-      <c r="J13">
-        <v>80</v>
-      </c>
       <c r="K13">
-        <v>80</v>
+        <v>110</v>
       </c>
       <c r="L13">
+        <v>105</v>
+      </c>
+      <c r="M13">
         <v>110</v>
-      </c>
-      <c r="M13">
-        <v>90</v>
       </c>
       <c r="N13">
         <v>1</v>
@@ -36170,43 +36170,43 @@
     </row>
     <row r="14" spans="1:14" x14ac:dyDescent="0.4">
       <c r="A14" t="s">
-        <v>856</v>
+        <v>588</v>
       </c>
       <c r="B14">
-        <v>150</v>
+        <v>130</v>
       </c>
       <c r="C14">
+        <v>110</v>
+      </c>
+      <c r="D14">
+        <v>130</v>
+      </c>
+      <c r="E14">
+        <v>100</v>
+      </c>
+      <c r="F14">
         <v>120</v>
       </c>
-      <c r="D14">
-        <v>110</v>
-      </c>
-      <c r="E14">
+      <c r="G14">
         <v>70</v>
-      </c>
-      <c r="F14">
-        <v>130</v>
-      </c>
-      <c r="G14">
-        <v>90</v>
       </c>
       <c r="H14">
         <v>90</v>
       </c>
       <c r="I14">
+        <v>80</v>
+      </c>
+      <c r="J14">
+        <v>80</v>
+      </c>
+      <c r="K14">
+        <v>80</v>
+      </c>
+      <c r="L14">
+        <v>110</v>
+      </c>
+      <c r="M14">
         <v>90</v>
-      </c>
-      <c r="J14">
-        <v>130</v>
-      </c>
-      <c r="K14">
-        <v>110</v>
-      </c>
-      <c r="L14">
-        <v>135</v>
-      </c>
-      <c r="M14">
-        <v>125</v>
       </c>
       <c r="N14">
         <v>1</v>
@@ -36214,25 +36214,25 @@
     </row>
     <row r="15" spans="1:14" x14ac:dyDescent="0.4">
       <c r="A15" t="s">
-        <v>302</v>
+        <v>856</v>
       </c>
       <c r="B15">
+        <v>150</v>
+      </c>
+      <c r="C15">
+        <v>120</v>
+      </c>
+      <c r="D15">
+        <v>110</v>
+      </c>
+      <c r="E15">
+        <v>70</v>
+      </c>
+      <c r="F15">
         <v>130</v>
       </c>
-      <c r="C15">
-        <v>110</v>
-      </c>
-      <c r="D15">
-        <v>120</v>
-      </c>
-      <c r="E15">
-        <v>60</v>
-      </c>
-      <c r="F15">
-        <v>150</v>
-      </c>
       <c r="G15">
-        <v>80</v>
+        <v>90</v>
       </c>
       <c r="H15">
         <v>90</v>
@@ -36241,16 +36241,16 @@
         <v>90</v>
       </c>
       <c r="J15">
-        <v>150</v>
+        <v>130</v>
       </c>
       <c r="K15">
-        <v>105</v>
+        <v>110</v>
       </c>
       <c r="L15">
+        <v>135</v>
+      </c>
+      <c r="M15">
         <v>125</v>
-      </c>
-      <c r="M15">
-        <v>135</v>
       </c>
       <c r="N15">
         <v>1</v>
@@ -36258,87 +36258,87 @@
     </row>
     <row r="16" spans="1:14" x14ac:dyDescent="0.4">
       <c r="A16" t="s">
-        <v>826</v>
+        <v>302</v>
       </c>
       <c r="B16">
-        <v>250</v>
+        <v>130</v>
       </c>
       <c r="C16">
-        <v>130</v>
+        <v>110</v>
       </c>
       <c r="D16">
-        <v>110</v>
+        <v>120</v>
       </c>
       <c r="E16">
-        <v>110</v>
+        <v>60</v>
       </c>
       <c r="F16">
-        <v>110</v>
+        <v>150</v>
       </c>
       <c r="G16">
-        <v>110</v>
+        <v>80</v>
       </c>
       <c r="H16">
-        <v>110</v>
+        <v>90</v>
       </c>
       <c r="I16">
-        <v>110</v>
+        <v>90</v>
       </c>
       <c r="J16">
-        <v>110</v>
+        <v>150</v>
       </c>
       <c r="K16">
-        <v>110</v>
+        <v>105</v>
       </c>
       <c r="L16">
-        <v>180</v>
+        <v>125</v>
       </c>
       <c r="M16">
-        <v>180</v>
+        <v>135</v>
       </c>
       <c r="N16">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="17" spans="1:14" x14ac:dyDescent="0.4">
       <c r="A17" t="s">
-        <v>18</v>
+        <v>826</v>
       </c>
       <c r="B17">
-        <v>350</v>
+        <v>250</v>
       </c>
       <c r="C17">
-        <v>160</v>
+        <v>130</v>
       </c>
       <c r="D17">
-        <v>120</v>
+        <v>110</v>
       </c>
       <c r="E17">
-        <v>120</v>
+        <v>110</v>
       </c>
       <c r="F17">
-        <v>120</v>
+        <v>110</v>
       </c>
       <c r="G17">
-        <v>120</v>
+        <v>110</v>
       </c>
       <c r="H17">
-        <v>120</v>
+        <v>110</v>
       </c>
       <c r="I17">
-        <v>120</v>
+        <v>110</v>
       </c>
       <c r="J17">
-        <v>120</v>
+        <v>110</v>
       </c>
       <c r="K17">
-        <v>120</v>
+        <v>110</v>
       </c>
       <c r="L17">
-        <v>300</v>
+        <v>180</v>
       </c>
       <c r="M17">
-        <v>250</v>
+        <v>180</v>
       </c>
       <c r="N17">
         <v>2</v>
@@ -36346,75 +36346,75 @@
     </row>
     <row r="18" spans="1:14" x14ac:dyDescent="0.4">
       <c r="A18" t="s">
-        <v>689</v>
+        <v>18</v>
       </c>
       <c r="B18">
-        <v>1000</v>
+        <v>350</v>
       </c>
       <c r="C18">
-        <v>175</v>
+        <v>160</v>
       </c>
       <c r="D18">
-        <v>130</v>
+        <v>120</v>
       </c>
       <c r="E18">
-        <v>130</v>
+        <v>120</v>
       </c>
       <c r="F18">
-        <v>130</v>
+        <v>120</v>
       </c>
       <c r="G18">
-        <v>130</v>
+        <v>120</v>
       </c>
       <c r="H18">
-        <v>130</v>
+        <v>120</v>
       </c>
       <c r="I18">
-        <v>130</v>
+        <v>120</v>
       </c>
       <c r="J18">
-        <v>130</v>
+        <v>120</v>
       </c>
       <c r="K18">
-        <v>130</v>
+        <v>120</v>
       </c>
       <c r="L18">
-        <v>550</v>
+        <v>300</v>
       </c>
       <c r="M18">
-        <v>450</v>
+        <v>250</v>
       </c>
       <c r="N18">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="19" spans="1:14" x14ac:dyDescent="0.4">
       <c r="A19" t="s">
-        <v>20</v>
+        <v>689</v>
       </c>
       <c r="B19">
-        <v>2000</v>
+        <v>1000</v>
       </c>
       <c r="C19">
-        <v>200</v>
+        <v>175</v>
       </c>
       <c r="D19">
-        <v>140</v>
+        <v>130</v>
       </c>
       <c r="E19">
-        <v>140</v>
+        <v>130</v>
       </c>
       <c r="F19">
-        <v>140</v>
+        <v>130</v>
       </c>
       <c r="G19">
-        <v>140</v>
+        <v>130</v>
       </c>
       <c r="H19">
-        <v>140</v>
+        <v>130</v>
       </c>
       <c r="I19">
-        <v>140</v>
+        <v>130</v>
       </c>
       <c r="J19">
         <v>130</v>
@@ -36423,56 +36423,100 @@
         <v>130</v>
       </c>
       <c r="L19">
-        <v>1200</v>
+        <v>550</v>
       </c>
       <c r="M19">
-        <v>1000</v>
+        <v>450</v>
       </c>
       <c r="N19">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="20" spans="1:14" x14ac:dyDescent="0.4">
       <c r="A20" t="s">
+        <v>20</v>
+      </c>
+      <c r="B20">
+        <v>2000</v>
+      </c>
+      <c r="C20">
+        <v>200</v>
+      </c>
+      <c r="D20">
+        <v>140</v>
+      </c>
+      <c r="E20">
+        <v>140</v>
+      </c>
+      <c r="F20">
+        <v>140</v>
+      </c>
+      <c r="G20">
+        <v>140</v>
+      </c>
+      <c r="H20">
+        <v>140</v>
+      </c>
+      <c r="I20">
+        <v>140</v>
+      </c>
+      <c r="J20">
+        <v>130</v>
+      </c>
+      <c r="K20">
+        <v>130</v>
+      </c>
+      <c r="L20">
+        <v>1200</v>
+      </c>
+      <c r="M20">
+        <v>1000</v>
+      </c>
+      <c r="N20">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="21" spans="1:14" x14ac:dyDescent="0.4">
+      <c r="A21" t="s">
         <v>19</v>
       </c>
-      <c r="B20">
+      <c r="B21">
         <v>5000</v>
       </c>
-      <c r="C20">
+      <c r="C21">
         <v>230</v>
       </c>
-      <c r="D20">
+      <c r="D21">
         <v>180</v>
       </c>
-      <c r="E20">
+      <c r="E21">
         <v>180</v>
       </c>
-      <c r="F20">
+      <c r="F21">
         <v>180</v>
       </c>
-      <c r="G20">
+      <c r="G21">
         <v>180</v>
       </c>
-      <c r="H20">
+      <c r="H21">
         <v>180</v>
       </c>
-      <c r="I20">
+      <c r="I21">
         <v>180</v>
       </c>
-      <c r="J20">
+      <c r="J21">
         <v>140</v>
       </c>
-      <c r="K20">
+      <c r="K21">
         <v>140</v>
       </c>
-      <c r="L20">
+      <c r="L21">
         <v>5000</v>
       </c>
-      <c r="M20">
+      <c r="M21">
         <v>5000</v>
       </c>
-      <c r="N20">
+      <c r="N21">
         <v>5</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Fixing some missing or out of date stuff.
</commit_message>
<xml_diff>
--- a/Other/RoStatProcessing.xlsx
+++ b/Other/RoStatProcessing.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\ProjectsSSD\RagnarokRebuildTcp\Other\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0DEFC7A2-F64C-4130-856F-8F90FBA85FC6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BA7BBFBE-10D4-4DE3-A1D3-528A1A4D06D6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="377" yWindow="377" windowWidth="29494" windowHeight="16594" activeTab="1" xr2:uid="{1C41742B-2950-4FF8-AA39-6557869B44EA}"/>
   </bookViews>
@@ -48,7 +48,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2817" uniqueCount="1045">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2818" uniqueCount="1046">
   <si>
     <t>Level</t>
   </si>
@@ -3183,6 +3183,9 @@
   </si>
   <si>
     <t>Demon,Golem,WorldBoss</t>
+  </si>
+  <si>
+    <t>Golem,Elite</t>
   </si>
 </sst>
 </file>
@@ -3575,10 +3578,10 @@
   <dimension ref="A1:AI286"/>
   <sheetViews>
     <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <pane xSplit="2" ySplit="1" topLeftCell="C154" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="1" topLeftCell="C228" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="AC173" sqref="AC173"/>
+      <selection pane="bottomRight" activeCell="AC259" sqref="AC259"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
@@ -14082,7 +14085,7 @@
         <v>42</v>
       </c>
       <c r="AC98" t="s">
-        <v>42</v>
+        <v>354</v>
       </c>
       <c r="AD98" t="s">
         <v>72</v>
@@ -14189,7 +14192,7 @@
         <v>42</v>
       </c>
       <c r="AC99" t="s">
-        <v>42</v>
+        <v>354</v>
       </c>
       <c r="AD99" t="s">
         <v>72</v>
@@ -15615,7 +15618,7 @@
         <v>38</v>
       </c>
       <c r="E113">
-        <v>100</v>
+        <v>90</v>
       </c>
       <c r="F113">
         <v>100</v>
@@ -15624,19 +15627,19 @@
         <v>100</v>
       </c>
       <c r="H113">
-        <v>100</v>
+        <v>70</v>
       </c>
       <c r="I113">
         <v>100</v>
       </c>
       <c r="J113">
-        <v>100</v>
+        <v>130</v>
       </c>
       <c r="K113">
         <v>100</v>
       </c>
       <c r="L113">
-        <v>100</v>
+        <v>90</v>
       </c>
       <c r="M113">
         <v>10</v>
@@ -15645,7 +15648,7 @@
         <v>1</v>
       </c>
       <c r="O113">
-        <v>100</v>
+        <v>80</v>
       </c>
       <c r="P113">
         <v>100</v>
@@ -15654,7 +15657,7 @@
         <v>100</v>
       </c>
       <c r="R113">
-        <v>100</v>
+        <v>95</v>
       </c>
       <c r="S113">
         <v>10</v>
@@ -16650,7 +16653,7 @@
         <v>42</v>
       </c>
       <c r="AC122" t="s">
-        <v>42</v>
+        <v>826</v>
       </c>
       <c r="AD122" t="s">
         <v>72</v>
@@ -18041,7 +18044,7 @@
         <v>42</v>
       </c>
       <c r="AC135" t="s">
-        <v>42</v>
+        <v>588</v>
       </c>
       <c r="AD135" t="s">
         <v>72</v>
@@ -18516,7 +18519,7 @@
         <v>100</v>
       </c>
       <c r="I140">
-        <v>100</v>
+        <v>110</v>
       </c>
       <c r="J140">
         <v>100</v>
@@ -18525,7 +18528,7 @@
         <v>100</v>
       </c>
       <c r="L140">
-        <v>100</v>
+        <v>95</v>
       </c>
       <c r="M140">
         <v>10</v>
@@ -19004,7 +19007,7 @@
         <v>42</v>
       </c>
       <c r="AC144" t="s">
-        <v>42</v>
+        <v>1045</v>
       </c>
       <c r="AD144" t="s">
         <v>72</v>
@@ -19684,7 +19687,7 @@
         <v>100</v>
       </c>
       <c r="F151">
-        <v>100</v>
+        <v>130</v>
       </c>
       <c r="G151">
         <v>100</v>
@@ -19791,7 +19794,7 @@
         <v>100</v>
       </c>
       <c r="F152">
-        <v>100</v>
+        <v>130</v>
       </c>
       <c r="G152">
         <v>100</v>
@@ -20430,7 +20433,7 @@
         <v>59</v>
       </c>
       <c r="E158">
-        <v>100</v>
+        <v>85</v>
       </c>
       <c r="F158">
         <v>100</v>
@@ -20442,16 +20445,16 @@
         <v>100</v>
       </c>
       <c r="I158">
-        <v>100</v>
+        <v>130</v>
       </c>
       <c r="J158">
         <v>100</v>
       </c>
       <c r="K158">
-        <v>100</v>
+        <v>110</v>
       </c>
       <c r="L158">
-        <v>100</v>
+        <v>105</v>
       </c>
       <c r="M158">
         <v>10</v>
@@ -20460,16 +20463,16 @@
         <v>1</v>
       </c>
       <c r="O158">
-        <v>100</v>
+        <v>90</v>
       </c>
       <c r="P158">
-        <v>100</v>
+        <v>90</v>
       </c>
       <c r="Q158">
-        <v>100</v>
+        <v>102</v>
       </c>
       <c r="R158">
-        <v>100</v>
+        <v>105</v>
       </c>
       <c r="S158">
         <v>10</v>
@@ -20537,16 +20540,16 @@
         <v>44</v>
       </c>
       <c r="E159">
-        <v>100</v>
+        <v>90</v>
       </c>
       <c r="F159">
         <v>100</v>
       </c>
       <c r="G159">
-        <v>100</v>
+        <v>110</v>
       </c>
       <c r="H159">
-        <v>100</v>
+        <v>80</v>
       </c>
       <c r="I159">
         <v>100</v>
@@ -20555,7 +20558,7 @@
         <v>100</v>
       </c>
       <c r="K159">
-        <v>100</v>
+        <v>110</v>
       </c>
       <c r="L159">
         <v>100</v>
@@ -20567,16 +20570,16 @@
         <v>1</v>
       </c>
       <c r="O159">
-        <v>100</v>
+        <v>80</v>
       </c>
       <c r="P159">
-        <v>100</v>
+        <v>110</v>
       </c>
       <c r="Q159">
         <v>100</v>
       </c>
       <c r="R159">
-        <v>100</v>
+        <v>90</v>
       </c>
       <c r="S159">
         <v>10</v>
@@ -20757,7 +20760,7 @@
         <v>100</v>
       </c>
       <c r="G161">
-        <v>100</v>
+        <v>130</v>
       </c>
       <c r="H161">
         <v>100</v>
@@ -20790,7 +20793,7 @@
         <v>100</v>
       </c>
       <c r="R161">
-        <v>100</v>
+        <v>110</v>
       </c>
       <c r="S161">
         <v>10</v>
@@ -21286,7 +21289,7 @@
         <v>60</v>
       </c>
       <c r="E166">
-        <v>100</v>
+        <v>120</v>
       </c>
       <c r="F166">
         <v>100</v>
@@ -21307,7 +21310,7 @@
         <v>100</v>
       </c>
       <c r="L166">
-        <v>100</v>
+        <v>110</v>
       </c>
       <c r="M166">
         <v>10</v>
@@ -21316,16 +21319,16 @@
         <v>1</v>
       </c>
       <c r="O166">
-        <v>100</v>
+        <v>90</v>
       </c>
       <c r="P166">
-        <v>100</v>
+        <v>80</v>
       </c>
       <c r="Q166">
-        <v>100</v>
+        <v>105</v>
       </c>
       <c r="R166">
-        <v>100</v>
+        <v>110</v>
       </c>
       <c r="S166">
         <v>10</v>
@@ -28741,7 +28744,7 @@
         <v>42</v>
       </c>
       <c r="AC235" t="s">
-        <v>42</v>
+        <v>57</v>
       </c>
       <c r="AD235" t="s">
         <v>43</v>
@@ -29597,7 +29600,7 @@
         <v>42</v>
       </c>
       <c r="AC243" t="s">
-        <v>42</v>
+        <v>588</v>
       </c>
       <c r="AD243" t="s">
         <v>94</v>
@@ -29811,7 +29814,7 @@
         <v>42</v>
       </c>
       <c r="AC245" t="s">
-        <v>42</v>
+        <v>354</v>
       </c>
       <c r="AD245" t="s">
         <v>72</v>
@@ -29918,7 +29921,7 @@
         <v>42</v>
       </c>
       <c r="AC246" t="s">
-        <v>42</v>
+        <v>354</v>
       </c>
       <c r="AD246" t="s">
         <v>72</v>
@@ -30453,7 +30456,7 @@
         <v>42</v>
       </c>
       <c r="AC251" t="s">
-        <v>42</v>
+        <v>588</v>
       </c>
       <c r="AD251" t="s">
         <v>94</v>
@@ -30560,7 +30563,7 @@
         <v>42</v>
       </c>
       <c r="AC252" t="s">
-        <v>42</v>
+        <v>76</v>
       </c>
       <c r="AD252" t="s">
         <v>72</v>
@@ -30667,7 +30670,7 @@
         <v>42</v>
       </c>
       <c r="AC253" t="s">
-        <v>42</v>
+        <v>588</v>
       </c>
       <c r="AD253" t="s">
         <v>72</v>
@@ -35584,11 +35587,11 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0E19C42E-4D03-4797-B846-FB5E09BB39D3}">
-  <dimension ref="A1:N21"/>
+  <dimension ref="A1:N22"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B6" sqref="B6"/>
+      <selection pane="bottomLeft" activeCell="L15" sqref="L15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
@@ -36214,43 +36217,43 @@
     </row>
     <row r="15" spans="1:14" x14ac:dyDescent="0.4">
       <c r="A15" t="s">
-        <v>856</v>
+        <v>354</v>
       </c>
       <c r="B15">
-        <v>150</v>
+        <v>125</v>
       </c>
       <c r="C15">
         <v>120</v>
       </c>
       <c r="D15">
+        <v>120</v>
+      </c>
+      <c r="E15">
         <v>110</v>
       </c>
-      <c r="E15">
-        <v>70</v>
-      </c>
       <c r="F15">
-        <v>130</v>
+        <v>110</v>
       </c>
       <c r="G15">
         <v>90</v>
       </c>
       <c r="H15">
-        <v>90</v>
+        <v>100</v>
       </c>
       <c r="I15">
-        <v>90</v>
+        <v>100</v>
       </c>
       <c r="J15">
-        <v>130</v>
+        <v>100</v>
       </c>
       <c r="K15">
-        <v>110</v>
+        <v>100</v>
       </c>
       <c r="L15">
-        <v>135</v>
+        <v>115</v>
       </c>
       <c r="M15">
-        <v>125</v>
+        <v>105</v>
       </c>
       <c r="N15">
         <v>1</v>
@@ -36258,25 +36261,25 @@
     </row>
     <row r="16" spans="1:14" x14ac:dyDescent="0.4">
       <c r="A16" t="s">
-        <v>302</v>
+        <v>856</v>
       </c>
       <c r="B16">
+        <v>150</v>
+      </c>
+      <c r="C16">
+        <v>120</v>
+      </c>
+      <c r="D16">
+        <v>110</v>
+      </c>
+      <c r="E16">
+        <v>70</v>
+      </c>
+      <c r="F16">
         <v>130</v>
       </c>
-      <c r="C16">
-        <v>110</v>
-      </c>
-      <c r="D16">
-        <v>120</v>
-      </c>
-      <c r="E16">
-        <v>60</v>
-      </c>
-      <c r="F16">
-        <v>150</v>
-      </c>
       <c r="G16">
-        <v>80</v>
+        <v>90</v>
       </c>
       <c r="H16">
         <v>90</v>
@@ -36285,16 +36288,16 @@
         <v>90</v>
       </c>
       <c r="J16">
-        <v>150</v>
+        <v>130</v>
       </c>
       <c r="K16">
-        <v>105</v>
+        <v>110</v>
       </c>
       <c r="L16">
+        <v>135</v>
+      </c>
+      <c r="M16">
         <v>125</v>
-      </c>
-      <c r="M16">
-        <v>135</v>
       </c>
       <c r="N16">
         <v>1</v>
@@ -36302,87 +36305,87 @@
     </row>
     <row r="17" spans="1:14" x14ac:dyDescent="0.4">
       <c r="A17" t="s">
-        <v>826</v>
+        <v>302</v>
       </c>
       <c r="B17">
-        <v>250</v>
+        <v>130</v>
       </c>
       <c r="C17">
-        <v>130</v>
+        <v>110</v>
       </c>
       <c r="D17">
-        <v>110</v>
+        <v>120</v>
       </c>
       <c r="E17">
-        <v>110</v>
+        <v>60</v>
       </c>
       <c r="F17">
-        <v>110</v>
+        <v>150</v>
       </c>
       <c r="G17">
-        <v>110</v>
+        <v>80</v>
       </c>
       <c r="H17">
-        <v>110</v>
+        <v>90</v>
       </c>
       <c r="I17">
-        <v>110</v>
+        <v>90</v>
       </c>
       <c r="J17">
-        <v>110</v>
+        <v>150</v>
       </c>
       <c r="K17">
-        <v>110</v>
+        <v>105</v>
       </c>
       <c r="L17">
-        <v>180</v>
+        <v>125</v>
       </c>
       <c r="M17">
-        <v>180</v>
+        <v>135</v>
       </c>
       <c r="N17">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="18" spans="1:14" x14ac:dyDescent="0.4">
       <c r="A18" t="s">
-        <v>18</v>
+        <v>826</v>
       </c>
       <c r="B18">
-        <v>350</v>
+        <v>250</v>
       </c>
       <c r="C18">
-        <v>160</v>
+        <v>130</v>
       </c>
       <c r="D18">
-        <v>120</v>
+        <v>110</v>
       </c>
       <c r="E18">
-        <v>120</v>
+        <v>110</v>
       </c>
       <c r="F18">
-        <v>120</v>
+        <v>110</v>
       </c>
       <c r="G18">
-        <v>120</v>
+        <v>110</v>
       </c>
       <c r="H18">
-        <v>120</v>
+        <v>110</v>
       </c>
       <c r="I18">
-        <v>120</v>
+        <v>110</v>
       </c>
       <c r="J18">
-        <v>120</v>
+        <v>110</v>
       </c>
       <c r="K18">
-        <v>120</v>
+        <v>110</v>
       </c>
       <c r="L18">
-        <v>300</v>
+        <v>180</v>
       </c>
       <c r="M18">
-        <v>250</v>
+        <v>180</v>
       </c>
       <c r="N18">
         <v>2</v>
@@ -36390,75 +36393,75 @@
     </row>
     <row r="19" spans="1:14" x14ac:dyDescent="0.4">
       <c r="A19" t="s">
-        <v>689</v>
+        <v>18</v>
       </c>
       <c r="B19">
-        <v>1000</v>
+        <v>350</v>
       </c>
       <c r="C19">
-        <v>175</v>
+        <v>160</v>
       </c>
       <c r="D19">
-        <v>130</v>
+        <v>120</v>
       </c>
       <c r="E19">
-        <v>130</v>
+        <v>120</v>
       </c>
       <c r="F19">
-        <v>130</v>
+        <v>120</v>
       </c>
       <c r="G19">
-        <v>130</v>
+        <v>120</v>
       </c>
       <c r="H19">
-        <v>130</v>
+        <v>120</v>
       </c>
       <c r="I19">
-        <v>130</v>
+        <v>120</v>
       </c>
       <c r="J19">
-        <v>130</v>
+        <v>120</v>
       </c>
       <c r="K19">
-        <v>130</v>
+        <v>120</v>
       </c>
       <c r="L19">
-        <v>550</v>
+        <v>300</v>
       </c>
       <c r="M19">
-        <v>450</v>
+        <v>250</v>
       </c>
       <c r="N19">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="20" spans="1:14" x14ac:dyDescent="0.4">
       <c r="A20" t="s">
-        <v>20</v>
+        <v>689</v>
       </c>
       <c r="B20">
-        <v>2000</v>
+        <v>1000</v>
       </c>
       <c r="C20">
-        <v>200</v>
+        <v>175</v>
       </c>
       <c r="D20">
-        <v>140</v>
+        <v>130</v>
       </c>
       <c r="E20">
-        <v>140</v>
+        <v>130</v>
       </c>
       <c r="F20">
-        <v>140</v>
+        <v>130</v>
       </c>
       <c r="G20">
-        <v>140</v>
+        <v>130</v>
       </c>
       <c r="H20">
-        <v>140</v>
+        <v>130</v>
       </c>
       <c r="I20">
-        <v>140</v>
+        <v>130</v>
       </c>
       <c r="J20">
         <v>130</v>
@@ -36467,56 +36470,100 @@
         <v>130</v>
       </c>
       <c r="L20">
-        <v>1200</v>
+        <v>550</v>
       </c>
       <c r="M20">
-        <v>1000</v>
+        <v>450</v>
       </c>
       <c r="N20">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="21" spans="1:14" x14ac:dyDescent="0.4">
       <c r="A21" t="s">
+        <v>20</v>
+      </c>
+      <c r="B21">
+        <v>2000</v>
+      </c>
+      <c r="C21">
+        <v>200</v>
+      </c>
+      <c r="D21">
+        <v>140</v>
+      </c>
+      <c r="E21">
+        <v>140</v>
+      </c>
+      <c r="F21">
+        <v>140</v>
+      </c>
+      <c r="G21">
+        <v>140</v>
+      </c>
+      <c r="H21">
+        <v>140</v>
+      </c>
+      <c r="I21">
+        <v>140</v>
+      </c>
+      <c r="J21">
+        <v>130</v>
+      </c>
+      <c r="K21">
+        <v>130</v>
+      </c>
+      <c r="L21">
+        <v>1200</v>
+      </c>
+      <c r="M21">
+        <v>1000</v>
+      </c>
+      <c r="N21">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="22" spans="1:14" x14ac:dyDescent="0.4">
+      <c r="A22" t="s">
         <v>19</v>
       </c>
-      <c r="B21">
+      <c r="B22">
         <v>5000</v>
       </c>
-      <c r="C21">
+      <c r="C22">
         <v>230</v>
       </c>
-      <c r="D21">
+      <c r="D22">
         <v>180</v>
       </c>
-      <c r="E21">
+      <c r="E22">
         <v>180</v>
       </c>
-      <c r="F21">
+      <c r="F22">
         <v>180</v>
       </c>
-      <c r="G21">
+      <c r="G22">
         <v>180</v>
       </c>
-      <c r="H21">
+      <c r="H22">
         <v>180</v>
       </c>
-      <c r="I21">
+      <c r="I22">
         <v>180</v>
       </c>
-      <c r="J21">
+      <c r="J22">
         <v>140</v>
       </c>
-      <c r="K21">
+      <c r="K22">
         <v>140</v>
       </c>
-      <c r="L21">
+      <c r="L22">
         <v>5000</v>
       </c>
-      <c r="M21">
+      <c r="M22">
         <v>5000</v>
       </c>
-      <c r="N21">
+      <c r="N22">
         <v>5</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Some client data stuff.
</commit_message>
<xml_diff>
--- a/Other/RoStatProcessing.xlsx
+++ b/Other/RoStatProcessing.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26626"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26924"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\ProjectsSSD\RagnarokRebuildTcp\Other\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BA7BBFBE-10D4-4DE3-A1D3-528A1A4D06D6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6239883E-C4C3-46ED-8BF9-BAB92769CE28}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="377" yWindow="377" windowWidth="29494" windowHeight="16594" activeTab="1" xr2:uid="{1C41742B-2950-4FF8-AA39-6557869B44EA}"/>
+    <workbookView xWindow="3651" yWindow="677" windowWidth="22252" windowHeight="16740" xr2:uid="{1C41742B-2950-4FF8-AA39-6557869B44EA}"/>
   </bookViews>
   <sheets>
     <sheet name="StatDef" sheetId="3" r:id="rId1"/>
@@ -24,6 +24,7 @@
     <sheet name="WeaponClass" sheetId="13" r:id="rId9"/>
     <sheet name="JobWeaponClass" sheetId="14" r:id="rId10"/>
     <sheet name="Sheet1" sheetId="1" r:id="rId11"/>
+    <sheet name="Sheet2" sheetId="15" r:id="rId12"/>
   </sheets>
   <definedNames>
     <definedName name="BaseMonStatTable">StatCharts!$A:$H</definedName>
@@ -48,7 +49,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2818" uniqueCount="1046">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2826" uniqueCount="1046">
   <si>
     <t>Level</t>
   </si>
@@ -3239,7 +3240,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -3247,11 +3248,20 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
@@ -3261,6 +3271,8 @@
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -3577,11 +3589,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{811A97A5-94A7-4FFA-A162-65D076B52481}">
   <dimension ref="A1:AI286"/>
   <sheetViews>
-    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <pane xSplit="2" ySplit="1" topLeftCell="C228" activePane="bottomRight" state="frozen"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <pane xSplit="2" ySplit="1" topLeftCell="C34" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="AC259" sqref="AC259"/>
+      <selection pane="bottomRight" activeCell="F46" sqref="F46"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
@@ -34367,7 +34379,7 @@
   <dimension ref="A1:R22"/>
   <sheetViews>
     <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="T2" sqref="T2"/>
+      <selection activeCell="D27" sqref="D27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
@@ -35578,6 +35590,743 @@
       <c r="R22">
         <f t="shared" si="12"/>
         <v>1964.5109400004289</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4CDA1E1B-7E76-4F6C-9799-F663030F0908}">
+  <dimension ref="A1:H22"/>
+  <sheetViews>
+    <sheetView topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="J22" sqref="J1:J22"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
+  <cols>
+    <col min="5" max="5" width="11" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:8" x14ac:dyDescent="0.4">
+      <c r="A1" s="7" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="8" t="s">
+        <v>2</v>
+      </c>
+      <c r="C1" s="8" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" s="8" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="8" t="s">
+        <v>45</v>
+      </c>
+      <c r="F1" s="8" t="s">
+        <v>21</v>
+      </c>
+      <c r="G1" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" s="7" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.4">
+      <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="B2" s="1">
+        <f ca="1">OFFSET(StatCharts!B$2,Sheet2!$A2-1,0)</f>
+        <v>0.10717734625362932</v>
+      </c>
+      <c r="C2" s="1">
+        <f ca="1">OFFSET(StatCharts!C$2,Sheet2!$A2-1,0)</f>
+        <v>35.15004828475508</v>
+      </c>
+      <c r="D2" s="1">
+        <f ca="1">OFFSET(StatCharts!D$2,Sheet2!$A2-1,0)</f>
+        <v>8.5717734625362922</v>
+      </c>
+      <c r="E2" s="1">
+        <f ca="1">OFFSET(StatCharts!E$2,Sheet2!$A2-1,0)</f>
+        <v>0.79200000000000159</v>
+      </c>
+      <c r="F2" s="1">
+        <f ca="1">OFFSET(StatCharts!F$2,Sheet2!$A2-1,0)</f>
+        <v>7.5757575757575601</v>
+      </c>
+      <c r="G2">
+        <f ca="1">OFFSET(StatCharts!G$2,Sheet2!$A2-1,0)</f>
+        <v>1</v>
+      </c>
+      <c r="H2">
+        <f ca="1">OFFSET(StatCharts!H$2,Sheet2!$A2-1,0)</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.4">
+      <c r="A3">
+        <v>5</v>
+      </c>
+      <c r="B3" s="1">
+        <f ca="1">OFFSET(StatCharts!B$2,Sheet2!$A3-1,0)</f>
+        <v>0.1414213562373095</v>
+      </c>
+      <c r="C3" s="1">
+        <f ca="1">OFFSET(StatCharts!C$2,Sheet2!$A3-1,0)</f>
+        <v>91.989949493661172</v>
+      </c>
+      <c r="D3" s="1">
+        <f ca="1">OFFSET(StatCharts!D$2,Sheet2!$A3-1,0)</f>
+        <v>18.914213562373096</v>
+      </c>
+      <c r="E3" s="1">
+        <f ca="1">OFFSET(StatCharts!E$2,Sheet2!$A3-1,0)</f>
+        <v>2.3280000000000012</v>
+      </c>
+      <c r="F3" s="1">
+        <f ca="1">OFFSET(StatCharts!F$2,Sheet2!$A3-1,0)</f>
+        <v>12.886597938144323</v>
+      </c>
+      <c r="G3">
+        <f ca="1">OFFSET(StatCharts!G$2,Sheet2!$A3-1,0)</f>
+        <v>5</v>
+      </c>
+      <c r="H3">
+        <f ca="1">OFFSET(StatCharts!H$2,Sheet2!$A3-1,0)</f>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.4">
+      <c r="A4">
+        <v>10</v>
+      </c>
+      <c r="B4" s="1">
+        <f ca="1">OFFSET(StatCharts!B$2,Sheet2!$A4-1,0)</f>
+        <v>0.2</v>
+      </c>
+      <c r="C4" s="1">
+        <f ca="1">OFFSET(StatCharts!C$2,Sheet2!$A4-1,0)</f>
+        <v>163.79999999999998</v>
+      </c>
+      <c r="D4" s="1">
+        <f ca="1">OFFSET(StatCharts!D$2,Sheet2!$A4-1,0)</f>
+        <v>32</v>
+      </c>
+      <c r="E4" s="1">
+        <f ca="1">OFFSET(StatCharts!E$2,Sheet2!$A4-1,0)</f>
+        <v>4.1579999999999995</v>
+      </c>
+      <c r="F4" s="1">
+        <f ca="1">OFFSET(StatCharts!F$2,Sheet2!$A4-1,0)</f>
+        <v>49.302549302549309</v>
+      </c>
+      <c r="G4">
+        <f ca="1">OFFSET(StatCharts!G$2,Sheet2!$A4-1,0)</f>
+        <v>9</v>
+      </c>
+      <c r="H4">
+        <f ca="1">OFFSET(StatCharts!H$2,Sheet2!$A4-1,0)</f>
+        <v>4</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.4">
+      <c r="A5">
+        <v>15</v>
+      </c>
+      <c r="B5" s="1">
+        <f ca="1">OFFSET(StatCharts!B$2,Sheet2!$A5-1,0)</f>
+        <v>0.28284271247461901</v>
+      </c>
+      <c r="C5" s="1">
+        <f ca="1">OFFSET(StatCharts!C$2,Sheet2!$A5-1,0)</f>
+        <v>236.939696961967</v>
+      </c>
+      <c r="D5" s="1">
+        <f ca="1">OFFSET(StatCharts!D$2,Sheet2!$A5-1,0)</f>
+        <v>45.328427124746192</v>
+      </c>
+      <c r="E5" s="1">
+        <f ca="1">OFFSET(StatCharts!E$2,Sheet2!$A5-1,0)</f>
+        <v>5.8880000000000017</v>
+      </c>
+      <c r="F5" s="1">
+        <f ca="1">OFFSET(StatCharts!F$2,Sheet2!$A5-1,0)</f>
+        <v>115.48913043478258</v>
+      </c>
+      <c r="G5">
+        <f ca="1">OFFSET(StatCharts!G$2,Sheet2!$A5-1,0)</f>
+        <v>13</v>
+      </c>
+      <c r="H5">
+        <f ca="1">OFFSET(StatCharts!H$2,Sheet2!$A5-1,0)</f>
+        <v>6</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.4">
+      <c r="A6">
+        <v>20</v>
+      </c>
+      <c r="B6" s="1">
+        <f ca="1">OFFSET(StatCharts!B$2,Sheet2!$A6-1,0)</f>
+        <v>1.4</v>
+      </c>
+      <c r="C6" s="1">
+        <f ca="1">OFFSET(StatCharts!C$2,Sheet2!$A6-1,0)</f>
+        <v>340.2</v>
+      </c>
+      <c r="D6" s="1">
+        <f ca="1">OFFSET(StatCharts!D$2,Sheet2!$A6-1,0)</f>
+        <v>69</v>
+      </c>
+      <c r="E6" s="1">
+        <f ca="1">OFFSET(StatCharts!E$2,Sheet2!$A6-1,0)</f>
+        <v>7.517999999999998</v>
+      </c>
+      <c r="F6" s="1">
+        <f ca="1">OFFSET(StatCharts!F$2,Sheet2!$A6-1,0)</f>
+        <v>213.48762968874706</v>
+      </c>
+      <c r="G6">
+        <f ca="1">OFFSET(StatCharts!G$2,Sheet2!$A6-1,0)</f>
+        <v>17</v>
+      </c>
+      <c r="H6">
+        <f ca="1">OFFSET(StatCharts!H$2,Sheet2!$A6-1,0)</f>
+        <v>7</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.4">
+      <c r="A7">
+        <v>25</v>
+      </c>
+      <c r="B7" s="1">
+        <f ca="1">OFFSET(StatCharts!B$2,Sheet2!$A7-1,0)</f>
+        <v>1.565685424949238</v>
+      </c>
+      <c r="C7" s="1">
+        <f ca="1">OFFSET(StatCharts!C$2,Sheet2!$A7-1,0)</f>
+        <v>425.79898987322332</v>
+      </c>
+      <c r="D7" s="1">
+        <f ca="1">OFFSET(StatCharts!D$2,Sheet2!$A7-1,0)</f>
+        <v>83.156854249492383</v>
+      </c>
+      <c r="E7" s="1">
+        <f ca="1">OFFSET(StatCharts!E$2,Sheet2!$A7-1,0)</f>
+        <v>9.048</v>
+      </c>
+      <c r="F7" s="1">
+        <f ca="1">OFFSET(StatCharts!F$2,Sheet2!$A7-1,0)</f>
+        <v>345.93280282935456</v>
+      </c>
+      <c r="G7">
+        <f ca="1">OFFSET(StatCharts!G$2,Sheet2!$A7-1,0)</f>
+        <v>21</v>
+      </c>
+      <c r="H7">
+        <f ca="1">OFFSET(StatCharts!H$2,Sheet2!$A7-1,0)</f>
+        <v>9</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.4">
+      <c r="A8">
+        <v>30</v>
+      </c>
+      <c r="B8" s="1">
+        <f ca="1">OFFSET(StatCharts!B$2,Sheet2!$A8-1,0)</f>
+        <v>4.8</v>
+      </c>
+      <c r="C8" s="1">
+        <f ca="1">OFFSET(StatCharts!C$2,Sheet2!$A8-1,0)</f>
+        <v>642.59999999999991</v>
+      </c>
+      <c r="D8" s="1">
+        <f ca="1">OFFSET(StatCharts!D$2,Sheet2!$A8-1,0)</f>
+        <v>128</v>
+      </c>
+      <c r="E8" s="1">
+        <f ca="1">OFFSET(StatCharts!E$2,Sheet2!$A8-1,0)</f>
+        <v>10.478000000000002</v>
+      </c>
+      <c r="F8" s="1">
+        <f ca="1">OFFSET(StatCharts!F$2,Sheet2!$A8-1,0)</f>
+        <v>515.84271807596861</v>
+      </c>
+      <c r="G8">
+        <f ca="1">OFFSET(StatCharts!G$2,Sheet2!$A8-1,0)</f>
+        <v>25</v>
+      </c>
+      <c r="H8">
+        <f ca="1">OFFSET(StatCharts!H$2,Sheet2!$A8-1,0)</f>
+        <v>11</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.4">
+      <c r="A9">
+        <v>35</v>
+      </c>
+      <c r="B9" s="1">
+        <f ca="1">OFFSET(StatCharts!B$2,Sheet2!$A9-1,0)</f>
+        <v>5.1313708498984756</v>
+      </c>
+      <c r="C9" s="1">
+        <f ca="1">OFFSET(StatCharts!C$2,Sheet2!$A9-1,0)</f>
+        <v>762.43717164502527</v>
+      </c>
+      <c r="D9" s="1">
+        <f ca="1">OFFSET(StatCharts!D$2,Sheet2!$A9-1,0)</f>
+        <v>143.81370849898474</v>
+      </c>
+      <c r="E9" s="1">
+        <f ca="1">OFFSET(StatCharts!E$2,Sheet2!$A9-1,0)</f>
+        <v>11.808</v>
+      </c>
+      <c r="F9" s="1">
+        <f ca="1">OFFSET(StatCharts!F$2,Sheet2!$A9-1,0)</f>
+        <v>726.6260162601626</v>
+      </c>
+      <c r="G9">
+        <f ca="1">OFFSET(StatCharts!G$2,Sheet2!$A9-1,0)</f>
+        <v>29</v>
+      </c>
+      <c r="H9">
+        <f ca="1">OFFSET(StatCharts!H$2,Sheet2!$A9-1,0)</f>
+        <v>12</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.4">
+      <c r="A10">
+        <v>40</v>
+      </c>
+      <c r="B10" s="1">
+        <f ca="1">OFFSET(StatCharts!B$2,Sheet2!$A10-1,0)</f>
+        <v>8.6</v>
+      </c>
+      <c r="C10" s="1">
+        <f ca="1">OFFSET(StatCharts!C$2,Sheet2!$A10-1,0)</f>
+        <v>1062.5999999999999</v>
+      </c>
+      <c r="D10" s="1">
+        <f ca="1">OFFSET(StatCharts!D$2,Sheet2!$A10-1,0)</f>
+        <v>191</v>
+      </c>
+      <c r="E10" s="1">
+        <f ca="1">OFFSET(StatCharts!E$2,Sheet2!$A10-1,0)</f>
+        <v>13.037999999999998</v>
+      </c>
+      <c r="F10" s="1">
+        <f ca="1">OFFSET(StatCharts!F$2,Sheet2!$A10-1,0)</f>
+        <v>982.12916091425075</v>
+      </c>
+      <c r="G10">
+        <f ca="1">OFFSET(StatCharts!G$2,Sheet2!$A10-1,0)</f>
+        <v>33</v>
+      </c>
+      <c r="H10">
+        <f ca="1">OFFSET(StatCharts!H$2,Sheet2!$A10-1,0)</f>
+        <v>14</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.4">
+      <c r="A11">
+        <v>45</v>
+      </c>
+      <c r="B11" s="1">
+        <f ca="1">OFFSET(StatCharts!B$2,Sheet2!$A11-1,0)</f>
+        <v>9.2627416997969512</v>
+      </c>
+      <c r="C11" s="1">
+        <f ca="1">OFFSET(StatCharts!C$2,Sheet2!$A11-1,0)</f>
+        <v>1234.5527270872078</v>
+      </c>
+      <c r="D11" s="1">
+        <f ca="1">OFFSET(StatCharts!D$2,Sheet2!$A11-1,0)</f>
+        <v>210.1274169979695</v>
+      </c>
+      <c r="E11" s="1">
+        <f ca="1">OFFSET(StatCharts!E$2,Sheet2!$A11-1,0)</f>
+        <v>14.167999999999999</v>
+      </c>
+      <c r="F11" s="1">
+        <f ca="1">OFFSET(StatCharts!F$2,Sheet2!$A11-1,0)</f>
+        <v>1286.7024280067758</v>
+      </c>
+      <c r="G11">
+        <f ca="1">OFFSET(StatCharts!G$2,Sheet2!$A11-1,0)</f>
+        <v>37</v>
+      </c>
+      <c r="H11">
+        <f ca="1">OFFSET(StatCharts!H$2,Sheet2!$A11-1,0)</f>
+        <v>16</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.4">
+      <c r="A12">
+        <v>50</v>
+      </c>
+      <c r="B12" s="1">
+        <f ca="1">OFFSET(StatCharts!B$2,Sheet2!$A12-1,0)</f>
+        <v>10.199999999999999</v>
+      </c>
+      <c r="C12" s="1">
+        <f ca="1">OFFSET(StatCharts!C$2,Sheet2!$A12-1,0)</f>
+        <v>1435</v>
+      </c>
+      <c r="D12" s="1">
+        <f ca="1">OFFSET(StatCharts!D$2,Sheet2!$A12-1,0)</f>
+        <v>232</v>
+      </c>
+      <c r="E12" s="1">
+        <f ca="1">OFFSET(StatCharts!E$2,Sheet2!$A12-1,0)</f>
+        <v>15.198</v>
+      </c>
+      <c r="F12" s="1">
+        <f ca="1">OFFSET(StatCharts!F$2,Sheet2!$A12-1,0)</f>
+        <v>1645.2822739834189</v>
+      </c>
+      <c r="G12">
+        <f ca="1">OFFSET(StatCharts!G$2,Sheet2!$A12-1,0)</f>
+        <v>41</v>
+      </c>
+      <c r="H12">
+        <f ca="1">OFFSET(StatCharts!H$2,Sheet2!$A12-1,0)</f>
+        <v>17</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.4">
+      <c r="A13">
+        <v>55</v>
+      </c>
+      <c r="B13" s="1">
+        <f ca="1">OFFSET(StatCharts!B$2,Sheet2!$A13-1,0)</f>
+        <v>11.525483399593904</v>
+      </c>
+      <c r="C13" s="1">
+        <f ca="1">OFFSET(StatCharts!C$2,Sheet2!$A13-1,0)</f>
+        <v>1678.4622217687304</v>
+      </c>
+      <c r="D13" s="1">
+        <f ca="1">OFFSET(StatCharts!D$2,Sheet2!$A13-1,0)</f>
+        <v>257.75483399593907</v>
+      </c>
+      <c r="E13" s="1">
+        <f ca="1">OFFSET(StatCharts!E$2,Sheet2!$A13-1,0)</f>
+        <v>16.128</v>
+      </c>
+      <c r="F13" s="1">
+        <f ca="1">OFFSET(StatCharts!F$2,Sheet2!$A13-1,0)</f>
+        <v>2063.4920634920636</v>
+      </c>
+      <c r="G13">
+        <f ca="1">OFFSET(StatCharts!G$2,Sheet2!$A13-1,0)</f>
+        <v>45</v>
+      </c>
+      <c r="H13">
+        <f ca="1">OFFSET(StatCharts!H$2,Sheet2!$A13-1,0)</f>
+        <v>19</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.4">
+      <c r="A14">
+        <v>60</v>
+      </c>
+      <c r="B14" s="1">
+        <f ca="1">OFFSET(StatCharts!B$2,Sheet2!$A14-1,0)</f>
+        <v>27.4</v>
+      </c>
+      <c r="C14" s="1">
+        <f ca="1">OFFSET(StatCharts!C$2,Sheet2!$A14-1,0)</f>
+        <v>3162.6</v>
+      </c>
+      <c r="D14" s="1">
+        <f ca="1">OFFSET(StatCharts!D$2,Sheet2!$A14-1,0)</f>
+        <v>429</v>
+      </c>
+      <c r="E14" s="1">
+        <f ca="1">OFFSET(StatCharts!E$2,Sheet2!$A14-1,0)</f>
+        <v>16.957999999999998</v>
+      </c>
+      <c r="F14" s="1">
+        <f ca="1">OFFSET(StatCharts!F$2,Sheet2!$A14-1,0)</f>
+        <v>2547.7650666352165</v>
+      </c>
+      <c r="G14">
+        <f ca="1">OFFSET(StatCharts!G$2,Sheet2!$A14-1,0)</f>
+        <v>49</v>
+      </c>
+      <c r="H14">
+        <f ca="1">OFFSET(StatCharts!H$2,Sheet2!$A14-1,0)</f>
+        <v>21</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.4">
+      <c r="A15">
+        <v>65</v>
+      </c>
+      <c r="B15" s="1">
+        <f ca="1">OFFSET(StatCharts!B$2,Sheet2!$A15-1,0)</f>
+        <v>30.050966799187805</v>
+      </c>
+      <c r="C15" s="1">
+        <f ca="1">OFFSET(StatCharts!C$2,Sheet2!$A15-1,0)</f>
+        <v>3665.6379787260898</v>
+      </c>
+      <c r="D15" s="1">
+        <f ca="1">OFFSET(StatCharts!D$2,Sheet2!$A15-1,0)</f>
+        <v>468.00966799187802</v>
+      </c>
+      <c r="E15" s="1">
+        <f ca="1">OFFSET(StatCharts!E$2,Sheet2!$A15-1,0)</f>
+        <v>17.688000000000002</v>
+      </c>
+      <c r="F15" s="1">
+        <f ca="1">OFFSET(StatCharts!F$2,Sheet2!$A15-1,0)</f>
+        <v>3105.4952510176386</v>
+      </c>
+      <c r="G15">
+        <f ca="1">OFFSET(StatCharts!G$2,Sheet2!$A15-1,0)</f>
+        <v>53</v>
+      </c>
+      <c r="H15">
+        <f ca="1">OFFSET(StatCharts!H$2,Sheet2!$A15-1,0)</f>
+        <v>22</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.4">
+      <c r="A16">
+        <v>70</v>
+      </c>
+      <c r="B16" s="1">
+        <f ca="1">OFFSET(StatCharts!B$2,Sheet2!$A16-1,0)</f>
+        <v>33.799999999999997</v>
+      </c>
+      <c r="C16" s="1">
+        <f ca="1">OFFSET(StatCharts!C$2,Sheet2!$A16-1,0)</f>
+        <v>4313.3999999999996</v>
+      </c>
+      <c r="D16" s="1">
+        <f ca="1">OFFSET(StatCharts!D$2,Sheet2!$A16-1,0)</f>
+        <v>518</v>
+      </c>
+      <c r="E16" s="1">
+        <f ca="1">OFFSET(StatCharts!E$2,Sheet2!$A16-1,0)</f>
+        <v>18.317999999999998</v>
+      </c>
+      <c r="F16" s="1">
+        <f ca="1">OFFSET(StatCharts!F$2,Sheet2!$A16-1,0)</f>
+        <v>3745.2232776503988</v>
+      </c>
+      <c r="G16">
+        <f ca="1">OFFSET(StatCharts!G$2,Sheet2!$A16-1,0)</f>
+        <v>57</v>
+      </c>
+      <c r="H16">
+        <f ca="1">OFFSET(StatCharts!H$2,Sheet2!$A16-1,0)</f>
+        <v>24</v>
+      </c>
+    </row>
+    <row r="17" spans="1:8" x14ac:dyDescent="0.4">
+      <c r="A17">
+        <v>75</v>
+      </c>
+      <c r="B17" s="1">
+        <f ca="1">OFFSET(StatCharts!B$2,Sheet2!$A17-1,0)</f>
+        <v>39.101933598375609</v>
+      </c>
+      <c r="C17" s="1">
+        <f ca="1">OFFSET(StatCharts!C$2,Sheet2!$A17-1,0)</f>
+        <v>5176.7030278294387</v>
+      </c>
+      <c r="D17" s="1">
+        <f ca="1">OFFSET(StatCharts!D$2,Sheet2!$A17-1,0)</f>
+        <v>583.51933598375604</v>
+      </c>
+      <c r="E17" s="1">
+        <f ca="1">OFFSET(StatCharts!E$2,Sheet2!$A17-1,0)</f>
+        <v>18.847999999999999</v>
+      </c>
+      <c r="F17" s="1">
+        <f ca="1">OFFSET(StatCharts!F$2,Sheet2!$A17-1,0)</f>
+        <v>4476.8675721561976</v>
+      </c>
+      <c r="G17">
+        <f ca="1">OFFSET(StatCharts!G$2,Sheet2!$A17-1,0)</f>
+        <v>61</v>
+      </c>
+      <c r="H17">
+        <f ca="1">OFFSET(StatCharts!H$2,Sheet2!$A17-1,0)</f>
+        <v>26</v>
+      </c>
+    </row>
+    <row r="18" spans="1:8" x14ac:dyDescent="0.4">
+      <c r="A18">
+        <v>80</v>
+      </c>
+      <c r="B18" s="1">
+        <f ca="1">OFFSET(StatCharts!B$2,Sheet2!$A18-1,0)</f>
+        <v>53.6</v>
+      </c>
+      <c r="C18" s="1">
+        <f ca="1">OFFSET(StatCharts!C$2,Sheet2!$A18-1,0)</f>
+        <v>7144.2</v>
+      </c>
+      <c r="D18" s="1">
+        <f ca="1">OFFSET(StatCharts!D$2,Sheet2!$A18-1,0)</f>
+        <v>741</v>
+      </c>
+      <c r="E18" s="1">
+        <f ca="1">OFFSET(StatCharts!E$2,Sheet2!$A18-1,0)</f>
+        <v>19.277999999999999</v>
+      </c>
+      <c r="F18" s="1">
+        <f ca="1">OFFSET(StatCharts!F$2,Sheet2!$A18-1,0)</f>
+        <v>5312.0136943666357</v>
+      </c>
+      <c r="G18">
+        <f ca="1">OFFSET(StatCharts!G$2,Sheet2!$A18-1,0)</f>
+        <v>65</v>
+      </c>
+      <c r="H18">
+        <f ca="1">OFFSET(StatCharts!H$2,Sheet2!$A18-1,0)</f>
+        <v>27</v>
+      </c>
+    </row>
+    <row r="19" spans="1:8" x14ac:dyDescent="0.4">
+      <c r="A19">
+        <v>85</v>
+      </c>
+      <c r="B19" s="1">
+        <f ca="1">OFFSET(StatCharts!B$2,Sheet2!$A19-1,0)</f>
+        <v>64.203867196751233</v>
+      </c>
+      <c r="C19" s="1">
+        <f ca="1">OFFSET(StatCharts!C$2,Sheet2!$A19-1,0)</f>
+        <v>8851.2601964133974</v>
+      </c>
+      <c r="D19" s="1">
+        <f ca="1">OFFSET(StatCharts!D$2,Sheet2!$A19-1,0)</f>
+        <v>859.5386719675123</v>
+      </c>
+      <c r="E19" s="1">
+        <f ca="1">OFFSET(StatCharts!E$2,Sheet2!$A19-1,0)</f>
+        <v>19.608000000000001</v>
+      </c>
+      <c r="F19" s="1">
+        <f ca="1">OFFSET(StatCharts!F$2,Sheet2!$A19-1,0)</f>
+        <v>9396.2668298653607</v>
+      </c>
+      <c r="G19">
+        <f ca="1">OFFSET(StatCharts!G$2,Sheet2!$A19-1,0)</f>
+        <v>69</v>
+      </c>
+      <c r="H19">
+        <f ca="1">OFFSET(StatCharts!H$2,Sheet2!$A19-1,0)</f>
+        <v>29</v>
+      </c>
+    </row>
+    <row r="20" spans="1:8" x14ac:dyDescent="0.4">
+      <c r="A20">
+        <v>90</v>
+      </c>
+      <c r="B20" s="1">
+        <f ca="1">OFFSET(StatCharts!B$2,Sheet2!$A20-1,0)</f>
+        <v>94.2</v>
+      </c>
+      <c r="C20" s="1">
+        <f ca="1">OFFSET(StatCharts!C$2,Sheet2!$A20-1,0)</f>
+        <v>13150.199999999999</v>
+      </c>
+      <c r="D20" s="1">
+        <f ca="1">OFFSET(StatCharts!D$2,Sheet2!$A20-1,0)</f>
+        <v>1172</v>
+      </c>
+      <c r="E20" s="1">
+        <f ca="1">OFFSET(StatCharts!E$2,Sheet2!$A20-1,0)</f>
+        <v>19.838000000000001</v>
+      </c>
+      <c r="F20" s="1">
+        <f ca="1">OFFSET(StatCharts!F$2,Sheet2!$A20-1,0)</f>
+        <v>14699.314447020868</v>
+      </c>
+      <c r="G20">
+        <f ca="1">OFFSET(StatCharts!G$2,Sheet2!$A20-1,0)</f>
+        <v>73</v>
+      </c>
+      <c r="H20">
+        <f ca="1">OFFSET(StatCharts!H$2,Sheet2!$A20-1,0)</f>
+        <v>31</v>
+      </c>
+    </row>
+    <row r="21" spans="1:8" x14ac:dyDescent="0.4">
+      <c r="A21">
+        <v>95</v>
+      </c>
+      <c r="B21" s="1">
+        <f ca="1">OFFSET(StatCharts!B$2,Sheet2!$A21-1,0)</f>
+        <v>115.40773439350247</v>
+      </c>
+      <c r="C21" s="1">
+        <f ca="1">OFFSET(StatCharts!C$2,Sheet2!$A21-1,0)</f>
+        <v>16700.228674335827</v>
+      </c>
+      <c r="D21" s="1">
+        <f ca="1">OFFSET(StatCharts!D$2,Sheet2!$A21-1,0)</f>
+        <v>1396.5773439350246</v>
+      </c>
+      <c r="E21" s="1">
+        <f ca="1">OFFSET(StatCharts!E$2,Sheet2!$A21-1,0)</f>
+        <v>19.968</v>
+      </c>
+      <c r="F21" s="1">
+        <f ca="1">OFFSET(StatCharts!F$2,Sheet2!$A21-1,0)</f>
+        <v>21468.95032051282</v>
+      </c>
+      <c r="G21">
+        <f ca="1">OFFSET(StatCharts!G$2,Sheet2!$A21-1,0)</f>
+        <v>77</v>
+      </c>
+      <c r="H21">
+        <f ca="1">OFFSET(StatCharts!H$2,Sheet2!$A21-1,0)</f>
+        <v>32</v>
+      </c>
+    </row>
+    <row r="22" spans="1:8" x14ac:dyDescent="0.4">
+      <c r="A22">
+        <v>99</v>
+      </c>
+      <c r="B22" s="1">
+        <f ca="1">OFFSET(StatCharts!B$2,Sheet2!$A22-1,0)</f>
+        <v>138.54257833336908</v>
+      </c>
+      <c r="C22" s="1">
+        <f ca="1">OFFSET(StatCharts!C$2,Sheet2!$A22-1,0)</f>
+        <v>20609.001357004952</v>
+      </c>
+      <c r="D22" s="1">
+        <f ca="1">OFFSET(StatCharts!D$2,Sheet2!$A22-1,0)</f>
+        <v>1637.9257833336908</v>
+      </c>
+      <c r="E22" s="1">
+        <f ca="1">OFFSET(StatCharts!E$2,Sheet2!$A22-1,0)</f>
+        <v>20</v>
+      </c>
+      <c r="F22" s="1">
+        <f ca="1">OFFSET(StatCharts!F$2,Sheet2!$A22-1,0)</f>
+        <v>28138.9</v>
+      </c>
+      <c r="G22">
+        <f ca="1">OFFSET(StatCharts!G$2,Sheet2!$A22-1,0)</f>
+        <v>80</v>
+      </c>
+      <c r="H22">
+        <f ca="1">OFFSET(StatCharts!H$2,Sheet2!$A22-1,0)</f>
+        <v>34</v>
       </c>
     </row>
   </sheetData>
@@ -35589,9 +36338,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0E19C42E-4D03-4797-B846-FB5E09BB39D3}">
   <dimension ref="A1:N22"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="L15" sqref="L15"/>
+      <selection pane="bottomLeft" activeCell="P24" sqref="P24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
@@ -36578,7 +37327,7 @@
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C27" sqref="C27"/>
+      <selection pane="bottomLeft" activeCell="Q27" sqref="Q27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
@@ -38275,7 +39024,7 @@
   <dimension ref="A1:M11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
+      <selection activeCell="K23" sqref="K23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
@@ -38744,10 +39493,10 @@
   <dimension ref="A1:H100"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B71" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="C100" sqref="C100"/>
+      <selection pane="bottomRight" sqref="A1:H1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
@@ -42062,7 +42811,7 @@
   <dimension ref="A1:C11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D11" sqref="D11"/>
+      <selection activeCell="F12" sqref="F12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
@@ -42197,8 +42946,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{62CCB73E-E5CD-449F-AA09-CCF4B08E4898}">
   <dimension ref="A1:G100"/>
   <sheetViews>
-    <sheetView topLeftCell="A73" workbookViewId="0">
-      <selection activeCell="B100" sqref="B100"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G2" sqref="G2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>

</xml_diff>

<commit_message>
Big changes on movement and skill usage. Started work on monster skill AI.
</commit_message>
<xml_diff>
--- a/Other/RoStatProcessing.xlsx
+++ b/Other/RoStatProcessing.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26924"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27531"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\ProjectsSSD\RagnarokRebuildTcp\Other\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6239883E-C4C3-46ED-8BF9-BAB92769CE28}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{764F9E13-866A-4351-B5FA-D19957F018FD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3651" yWindow="677" windowWidth="22252" windowHeight="16740" xr2:uid="{1C41742B-2950-4FF8-AA39-6557869B44EA}"/>
+    <workbookView xWindow="720" yWindow="720" windowWidth="27917" windowHeight="13200" xr2:uid="{1C41742B-2950-4FF8-AA39-6557869B44EA}"/>
   </bookViews>
   <sheets>
     <sheet name="StatDef" sheetId="3" r:id="rId1"/>
@@ -49,7 +49,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2826" uniqueCount="1046">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2865" uniqueCount="1063">
   <si>
     <t>Level</t>
   </si>
@@ -3187,6 +3187,57 @@
   </si>
   <si>
     <t>Golem,Elite</t>
+  </si>
+  <si>
+    <t>TARGET_DUMMY</t>
+  </si>
+  <si>
+    <t>Target Dummy</t>
+  </si>
+  <si>
+    <t>barricade.spr</t>
+  </si>
+  <si>
+    <t>Flags</t>
+  </si>
+  <si>
+    <t>Hp#100000</t>
+  </si>
+  <si>
+    <t>constant.spr</t>
+  </si>
+  <si>
+    <t>Test Drone</t>
+  </si>
+  <si>
+    <t>TEST_DRONE</t>
+  </si>
+  <si>
+    <t>AiHyperPacifist</t>
+  </si>
+  <si>
+    <t>RANDGRIS</t>
+  </si>
+  <si>
+    <t>randgris.spr</t>
+  </si>
+  <si>
+    <t>Valkyrie Randgris</t>
+  </si>
+  <si>
+    <t>Angel,WorldBoss</t>
+  </si>
+  <si>
+    <t>Valkyrie</t>
+  </si>
+  <si>
+    <t>VALKYRIE</t>
+  </si>
+  <si>
+    <t>g_randgris.spr</t>
+  </si>
+  <si>
+    <t>Angel,Elite2</t>
   </si>
 </sst>
 </file>
@@ -3268,11 +3319,11 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -3291,9 +3342,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 Theme">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -3331,7 +3382,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2013 - 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -3437,7 +3488,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2013 - 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -3579,7 +3630,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -3587,13 +3638,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{811A97A5-94A7-4FFA-A162-65D076B52481}">
-  <dimension ref="A1:AI286"/>
+  <dimension ref="A1:AJ290"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <pane xSplit="2" ySplit="1" topLeftCell="C34" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="1" topLeftCell="C2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="F46" sqref="F46"/>
+      <selection pane="bottomRight" activeCell="AA1" sqref="AA1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
@@ -3630,9 +3681,10 @@
     <col min="33" max="33" width="11.23046875" bestFit="1" customWidth="1"/>
     <col min="34" max="34" width="12.84375" bestFit="1" customWidth="1"/>
     <col min="35" max="35" width="9.53515625" bestFit="1" customWidth="1"/>
+    <col min="36" max="36" width="15.69140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:35" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:36" x14ac:dyDescent="0.4">
       <c r="A1" t="s">
         <v>46</v>
       </c>
@@ -3738,8 +3790,11 @@
       <c r="AI1" t="s">
         <v>38</v>
       </c>
-    </row>
-    <row r="2" spans="1:35" x14ac:dyDescent="0.4">
+      <c r="AJ1" t="s">
+        <v>1049</v>
+      </c>
+    </row>
+    <row r="2" spans="1:36" x14ac:dyDescent="0.4">
       <c r="A2">
         <v>4000</v>
       </c>
@@ -3846,7 +3901,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:35" x14ac:dyDescent="0.4">
+    <row r="3" spans="1:36" x14ac:dyDescent="0.4">
       <c r="A3">
         <v>5000</v>
       </c>
@@ -3953,7 +4008,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:35" x14ac:dyDescent="0.4">
+    <row r="4" spans="1:36" x14ac:dyDescent="0.4">
       <c r="A4">
         <v>4001</v>
       </c>
@@ -4060,7 +4115,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:35" x14ac:dyDescent="0.4">
+    <row r="5" spans="1:36" x14ac:dyDescent="0.4">
       <c r="A5">
         <v>4002</v>
       </c>
@@ -4167,7 +4222,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:35" x14ac:dyDescent="0.4">
+    <row r="6" spans="1:36" x14ac:dyDescent="0.4">
       <c r="A6">
         <v>4003</v>
       </c>
@@ -4247,7 +4302,7 @@
         <v>1</v>
       </c>
       <c r="AA6">
-        <v>1000</v>
+        <v>-1</v>
       </c>
       <c r="AB6" t="s">
         <v>42</v>
@@ -4274,7 +4329,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:35" x14ac:dyDescent="0.4">
+    <row r="7" spans="1:36" x14ac:dyDescent="0.4">
       <c r="A7">
         <v>4004</v>
       </c>
@@ -4381,7 +4436,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="1:35" x14ac:dyDescent="0.4">
+    <row r="8" spans="1:36" x14ac:dyDescent="0.4">
       <c r="A8">
         <v>4005</v>
       </c>
@@ -4488,7 +4543,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="1:35" x14ac:dyDescent="0.4">
+    <row r="9" spans="1:36" x14ac:dyDescent="0.4">
       <c r="A9">
         <v>4006</v>
       </c>
@@ -4595,7 +4650,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="10" spans="1:35" x14ac:dyDescent="0.4">
+    <row r="10" spans="1:36" x14ac:dyDescent="0.4">
       <c r="A10">
         <v>4007</v>
       </c>
@@ -4702,7 +4757,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="11" spans="1:35" x14ac:dyDescent="0.4">
+    <row r="11" spans="1:36" x14ac:dyDescent="0.4">
       <c r="A11">
         <v>4008</v>
       </c>
@@ -4782,7 +4837,7 @@
         <v>1</v>
       </c>
       <c r="AA11">
-        <v>1000</v>
+        <v>-1</v>
       </c>
       <c r="AB11" t="s">
         <v>42</v>
@@ -4809,7 +4864,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="12" spans="1:35" x14ac:dyDescent="0.4">
+    <row r="12" spans="1:36" x14ac:dyDescent="0.4">
       <c r="A12">
         <v>4009</v>
       </c>
@@ -4916,7 +4971,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="13" spans="1:35" x14ac:dyDescent="0.4">
+    <row r="13" spans="1:36" x14ac:dyDescent="0.4">
       <c r="A13">
         <v>4010</v>
       </c>
@@ -5023,7 +5078,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="14" spans="1:35" x14ac:dyDescent="0.4">
+    <row r="14" spans="1:36" x14ac:dyDescent="0.4">
       <c r="A14">
         <v>4011</v>
       </c>
@@ -5130,7 +5185,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="15" spans="1:35" x14ac:dyDescent="0.4">
+    <row r="15" spans="1:36" x14ac:dyDescent="0.4">
       <c r="A15">
         <v>4012</v>
       </c>
@@ -5237,7 +5292,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="16" spans="1:35" x14ac:dyDescent="0.4">
+    <row r="16" spans="1:36" x14ac:dyDescent="0.4">
       <c r="A16">
         <v>4013</v>
       </c>
@@ -5367,16 +5422,16 @@
         <v>100</v>
       </c>
       <c r="H17">
-        <v>100</v>
+        <v>50</v>
       </c>
       <c r="I17">
-        <v>100</v>
+        <v>110</v>
       </c>
       <c r="J17">
-        <v>100</v>
+        <v>110</v>
       </c>
       <c r="K17">
-        <v>100</v>
+        <v>40</v>
       </c>
       <c r="L17">
         <v>100</v>
@@ -5388,16 +5443,16 @@
         <v>1</v>
       </c>
       <c r="O17">
-        <v>100</v>
+        <v>80</v>
       </c>
       <c r="P17">
-        <v>100</v>
+        <v>80</v>
       </c>
       <c r="Q17">
-        <v>100</v>
+        <v>105</v>
       </c>
       <c r="R17">
-        <v>100</v>
+        <v>90</v>
       </c>
       <c r="S17">
         <v>10</v>
@@ -5801,7 +5856,7 @@
         <v>100</v>
       </c>
       <c r="J21">
-        <v>100</v>
+        <v>75</v>
       </c>
       <c r="K21">
         <v>100</v>
@@ -5852,7 +5907,7 @@
         <v>768</v>
       </c>
       <c r="AA21">
-        <v>1000</v>
+        <v>-1</v>
       </c>
       <c r="AB21" t="s">
         <v>42</v>
@@ -6006,16 +6061,16 @@
         <v>100</v>
       </c>
       <c r="G23">
-        <v>100</v>
+        <v>70</v>
       </c>
       <c r="H23">
-        <v>100</v>
+        <v>80</v>
       </c>
       <c r="I23">
         <v>100</v>
       </c>
       <c r="J23">
-        <v>100</v>
+        <v>110</v>
       </c>
       <c r="K23">
         <v>100</v>
@@ -6220,16 +6275,16 @@
         <v>100</v>
       </c>
       <c r="G25">
-        <v>100</v>
+        <v>70</v>
       </c>
       <c r="H25">
-        <v>100</v>
+        <v>80</v>
       </c>
       <c r="I25">
         <v>100</v>
       </c>
       <c r="J25">
-        <v>100</v>
+        <v>110</v>
       </c>
       <c r="K25">
         <v>100</v>
@@ -6601,7 +6656,7 @@
         <v>1</v>
       </c>
       <c r="AA28">
-        <v>1000</v>
+        <v>-1</v>
       </c>
       <c r="AB28" t="s">
         <v>42</v>
@@ -6972,7 +7027,7 @@
         <v>100</v>
       </c>
       <c r="H32">
-        <v>100</v>
+        <v>150</v>
       </c>
       <c r="I32">
         <v>100</v>
@@ -6984,7 +7039,7 @@
         <v>100</v>
       </c>
       <c r="L32">
-        <v>100</v>
+        <v>110</v>
       </c>
       <c r="M32">
         <v>10</v>
@@ -6993,16 +7048,16 @@
         <v>1</v>
       </c>
       <c r="O32">
-        <v>100</v>
+        <v>140</v>
       </c>
       <c r="P32">
-        <v>100</v>
+        <v>130</v>
       </c>
       <c r="Q32">
-        <v>100</v>
+        <v>120</v>
       </c>
       <c r="R32">
-        <v>100</v>
+        <v>110</v>
       </c>
       <c r="S32">
         <v>10</v>
@@ -10346,7 +10401,7 @@
         <v>1152</v>
       </c>
       <c r="AA63">
-        <v>200</v>
+        <v>-1</v>
       </c>
       <c r="AB63" t="s">
         <v>42</v>
@@ -14305,7 +14360,7 @@
         <v>432</v>
       </c>
       <c r="AA100">
-        <v>1000</v>
+        <v>-1</v>
       </c>
       <c r="AB100" t="s">
         <v>42</v>
@@ -17351,16 +17406,16 @@
         <v>100</v>
       </c>
       <c r="H129">
-        <v>100</v>
+        <v>50</v>
       </c>
       <c r="I129">
-        <v>100</v>
+        <v>110</v>
       </c>
       <c r="J129">
-        <v>100</v>
+        <v>110</v>
       </c>
       <c r="K129">
-        <v>100</v>
+        <v>40</v>
       </c>
       <c r="L129">
         <v>100</v>
@@ -17372,16 +17427,16 @@
         <v>1</v>
       </c>
       <c r="O129">
-        <v>100</v>
+        <v>80</v>
       </c>
       <c r="P129">
-        <v>100</v>
+        <v>80</v>
       </c>
       <c r="Q129">
-        <v>100</v>
+        <v>105</v>
       </c>
       <c r="R129">
-        <v>100</v>
+        <v>90</v>
       </c>
       <c r="S129">
         <v>10</v>
@@ -18692,7 +18747,7 @@
         <v>2016</v>
       </c>
       <c r="AA141">
-        <v>170</v>
+        <v>-1</v>
       </c>
       <c r="AB141" t="s">
         <v>71</v>
@@ -19227,7 +19282,7 @@
         <v>432</v>
       </c>
       <c r="AA146">
-        <v>1000</v>
+        <v>-1</v>
       </c>
       <c r="AB146" t="s">
         <v>42</v>
@@ -32736,7 +32791,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="273" spans="1:35" x14ac:dyDescent="0.4">
+    <row r="273" spans="1:36" x14ac:dyDescent="0.4">
       <c r="A273">
         <v>4270</v>
       </c>
@@ -32843,7 +32898,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="274" spans="1:35" x14ac:dyDescent="0.4">
+    <row r="274" spans="1:36" x14ac:dyDescent="0.4">
       <c r="A274">
         <v>4271</v>
       </c>
@@ -32950,7 +33005,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="275" spans="1:35" x14ac:dyDescent="0.4">
+    <row r="275" spans="1:36" x14ac:dyDescent="0.4">
       <c r="A275">
         <v>4272</v>
       </c>
@@ -33057,7 +33112,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="276" spans="1:35" x14ac:dyDescent="0.4">
+    <row r="276" spans="1:36" x14ac:dyDescent="0.4">
       <c r="A276">
         <v>4273</v>
       </c>
@@ -33164,7 +33219,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="277" spans="1:35" x14ac:dyDescent="0.4">
+    <row r="277" spans="1:36" x14ac:dyDescent="0.4">
       <c r="A277">
         <v>4274</v>
       </c>
@@ -33271,7 +33326,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="278" spans="1:35" x14ac:dyDescent="0.4">
+    <row r="278" spans="1:36" x14ac:dyDescent="0.4">
       <c r="A278">
         <v>4275</v>
       </c>
@@ -33378,7 +33433,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="279" spans="1:35" x14ac:dyDescent="0.4">
+    <row r="279" spans="1:36" x14ac:dyDescent="0.4">
       <c r="A279">
         <v>4276</v>
       </c>
@@ -33485,7 +33540,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="280" spans="1:35" x14ac:dyDescent="0.4">
+    <row r="280" spans="1:36" x14ac:dyDescent="0.4">
       <c r="A280">
         <v>4277</v>
       </c>
@@ -33592,7 +33647,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="281" spans="1:35" x14ac:dyDescent="0.4">
+    <row r="281" spans="1:36" x14ac:dyDescent="0.4">
       <c r="A281">
         <v>4278</v>
       </c>
@@ -33699,7 +33754,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="282" spans="1:35" x14ac:dyDescent="0.4">
+    <row r="282" spans="1:36" x14ac:dyDescent="0.4">
       <c r="A282">
         <v>4279</v>
       </c>
@@ -33806,7 +33861,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="283" spans="1:35" x14ac:dyDescent="0.4">
+    <row r="283" spans="1:36" x14ac:dyDescent="0.4">
       <c r="A283">
         <v>4280</v>
       </c>
@@ -33913,7 +33968,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="284" spans="1:35" x14ac:dyDescent="0.4">
+    <row r="284" spans="1:36" x14ac:dyDescent="0.4">
       <c r="A284">
         <v>4281</v>
       </c>
@@ -34020,7 +34075,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="285" spans="1:35" x14ac:dyDescent="0.4">
+    <row r="285" spans="1:36" x14ac:dyDescent="0.4">
       <c r="A285">
         <v>4282</v>
       </c>
@@ -34100,7 +34155,7 @@
         <v>1332</v>
       </c>
       <c r="AA285">
-        <v>200</v>
+        <v>-1</v>
       </c>
       <c r="AB285" t="s">
         <v>42</v>
@@ -34127,7 +34182,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="286" spans="1:35" x14ac:dyDescent="0.4">
+    <row r="286" spans="1:36" x14ac:dyDescent="0.4">
       <c r="A286">
         <v>4283</v>
       </c>
@@ -34231,6 +34286,440 @@
         <v>0.5</v>
       </c>
       <c r="AI286">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="287" spans="1:36" x14ac:dyDescent="0.4">
+      <c r="A287">
+        <v>4284</v>
+      </c>
+      <c r="B287" t="s">
+        <v>1046</v>
+      </c>
+      <c r="C287" t="s">
+        <v>1047</v>
+      </c>
+      <c r="D287">
+        <v>50</v>
+      </c>
+      <c r="E287">
+        <v>100</v>
+      </c>
+      <c r="F287">
+        <v>100</v>
+      </c>
+      <c r="G287">
+        <v>100</v>
+      </c>
+      <c r="H287">
+        <v>100</v>
+      </c>
+      <c r="I287">
+        <v>100</v>
+      </c>
+      <c r="J287">
+        <v>100</v>
+      </c>
+      <c r="K287">
+        <v>100</v>
+      </c>
+      <c r="L287">
+        <v>100</v>
+      </c>
+      <c r="M287">
+        <v>10</v>
+      </c>
+      <c r="N287">
+        <v>0</v>
+      </c>
+      <c r="O287">
+        <v>100</v>
+      </c>
+      <c r="P287">
+        <v>100</v>
+      </c>
+      <c r="Q287">
+        <v>0</v>
+      </c>
+      <c r="R287">
+        <v>0</v>
+      </c>
+      <c r="S287">
+        <v>10</v>
+      </c>
+      <c r="T287">
+        <v>12</v>
+      </c>
+      <c r="U287" t="s">
+        <v>56</v>
+      </c>
+      <c r="V287" t="s">
+        <v>50</v>
+      </c>
+      <c r="W287" t="s">
+        <v>541</v>
+      </c>
+      <c r="X287">
+        <v>1001</v>
+      </c>
+      <c r="Y287">
+        <v>1</v>
+      </c>
+      <c r="Z287">
+        <v>1000</v>
+      </c>
+      <c r="AA287">
+        <v>-1</v>
+      </c>
+      <c r="AB287" t="s">
+        <v>42</v>
+      </c>
+      <c r="AC287" t="s">
+        <v>587</v>
+      </c>
+      <c r="AD287" t="s">
+        <v>67</v>
+      </c>
+      <c r="AE287">
+        <v>1</v>
+      </c>
+      <c r="AF287" t="s">
+        <v>1048</v>
+      </c>
+      <c r="AG287">
+        <v>0</v>
+      </c>
+      <c r="AH287">
+        <v>-1</v>
+      </c>
+      <c r="AI287">
+        <v>1</v>
+      </c>
+      <c r="AJ287" t="s">
+        <v>1050</v>
+      </c>
+    </row>
+    <row r="288" spans="1:36" x14ac:dyDescent="0.4">
+      <c r="A288">
+        <v>4285</v>
+      </c>
+      <c r="B288" t="s">
+        <v>1053</v>
+      </c>
+      <c r="C288" t="s">
+        <v>1052</v>
+      </c>
+      <c r="D288">
+        <v>50</v>
+      </c>
+      <c r="E288">
+        <v>100</v>
+      </c>
+      <c r="F288">
+        <v>100</v>
+      </c>
+      <c r="G288">
+        <v>100</v>
+      </c>
+      <c r="H288">
+        <v>100</v>
+      </c>
+      <c r="I288">
+        <v>100</v>
+      </c>
+      <c r="J288">
+        <v>100</v>
+      </c>
+      <c r="K288">
+        <v>100</v>
+      </c>
+      <c r="L288">
+        <v>100</v>
+      </c>
+      <c r="M288">
+        <v>10</v>
+      </c>
+      <c r="N288">
+        <v>1</v>
+      </c>
+      <c r="O288">
+        <v>100</v>
+      </c>
+      <c r="P288">
+        <v>100</v>
+      </c>
+      <c r="Q288">
+        <v>0</v>
+      </c>
+      <c r="R288">
+        <v>0</v>
+      </c>
+      <c r="S288">
+        <v>10</v>
+      </c>
+      <c r="T288">
+        <v>12</v>
+      </c>
+      <c r="U288" t="s">
+        <v>56</v>
+      </c>
+      <c r="V288" t="s">
+        <v>50</v>
+      </c>
+      <c r="W288" t="s">
+        <v>575</v>
+      </c>
+      <c r="X288">
+        <v>1000</v>
+      </c>
+      <c r="Y288">
+        <v>0</v>
+      </c>
+      <c r="Z288">
+        <v>1000</v>
+      </c>
+      <c r="AA288">
+        <v>150</v>
+      </c>
+      <c r="AB288" t="s">
+        <v>42</v>
+      </c>
+      <c r="AC288" t="s">
+        <v>42</v>
+      </c>
+      <c r="AD288" t="s">
+        <v>1054</v>
+      </c>
+      <c r="AE288">
+        <v>1</v>
+      </c>
+      <c r="AF288" t="s">
+        <v>1051</v>
+      </c>
+      <c r="AG288">
+        <v>0</v>
+      </c>
+      <c r="AH288">
+        <v>0.5</v>
+      </c>
+      <c r="AI288">
+        <v>1</v>
+      </c>
+      <c r="AJ288" t="s">
+        <v>1050</v>
+      </c>
+    </row>
+    <row r="289" spans="1:35" x14ac:dyDescent="0.4">
+      <c r="A289">
+        <v>4286</v>
+      </c>
+      <c r="B289" t="s">
+        <v>1055</v>
+      </c>
+      <c r="C289" t="s">
+        <v>1057</v>
+      </c>
+      <c r="D289">
+        <v>99</v>
+      </c>
+      <c r="E289">
+        <v>100</v>
+      </c>
+      <c r="F289">
+        <v>100</v>
+      </c>
+      <c r="G289">
+        <v>100</v>
+      </c>
+      <c r="H289">
+        <v>100</v>
+      </c>
+      <c r="I289">
+        <v>100</v>
+      </c>
+      <c r="J289">
+        <v>100</v>
+      </c>
+      <c r="K289">
+        <v>100</v>
+      </c>
+      <c r="L289">
+        <v>100</v>
+      </c>
+      <c r="M289">
+        <v>10</v>
+      </c>
+      <c r="N289">
+        <v>3</v>
+      </c>
+      <c r="O289">
+        <v>100</v>
+      </c>
+      <c r="P289">
+        <v>100</v>
+      </c>
+      <c r="Q289">
+        <v>100</v>
+      </c>
+      <c r="R289">
+        <v>100</v>
+      </c>
+      <c r="S289">
+        <v>10</v>
+      </c>
+      <c r="T289">
+        <v>12</v>
+      </c>
+      <c r="U289" t="s">
+        <v>156</v>
+      </c>
+      <c r="V289" t="s">
+        <v>228</v>
+      </c>
+      <c r="W289" t="s">
+        <v>229</v>
+      </c>
+      <c r="X289">
+        <v>576</v>
+      </c>
+      <c r="Y289">
+        <v>480</v>
+      </c>
+      <c r="Z289">
+        <v>576</v>
+      </c>
+      <c r="AA289">
+        <v>100</v>
+      </c>
+      <c r="AB289" t="s">
+        <v>71</v>
+      </c>
+      <c r="AC289" t="s">
+        <v>1058</v>
+      </c>
+      <c r="AD289" t="s">
+        <v>72</v>
+      </c>
+      <c r="AE289">
+        <v>525</v>
+      </c>
+      <c r="AF289" t="s">
+        <v>1056</v>
+      </c>
+      <c r="AG289">
+        <v>0</v>
+      </c>
+      <c r="AH289">
+        <v>0.5</v>
+      </c>
+      <c r="AI289">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="290" spans="1:35" x14ac:dyDescent="0.4">
+      <c r="A290">
+        <v>4287</v>
+      </c>
+      <c r="B290" t="s">
+        <v>1060</v>
+      </c>
+      <c r="C290" t="s">
+        <v>1059</v>
+      </c>
+      <c r="D290">
+        <v>99</v>
+      </c>
+      <c r="E290">
+        <v>100</v>
+      </c>
+      <c r="F290">
+        <v>100</v>
+      </c>
+      <c r="G290">
+        <v>100</v>
+      </c>
+      <c r="H290">
+        <v>100</v>
+      </c>
+      <c r="I290">
+        <v>100</v>
+      </c>
+      <c r="J290">
+        <v>100</v>
+      </c>
+      <c r="K290">
+        <v>100</v>
+      </c>
+      <c r="L290">
+        <v>90</v>
+      </c>
+      <c r="M290">
+        <v>10</v>
+      </c>
+      <c r="N290">
+        <v>3</v>
+      </c>
+      <c r="O290">
+        <v>100</v>
+      </c>
+      <c r="P290">
+        <v>100</v>
+      </c>
+      <c r="Q290">
+        <v>100</v>
+      </c>
+      <c r="R290">
+        <v>100</v>
+      </c>
+      <c r="S290">
+        <v>10</v>
+      </c>
+      <c r="T290">
+        <v>12</v>
+      </c>
+      <c r="U290" t="s">
+        <v>156</v>
+      </c>
+      <c r="V290" t="s">
+        <v>228</v>
+      </c>
+      <c r="W290" t="s">
+        <v>229</v>
+      </c>
+      <c r="X290">
+        <v>576</v>
+      </c>
+      <c r="Y290">
+        <v>480</v>
+      </c>
+      <c r="Z290">
+        <v>576</v>
+      </c>
+      <c r="AA290">
+        <v>100</v>
+      </c>
+      <c r="AB290" t="s">
+        <v>71</v>
+      </c>
+      <c r="AC290" t="s">
+        <v>1062</v>
+      </c>
+      <c r="AD290" t="s">
+        <v>72</v>
+      </c>
+      <c r="AE290">
+        <v>525</v>
+      </c>
+      <c r="AF290" t="s">
+        <v>1061</v>
+      </c>
+      <c r="AG290">
+        <v>0</v>
+      </c>
+      <c r="AH290">
+        <v>0.5</v>
+      </c>
+      <c r="AI290">
         <v>1</v>
       </c>
     </row>
@@ -34247,7 +34736,7 @@
   <dimension ref="A1:F6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E28" sqref="E28"/>
+      <selection activeCell="E11" sqref="E11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
@@ -35611,28 +36100,28 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.4">
-      <c r="A1" s="7" t="s">
+      <c r="A1" s="6" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="8" t="s">
+      <c r="B1" s="7" t="s">
         <v>2</v>
       </c>
-      <c r="C1" s="8" t="s">
-        <v>1</v>
-      </c>
-      <c r="D1" s="8" t="s">
+      <c r="C1" s="7" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" s="7" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="8" t="s">
+      <c r="E1" s="7" t="s">
         <v>45</v>
       </c>
-      <c r="F1" s="8" t="s">
+      <c r="F1" s="7" t="s">
         <v>21</v>
       </c>
-      <c r="G1" s="7" t="s">
+      <c r="G1" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="7" t="s">
+      <c r="H1" s="6" t="s">
         <v>7</v>
       </c>
     </row>
@@ -36340,7 +36829,7 @@
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="P24" sqref="P24"/>
+      <selection pane="bottomLeft" activeCell="H8" sqref="E8:H8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
@@ -39024,7 +39513,7 @@
   <dimension ref="A1:M11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="K23" sqref="K23"/>
+      <selection activeCell="C16" sqref="C16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
@@ -39493,10 +39982,10 @@
   <dimension ref="A1:H100"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="B74" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" sqref="A1:H1"/>
+      <selection pane="bottomRight" activeCell="H100" sqref="H100"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
@@ -45445,7 +45934,7 @@
   <dimension ref="A1:S10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A3" sqref="A3:S10"/>
+      <selection activeCell="H24" sqref="H24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
@@ -45454,21 +45943,21 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:19" x14ac:dyDescent="0.4">
-      <c r="G1" s="6" t="s">
+      <c r="G1" s="8" t="s">
         <v>918</v>
       </c>
-      <c r="H1" s="6"/>
-      <c r="I1" s="6"/>
-      <c r="J1" s="6"/>
-      <c r="K1" s="6"/>
-      <c r="L1" s="6"/>
-      <c r="M1" s="6"/>
-      <c r="N1" s="6"/>
-      <c r="O1" s="6"/>
-      <c r="P1" s="6"/>
-      <c r="Q1" s="6"/>
-      <c r="R1" s="6"/>
-      <c r="S1" s="6"/>
+      <c r="H1" s="8"/>
+      <c r="I1" s="8"/>
+      <c r="J1" s="8"/>
+      <c r="K1" s="8"/>
+      <c r="L1" s="8"/>
+      <c r="M1" s="8"/>
+      <c r="N1" s="8"/>
+      <c r="O1" s="8"/>
+      <c r="P1" s="8"/>
+      <c r="Q1" s="8"/>
+      <c r="R1" s="8"/>
+      <c r="S1" s="8"/>
     </row>
     <row r="2" spans="1:19" x14ac:dyDescent="0.4">
       <c r="A2" s="5" t="s">
@@ -46015,7 +46504,7 @@
   <dimension ref="A1:B14"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B14" sqref="A1:B14"/>
+      <selection activeCell="H16" sqref="H16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>

</xml_diff>

<commit_message>
Re-balancing mjolnir dead pit for some reason.
</commit_message>
<xml_diff>
--- a/Other/RoStatProcessing.xlsx
+++ b/Other/RoStatProcessing.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\ProjectsSSD\RagnarokRebuildTcp\Other\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B1928F0A-0C17-4BA0-B91C-C0FBE7E7713A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8E911FF2-4999-4EA3-9D4A-163CE4375039}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1191" yWindow="2074" windowWidth="27918" windowHeight="13200" xr2:uid="{1C41742B-2950-4FF8-AA39-6557869B44EA}"/>
   </bookViews>
@@ -51,7 +51,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2957" uniqueCount="1096">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2957" uniqueCount="1098">
   <si>
     <t>Id</t>
   </si>
@@ -3080,6 +3080,78 @@
     <t>shinobi.spr</t>
   </si>
   <si>
+    <t>KAPHA</t>
+  </si>
+  <si>
+    <t>Kappa</t>
+  </si>
+  <si>
+    <t>kapha.spr</t>
+  </si>
+  <si>
+    <t>KARAKASA</t>
+  </si>
+  <si>
+    <t>Karakasa</t>
+  </si>
+  <si>
+    <t>karakasa.spr</t>
+  </si>
+  <si>
+    <t>TENGU</t>
+  </si>
+  <si>
+    <t>Sake Tengu</t>
+  </si>
+  <si>
+    <t>tengu.spr</t>
+  </si>
+  <si>
+    <t>ANTIQUE_FIRELOCK</t>
+  </si>
+  <si>
+    <t>Firelock Soldier</t>
+  </si>
+  <si>
+    <t>antique_firelock.spr</t>
+  </si>
+  <si>
+    <t>INCANTATION_SAMURAI</t>
+  </si>
+  <si>
+    <t>Samurai Specter</t>
+  </si>
+  <si>
+    <t>incantation_samurai.spr</t>
+  </si>
+  <si>
+    <t>MIYABI_NINGYO</t>
+  </si>
+  <si>
+    <t>Miyabi Doll</t>
+  </si>
+  <si>
+    <t>miyabi_ningyo.spr</t>
+  </si>
+  <si>
+    <t>THE_PAPER</t>
+  </si>
+  <si>
+    <t>Ittan-Momen</t>
+  </si>
+  <si>
+    <t>the_paper.spr</t>
+  </si>
+  <si>
+    <t>POISON_TOAD</t>
+  </si>
+  <si>
+    <t>Poison Toad</t>
+  </si>
+  <si>
+    <t>poison_toad.spr</t>
+  </si>
+  <si>
     <t>Mdef</t>
   </si>
   <si>
@@ -3269,92 +3341,20 @@
     <t>Assets/Sprites/Weapons/Swordsman/Female/검사_여_1207.spr</t>
   </si>
   <si>
-    <t>KAPHA</t>
-  </si>
-  <si>
-    <t>kapha.spr</t>
-  </si>
-  <si>
-    <t>KARAKASA</t>
-  </si>
-  <si>
-    <t>karakasa.spr</t>
-  </si>
-  <si>
-    <t>TENGU</t>
-  </si>
-  <si>
-    <t>tengu.spr</t>
-  </si>
-  <si>
-    <t>ANTIQUE_FIRELOCK</t>
-  </si>
-  <si>
-    <t>antique_firelock.spr</t>
-  </si>
-  <si>
-    <t>INCANTATION_SAMURAI</t>
-  </si>
-  <si>
-    <t>incantation_samurai.spr</t>
-  </si>
-  <si>
-    <t>MIYABI_NINGYO</t>
-  </si>
-  <si>
-    <t>miyabi_ningyo.spr</t>
-  </si>
-  <si>
-    <t>THE_PAPER</t>
-  </si>
-  <si>
-    <t>the_paper.spr</t>
-  </si>
-  <si>
-    <t>Kappa</t>
-  </si>
-  <si>
-    <t>Karakasa</t>
-  </si>
-  <si>
-    <t>Firelock Soldier</t>
-  </si>
-  <si>
-    <t>Ittan-Momen</t>
-  </si>
-  <si>
-    <t>Samurai Specter</t>
-  </si>
-  <si>
-    <t>Sake Tengu</t>
-  </si>
-  <si>
-    <t>POISON_TOAD</t>
-  </si>
-  <si>
-    <t>poison_toad.spr</t>
-  </si>
-  <si>
-    <t>Poison Toad</t>
-  </si>
-  <si>
-    <t>Miyabi Doll</t>
+    <t>Small,Brute</t>
+  </si>
+  <si>
+    <t>Undead,Buff</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="8"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -3787,11 +3787,11 @@
   <dimension ref="A1:AJ300"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A13" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <pane xSplit="3" ySplit="1" topLeftCell="M226" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="3" ySplit="1" topLeftCell="D214" activePane="bottomRight" state="frozen"/>
       <selection activeCell="A13" sqref="A13"/>
       <selection pane="topRight" activeCell="D13" sqref="D13"/>
       <selection pane="bottomLeft" activeCell="A14" sqref="A14"/>
-      <selection pane="bottomRight" activeCell="AE244" sqref="AE244"/>
+      <selection pane="bottomRight" activeCell="Q231" sqref="Q231"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
@@ -5210,7 +5210,7 @@
         <v>59</v>
       </c>
       <c r="AE13">
-        <v>960</v>
+        <v>166</v>
       </c>
       <c r="AF13" t="s">
         <v>86</v>
@@ -5531,7 +5531,7 @@
         <v>59</v>
       </c>
       <c r="AE16">
-        <v>960</v>
+        <v>166</v>
       </c>
       <c r="AF16" t="s">
         <v>96</v>
@@ -5959,7 +5959,7 @@
         <v>59</v>
       </c>
       <c r="AE20">
-        <v>2016</v>
+        <v>182</v>
       </c>
       <c r="AF20" t="s">
         <v>110</v>
@@ -8099,7 +8099,7 @@
         <v>99</v>
       </c>
       <c r="AE40">
-        <v>864</v>
+        <v>324</v>
       </c>
       <c r="AF40" t="s">
         <v>182</v>
@@ -8420,7 +8420,7 @@
         <v>99</v>
       </c>
       <c r="AE43">
-        <v>672</v>
+        <v>603</v>
       </c>
       <c r="AF43" t="s">
         <v>193</v>
@@ -8527,7 +8527,7 @@
         <v>59</v>
       </c>
       <c r="AE44">
-        <v>960</v>
+        <v>166</v>
       </c>
       <c r="AF44" t="s">
         <v>196</v>
@@ -10453,7 +10453,7 @@
         <v>99</v>
       </c>
       <c r="AE62">
-        <v>672</v>
+        <v>336</v>
       </c>
       <c r="AF62" t="s">
         <v>264</v>
@@ -12084,7 +12084,7 @@
         <v>317</v>
       </c>
       <c r="D78">
-        <v>29</v>
+        <v>33</v>
       </c>
       <c r="E78">
         <v>100</v>
@@ -15482,7 +15482,7 @@
         <v>59</v>
       </c>
       <c r="AE109">
-        <v>960</v>
+        <v>166</v>
       </c>
       <c r="AF109" t="s">
         <v>416</v>
@@ -15910,7 +15910,7 @@
         <v>42</v>
       </c>
       <c r="AE113">
-        <v>840</v>
+        <v>562</v>
       </c>
       <c r="AF113" t="s">
         <v>429</v>
@@ -20511,7 +20511,7 @@
         <v>59</v>
       </c>
       <c r="AE156">
-        <v>960</v>
+        <v>166</v>
       </c>
       <c r="AF156" t="s">
         <v>574</v>
@@ -20618,7 +20618,7 @@
         <v>99</v>
       </c>
       <c r="AE157">
-        <v>1152</v>
+        <v>900</v>
       </c>
       <c r="AF157" t="s">
         <v>577</v>
@@ -21682,13 +21682,13 @@
         <v>41</v>
       </c>
       <c r="AC167" t="s">
-        <v>41</v>
+        <v>1096</v>
       </c>
       <c r="AD167" t="s">
         <v>99</v>
       </c>
       <c r="AE167">
-        <v>648</v>
+        <v>620</v>
       </c>
       <c r="AF167" t="s">
         <v>608</v>
@@ -22249,7 +22249,7 @@
         <v>626</v>
       </c>
       <c r="D173">
-        <v>18</v>
+        <v>28</v>
       </c>
       <c r="E173">
         <v>100</v>
@@ -22544,7 +22544,7 @@
         <v>99</v>
       </c>
       <c r="AE175">
-        <v>1152</v>
+        <v>1080</v>
       </c>
       <c r="AF175" t="s">
         <v>633</v>
@@ -27038,7 +27038,7 @@
         <v>99</v>
       </c>
       <c r="AE217">
-        <v>263</v>
+        <v>269</v>
       </c>
       <c r="AF217" t="s">
         <v>768</v>
@@ -27573,7 +27573,7 @@
         <v>99</v>
       </c>
       <c r="AE222">
-        <v>1152</v>
+        <v>660</v>
       </c>
       <c r="AF222" t="s">
         <v>785</v>
@@ -28455,7 +28455,7 @@
         <v>814</v>
       </c>
       <c r="D231">
-        <v>30</v>
+        <v>40</v>
       </c>
       <c r="E231">
         <v>100</v>
@@ -28470,7 +28470,7 @@
         <v>100</v>
       </c>
       <c r="I231">
-        <v>100</v>
+        <v>90</v>
       </c>
       <c r="J231">
         <v>100</v>
@@ -28479,7 +28479,7 @@
         <v>100</v>
       </c>
       <c r="L231">
-        <v>100</v>
+        <v>130</v>
       </c>
       <c r="M231">
         <v>5</v>
@@ -28494,7 +28494,7 @@
         <v>100</v>
       </c>
       <c r="Q231">
-        <v>100</v>
+        <v>110</v>
       </c>
       <c r="R231">
         <v>100</v>
@@ -28530,7 +28530,7 @@
         <v>41</v>
       </c>
       <c r="AC231" t="s">
-        <v>470</v>
+        <v>1097</v>
       </c>
       <c r="AD231" t="s">
         <v>99</v>
@@ -28562,7 +28562,7 @@
         <v>817</v>
       </c>
       <c r="D232">
-        <v>38</v>
+        <v>48</v>
       </c>
       <c r="E232">
         <v>100</v>
@@ -28637,7 +28637,7 @@
         <v>41</v>
       </c>
       <c r="AC232" t="s">
-        <v>41</v>
+        <v>286</v>
       </c>
       <c r="AD232" t="s">
         <v>99</v>
@@ -29392,7 +29392,7 @@
         <v>99</v>
       </c>
       <c r="AE239">
-        <v>540</v>
+        <v>522</v>
       </c>
       <c r="AF239" t="s">
         <v>840</v>
@@ -35069,7 +35069,7 @@
         <v>99</v>
       </c>
       <c r="AE292">
-        <v>720</v>
+        <v>480</v>
       </c>
       <c r="AF292" t="s">
         <v>1008</v>
@@ -35089,10 +35089,10 @@
         <v>4290</v>
       </c>
       <c r="B293" t="s">
-        <v>1072</v>
+        <v>1009</v>
       </c>
       <c r="C293" t="s">
-        <v>1086</v>
+        <v>1010</v>
       </c>
       <c r="D293">
         <v>41</v>
@@ -35179,7 +35179,7 @@
         <v>576</v>
       </c>
       <c r="AF293" t="s">
-        <v>1073</v>
+        <v>1011</v>
       </c>
       <c r="AG293">
         <v>0</v>
@@ -35196,10 +35196,10 @@
         <v>4291</v>
       </c>
       <c r="B294" t="s">
-        <v>1074</v>
+        <v>1012</v>
       </c>
       <c r="C294" t="s">
-        <v>1087</v>
+        <v>1013</v>
       </c>
       <c r="D294">
         <v>30</v>
@@ -35286,7 +35286,7 @@
         <v>432</v>
       </c>
       <c r="AF294" t="s">
-        <v>1075</v>
+        <v>1014</v>
       </c>
       <c r="AG294">
         <v>0</v>
@@ -35303,10 +35303,10 @@
         <v>4292</v>
       </c>
       <c r="B295" t="s">
-        <v>1076</v>
+        <v>1015</v>
       </c>
       <c r="C295" t="s">
-        <v>1091</v>
+        <v>1016</v>
       </c>
       <c r="D295">
         <v>65</v>
@@ -35393,7 +35393,7 @@
         <v>624</v>
       </c>
       <c r="AF295" t="s">
-        <v>1077</v>
+        <v>1017</v>
       </c>
       <c r="AG295">
         <v>0</v>
@@ -35410,10 +35410,10 @@
         <v>4293</v>
       </c>
       <c r="B296" t="s">
-        <v>1078</v>
+        <v>1018</v>
       </c>
       <c r="C296" t="s">
-        <v>1088</v>
+        <v>1019</v>
       </c>
       <c r="D296">
         <v>47</v>
@@ -35500,7 +35500,7 @@
         <v>480</v>
       </c>
       <c r="AF296" t="s">
-        <v>1079</v>
+        <v>1020</v>
       </c>
       <c r="AG296">
         <v>0</v>
@@ -35517,10 +35517,10 @@
         <v>4294</v>
       </c>
       <c r="B297" t="s">
-        <v>1080</v>
+        <v>1021</v>
       </c>
       <c r="C297" t="s">
-        <v>1090</v>
+        <v>1022</v>
       </c>
       <c r="D297">
         <v>71</v>
@@ -35604,10 +35604,10 @@
         <v>99</v>
       </c>
       <c r="AE297">
-        <v>768</v>
+        <v>425</v>
       </c>
       <c r="AF297" t="s">
-        <v>1081</v>
+        <v>1023</v>
       </c>
       <c r="AG297">
         <v>0</v>
@@ -35624,10 +35624,10 @@
         <v>4295</v>
       </c>
       <c r="B298" t="s">
-        <v>1082</v>
+        <v>1024</v>
       </c>
       <c r="C298" t="s">
-        <v>1095</v>
+        <v>1025</v>
       </c>
       <c r="D298">
         <v>33</v>
@@ -35714,7 +35714,7 @@
         <v>672</v>
       </c>
       <c r="AF298" t="s">
-        <v>1083</v>
+        <v>1026</v>
       </c>
       <c r="AG298">
         <v>0</v>
@@ -35731,10 +35731,10 @@
         <v>4296</v>
       </c>
       <c r="B299" t="s">
-        <v>1084</v>
+        <v>1027</v>
       </c>
       <c r="C299" t="s">
-        <v>1089</v>
+        <v>1028</v>
       </c>
       <c r="D299">
         <v>56</v>
@@ -35821,7 +35821,7 @@
         <v>540</v>
       </c>
       <c r="AF299" t="s">
-        <v>1085</v>
+        <v>1029</v>
       </c>
       <c r="AG299">
         <v>0</v>
@@ -35838,10 +35838,10 @@
         <v>4297</v>
       </c>
       <c r="B300" t="s">
-        <v>1092</v>
+        <v>1030</v>
       </c>
       <c r="C300" t="s">
-        <v>1094</v>
+        <v>1031</v>
       </c>
       <c r="D300">
         <v>46</v>
@@ -35928,7 +35928,7 @@
         <v>624</v>
       </c>
       <c r="AF300" t="s">
-        <v>1093</v>
+        <v>1032</v>
       </c>
       <c r="AG300">
         <v>0</v>
@@ -35944,7 +35944,6 @@
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:AI179">
     <sortCondition ref="D2:D179"/>
   </sortState>
-  <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <tableParts count="1">
     <tablePart r:id="rId1"/>
@@ -35972,30 +35971,30 @@
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A1" t="s">
-        <v>1010</v>
+        <v>1034</v>
       </c>
       <c r="B1" t="s">
         <v>28</v>
       </c>
       <c r="C1" t="s">
-        <v>1064</v>
+        <v>1088</v>
       </c>
       <c r="D1" t="s">
-        <v>1065</v>
+        <v>1089</v>
       </c>
       <c r="E1" t="s">
-        <v>1024</v>
+        <v>1048</v>
       </c>
       <c r="F1" t="s">
-        <v>1025</v>
+        <v>1049</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A2" t="s">
-        <v>1039</v>
+        <v>1063</v>
       </c>
       <c r="B2" t="s">
-        <v>1026</v>
+        <v>1050</v>
       </c>
       <c r="C2">
         <v>0</v>
@@ -36006,10 +36005,10 @@
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A3" t="s">
-        <v>1039</v>
+        <v>1063</v>
       </c>
       <c r="B3" t="s">
-        <v>1027</v>
+        <v>1051</v>
       </c>
       <c r="C3">
         <v>0</v>
@@ -36018,18 +36017,18 @@
         <v>2</v>
       </c>
       <c r="E3" t="s">
-        <v>1066</v>
+        <v>1090</v>
       </c>
       <c r="F3" t="s">
-        <v>1067</v>
+        <v>1091</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A4" t="s">
-        <v>1039</v>
+        <v>1063</v>
       </c>
       <c r="B4" t="s">
-        <v>1028</v>
+        <v>1052</v>
       </c>
       <c r="C4">
         <v>0</v>
@@ -36038,18 +36037,18 @@
         <v>2</v>
       </c>
       <c r="E4" t="s">
-        <v>1068</v>
+        <v>1092</v>
       </c>
       <c r="F4" t="s">
-        <v>1069</v>
+        <v>1093</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A5" t="s">
-        <v>1042</v>
+        <v>1066</v>
       </c>
       <c r="B5" t="s">
-        <v>1026</v>
+        <v>1050</v>
       </c>
       <c r="C5">
         <v>0</v>
@@ -36060,10 +36059,10 @@
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A6" t="s">
-        <v>1042</v>
+        <v>1066</v>
       </c>
       <c r="B6" t="s">
-        <v>1027</v>
+        <v>1051</v>
       </c>
       <c r="C6">
         <v>0</v>
@@ -36072,10 +36071,10 @@
         <v>2</v>
       </c>
       <c r="E6" t="s">
-        <v>1070</v>
+        <v>1094</v>
       </c>
       <c r="F6" t="s">
-        <v>1071</v>
+        <v>1095</v>
       </c>
     </row>
   </sheetData>
@@ -36099,7 +36098,7 @@
         <v>3</v>
       </c>
       <c r="B1" t="s">
-        <v>1015</v>
+        <v>1039</v>
       </c>
       <c r="C1" t="s">
         <v>4</v>
@@ -37325,7 +37324,7 @@
         <v>3</v>
       </c>
       <c r="B1" s="7" t="s">
-        <v>1015</v>
+        <v>1039</v>
       </c>
       <c r="C1" s="7" t="s">
         <v>4</v>
@@ -37334,13 +37333,13 @@
         <v>11</v>
       </c>
       <c r="E1" s="7" t="s">
-        <v>1016</v>
+        <v>1040</v>
       </c>
       <c r="F1" s="7" t="s">
         <v>16</v>
       </c>
       <c r="G1" s="6" t="s">
-        <v>1017</v>
+        <v>1041</v>
       </c>
       <c r="H1" s="6" t="s">
         <v>14</v>
@@ -38090,21 +38089,21 @@
         <v>14</v>
       </c>
       <c r="K1" t="s">
-        <v>1009</v>
+        <v>1033</v>
       </c>
       <c r="L1" t="s">
         <v>16</v>
       </c>
       <c r="M1" t="s">
-        <v>1010</v>
+        <v>1034</v>
       </c>
       <c r="N1" t="s">
-        <v>1011</v>
+        <v>1035</v>
       </c>
     </row>
     <row r="2" spans="1:14" x14ac:dyDescent="0.4">
       <c r="A2" t="s">
-        <v>1012</v>
+        <v>1036</v>
       </c>
       <c r="B2">
         <v>0</v>
@@ -38324,7 +38323,7 @@
     </row>
     <row r="7" spans="1:14" x14ac:dyDescent="0.4">
       <c r="A7" t="s">
-        <v>1013</v>
+        <v>1037</v>
       </c>
       <c r="B7">
         <v>100</v>
@@ -39162,13 +39161,13 @@
         <v>14</v>
       </c>
       <c r="K1" t="s">
-        <v>1009</v>
+        <v>1033</v>
       </c>
       <c r="L1" t="s">
         <v>16</v>
       </c>
       <c r="M1" t="s">
-        <v>1010</v>
+        <v>1034</v>
       </c>
     </row>
     <row r="2" spans="1:13" x14ac:dyDescent="0.4">
@@ -40116,7 +40115,7 @@
     </row>
     <row r="25" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A25" t="s">
-        <v>1014</v>
+        <v>1038</v>
       </c>
       <c r="B25">
         <v>100</v>
@@ -40862,13 +40861,13 @@
         <v>14</v>
       </c>
       <c r="K1" t="s">
-        <v>1009</v>
+        <v>1033</v>
       </c>
       <c r="L1" t="s">
         <v>16</v>
       </c>
       <c r="M1" t="s">
-        <v>1010</v>
+        <v>1034</v>
       </c>
     </row>
     <row r="2" spans="1:13" x14ac:dyDescent="0.4">
@@ -41310,7 +41309,7 @@
         <v>3</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>1015</v>
+        <v>1039</v>
       </c>
       <c r="C1" s="1" t="s">
         <v>4</v>
@@ -41319,13 +41318,13 @@
         <v>11</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>1016</v>
+        <v>1040</v>
       </c>
       <c r="F1" s="1" t="s">
         <v>16</v>
       </c>
       <c r="G1" t="s">
-        <v>1017</v>
+        <v>1041</v>
       </c>
       <c r="H1" t="s">
         <v>14</v>
@@ -44616,18 +44615,18 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A1" t="s">
-        <v>1018</v>
+        <v>1042</v>
       </c>
       <c r="B1" t="s">
-        <v>1019</v>
+        <v>1043</v>
       </c>
       <c r="C1" t="s">
-        <v>1020</v>
+        <v>1044</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A2" t="s">
-        <v>1021</v>
+        <v>1045</v>
       </c>
       <c r="B2">
         <v>0.1</v>
@@ -44726,7 +44725,7 @@
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A11" t="s">
-        <v>1009</v>
+        <v>1033</v>
       </c>
       <c r="B11">
         <v>7.4999999999999997E-2</v>
@@ -47253,7 +47252,7 @@
   <sheetData>
     <row r="1" spans="1:19" x14ac:dyDescent="0.4">
       <c r="G1" s="8" t="s">
-        <v>1022</v>
+        <v>1046</v>
       </c>
       <c r="H1" s="8"/>
       <c r="I1" s="8"/>
@@ -47279,52 +47278,52 @@
         <v>4</v>
       </c>
       <c r="D2" s="5" t="s">
-        <v>1023</v>
+        <v>1047</v>
       </c>
       <c r="E2" s="5" t="s">
-        <v>1024</v>
+        <v>1048</v>
       </c>
       <c r="F2" s="5" t="s">
-        <v>1025</v>
+        <v>1049</v>
       </c>
       <c r="G2" s="4" t="s">
-        <v>1026</v>
+        <v>1050</v>
       </c>
       <c r="H2" s="4" t="s">
-        <v>1027</v>
+        <v>1051</v>
       </c>
       <c r="I2" s="4" t="s">
-        <v>1028</v>
+        <v>1052</v>
       </c>
       <c r="J2" s="4" t="s">
-        <v>1029</v>
+        <v>1053</v>
       </c>
       <c r="K2" s="4" t="s">
-        <v>1030</v>
+        <v>1054</v>
       </c>
       <c r="L2" s="4" t="s">
-        <v>1031</v>
+        <v>1055</v>
       </c>
       <c r="M2" s="4" t="s">
-        <v>1032</v>
+        <v>1056</v>
       </c>
       <c r="N2" s="4" t="s">
-        <v>1033</v>
+        <v>1057</v>
       </c>
       <c r="O2" s="4" t="s">
-        <v>1034</v>
+        <v>1058</v>
       </c>
       <c r="P2" s="4" t="s">
-        <v>1035</v>
+        <v>1059</v>
       </c>
       <c r="Q2" s="4" t="s">
-        <v>1036</v>
+        <v>1060</v>
       </c>
       <c r="R2" s="4" t="s">
-        <v>1037</v>
+        <v>1061</v>
       </c>
       <c r="S2" s="4" t="s">
-        <v>1038</v>
+        <v>1062</v>
       </c>
     </row>
     <row r="3" spans="1:19" x14ac:dyDescent="0.4">
@@ -47332,7 +47331,7 @@
         <v>0</v>
       </c>
       <c r="B3" t="s">
-        <v>1039</v>
+        <v>1063</v>
       </c>
       <c r="C3">
         <v>1</v>
@@ -47341,10 +47340,10 @@
         <v>1</v>
       </c>
       <c r="E3" t="s">
-        <v>1040</v>
+        <v>1064</v>
       </c>
       <c r="F3" t="s">
-        <v>1041</v>
+        <v>1065</v>
       </c>
       <c r="G3">
         <v>1</v>
@@ -47391,7 +47390,7 @@
         <v>1</v>
       </c>
       <c r="B4" t="s">
-        <v>1042</v>
+        <v>1066</v>
       </c>
       <c r="C4">
         <v>1.6</v>
@@ -47400,10 +47399,10 @@
         <v>1</v>
       </c>
       <c r="E4" t="s">
-        <v>1043</v>
+        <v>1067</v>
       </c>
       <c r="F4" t="s">
-        <v>1044</v>
+        <v>1068</v>
       </c>
       <c r="G4">
         <v>1</v>
@@ -47450,7 +47449,7 @@
         <v>2</v>
       </c>
       <c r="B5" t="s">
-        <v>1045</v>
+        <v>1069</v>
       </c>
       <c r="C5">
         <v>1.1499999999999999</v>
@@ -47459,10 +47458,10 @@
         <v>1.5</v>
       </c>
       <c r="E5" t="s">
-        <v>1046</v>
+        <v>1070</v>
       </c>
       <c r="F5" t="s">
-        <v>1047</v>
+        <v>1071</v>
       </c>
       <c r="G5">
         <v>1</v>
@@ -47509,7 +47508,7 @@
         <v>3</v>
       </c>
       <c r="B6" t="s">
-        <v>1048</v>
+        <v>1072</v>
       </c>
       <c r="C6">
         <v>1.1000000000000001</v>
@@ -47518,10 +47517,10 @@
         <v>1.8</v>
       </c>
       <c r="E6" t="s">
-        <v>1049</v>
+        <v>1073</v>
       </c>
       <c r="F6" t="s">
-        <v>1050</v>
+        <v>1074</v>
       </c>
       <c r="G6">
         <v>1</v>
@@ -47568,7 +47567,7 @@
         <v>4</v>
       </c>
       <c r="B7" t="s">
-        <v>1051</v>
+        <v>1075</v>
       </c>
       <c r="C7">
         <v>1.2</v>
@@ -47577,10 +47576,10 @@
         <v>1.6</v>
       </c>
       <c r="E7" t="s">
-        <v>1052</v>
+        <v>1076</v>
       </c>
       <c r="F7" t="s">
-        <v>1053</v>
+        <v>1077</v>
       </c>
       <c r="G7">
         <v>1</v>
@@ -47627,7 +47626,7 @@
         <v>5</v>
       </c>
       <c r="B8" t="s">
-        <v>1054</v>
+        <v>1078</v>
       </c>
       <c r="C8">
         <v>1.3</v>
@@ -47636,10 +47635,10 @@
         <v>1.3</v>
       </c>
       <c r="E8" t="s">
-        <v>1055</v>
+        <v>1079</v>
       </c>
       <c r="F8" t="s">
-        <v>1056</v>
+        <v>1080</v>
       </c>
       <c r="G8">
         <v>1</v>
@@ -47686,7 +47685,7 @@
         <v>6</v>
       </c>
       <c r="B9" t="s">
-        <v>1057</v>
+        <v>1081</v>
       </c>
       <c r="C9">
         <v>1.4</v>
@@ -47695,10 +47694,10 @@
         <v>1.4</v>
       </c>
       <c r="E9" t="s">
-        <v>1058</v>
+        <v>1082</v>
       </c>
       <c r="F9" t="s">
-        <v>1059</v>
+        <v>1083</v>
       </c>
       <c r="G9">
         <v>1</v>
@@ -47745,7 +47744,7 @@
         <v>200</v>
       </c>
       <c r="B10" t="s">
-        <v>1060</v>
+        <v>1084</v>
       </c>
       <c r="C10">
         <v>1</v>
@@ -47754,10 +47753,10 @@
         <v>1</v>
       </c>
       <c r="E10" t="s">
-        <v>1061</v>
+        <v>1085</v>
       </c>
       <c r="F10" t="s">
-        <v>1062</v>
+        <v>1086</v>
       </c>
       <c r="G10">
         <v>1</v>
@@ -47826,7 +47825,7 @@
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>1063</v>
+        <v>1087</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.4">
@@ -47834,7 +47833,7 @@
         <v>0</v>
       </c>
       <c r="B2" t="s">
-        <v>1026</v>
+        <v>1050</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.4">
@@ -47842,7 +47841,7 @@
         <v>1</v>
       </c>
       <c r="B3" t="s">
-        <v>1027</v>
+        <v>1051</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.4">
@@ -47850,7 +47849,7 @@
         <v>2</v>
       </c>
       <c r="B4" t="s">
-        <v>1028</v>
+        <v>1052</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.4">
@@ -47858,7 +47857,7 @@
         <v>3</v>
       </c>
       <c r="B5" t="s">
-        <v>1029</v>
+        <v>1053</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.4">
@@ -47866,7 +47865,7 @@
         <v>4</v>
       </c>
       <c r="B6" t="s">
-        <v>1030</v>
+        <v>1054</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.4">
@@ -47874,7 +47873,7 @@
         <v>5</v>
       </c>
       <c r="B7" t="s">
-        <v>1031</v>
+        <v>1055</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.4">
@@ -47882,7 +47881,7 @@
         <v>6</v>
       </c>
       <c r="B8" t="s">
-        <v>1032</v>
+        <v>1056</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.4">
@@ -47890,7 +47889,7 @@
         <v>7</v>
       </c>
       <c r="B9" t="s">
-        <v>1033</v>
+        <v>1057</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.4">
@@ -47898,7 +47897,7 @@
         <v>8</v>
       </c>
       <c r="B10" t="s">
-        <v>1034</v>
+        <v>1058</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.4">
@@ -47906,7 +47905,7 @@
         <v>9</v>
       </c>
       <c r="B11" t="s">
-        <v>1035</v>
+        <v>1059</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.4">
@@ -47914,7 +47913,7 @@
         <v>10</v>
       </c>
       <c r="B12" t="s">
-        <v>1036</v>
+        <v>1060</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.4">
@@ -47922,7 +47921,7 @@
         <v>11</v>
       </c>
       <c r="B13" t="s">
-        <v>1037</v>
+        <v>1061</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.4">
@@ -47930,7 +47929,7 @@
         <v>12</v>
       </c>
       <c r="B14" t="s">
-        <v>1038</v>
+        <v>1062</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Movement rework and a bunch of other stuff too.
</commit_message>
<xml_diff>
--- a/Other/RoStatProcessing.xlsx
+++ b/Other/RoStatProcessing.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27628"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27830"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\ProjectsSSD\RagnarokRebuildTcp\Other\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{49A408D0-40F3-4509-BFAF-FC40EBED44AE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D23214C7-82EB-49CF-9DCD-2C1DCCA85CA4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3583" yWindow="2923" windowWidth="27797" windowHeight="13903" xr2:uid="{1C41742B-2950-4FF8-AA39-6557869B44EA}"/>
+    <workbookView xWindow="3771" yWindow="3771" windowWidth="24686" windowHeight="13055" xr2:uid="{1C41742B-2950-4FF8-AA39-6557869B44EA}"/>
   </bookViews>
   <sheets>
     <sheet name="StatDef" sheetId="3" r:id="rId1"/>
@@ -51,7 +51,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2966" uniqueCount="1105">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2976" uniqueCount="1108">
   <si>
     <t>Id</t>
   </si>
@@ -3366,6 +3366,15 @@
   </si>
   <si>
     <t>V3</t>
+  </si>
+  <si>
+    <t>Golem,Ranged</t>
+  </si>
+  <si>
+    <t>MOONLIGHT_CLONE</t>
+  </si>
+  <si>
+    <t>Color#FFFFFF80</t>
   </si>
 </sst>
 </file>
@@ -3805,13 +3814,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{811A97A5-94A7-4FFA-A162-65D076B52481}">
-  <dimension ref="A1:AJ300"/>
+  <dimension ref="A1:AJ301"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <pane xSplit="3" ySplit="1" topLeftCell="D278" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="3" ySplit="1" topLeftCell="D269" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="Q296" sqref="Q296"/>
+      <selection pane="bottomRight" activeCell="A301" sqref="A301"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
@@ -3848,7 +3857,7 @@
     <col min="33" max="33" width="13.3828125" bestFit="1" customWidth="1"/>
     <col min="34" max="34" width="14.84375" bestFit="1" customWidth="1"/>
     <col min="35" max="35" width="11.3828125" bestFit="1" customWidth="1"/>
-    <col min="36" max="36" width="10.15234375" bestFit="1" customWidth="1"/>
+    <col min="36" max="36" width="13.84375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:36" x14ac:dyDescent="0.4">
@@ -4403,7 +4412,7 @@
         <v>6</v>
       </c>
       <c r="E6">
-        <v>70</v>
+        <v>80</v>
       </c>
       <c r="F6">
         <v>100</v>
@@ -25268,7 +25277,7 @@
         <v>28</v>
       </c>
       <c r="E201">
-        <v>100</v>
+        <v>150</v>
       </c>
       <c r="F201">
         <v>100</v>
@@ -25277,19 +25286,19 @@
         <v>100</v>
       </c>
       <c r="H201">
-        <v>100</v>
+        <v>30</v>
       </c>
       <c r="I201">
-        <v>100</v>
+        <v>30</v>
       </c>
       <c r="J201">
-        <v>100</v>
+        <v>30</v>
       </c>
       <c r="K201">
         <v>100</v>
       </c>
       <c r="L201">
-        <v>100</v>
+        <v>30</v>
       </c>
       <c r="M201">
         <v>5</v>
@@ -25298,10 +25307,10 @@
         <v>1</v>
       </c>
       <c r="O201">
-        <v>100</v>
+        <v>50</v>
       </c>
       <c r="P201">
-        <v>100</v>
+        <v>50</v>
       </c>
       <c r="Q201">
         <v>100</v>
@@ -25340,7 +25349,7 @@
         <v>41</v>
       </c>
       <c r="AC201" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="AD201" t="s">
         <v>59</v>
@@ -34328,7 +34337,7 @@
         <v>41</v>
       </c>
       <c r="AC285" t="s">
-        <v>188</v>
+        <v>1105</v>
       </c>
       <c r="AD285" t="s">
         <v>115</v>
@@ -34640,7 +34649,7 @@
         <v>1000</v>
       </c>
       <c r="Y288">
-        <v>0</v>
+        <v>500</v>
       </c>
       <c r="Z288">
         <v>1000</v>
@@ -34676,7 +34685,7 @@
         <v>990</v>
       </c>
     </row>
-    <row r="289" spans="1:35" x14ac:dyDescent="0.4">
+    <row r="289" spans="1:36" x14ac:dyDescent="0.4">
       <c r="A289">
         <v>4286</v>
       </c>
@@ -34783,7 +34792,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="290" spans="1:35" x14ac:dyDescent="0.4">
+    <row r="290" spans="1:36" x14ac:dyDescent="0.4">
       <c r="A290">
         <v>4287</v>
       </c>
@@ -34890,7 +34899,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="291" spans="1:35" x14ac:dyDescent="0.4">
+    <row r="291" spans="1:36" x14ac:dyDescent="0.4">
       <c r="A291">
         <v>4288</v>
       </c>
@@ -34997,7 +35006,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="292" spans="1:35" x14ac:dyDescent="0.4">
+    <row r="292" spans="1:36" x14ac:dyDescent="0.4">
       <c r="A292">
         <v>4289</v>
       </c>
@@ -35104,7 +35113,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="293" spans="1:35" x14ac:dyDescent="0.4">
+    <row r="293" spans="1:36" x14ac:dyDescent="0.4">
       <c r="A293">
         <v>4290</v>
       </c>
@@ -35211,7 +35220,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="294" spans="1:35" x14ac:dyDescent="0.4">
+    <row r="294" spans="1:36" x14ac:dyDescent="0.4">
       <c r="A294">
         <v>4291</v>
       </c>
@@ -35318,7 +35327,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="295" spans="1:35" x14ac:dyDescent="0.4">
+    <row r="295" spans="1:36" x14ac:dyDescent="0.4">
       <c r="A295">
         <v>4292</v>
       </c>
@@ -35425,7 +35434,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="296" spans="1:35" x14ac:dyDescent="0.4">
+    <row r="296" spans="1:36" x14ac:dyDescent="0.4">
       <c r="A296">
         <v>4293</v>
       </c>
@@ -35460,7 +35469,7 @@
         <v>100</v>
       </c>
       <c r="L296">
-        <v>120</v>
+        <v>150</v>
       </c>
       <c r="M296">
         <v>10</v>
@@ -35475,10 +35484,10 @@
         <v>100</v>
       </c>
       <c r="Q296">
-        <v>110</v>
+        <v>130</v>
       </c>
       <c r="R296">
-        <v>100</v>
+        <v>130</v>
       </c>
       <c r="S296">
         <v>10</v>
@@ -35532,7 +35541,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="297" spans="1:35" x14ac:dyDescent="0.4">
+    <row r="297" spans="1:36" x14ac:dyDescent="0.4">
       <c r="A297">
         <v>4294</v>
       </c>
@@ -35639,7 +35648,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="298" spans="1:35" x14ac:dyDescent="0.4">
+    <row r="298" spans="1:36" x14ac:dyDescent="0.4">
       <c r="A298">
         <v>4295</v>
       </c>
@@ -35746,7 +35755,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="299" spans="1:35" x14ac:dyDescent="0.4">
+    <row r="299" spans="1:36" x14ac:dyDescent="0.4">
       <c r="A299">
         <v>4296</v>
       </c>
@@ -35853,7 +35862,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="300" spans="1:35" x14ac:dyDescent="0.4">
+    <row r="300" spans="1:36" x14ac:dyDescent="0.4">
       <c r="A300">
         <v>4297</v>
       </c>
@@ -35958,6 +35967,116 @@
       </c>
       <c r="AI300">
         <v>1</v>
+      </c>
+    </row>
+    <row r="301" spans="1:36" x14ac:dyDescent="0.4">
+      <c r="A301">
+        <v>4298</v>
+      </c>
+      <c r="B301" t="s">
+        <v>1106</v>
+      </c>
+      <c r="C301" t="s">
+        <v>566</v>
+      </c>
+      <c r="D301">
+        <v>67</v>
+      </c>
+      <c r="E301">
+        <v>15</v>
+      </c>
+      <c r="F301">
+        <v>100</v>
+      </c>
+      <c r="G301">
+        <v>80</v>
+      </c>
+      <c r="H301">
+        <v>100</v>
+      </c>
+      <c r="I301">
+        <v>100</v>
+      </c>
+      <c r="J301">
+        <v>100</v>
+      </c>
+      <c r="K301">
+        <v>130</v>
+      </c>
+      <c r="L301">
+        <v>80</v>
+      </c>
+      <c r="M301">
+        <v>10</v>
+      </c>
+      <c r="N301">
+        <v>1</v>
+      </c>
+      <c r="O301">
+        <v>100</v>
+      </c>
+      <c r="P301">
+        <v>100</v>
+      </c>
+      <c r="Q301">
+        <v>0</v>
+      </c>
+      <c r="R301">
+        <v>0</v>
+      </c>
+      <c r="S301">
+        <v>10</v>
+      </c>
+      <c r="T301">
+        <v>12</v>
+      </c>
+      <c r="U301" t="s">
+        <v>38</v>
+      </c>
+      <c r="V301" t="s">
+        <v>219</v>
+      </c>
+      <c r="W301" t="s">
+        <v>274</v>
+      </c>
+      <c r="X301">
+        <v>1276</v>
+      </c>
+      <c r="Y301">
+        <v>288</v>
+      </c>
+      <c r="Z301">
+        <v>576</v>
+      </c>
+      <c r="AA301">
+        <v>150</v>
+      </c>
+      <c r="AB301" t="s">
+        <v>119</v>
+      </c>
+      <c r="AC301" t="s">
+        <v>567</v>
+      </c>
+      <c r="AD301" t="s">
+        <v>99</v>
+      </c>
+      <c r="AE301">
+        <v>180</v>
+      </c>
+      <c r="AF301" t="s">
+        <v>568</v>
+      </c>
+      <c r="AG301">
+        <v>0</v>
+      </c>
+      <c r="AH301">
+        <v>0.5</v>
+      </c>
+      <c r="AI301">
+        <v>1</v>
+      </c>
+      <c r="AJ301" t="s">
+        <v>1107</v>
       </c>
     </row>
   </sheetData>
@@ -38069,7 +38188,7 @@
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C25" sqref="C25"/>
+      <selection pane="bottomLeft" activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
@@ -38214,7 +38333,7 @@
         <v>58</v>
       </c>
       <c r="B4">
-        <v>300</v>
+        <v>220</v>
       </c>
       <c r="C4">
         <v>10</v>

</xml_diff>

<commit_message>
Added optional color data for monsters and cleaned up moonlight flower's AI.
</commit_message>
<xml_diff>
--- a/Other/RoStatProcessing.xlsx
+++ b/Other/RoStatProcessing.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\ProjectsSSD\RagnarokRebuildTcp\Other\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D23214C7-82EB-49CF-9DCD-2C1DCCA85CA4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4DAD45C8-8EDC-43BC-B534-8954001128FF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="3771" yWindow="3771" windowWidth="24686" windowHeight="13055" xr2:uid="{1C41742B-2950-4FF8-AA39-6557869B44EA}"/>
   </bookViews>
@@ -3374,7 +3374,7 @@
     <t>MOONLIGHT_CLONE</t>
   </si>
   <si>
-    <t>Color#FFFFFF80</t>
+    <t>Color#FFFFFFAA</t>
   </si>
 </sst>
 </file>
@@ -3817,10 +3817,10 @@
   <dimension ref="A1:AJ301"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <pane xSplit="3" ySplit="1" topLeftCell="D269" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="3" ySplit="1" topLeftCell="W281" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="A301" sqref="A301"/>
+      <selection pane="bottomRight" activeCell="AJ302" sqref="AJ302"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>

</xml_diff>

<commit_message>
Implemented the heal skill and related visual effects.
</commit_message>
<xml_diff>
--- a/Other/RoStatProcessing.xlsx
+++ b/Other/RoStatProcessing.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\ProjectsSSD\RagnarokRebuildTcp\Other\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4DAD45C8-8EDC-43BC-B534-8954001128FF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9B6CDA93-0B70-417C-B2F2-D3CC1CA427E4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="3771" yWindow="3771" windowWidth="24686" windowHeight="13055" xr2:uid="{1C41742B-2950-4FF8-AA39-6557869B44EA}"/>
   </bookViews>
@@ -51,7 +51,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2976" uniqueCount="1108">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2976" uniqueCount="1109">
   <si>
     <t>Id</t>
   </si>
@@ -3375,6 +3375,9 @@
   </si>
   <si>
     <t>Color#FFFFFFAA</t>
+  </si>
+  <si>
+    <t>Plant,Buff</t>
   </si>
 </sst>
 </file>
@@ -3817,10 +3820,10 @@
   <dimension ref="A1:AJ301"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <pane xSplit="3" ySplit="1" topLeftCell="W281" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="3" ySplit="1" topLeftCell="D50" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="AJ302" sqref="AJ302"/>
+      <selection pane="bottomRight" activeCell="I53" sqref="I53"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
@@ -9447,7 +9450,7 @@
         <v>100</v>
       </c>
       <c r="G53">
-        <v>100</v>
+        <v>180</v>
       </c>
       <c r="H53">
         <v>100</v>
@@ -18923,7 +18926,7 @@
         <v>2016</v>
       </c>
       <c r="AA141">
-        <v>-1</v>
+        <v>100</v>
       </c>
       <c r="AB141" t="s">
         <v>119</v>
@@ -30199,16 +30202,16 @@
         <v>56</v>
       </c>
       <c r="E247">
-        <v>100</v>
+        <v>95</v>
       </c>
       <c r="F247">
         <v>100</v>
       </c>
       <c r="G247">
-        <v>130</v>
+        <v>160</v>
       </c>
       <c r="H247">
-        <v>100</v>
+        <v>120</v>
       </c>
       <c r="I247">
         <v>100</v>
@@ -30217,7 +30220,7 @@
         <v>100</v>
       </c>
       <c r="K247">
-        <v>100</v>
+        <v>80</v>
       </c>
       <c r="L247">
         <v>100</v>
@@ -30229,16 +30232,16 @@
         <v>3</v>
       </c>
       <c r="O247">
-        <v>100</v>
+        <v>110</v>
       </c>
       <c r="P247">
-        <v>100</v>
+        <v>110</v>
       </c>
       <c r="Q247">
-        <v>100</v>
+        <v>120</v>
       </c>
       <c r="R247">
-        <v>100</v>
+        <v>115</v>
       </c>
       <c r="S247">
         <v>10</v>
@@ -30271,7 +30274,7 @@
         <v>41</v>
       </c>
       <c r="AC247" t="s">
-        <v>39</v>
+        <v>1108</v>
       </c>
       <c r="AD247" t="s">
         <v>115</v>

</xml_diff>

<commit_message>
Skill and attack timing shenanigans.
</commit_message>
<xml_diff>
--- a/Other/RoStatProcessing.xlsx
+++ b/Other/RoStatProcessing.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\ProjectsSSD\RagnarokRebuildTcp\Other\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9B6CDA93-0B70-417C-B2F2-D3CC1CA427E4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{810BA49F-5F5D-43DD-9A27-DC71B9F75010}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="3771" yWindow="3771" windowWidth="24686" windowHeight="13055" xr2:uid="{1C41742B-2950-4FF8-AA39-6557869B44EA}"/>
   </bookViews>
@@ -3820,10 +3820,10 @@
   <dimension ref="A1:AJ301"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <pane xSplit="3" ySplit="1" topLeftCell="D50" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="3" ySplit="1" topLeftCell="D145" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="I53" sqref="I53"/>
+      <selection pane="bottomRight" activeCell="N161" sqref="N161"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
@@ -21000,22 +21000,22 @@
         <v>64</v>
       </c>
       <c r="E161">
-        <v>100</v>
+        <v>90</v>
       </c>
       <c r="F161">
         <v>100</v>
       </c>
       <c r="G161">
-        <v>130</v>
+        <v>180</v>
       </c>
       <c r="H161">
-        <v>100</v>
+        <v>90</v>
       </c>
       <c r="I161">
-        <v>100</v>
+        <v>110</v>
       </c>
       <c r="J161">
-        <v>100</v>
+        <v>80</v>
       </c>
       <c r="K161">
         <v>100</v>
@@ -21033,7 +21033,7 @@
         <v>100</v>
       </c>
       <c r="P161">
-        <v>100</v>
+        <v>110</v>
       </c>
       <c r="Q161">
         <v>100</v>

</xml_diff>

<commit_message>
Hit animation, sprite trail, and other bug fixes.
</commit_message>
<xml_diff>
--- a/Other/RoStatProcessing.xlsx
+++ b/Other/RoStatProcessing.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\ProjectsSSD\RagnarokRebuildTcp\Other\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{810BA49F-5F5D-43DD-9A27-DC71B9F75010}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AD5E5D14-C1BE-4D6A-BEA9-40FF37E16889}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="3771" yWindow="3771" windowWidth="24686" windowHeight="13055" xr2:uid="{1C41742B-2950-4FF8-AA39-6557869B44EA}"/>
   </bookViews>
@@ -3137,9 +3137,6 @@
     <t>THE_PAPER</t>
   </si>
   <si>
-    <t>Ittan-Momen</t>
-  </si>
-  <si>
     <t>the_paper.spr</t>
   </si>
   <si>
@@ -3378,6 +3375,9 @@
   </si>
   <si>
     <t>Plant,Buff</t>
+  </si>
+  <si>
+    <t>The Paper</t>
   </si>
 </sst>
 </file>
@@ -3820,10 +3820,10 @@
   <dimension ref="A1:AJ301"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <pane xSplit="3" ySplit="1" topLeftCell="D145" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="3" ySplit="1" topLeftCell="D283" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="N161" sqref="N161"/>
+      <selection pane="bottomRight" activeCell="C299" sqref="C299"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
@@ -5022,7 +5022,7 @@
         <v>41</v>
       </c>
       <c r="AC11" t="s">
-        <v>1102</v>
+        <v>1101</v>
       </c>
       <c r="AD11" t="s">
         <v>59</v>
@@ -11121,7 +11121,7 @@
         <v>41</v>
       </c>
       <c r="AC68" t="s">
-        <v>1101</v>
+        <v>1100</v>
       </c>
       <c r="AD68" t="s">
         <v>99</v>
@@ -21006,7 +21006,7 @@
         <v>100</v>
       </c>
       <c r="G161">
-        <v>180</v>
+        <v>150</v>
       </c>
       <c r="H161">
         <v>90</v>
@@ -21030,16 +21030,16 @@
         <v>3</v>
       </c>
       <c r="O161">
-        <v>100</v>
+        <v>90</v>
       </c>
       <c r="P161">
         <v>110</v>
       </c>
       <c r="Q161">
-        <v>100</v>
+        <v>110</v>
       </c>
       <c r="R161">
-        <v>110</v>
+        <v>120</v>
       </c>
       <c r="S161">
         <v>10</v>
@@ -21714,7 +21714,7 @@
         <v>41</v>
       </c>
       <c r="AC167" t="s">
-        <v>1096</v>
+        <v>1095</v>
       </c>
       <c r="AD167" t="s">
         <v>99</v>
@@ -28562,7 +28562,7 @@
         <v>41</v>
       </c>
       <c r="AC231" t="s">
-        <v>1097</v>
+        <v>1096</v>
       </c>
       <c r="AD231" t="s">
         <v>99</v>
@@ -30274,7 +30274,7 @@
         <v>41</v>
       </c>
       <c r="AC247" t="s">
-        <v>1108</v>
+        <v>1107</v>
       </c>
       <c r="AD247" t="s">
         <v>115</v>
@@ -34340,7 +34340,7 @@
         <v>41</v>
       </c>
       <c r="AC285" t="s">
-        <v>1105</v>
+        <v>1104</v>
       </c>
       <c r="AD285" t="s">
         <v>115</v>
@@ -35766,7 +35766,7 @@
         <v>1027</v>
       </c>
       <c r="C299" t="s">
-        <v>1028</v>
+        <v>1108</v>
       </c>
       <c r="D299">
         <v>56</v>
@@ -35853,7 +35853,7 @@
         <v>540</v>
       </c>
       <c r="AF299" t="s">
-        <v>1029</v>
+        <v>1028</v>
       </c>
       <c r="AG299">
         <v>0</v>
@@ -35870,10 +35870,10 @@
         <v>4297</v>
       </c>
       <c r="B300" t="s">
+        <v>1029</v>
+      </c>
+      <c r="C300" t="s">
         <v>1030</v>
-      </c>
-      <c r="C300" t="s">
-        <v>1031</v>
       </c>
       <c r="D300">
         <v>46</v>
@@ -35960,7 +35960,7 @@
         <v>624</v>
       </c>
       <c r="AF300" t="s">
-        <v>1032</v>
+        <v>1031</v>
       </c>
       <c r="AG300">
         <v>0</v>
@@ -35977,7 +35977,7 @@
         <v>4298</v>
       </c>
       <c r="B301" t="s">
-        <v>1106</v>
+        <v>1105</v>
       </c>
       <c r="C301" t="s">
         <v>566</v>
@@ -36079,7 +36079,7 @@
         <v>1</v>
       </c>
       <c r="AJ301" t="s">
-        <v>1107</v>
+        <v>1106</v>
       </c>
     </row>
   </sheetData>
@@ -36113,30 +36113,30 @@
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A1" t="s">
-        <v>1034</v>
+        <v>1033</v>
       </c>
       <c r="B1" t="s">
         <v>28</v>
       </c>
       <c r="C1" t="s">
+        <v>1087</v>
+      </c>
+      <c r="D1" t="s">
         <v>1088</v>
       </c>
-      <c r="D1" t="s">
-        <v>1089</v>
-      </c>
       <c r="E1" t="s">
+        <v>1047</v>
+      </c>
+      <c r="F1" t="s">
         <v>1048</v>
-      </c>
-      <c r="F1" t="s">
-        <v>1049</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A2" t="s">
-        <v>1063</v>
+        <v>1062</v>
       </c>
       <c r="B2" t="s">
-        <v>1050</v>
+        <v>1049</v>
       </c>
       <c r="C2">
         <v>0</v>
@@ -36147,10 +36147,10 @@
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A3" t="s">
-        <v>1063</v>
+        <v>1062</v>
       </c>
       <c r="B3" t="s">
-        <v>1051</v>
+        <v>1050</v>
       </c>
       <c r="C3">
         <v>0</v>
@@ -36159,18 +36159,18 @@
         <v>2</v>
       </c>
       <c r="E3" t="s">
+        <v>1089</v>
+      </c>
+      <c r="F3" t="s">
         <v>1090</v>
-      </c>
-      <c r="F3" t="s">
-        <v>1091</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A4" t="s">
-        <v>1063</v>
+        <v>1062</v>
       </c>
       <c r="B4" t="s">
-        <v>1052</v>
+        <v>1051</v>
       </c>
       <c r="C4">
         <v>0</v>
@@ -36179,18 +36179,18 @@
         <v>2</v>
       </c>
       <c r="E4" t="s">
+        <v>1091</v>
+      </c>
+      <c r="F4" t="s">
         <v>1092</v>
-      </c>
-      <c r="F4" t="s">
-        <v>1093</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A5" t="s">
-        <v>1066</v>
+        <v>1065</v>
       </c>
       <c r="B5" t="s">
-        <v>1050</v>
+        <v>1049</v>
       </c>
       <c r="C5">
         <v>0</v>
@@ -36201,10 +36201,10 @@
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A6" t="s">
-        <v>1066</v>
+        <v>1065</v>
       </c>
       <c r="B6" t="s">
-        <v>1051</v>
+        <v>1050</v>
       </c>
       <c r="C6">
         <v>0</v>
@@ -36213,10 +36213,10 @@
         <v>2</v>
       </c>
       <c r="E6" t="s">
+        <v>1093</v>
+      </c>
+      <c r="F6" t="s">
         <v>1094</v>
-      </c>
-      <c r="F6" t="s">
-        <v>1095</v>
       </c>
     </row>
   </sheetData>
@@ -36240,7 +36240,7 @@
         <v>3</v>
       </c>
       <c r="B1" t="s">
-        <v>1039</v>
+        <v>1038</v>
       </c>
       <c r="C1" t="s">
         <v>4</v>
@@ -37466,7 +37466,7 @@
         <v>3</v>
       </c>
       <c r="B1" s="7" t="s">
-        <v>1039</v>
+        <v>1038</v>
       </c>
       <c r="C1" s="7" t="s">
         <v>4</v>
@@ -37475,13 +37475,13 @@
         <v>11</v>
       </c>
       <c r="E1" s="7" t="s">
-        <v>1040</v>
+        <v>1039</v>
       </c>
       <c r="F1" s="7" t="s">
         <v>16</v>
       </c>
       <c r="G1" s="6" t="s">
-        <v>1041</v>
+        <v>1040</v>
       </c>
       <c r="H1" s="6" t="s">
         <v>14</v>
@@ -38231,21 +38231,21 @@
         <v>14</v>
       </c>
       <c r="K1" t="s">
-        <v>1033</v>
+        <v>1032</v>
       </c>
       <c r="L1" t="s">
         <v>16</v>
       </c>
       <c r="M1" t="s">
+        <v>1033</v>
+      </c>
+      <c r="N1" t="s">
         <v>1034</v>
-      </c>
-      <c r="N1" t="s">
-        <v>1035</v>
       </c>
     </row>
     <row r="2" spans="1:14" x14ac:dyDescent="0.4">
       <c r="A2" t="s">
-        <v>1036</v>
+        <v>1035</v>
       </c>
       <c r="B2">
         <v>0</v>
@@ -38465,7 +38465,7 @@
     </row>
     <row r="7" spans="1:14" x14ac:dyDescent="0.4">
       <c r="A7" t="s">
-        <v>1037</v>
+        <v>1036</v>
       </c>
       <c r="B7">
         <v>100</v>
@@ -39303,13 +39303,13 @@
         <v>14</v>
       </c>
       <c r="K1" t="s">
-        <v>1033</v>
+        <v>1032</v>
       </c>
       <c r="L1" t="s">
         <v>16</v>
       </c>
       <c r="M1" t="s">
-        <v>1034</v>
+        <v>1033</v>
       </c>
     </row>
     <row r="2" spans="1:13" x14ac:dyDescent="0.4">
@@ -40257,7 +40257,7 @@
     </row>
     <row r="25" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A25" t="s">
-        <v>1038</v>
+        <v>1037</v>
       </c>
       <c r="B25">
         <v>100</v>
@@ -41003,13 +41003,13 @@
         <v>14</v>
       </c>
       <c r="K1" t="s">
-        <v>1033</v>
+        <v>1032</v>
       </c>
       <c r="L1" t="s">
         <v>16</v>
       </c>
       <c r="M1" t="s">
-        <v>1034</v>
+        <v>1033</v>
       </c>
     </row>
     <row r="2" spans="1:13" x14ac:dyDescent="0.4">
@@ -41452,7 +41452,7 @@
         <v>3</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>1039</v>
+        <v>1038</v>
       </c>
       <c r="C1" s="1" t="s">
         <v>4</v>
@@ -41461,13 +41461,13 @@
         <v>11</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>1040</v>
+        <v>1039</v>
       </c>
       <c r="F1" s="1" t="s">
         <v>16</v>
       </c>
       <c r="G1" t="s">
-        <v>1041</v>
+        <v>1040</v>
       </c>
       <c r="H1" t="s">
         <v>14</v>
@@ -45160,21 +45160,21 @@
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A1" t="s">
+        <v>1041</v>
+      </c>
+      <c r="B1" t="s">
         <v>1042</v>
       </c>
-      <c r="B1" t="s">
+      <c r="C1" t="s">
         <v>1043</v>
       </c>
-      <c r="C1" t="s">
-        <v>1044</v>
-      </c>
       <c r="E1" t="s">
-        <v>1103</v>
+        <v>1102</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A2" t="s">
-        <v>1045</v>
+        <v>1044</v>
       </c>
       <c r="B2">
         <v>0.05</v>
@@ -45309,7 +45309,7 @@
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A11" t="s">
-        <v>1033</v>
+        <v>1032</v>
       </c>
       <c r="B11">
         <v>7.4999999999999997E-2</v>
@@ -45351,19 +45351,19 @@
         <v>3</v>
       </c>
       <c r="N1" t="s">
-        <v>1100</v>
+        <v>1099</v>
       </c>
       <c r="O1" t="s">
         <v>3</v>
       </c>
       <c r="P1" t="s">
-        <v>1099</v>
+        <v>1098</v>
       </c>
       <c r="Q1" t="s">
         <v>3</v>
       </c>
       <c r="R1" t="s">
-        <v>1104</v>
+        <v>1103</v>
       </c>
     </row>
     <row r="2" spans="1:20" x14ac:dyDescent="0.4">
@@ -51704,7 +51704,7 @@
     </row>
     <row r="106" spans="1:20" x14ac:dyDescent="0.4">
       <c r="L106" t="s">
-        <v>1098</v>
+        <v>1097</v>
       </c>
     </row>
   </sheetData>
@@ -51727,7 +51727,7 @@
   <sheetData>
     <row r="1" spans="1:19" x14ac:dyDescent="0.4">
       <c r="G1" s="8" t="s">
-        <v>1046</v>
+        <v>1045</v>
       </c>
       <c r="H1" s="8"/>
       <c r="I1" s="8"/>
@@ -51753,52 +51753,52 @@
         <v>4</v>
       </c>
       <c r="D2" s="5" t="s">
+        <v>1046</v>
+      </c>
+      <c r="E2" s="5" t="s">
         <v>1047</v>
       </c>
-      <c r="E2" s="5" t="s">
+      <c r="F2" s="5" t="s">
         <v>1048</v>
       </c>
-      <c r="F2" s="5" t="s">
+      <c r="G2" s="4" t="s">
         <v>1049</v>
       </c>
-      <c r="G2" s="4" t="s">
+      <c r="H2" s="4" t="s">
         <v>1050</v>
       </c>
-      <c r="H2" s="4" t="s">
+      <c r="I2" s="4" t="s">
         <v>1051</v>
       </c>
-      <c r="I2" s="4" t="s">
+      <c r="J2" s="4" t="s">
         <v>1052</v>
       </c>
-      <c r="J2" s="4" t="s">
+      <c r="K2" s="4" t="s">
         <v>1053</v>
       </c>
-      <c r="K2" s="4" t="s">
+      <c r="L2" s="4" t="s">
         <v>1054</v>
       </c>
-      <c r="L2" s="4" t="s">
+      <c r="M2" s="4" t="s">
         <v>1055</v>
       </c>
-      <c r="M2" s="4" t="s">
+      <c r="N2" s="4" t="s">
         <v>1056</v>
       </c>
-      <c r="N2" s="4" t="s">
+      <c r="O2" s="4" t="s">
         <v>1057</v>
       </c>
-      <c r="O2" s="4" t="s">
+      <c r="P2" s="4" t="s">
         <v>1058</v>
       </c>
-      <c r="P2" s="4" t="s">
+      <c r="Q2" s="4" t="s">
         <v>1059</v>
       </c>
-      <c r="Q2" s="4" t="s">
+      <c r="R2" s="4" t="s">
         <v>1060</v>
       </c>
-      <c r="R2" s="4" t="s">
+      <c r="S2" s="4" t="s">
         <v>1061</v>
-      </c>
-      <c r="S2" s="4" t="s">
-        <v>1062</v>
       </c>
     </row>
     <row r="3" spans="1:19" x14ac:dyDescent="0.4">
@@ -51806,19 +51806,19 @@
         <v>0</v>
       </c>
       <c r="B3" t="s">
+        <v>1062</v>
+      </c>
+      <c r="C3">
+        <v>1</v>
+      </c>
+      <c r="D3">
+        <v>1</v>
+      </c>
+      <c r="E3" t="s">
         <v>1063</v>
       </c>
-      <c r="C3">
-        <v>1</v>
-      </c>
-      <c r="D3">
-        <v>1</v>
-      </c>
-      <c r="E3" t="s">
+      <c r="F3" t="s">
         <v>1064</v>
-      </c>
-      <c r="F3" t="s">
-        <v>1065</v>
       </c>
       <c r="G3">
         <v>1</v>
@@ -51865,7 +51865,7 @@
         <v>1</v>
       </c>
       <c r="B4" t="s">
-        <v>1066</v>
+        <v>1065</v>
       </c>
       <c r="C4">
         <v>1.6</v>
@@ -51874,10 +51874,10 @@
         <v>1</v>
       </c>
       <c r="E4" t="s">
+        <v>1066</v>
+      </c>
+      <c r="F4" t="s">
         <v>1067</v>
-      </c>
-      <c r="F4" t="s">
-        <v>1068</v>
       </c>
       <c r="G4">
         <v>1</v>
@@ -51924,7 +51924,7 @@
         <v>2</v>
       </c>
       <c r="B5" t="s">
-        <v>1069</v>
+        <v>1068</v>
       </c>
       <c r="C5">
         <v>1.1499999999999999</v>
@@ -51933,10 +51933,10 @@
         <v>1.5</v>
       </c>
       <c r="E5" t="s">
+        <v>1069</v>
+      </c>
+      <c r="F5" t="s">
         <v>1070</v>
-      </c>
-      <c r="F5" t="s">
-        <v>1071</v>
       </c>
       <c r="G5">
         <v>1</v>
@@ -51983,7 +51983,7 @@
         <v>3</v>
       </c>
       <c r="B6" t="s">
-        <v>1072</v>
+        <v>1071</v>
       </c>
       <c r="C6">
         <v>1.1000000000000001</v>
@@ -51992,10 +51992,10 @@
         <v>1.8</v>
       </c>
       <c r="E6" t="s">
+        <v>1072</v>
+      </c>
+      <c r="F6" t="s">
         <v>1073</v>
-      </c>
-      <c r="F6" t="s">
-        <v>1074</v>
       </c>
       <c r="G6">
         <v>1</v>
@@ -52042,7 +52042,7 @@
         <v>4</v>
       </c>
       <c r="B7" t="s">
-        <v>1075</v>
+        <v>1074</v>
       </c>
       <c r="C7">
         <v>1.2</v>
@@ -52051,10 +52051,10 @@
         <v>1.6</v>
       </c>
       <c r="E7" t="s">
+        <v>1075</v>
+      </c>
+      <c r="F7" t="s">
         <v>1076</v>
-      </c>
-      <c r="F7" t="s">
-        <v>1077</v>
       </c>
       <c r="G7">
         <v>1</v>
@@ -52101,7 +52101,7 @@
         <v>5</v>
       </c>
       <c r="B8" t="s">
-        <v>1078</v>
+        <v>1077</v>
       </c>
       <c r="C8">
         <v>1.3</v>
@@ -52110,10 +52110,10 @@
         <v>1.3</v>
       </c>
       <c r="E8" t="s">
+        <v>1078</v>
+      </c>
+      <c r="F8" t="s">
         <v>1079</v>
-      </c>
-      <c r="F8" t="s">
-        <v>1080</v>
       </c>
       <c r="G8">
         <v>1</v>
@@ -52160,7 +52160,7 @@
         <v>6</v>
       </c>
       <c r="B9" t="s">
-        <v>1081</v>
+        <v>1080</v>
       </c>
       <c r="C9">
         <v>1.4</v>
@@ -52169,10 +52169,10 @@
         <v>1.4</v>
       </c>
       <c r="E9" t="s">
+        <v>1081</v>
+      </c>
+      <c r="F9" t="s">
         <v>1082</v>
-      </c>
-      <c r="F9" t="s">
-        <v>1083</v>
       </c>
       <c r="G9">
         <v>1</v>
@@ -52219,19 +52219,19 @@
         <v>200</v>
       </c>
       <c r="B10" t="s">
+        <v>1083</v>
+      </c>
+      <c r="C10">
+        <v>1</v>
+      </c>
+      <c r="D10">
+        <v>1</v>
+      </c>
+      <c r="E10" t="s">
         <v>1084</v>
       </c>
-      <c r="C10">
-        <v>1</v>
-      </c>
-      <c r="D10">
-        <v>1</v>
-      </c>
-      <c r="E10" t="s">
+      <c r="F10" t="s">
         <v>1085</v>
-      </c>
-      <c r="F10" t="s">
-        <v>1086</v>
       </c>
       <c r="G10">
         <v>1</v>
@@ -52300,7 +52300,7 @@
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>1087</v>
+        <v>1086</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.4">
@@ -52308,7 +52308,7 @@
         <v>0</v>
       </c>
       <c r="B2" t="s">
-        <v>1050</v>
+        <v>1049</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.4">
@@ -52316,7 +52316,7 @@
         <v>1</v>
       </c>
       <c r="B3" t="s">
-        <v>1051</v>
+        <v>1050</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.4">
@@ -52324,7 +52324,7 @@
         <v>2</v>
       </c>
       <c r="B4" t="s">
-        <v>1052</v>
+        <v>1051</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.4">
@@ -52332,7 +52332,7 @@
         <v>3</v>
       </c>
       <c r="B5" t="s">
-        <v>1053</v>
+        <v>1052</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.4">
@@ -52340,7 +52340,7 @@
         <v>4</v>
       </c>
       <c r="B6" t="s">
-        <v>1054</v>
+        <v>1053</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.4">
@@ -52348,7 +52348,7 @@
         <v>5</v>
       </c>
       <c r="B7" t="s">
-        <v>1055</v>
+        <v>1054</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.4">
@@ -52356,7 +52356,7 @@
         <v>6</v>
       </c>
       <c r="B8" t="s">
-        <v>1056</v>
+        <v>1055</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.4">
@@ -52364,7 +52364,7 @@
         <v>7</v>
       </c>
       <c r="B9" t="s">
-        <v>1057</v>
+        <v>1056</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.4">
@@ -52372,7 +52372,7 @@
         <v>8</v>
       </c>
       <c r="B10" t="s">
-        <v>1058</v>
+        <v>1057</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.4">
@@ -52380,7 +52380,7 @@
         <v>9</v>
       </c>
       <c r="B11" t="s">
-        <v>1059</v>
+        <v>1058</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.4">
@@ -52388,7 +52388,7 @@
         <v>10</v>
       </c>
       <c r="B12" t="s">
-        <v>1060</v>
+        <v>1059</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.4">
@@ -52396,7 +52396,7 @@
         <v>11</v>
       </c>
       <c r="B13" t="s">
-        <v>1061</v>
+        <v>1060</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.4">
@@ -52404,7 +52404,7 @@
         <v>12</v>
       </c>
       <c r="B14" t="s">
-        <v>1062</v>
+        <v>1061</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Various changes up to test build.
</commit_message>
<xml_diff>
--- a/Other/RoStatProcessing.xlsx
+++ b/Other/RoStatProcessing.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\ProjectsSSD\RagnarokRebuildTcp\Other\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AD5E5D14-C1BE-4D6A-BEA9-40FF37E16889}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5D5DB7D6-1A1B-49DF-80F0-4BF738D60E36}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="3771" yWindow="3771" windowWidth="24686" windowHeight="13055" xr2:uid="{1C41742B-2950-4FF8-AA39-6557869B44EA}"/>
   </bookViews>
@@ -51,7 +51,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2976" uniqueCount="1109">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2976" uniqueCount="1111">
   <si>
     <t>Id</t>
   </si>
@@ -3378,6 +3378,12 @@
   </si>
   <si>
     <t>The Paper</t>
+  </si>
+  <si>
+    <t>AiAggressiveAssist</t>
+  </si>
+  <si>
+    <t>Brute,Buff</t>
   </si>
 </sst>
 </file>
@@ -3820,10 +3826,10 @@
   <dimension ref="A1:AJ301"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <pane xSplit="3" ySplit="1" topLeftCell="D283" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="3" ySplit="1" topLeftCell="D176" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="C299" sqref="C299"/>
+      <selection pane="bottomRight" activeCell="D199" sqref="D199"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
@@ -6017,7 +6023,7 @@
         <v>112</v>
       </c>
       <c r="D21">
-        <v>12</v>
+        <v>18</v>
       </c>
       <c r="E21">
         <v>100</v>
@@ -6231,7 +6237,7 @@
         <v>123</v>
       </c>
       <c r="D23">
-        <v>21</v>
+        <v>28</v>
       </c>
       <c r="E23">
         <v>100</v>
@@ -6338,7 +6344,7 @@
         <v>126</v>
       </c>
       <c r="D24">
-        <v>18</v>
+        <v>22</v>
       </c>
       <c r="E24">
         <v>100</v>
@@ -6552,7 +6558,7 @@
         <v>133</v>
       </c>
       <c r="D26">
-        <v>7</v>
+        <v>12</v>
       </c>
       <c r="E26">
         <v>100</v>
@@ -6659,7 +6665,7 @@
         <v>136</v>
       </c>
       <c r="D27">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="E27">
         <v>100</v>
@@ -6980,7 +6986,7 @@
         <v>147</v>
       </c>
       <c r="D30">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="E30">
         <v>100</v>
@@ -7087,7 +7093,7 @@
         <v>150</v>
       </c>
       <c r="D31">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="E31">
         <v>100</v>
@@ -7194,7 +7200,7 @@
         <v>153</v>
       </c>
       <c r="D32">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="E32">
         <v>100</v>
@@ -7408,7 +7414,7 @@
         <v>159</v>
       </c>
       <c r="D34">
-        <v>25</v>
+        <v>29</v>
       </c>
       <c r="E34">
         <v>100</v>
@@ -7515,7 +7521,7 @@
         <v>163</v>
       </c>
       <c r="D35">
-        <v>24</v>
+        <v>28</v>
       </c>
       <c r="E35">
         <v>90</v>
@@ -7622,7 +7628,7 @@
         <v>166</v>
       </c>
       <c r="D36">
-        <v>24</v>
+        <v>28</v>
       </c>
       <c r="E36">
         <v>100</v>
@@ -7729,7 +7735,7 @@
         <v>169</v>
       </c>
       <c r="D37">
-        <v>23</v>
+        <v>27</v>
       </c>
       <c r="E37">
         <v>140</v>
@@ -7836,7 +7842,7 @@
         <v>172</v>
       </c>
       <c r="D38">
-        <v>22</v>
+        <v>26</v>
       </c>
       <c r="E38">
         <v>110</v>
@@ -7943,7 +7949,7 @@
         <v>175</v>
       </c>
       <c r="D39">
-        <v>24</v>
+        <v>28</v>
       </c>
       <c r="E39">
         <v>100</v>
@@ -8050,7 +8056,7 @@
         <v>179</v>
       </c>
       <c r="D40">
-        <v>34</v>
+        <v>38</v>
       </c>
       <c r="E40">
         <v>100</v>
@@ -8264,7 +8270,7 @@
         <v>187</v>
       </c>
       <c r="D42">
-        <v>25</v>
+        <v>30</v>
       </c>
       <c r="E42">
         <v>100</v>
@@ -8371,7 +8377,7 @@
         <v>191</v>
       </c>
       <c r="D43">
-        <v>38</v>
+        <v>41</v>
       </c>
       <c r="E43">
         <v>100</v>
@@ -8585,7 +8591,7 @@
         <v>198</v>
       </c>
       <c r="D45">
-        <v>26</v>
+        <v>29</v>
       </c>
       <c r="E45">
         <v>120</v>
@@ -9052,7 +9058,7 @@
         <v>90</v>
       </c>
       <c r="Q49">
-        <v>100</v>
+        <v>105</v>
       </c>
       <c r="R49">
         <v>100</v>
@@ -9762,7 +9768,7 @@
         <v>242</v>
       </c>
       <c r="D56">
-        <v>19</v>
+        <v>26</v>
       </c>
       <c r="E56">
         <v>100</v>
@@ -9774,16 +9780,16 @@
         <v>100</v>
       </c>
       <c r="H56">
-        <v>100</v>
+        <v>80</v>
       </c>
       <c r="I56">
-        <v>100</v>
+        <v>120</v>
       </c>
       <c r="J56">
-        <v>100</v>
+        <v>120</v>
       </c>
       <c r="K56">
-        <v>100</v>
+        <v>120</v>
       </c>
       <c r="L56">
         <v>100</v>
@@ -9795,16 +9801,16 @@
         <v>1</v>
       </c>
       <c r="O56">
-        <v>100</v>
+        <v>70</v>
       </c>
       <c r="P56">
-        <v>100</v>
+        <v>70</v>
       </c>
       <c r="Q56">
-        <v>100</v>
+        <v>95</v>
       </c>
       <c r="R56">
-        <v>100</v>
+        <v>90</v>
       </c>
       <c r="S56">
         <v>10</v>
@@ -10265,7 +10271,7 @@
         <v>41</v>
       </c>
       <c r="AC60" t="s">
-        <v>275</v>
+        <v>1110</v>
       </c>
       <c r="AD60" t="s">
         <v>42</v>
@@ -10297,10 +10303,10 @@
         <v>259</v>
       </c>
       <c r="D61">
-        <v>33</v>
+        <v>46</v>
       </c>
       <c r="E61">
-        <v>110</v>
+        <v>120</v>
       </c>
       <c r="F61">
         <v>100</v>
@@ -10312,16 +10318,16 @@
         <v>105</v>
       </c>
       <c r="I61">
-        <v>90</v>
+        <v>80</v>
       </c>
       <c r="J61">
-        <v>90</v>
+        <v>80</v>
       </c>
       <c r="K61">
-        <v>100</v>
+        <v>50</v>
       </c>
       <c r="L61">
-        <v>100</v>
+        <v>110</v>
       </c>
       <c r="M61">
         <v>10</v>
@@ -10330,7 +10336,7 @@
         <v>1</v>
       </c>
       <c r="O61">
-        <v>100</v>
+        <v>80</v>
       </c>
       <c r="P61">
         <v>90</v>
@@ -11412,7 +11418,7 @@
         <v>100</v>
       </c>
       <c r="S71">
-        <v>10</v>
+        <v>2</v>
       </c>
       <c r="T71">
         <v>12</v>
@@ -11445,7 +11451,7 @@
         <v>48</v>
       </c>
       <c r="AD71" t="s">
-        <v>99</v>
+        <v>1109</v>
       </c>
       <c r="AE71">
         <v>384</v>
@@ -13739,13 +13745,13 @@
         <v>130</v>
       </c>
       <c r="J93">
-        <v>100</v>
+        <v>160</v>
       </c>
       <c r="K93">
         <v>100</v>
       </c>
       <c r="L93">
-        <v>100</v>
+        <v>95</v>
       </c>
       <c r="M93">
         <v>10</v>
@@ -13760,7 +13766,7 @@
         <v>100</v>
       </c>
       <c r="Q93">
-        <v>100</v>
+        <v>110</v>
       </c>
       <c r="R93">
         <v>100</v>
@@ -15005,7 +15011,7 @@
         <v>403</v>
       </c>
       <c r="D105">
-        <v>13</v>
+        <v>23</v>
       </c>
       <c r="E105">
         <v>100</v>
@@ -18123,16 +18129,16 @@
         <v>30</v>
       </c>
       <c r="I134">
-        <v>140</v>
+        <v>150</v>
       </c>
       <c r="J134">
-        <v>180</v>
+        <v>240</v>
       </c>
       <c r="K134">
         <v>130</v>
       </c>
       <c r="L134">
-        <v>130</v>
+        <v>160</v>
       </c>
       <c r="M134">
         <v>65</v>
@@ -19285,7 +19291,7 @@
         <v>537</v>
       </c>
       <c r="D145">
-        <v>32</v>
+        <v>42</v>
       </c>
       <c r="E145">
         <v>120</v>
@@ -19294,7 +19300,7 @@
         <v>120</v>
       </c>
       <c r="G145">
-        <v>80</v>
+        <v>60</v>
       </c>
       <c r="H145">
         <v>110</v>
@@ -19309,7 +19315,7 @@
         <v>100</v>
       </c>
       <c r="L145">
-        <v>120</v>
+        <v>140</v>
       </c>
       <c r="M145">
         <v>15</v>
@@ -19318,10 +19324,10 @@
         <v>1</v>
       </c>
       <c r="O145">
-        <v>110</v>
+        <v>120</v>
       </c>
       <c r="P145">
-        <v>90</v>
+        <v>80</v>
       </c>
       <c r="Q145">
         <v>112</v>
@@ -19499,7 +19505,7 @@
         <v>543</v>
       </c>
       <c r="D147">
-        <v>30</v>
+        <v>38</v>
       </c>
       <c r="E147">
         <v>100</v>
@@ -19508,13 +19514,13 @@
         <v>100</v>
       </c>
       <c r="G147">
-        <v>90</v>
+        <v>80</v>
       </c>
       <c r="H147">
         <v>90</v>
       </c>
       <c r="I147">
-        <v>100</v>
+        <v>90</v>
       </c>
       <c r="J147">
         <v>100</v>
@@ -19523,7 +19529,7 @@
         <v>100</v>
       </c>
       <c r="L147">
-        <v>100</v>
+        <v>110</v>
       </c>
       <c r="M147">
         <v>10</v>
@@ -19532,10 +19538,10 @@
         <v>1</v>
       </c>
       <c r="O147">
-        <v>90</v>
+        <v>80</v>
       </c>
       <c r="P147">
-        <v>110</v>
+        <v>120</v>
       </c>
       <c r="Q147">
         <v>100</v>
@@ -21764,7 +21770,7 @@
         <v>90</v>
       </c>
       <c r="J168">
-        <v>150</v>
+        <v>200</v>
       </c>
       <c r="K168">
         <v>400</v>
@@ -24109,7 +24115,7 @@
         <v>100</v>
       </c>
       <c r="G190">
-        <v>100</v>
+        <v>120</v>
       </c>
       <c r="H190">
         <v>100</v>
@@ -24424,7 +24430,7 @@
         <v>21</v>
       </c>
       <c r="E193">
-        <v>100</v>
+        <v>110</v>
       </c>
       <c r="F193">
         <v>100</v>
@@ -24436,7 +24442,7 @@
         <v>100</v>
       </c>
       <c r="I193">
-        <v>100</v>
+        <v>90</v>
       </c>
       <c r="J193">
         <v>100</v>
@@ -24543,7 +24549,7 @@
         <v>100</v>
       </c>
       <c r="I194">
-        <v>100</v>
+        <v>90</v>
       </c>
       <c r="J194">
         <v>100</v>
@@ -24650,7 +24656,7 @@
         <v>100</v>
       </c>
       <c r="I195">
-        <v>100</v>
+        <v>90</v>
       </c>
       <c r="J195">
         <v>100</v>
@@ -24757,7 +24763,7 @@
         <v>100</v>
       </c>
       <c r="I196">
-        <v>100</v>
+        <v>90</v>
       </c>
       <c r="J196">
         <v>100</v>
@@ -24864,7 +24870,7 @@
         <v>100</v>
       </c>
       <c r="I197">
-        <v>100</v>
+        <v>90</v>
       </c>
       <c r="J197">
         <v>100</v>
@@ -24959,7 +24965,7 @@
         <v>31</v>
       </c>
       <c r="E198">
-        <v>100</v>
+        <v>110</v>
       </c>
       <c r="F198">
         <v>100</v>
@@ -24971,7 +24977,7 @@
         <v>100</v>
       </c>
       <c r="I198">
-        <v>100</v>
+        <v>90</v>
       </c>
       <c r="J198">
         <v>100</v>
@@ -25138,7 +25144,7 @@
         <v>41</v>
       </c>
       <c r="AC199" t="s">
-        <v>41</v>
+        <v>286</v>
       </c>
       <c r="AD199" t="s">
         <v>99</v>
@@ -25173,7 +25179,7 @@
         <v>26</v>
       </c>
       <c r="E200">
-        <v>100</v>
+        <v>120</v>
       </c>
       <c r="F200">
         <v>100</v>
@@ -25185,7 +25191,7 @@
         <v>100</v>
       </c>
       <c r="I200">
-        <v>100</v>
+        <v>90</v>
       </c>
       <c r="J200">
         <v>100</v>
@@ -25277,10 +25283,10 @@
         <v>713</v>
       </c>
       <c r="D201">
-        <v>28</v>
+        <v>31</v>
       </c>
       <c r="E201">
-        <v>150</v>
+        <v>220</v>
       </c>
       <c r="F201">
         <v>100</v>
@@ -25316,10 +25322,10 @@
         <v>50</v>
       </c>
       <c r="Q201">
-        <v>100</v>
+        <v>70</v>
       </c>
       <c r="R201">
-        <v>100</v>
+        <v>70</v>
       </c>
       <c r="S201">
         <v>10</v>
@@ -25387,7 +25393,7 @@
         <v>36</v>
       </c>
       <c r="E202">
-        <v>100</v>
+        <v>120</v>
       </c>
       <c r="F202">
         <v>100</v>
@@ -25396,10 +25402,10 @@
         <v>100</v>
       </c>
       <c r="H202">
-        <v>100</v>
+        <v>120</v>
       </c>
       <c r="I202">
-        <v>100</v>
+        <v>90</v>
       </c>
       <c r="J202">
         <v>100</v>
@@ -25417,13 +25423,13 @@
         <v>1</v>
       </c>
       <c r="O202">
-        <v>100</v>
+        <v>110</v>
       </c>
       <c r="P202">
         <v>100</v>
       </c>
       <c r="Q202">
-        <v>100</v>
+        <v>110</v>
       </c>
       <c r="R202">
         <v>100</v>
@@ -25494,7 +25500,7 @@
         <v>30</v>
       </c>
       <c r="E203">
-        <v>100</v>
+        <v>120</v>
       </c>
       <c r="F203">
         <v>100</v>
@@ -25506,7 +25512,7 @@
         <v>100</v>
       </c>
       <c r="I203">
-        <v>100</v>
+        <v>90</v>
       </c>
       <c r="J203">
         <v>100</v>
@@ -25812,7 +25818,7 @@
         <v>729</v>
       </c>
       <c r="D206">
-        <v>43</v>
+        <v>53</v>
       </c>
       <c r="E206">
         <v>100</v>
@@ -25919,7 +25925,7 @@
         <v>732</v>
       </c>
       <c r="D207">
-        <v>51</v>
+        <v>55</v>
       </c>
       <c r="E207">
         <v>100</v>
@@ -26133,7 +26139,7 @@
         <v>738</v>
       </c>
       <c r="D209">
-        <v>62</v>
+        <v>64</v>
       </c>
       <c r="E209">
         <v>200</v>
@@ -26240,7 +26246,7 @@
         <v>741</v>
       </c>
       <c r="D210">
-        <v>52</v>
+        <v>62</v>
       </c>
       <c r="E210">
         <v>100</v>
@@ -26347,7 +26353,7 @@
         <v>744</v>
       </c>
       <c r="D211">
-        <v>52</v>
+        <v>62</v>
       </c>
       <c r="E211">
         <v>90</v>
@@ -26454,7 +26460,7 @@
         <v>748</v>
       </c>
       <c r="D212">
-        <v>70</v>
+        <v>72</v>
       </c>
       <c r="E212">
         <v>100</v>
@@ -26775,7 +26781,7 @@
         <v>760</v>
       </c>
       <c r="D215">
-        <v>63</v>
+        <v>65</v>
       </c>
       <c r="E215">
         <v>100</v>
@@ -34916,7 +34922,7 @@
         <v>43</v>
       </c>
       <c r="E291">
-        <v>100</v>
+        <v>90</v>
       </c>
       <c r="F291">
         <v>100</v>
@@ -34937,7 +34943,7 @@
         <v>100</v>
       </c>
       <c r="L291">
-        <v>100</v>
+        <v>130</v>
       </c>
       <c r="M291">
         <v>10</v>
@@ -34946,19 +34952,19 @@
         <v>1</v>
       </c>
       <c r="O291">
-        <v>100</v>
+        <v>110</v>
       </c>
       <c r="P291">
-        <v>100</v>
+        <v>90</v>
       </c>
       <c r="Q291">
-        <v>100</v>
+        <v>115</v>
       </c>
       <c r="R291">
         <v>100</v>
       </c>
       <c r="S291">
-        <v>10</v>
+        <v>3</v>
       </c>
       <c r="T291">
         <v>12</v>
@@ -34991,7 +34997,7 @@
         <v>48</v>
       </c>
       <c r="AD291" t="s">
-        <v>42</v>
+        <v>1109</v>
       </c>
       <c r="AE291">
         <v>384</v>
@@ -36007,7 +36013,7 @@
         <v>130</v>
       </c>
       <c r="L301">
-        <v>80</v>
+        <v>66</v>
       </c>
       <c r="M301">
         <v>10</v>
@@ -38191,7 +38197,7 @@
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B5" sqref="B5"/>
+      <selection pane="bottomLeft" activeCell="L13" sqref="L13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>

</xml_diff>

<commit_message>
Stats, blessing visual effect, custom particle system, and other skills and fixes.
</commit_message>
<xml_diff>
--- a/Other/RoStatProcessing.xlsx
+++ b/Other/RoStatProcessing.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\ProjectsSSD\RagnarokRebuildTcp\Other\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8BECCD1E-B60E-4A2F-984B-F0D1DE4EAE94}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{33C7F4F3-E3C7-4A60-AE9F-9F1FBD7698F1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="4106" yWindow="3300" windowWidth="20700" windowHeight="13123" xr2:uid="{1C41742B-2950-4FF8-AA39-6557869B44EA}"/>
   </bookViews>
@@ -3848,10 +3848,10 @@
   <dimension ref="A1:AJ303"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <pane xSplit="3" ySplit="1" topLeftCell="D74" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="3" ySplit="1" topLeftCell="D33" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="D92" sqref="D92"/>
+      <selection pane="bottomRight" activeCell="D51" sqref="D51"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
@@ -4036,7 +4036,7 @@
         <v>80</v>
       </c>
       <c r="L2">
-        <v>90</v>
+        <v>100</v>
       </c>
       <c r="M2">
         <v>5</v>
@@ -4250,7 +4250,7 @@
         <v>90</v>
       </c>
       <c r="L4">
-        <v>90</v>
+        <v>100</v>
       </c>
       <c r="M4">
         <v>5</v>
@@ -4354,10 +4354,10 @@
         <v>100</v>
       </c>
       <c r="K5">
-        <v>100</v>
+        <v>110</v>
       </c>
       <c r="L5">
-        <v>90</v>
+        <v>100</v>
       </c>
       <c r="M5">
         <v>10</v>
@@ -4761,7 +4761,7 @@
         <v>69</v>
       </c>
       <c r="D9">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="E9">
         <v>100</v>
@@ -4892,7 +4892,7 @@
         <v>100</v>
       </c>
       <c r="L10">
-        <v>90</v>
+        <v>100</v>
       </c>
       <c r="M10">
         <v>10</v>
@@ -5617,7 +5617,7 @@
         <v>98</v>
       </c>
       <c r="D17">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="E17">
         <v>100</v>
@@ -7246,7 +7246,7 @@
         <v>100</v>
       </c>
       <c r="L32">
-        <v>110</v>
+        <v>100</v>
       </c>
       <c r="M32">
         <v>10</v>
@@ -9148,7 +9148,7 @@
         <v>214</v>
       </c>
       <c r="D50">
-        <v>15</v>
+        <v>22</v>
       </c>
       <c r="E50">
         <v>100</v>
@@ -18992,7 +18992,7 @@
         <v>525</v>
       </c>
       <c r="D142">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="E142">
         <v>100</v>
@@ -19099,7 +19099,7 @@
         <v>528</v>
       </c>
       <c r="D143">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="E143">
         <v>100</v>
@@ -30334,7 +30334,7 @@
         <v>866</v>
       </c>
       <c r="D248">
-        <v>17</v>
+        <v>37</v>
       </c>
       <c r="E248">
         <v>100</v>
@@ -34186,7 +34186,7 @@
         <v>976</v>
       </c>
       <c r="D284">
-        <v>24</v>
+        <v>34</v>
       </c>
       <c r="E284">
         <v>100</v>
@@ -37746,7 +37746,7 @@
       </c>
       <c r="D2" s="1">
         <f ca="1">OFFSET(StatCharts!D$2,Sheet2!$A2-1,0)</f>
-        <v>8.5717734625362922</v>
+        <v>6.9859953719670784</v>
       </c>
       <c r="E2" s="1">
         <f ca="1">OFFSET(StatCharts!E$2,Sheet2!$A2-1,0)</f>
@@ -37779,7 +37779,7 @@
       </c>
       <c r="D3" s="1">
         <f ca="1">OFFSET(StatCharts!D$2,Sheet2!$A3-1,0)</f>
-        <v>18.914213562373096</v>
+        <v>16.549936867076458</v>
       </c>
       <c r="E3" s="1">
         <f ca="1">OFFSET(StatCharts!E$2,Sheet2!$A3-1,0)</f>
@@ -37812,7 +37812,7 @@
       </c>
       <c r="D4" s="1">
         <f ca="1">OFFSET(StatCharts!D$2,Sheet2!$A4-1,0)</f>
-        <v>32</v>
+        <v>30.400000000000002</v>
       </c>
       <c r="E4" s="1">
         <f ca="1">OFFSET(StatCharts!E$2,Sheet2!$A4-1,0)</f>
@@ -41677,10 +41677,10 @@
   <dimension ref="A1:N100"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B29" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="B11" sqref="B11"/>
+      <selection pane="bottomRight" activeCell="E11" sqref="E11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
@@ -41740,8 +41740,8 @@
         <v>35.15004828475508</v>
       </c>
       <c r="D2" s="1">
-        <f>(5+A2*2.5+10*B2)</f>
-        <v>8.5717734625362922</v>
+        <f>(5+A2*2.5+10*B2)*MIN(1,0.8+A2*0.015)</f>
+        <v>6.9859953719670784</v>
       </c>
       <c r="E2" s="1">
         <f>(1-POWER(1-((A2+1)/100),2))*20+MAX(0,(A2-10)/3)*N2</f>
@@ -41789,8 +41789,8 @@
         <v>49.321635539399168</v>
       </c>
       <c r="D3" s="1">
-        <f t="shared" ref="D3:D34" si="2">(5+A3*2.5+10*B3)</f>
-        <v>11.148698354997036</v>
+        <f t="shared" ref="D3:D28" si="2">(5+A3*2.5+10*B3)*MIN(1,0.8+A3*0.015)</f>
+        <v>9.2534196346475408</v>
       </c>
       <c r="E3" s="1">
         <f t="shared" ref="E3:E66" si="3">(1-POWER(1-((A3+1)/100),2))*20+MAX(0,(A3-10)/3)</f>
@@ -41839,7 +41839,7 @@
       </c>
       <c r="D4" s="1">
         <f t="shared" si="2"/>
-        <v>13.731144413344916</v>
+        <v>11.602817029276455</v>
       </c>
       <c r="E4" s="1">
         <f t="shared" si="3"/>
@@ -41888,7 +41888,7 @@
       </c>
       <c r="D5" s="1">
         <f t="shared" si="2"/>
-        <v>16.319507910772895</v>
+        <v>14.034776803264691</v>
       </c>
       <c r="E5" s="1">
         <f t="shared" si="3"/>
@@ -41937,7 +41937,7 @@
       </c>
       <c r="D6" s="1">
         <f t="shared" si="2"/>
-        <v>18.914213562373096</v>
+        <v>16.549936867076458</v>
       </c>
       <c r="E6" s="1">
         <f t="shared" si="3"/>
@@ -41986,7 +41986,7 @@
       </c>
       <c r="D7" s="1">
         <f t="shared" si="2"/>
-        <v>21.515716566510399</v>
+        <v>19.148987744194255</v>
       </c>
       <c r="E7" s="1">
         <f t="shared" si="3"/>
@@ -42035,7 +42035,7 @@
       </c>
       <c r="D8" s="1">
         <f t="shared" si="2"/>
-        <v>24.124504792712472</v>
+        <v>21.832676837404787</v>
       </c>
       <c r="E8" s="1">
         <f t="shared" si="3"/>
@@ -42084,7 +42084,7 @@
       </c>
       <c r="D9" s="1">
         <f t="shared" si="2"/>
-        <v>26.741101126592248</v>
+        <v>24.601813036464868</v>
       </c>
       <c r="E9" s="1">
         <f t="shared" si="3"/>
@@ -42133,7 +42133,7 @@
       </c>
       <c r="D10" s="1">
         <f t="shared" si="2"/>
-        <v>29.366065983073614</v>
+        <v>27.45727169417383</v>
       </c>
       <c r="E10" s="1">
         <f t="shared" si="3"/>
@@ -42182,7 +42182,7 @@
       </c>
       <c r="D11" s="1">
         <f t="shared" si="2"/>
-        <v>32</v>
+        <v>30.400000000000002</v>
       </c>
       <c r="E11" s="1">
         <f t="shared" si="3"/>
@@ -42231,7 +42231,7 @@
       </c>
       <c r="D12" s="1">
         <f t="shared" si="2"/>
-        <v>34.643546925072584</v>
+        <v>33.431022782695045</v>
       </c>
       <c r="E12" s="1">
         <f t="shared" si="3"/>
@@ -42280,7 +42280,7 @@
       </c>
       <c r="D13" s="1">
         <f t="shared" si="2"/>
-        <v>37.297396709994068</v>
+        <v>36.551448775794185</v>
       </c>
       <c r="E13" s="1">
         <f t="shared" si="3"/>
@@ -42329,7 +42329,7 @@
       </c>
       <c r="D14" s="1">
         <f t="shared" si="2"/>
-        <v>39.962288826689836</v>
+        <v>39.762477382556391</v>
       </c>
       <c r="E14" s="1">
         <f t="shared" si="3"/>
@@ -42720,7 +42720,7 @@
         <v>386.40405591942681</v>
       </c>
       <c r="D22" s="1">
-        <f>(5+A22*2.5+10*B22)</f>
+        <f t="shared" si="2"/>
         <v>81.787093850145169</v>
       </c>
       <c r="E22" s="1">
@@ -42818,7 +42818,7 @@
         <v>423.25714004388249</v>
       </c>
       <c r="D24" s="1">
-        <f t="shared" si="2"/>
+        <f>(5+A24*2.5+10*B24)*MIN(1,0.8+A24*0.015)</f>
         <v>87.424577653379657</v>
       </c>
       <c r="E24" s="1">
@@ -43063,7 +43063,7 @@
         <v>518.70046566496637</v>
       </c>
       <c r="D29" s="1">
-        <f t="shared" si="2"/>
+        <f t="shared" ref="D3:D34" si="8">(5+A29*2.5+10*B29)</f>
         <v>101.96440450636899</v>
       </c>
       <c r="E29" s="1">
@@ -43112,7 +43112,7 @@
         <v>538.50491156511544</v>
       </c>
       <c r="D30" s="1">
-        <f t="shared" si="2"/>
+        <f t="shared" si="8"/>
         <v>104.96426393229446</v>
       </c>
       <c r="E30" s="1">
@@ -43161,7 +43161,7 @@
         <v>726.59999999999991</v>
       </c>
       <c r="D31" s="1">
-        <f t="shared" si="2"/>
+        <f t="shared" si="8"/>
         <v>148</v>
       </c>
       <c r="E31" s="1">
@@ -43210,7 +43210,7 @@
         <v>752.61197461925997</v>
       </c>
       <c r="D32" s="1">
-        <f t="shared" si="2"/>
+        <f t="shared" si="8"/>
         <v>151.07418770029034</v>
       </c>
       <c r="E32" s="1">
@@ -43259,7 +43259,7 @@
         <v>778.96934904309376</v>
       </c>
       <c r="D33" s="1">
-        <f t="shared" si="2"/>
+        <f t="shared" si="8"/>
         <v>154.1895868399763</v>
       </c>
       <c r="E33" s="1">
@@ -43308,7 +43308,7 @@
         <v>805.703097517228</v>
       </c>
       <c r="D34" s="1">
-        <f t="shared" si="2"/>
+        <f t="shared" si="8"/>
         <v>157.34915530675931</v>
       </c>
       <c r="E34" s="1">
@@ -43357,7 +43357,7 @@
         <v>832.84686124223185</v>
       </c>
       <c r="D35" s="1">
-        <f t="shared" ref="D35:D66" si="8">(5+A35*2.5+10*B35)*MIN(A35/20*0.4+0.6,1)</f>
+        <f t="shared" ref="D35:D66" si="9">(5+A35*2.5+10*B35)*MIN(A35/20*0.4+0.6,1)</f>
         <v>160.55606328618316</v>
       </c>
       <c r="E35" s="1">
@@ -43406,7 +43406,7 @@
         <v>860.43717164502527</v>
       </c>
       <c r="D36" s="1">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>163.81370849898474</v>
       </c>
       <c r="E36" s="1">
@@ -43455,7 +43455,7 @@
         <v>888.51369196169912</v>
       </c>
       <c r="D37" s="1">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>167.12573253208319</v>
       </c>
       <c r="E37" s="1">
@@ -43504,7 +43504,7 @@
         <v>917.11947861000476</v>
       </c>
       <c r="D38" s="1">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>170.49603834169977</v>
       </c>
       <c r="E38" s="1">
@@ -43553,7 +43553,7 @@
         <v>946.30126394776607</v>
       </c>
       <c r="D39" s="1">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>173.92880901273799</v>
       </c>
       <c r="E39" s="1">
@@ -43602,7 +43602,7 @@
         <v>976.10976214065533</v>
       </c>
       <c r="D40" s="1">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>177.42852786458892</v>
       </c>
       <c r="E40" s="1">
@@ -43651,7 +43651,7 @@
         <v>1342.6</v>
       </c>
       <c r="D41" s="1">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>241</v>
       </c>
       <c r="E41" s="1">
@@ -43700,7 +43700,7 @@
         <v>1382.2316747993329</v>
       </c>
       <c r="D42" s="1">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>244.64837540058068</v>
       </c>
       <c r="E42" s="1">
@@ -43749,7 +43749,7 @@
         <v>1422.6695412381212</v>
       </c>
       <c r="D43" s="1">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>248.37917367995257</v>
       </c>
       <c r="E43" s="1">
@@ -43798,7 +43798,7 @@
         <v>1463.9838298933826</v>
       </c>
       <c r="D44" s="1">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>252.19831061351866</v>
       </c>
       <c r="E44" s="1">
@@ -43847,7 +43847,7 @@
         <v>1506.2506996857765</v>
       </c>
       <c r="D45" s="1">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>256.11212657236632</v>
       </c>
       <c r="E45" s="1">
@@ -43896,7 +43896,7 @@
         <v>1549.5527270872078</v>
       </c>
       <c r="D46" s="1">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>260.12741699796948</v>
       </c>
       <c r="E46" s="1">
@@ -43945,7 +43945,7 @@
         <v>1593.9794350132313</v>
       </c>
       <c r="D47" s="1">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>264.25146506416638</v>
       </c>
       <c r="E47" s="1">
@@ -43994,7 +43994,7 @@
         <v>1639.6278645767688</v>
       </c>
       <c r="D48" s="1">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>268.49207668339955</v>
       </c>
       <c r="E48" s="1">
@@ -44043,7 +44043,7 @@
         <v>1686.6031931311984</v>
       </c>
       <c r="D49" s="1">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>272.85761802547597</v>
       </c>
       <c r="E49" s="1">
@@ -44092,7 +44092,7 @@
         <v>1735.0194023021597</v>
       </c>
       <c r="D50" s="1">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>277.35705572917783</v>
       </c>
       <c r="E50" s="1">
@@ -44141,7 +44141,7 @@
         <v>1785</v>
       </c>
       <c r="D51" s="1">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>282</v>
       </c>
       <c r="E51" s="1">
@@ -44190,7 +44190,7 @@
         <v>1836.678800720292</v>
       </c>
       <c r="D52" s="1">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>286.79675080116135</v>
       </c>
       <c r="E52" s="1">
@@ -44239,7 +44239,7 @@
         <v>1890.200768780109</v>
       </c>
       <c r="D53" s="1">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>291.75834735990514</v>
       </c>
       <c r="E53" s="1">
@@ -44288,7 +44288,7 @@
         <v>1945.7229295046166</v>
       </c>
       <c r="D54" s="1">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>296.89662122703731</v>
       </c>
       <c r="E54" s="1">
@@ -44337,7 +44337,7 @@
         <v>2003.4153537741784</v>
       </c>
       <c r="D55" s="1">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>302.22425314473264</v>
       </c>
       <c r="E55" s="1">
@@ -44386,7 +44386,7 @@
         <v>2063.4622217687302</v>
       </c>
       <c r="D56" s="1">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>307.75483399593901</v>
       </c>
       <c r="E56" s="1">
@@ -44435,7 +44435,7 @@
         <v>2126.0629722061285</v>
       </c>
       <c r="D57" s="1">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>313.50293012833276</v>
       </c>
       <c r="E57" s="1">
@@ -44484,7 +44484,7 @@
         <v>2191.4335438670564</v>
       </c>
       <c r="D58" s="1">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>319.48415336679909</v>
       </c>
       <c r="E58" s="1">
@@ -44533,7 +44533,7 @@
         <v>2259.8077167337296</v>
       </c>
       <c r="D59" s="1">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>325.71523605095194</v>
       </c>
       <c r="E59" s="1">
@@ -44582,7 +44582,7 @@
         <v>2331.4385606460182</v>
       </c>
       <c r="D60" s="1">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>332.21411145835572</v>
       </c>
       <c r="E60" s="1">
@@ -44631,7 +44631,7 @@
         <v>4254.5999999999995</v>
       </c>
       <c r="D61" s="1">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>559</v>
       </c>
       <c r="E61" s="1">
@@ -44680,7 +44680,7 @@
         <v>4364.3885036838365</v>
       </c>
       <c r="D62" s="1">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>566.0935016023227</v>
       </c>
       <c r="E62" s="1">
@@ -44729,7 +44729,7 @@
         <v>4478.3249101679521</v>
       </c>
       <c r="D63" s="1">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>573.51669471981018</v>
       </c>
       <c r="E63" s="1">
@@ -44778,7 +44778,7 @@
         <v>4596.7563984449371</v>
       </c>
       <c r="D64" s="1">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>581.29324245407463</v>
       </c>
       <c r="E64" s="1">
@@ -44827,7 +44827,7 @@
         <v>4720.0586163536082</v>
       </c>
       <c r="D65" s="1">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>589.44850628946517</v>
       </c>
       <c r="E65" s="1">
@@ -44876,7 +44876,7 @@
         <v>4848.6379787260903</v>
       </c>
       <c r="D66" s="1">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>598.00966799187802</v>
       </c>
       <c r="E66" s="1">
@@ -44917,7 +44917,7 @@
         <v>66</v>
       </c>
       <c r="B67" s="1">
-        <f t="shared" ref="B67:B100" si="9">FLOOR(A67/20,1)*FLOOR(A67/20,1)*2+FLOOR(A67/30,1)*FLOOR(A67/30,1)*4+POWER(2,A67/10)/10</f>
+        <f t="shared" ref="B67:B100" si="10">FLOOR(A67/20,1)*FLOOR(A67/20,1)*2+FLOOR(A67/30,1)*FLOOR(A67/30,1)*4+POWER(2,A67/10)/10</f>
         <v>43.700586025666546</v>
       </c>
       <c r="C67" s="1">
@@ -44925,11 +44925,11 @@
         <v>4982.9341487715883</v>
       </c>
       <c r="D67" s="1">
-        <f t="shared" ref="D67:D100" si="10">(5+A67*2.5+10*B67)*MIN(A67/20*0.4+0.6,1)</f>
+        <f t="shared" ref="D67:D100" si="11">(5+A67*2.5+10*B67)*MIN(A67/20*0.4+0.6,1)</f>
         <v>607.00586025666553</v>
       </c>
       <c r="E67" s="1">
-        <f t="shared" ref="E67:E100" si="11">(1-POWER(1-((A67+1)/100),2))*20+MAX(0,(A67-10)/3)</f>
+        <f t="shared" ref="E67:E100" si="12">(1-POWER(1-((A67+1)/100),2))*20+MAX(0,(A67-10)/3)</f>
         <v>36.488666666666667</v>
       </c>
       <c r="F67" s="1">
@@ -44937,11 +44937,11 @@
         <v>7237.9734346737796</v>
       </c>
       <c r="G67">
-        <f t="shared" ref="G67:G100" si="12">FLOOR(A67*0.8,1)+1</f>
+        <f t="shared" ref="G67:G100" si="13">FLOOR(A67*0.8,1)+1</f>
         <v>53</v>
       </c>
       <c r="H67">
-        <f t="shared" ref="H67:H100" si="13">FLOOR(A67/3,1)+1</f>
+        <f t="shared" ref="H67:H100" si="14">FLOOR(A67/3,1)+1</f>
         <v>23</v>
       </c>
       <c r="J67" s="1">
@@ -44957,7 +44957,7 @@
         <v>4449.340424768975</v>
       </c>
       <c r="N67">
-        <f t="shared" ref="N67:N100" si="14">MAX(1,1+(1-POWER(1-(A67-10)/200,3)))</f>
+        <f t="shared" ref="N67:N100" si="15">MAX(1,1+(1-POWER(1-(A67-10)/200,3)))</f>
         <v>1.626752</v>
       </c>
     </row>
@@ -44966,7 +44966,7 @@
         <v>67</v>
       </c>
       <c r="B68" s="1">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>44.396830673359815</v>
       </c>
       <c r="C68" s="1">
@@ -44974,11 +44974,11 @@
         <v>5123.4227171611501</v>
       </c>
       <c r="D68" s="1">
-        <f t="shared" si="10"/>
+        <f t="shared" si="11"/>
         <v>616.46830673359818</v>
       </c>
       <c r="E68" s="1">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v>36.951999999999998</v>
       </c>
       <c r="F68" s="1">
@@ -44986,11 +44986,11 @@
         <v>7549.7943277765753</v>
       </c>
       <c r="G68">
-        <f t="shared" si="12"/>
+        <f t="shared" si="13"/>
         <v>54</v>
       </c>
       <c r="H68">
-        <f t="shared" si="13"/>
+        <f t="shared" si="14"/>
         <v>23</v>
       </c>
       <c r="J68" s="1">
@@ -45006,7 +45006,7 @@
         <v>4619.096877888217</v>
       </c>
       <c r="N68">
-        <f t="shared" si="14"/>
+        <f t="shared" si="15"/>
         <v>1.6344741249999999</v>
       </c>
     </row>
@@ -45015,7 +45015,7 @@
         <v>68</v>
       </c>
       <c r="B69" s="1">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>45.143047210190389</v>
       </c>
       <c r="C69" s="1">
@@ -45023,11 +45023,11 @@
         <v>5270.6180944101243</v>
       </c>
       <c r="D69" s="1">
-        <f t="shared" si="10"/>
+        <f t="shared" si="11"/>
         <v>626.43047210190389</v>
       </c>
       <c r="E69" s="1">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v>37.411333333333332</v>
       </c>
       <c r="F69" s="1">
@@ -45035,11 +45035,11 @@
         <v>8186.9041466935159</v>
       </c>
       <c r="G69">
-        <f t="shared" si="12"/>
+        <f t="shared" si="13"/>
         <v>55</v>
       </c>
       <c r="H69">
-        <f t="shared" si="13"/>
+        <f t="shared" si="14"/>
         <v>23</v>
       </c>
       <c r="J69" s="1">
@@ -45055,7 +45055,7 @@
         <v>4985.6640819672475</v>
       </c>
       <c r="N69">
-        <f t="shared" si="14"/>
+        <f t="shared" si="15"/>
         <v>1.6420889999999999</v>
       </c>
     </row>
@@ -45064,7 +45064,7 @@
         <v>69</v>
       </c>
       <c r="B70" s="1">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>45.942822291671135</v>
       </c>
       <c r="C70" s="1">
@@ -45072,11 +45072,11 @@
         <v>5425.0766333754309</v>
       </c>
       <c r="D70" s="1">
-        <f t="shared" si="10"/>
+        <f t="shared" si="11"/>
         <v>636.92822291671132</v>
       </c>
       <c r="E70" s="1">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v>37.866666666666667</v>
       </c>
       <c r="F70" s="1">
@@ -45084,11 +45084,11 @@
         <v>8530.6690140845076</v>
       </c>
       <c r="G70">
-        <f t="shared" si="12"/>
+        <f t="shared" si="13"/>
         <v>56</v>
       </c>
       <c r="H70">
-        <f t="shared" si="13"/>
+        <f t="shared" si="14"/>
         <v>24</v>
       </c>
       <c r="J70" s="1">
@@ -45104,7 +45104,7 @@
         <v>5171.3643240275569</v>
       </c>
       <c r="N70">
-        <f t="shared" si="14"/>
+        <f t="shared" si="15"/>
         <v>1.6495973749999999</v>
       </c>
     </row>
@@ -45113,7 +45113,7 @@
         <v>70</v>
       </c>
       <c r="B71" s="1">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>46.8</v>
       </c>
       <c r="C71" s="1">
@@ -45121,11 +45121,11 @@
         <v>5587.4</v>
       </c>
       <c r="D71" s="1">
-        <f t="shared" si="10"/>
+        <f t="shared" si="11"/>
         <v>648</v>
       </c>
       <c r="E71" s="1">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v>38.317999999999998</v>
       </c>
       <c r="F71" s="1">
@@ -45133,11 +45133,11 @@
         <v>9466.8302103450078</v>
       </c>
       <c r="G71">
-        <f t="shared" si="12"/>
+        <f t="shared" si="13"/>
         <v>57</v>
       </c>
       <c r="H71">
-        <f t="shared" si="13"/>
+        <f t="shared" si="14"/>
         <v>24</v>
       </c>
       <c r="J71" s="1">
@@ -45153,7 +45153,7 @@
         <v>5713.2348885606571</v>
       </c>
       <c r="N71">
-        <f t="shared" si="14"/>
+        <f t="shared" si="15"/>
         <v>1.657</v>
       </c>
     </row>
@@ -45162,7 +45162,7 @@
         <v>71</v>
       </c>
       <c r="B72" s="1">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>47.718700320464549</v>
       </c>
       <c r="C72" s="1">
@@ -45170,11 +45170,11 @@
         <v>5758.2388118541758</v>
       </c>
       <c r="D72" s="1">
-        <f t="shared" si="10"/>
+        <f t="shared" si="11"/>
         <v>659.68700320464552</v>
       </c>
       <c r="E72" s="1">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v>38.765333333333331</v>
       </c>
       <c r="F72" s="1">
@@ -45182,11 +45182,11 @@
         <v>9851.9467565522464</v>
       </c>
       <c r="G72">
-        <f t="shared" si="12"/>
+        <f t="shared" si="13"/>
         <v>57</v>
       </c>
       <c r="H72">
-        <f t="shared" si="13"/>
+        <f t="shared" si="14"/>
         <v>24</v>
       </c>
       <c r="J72" s="1">
@@ -45202,7 +45202,7 @@
         <v>5919.5822961967197</v>
       </c>
       <c r="N72">
-        <f t="shared" si="14"/>
+        <f t="shared" si="15"/>
         <v>1.6642976249999999</v>
       </c>
     </row>
@@ -45211,7 +45211,7 @@
         <v>72</v>
       </c>
       <c r="B73" s="1">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>48.703338943962045</v>
       </c>
       <c r="C73" s="1">
@@ -45219,11 +45219,11 @@
         <v>5938.2965655513735</v>
       </c>
       <c r="D73" s="1">
-        <f t="shared" si="10"/>
+        <f t="shared" si="11"/>
         <v>672.03338943962046</v>
       </c>
       <c r="E73" s="1">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v>39.208666666666673</v>
       </c>
       <c r="F73" s="1">
@@ -45231,11 +45231,11 @@
         <v>10549.198306496861</v>
       </c>
       <c r="G73">
-        <f t="shared" si="12"/>
+        <f t="shared" si="13"/>
         <v>58</v>
       </c>
       <c r="H73">
-        <f t="shared" si="13"/>
+        <f t="shared" si="14"/>
         <v>25</v>
       </c>
       <c r="J73" s="1">
@@ -45251,7 +45251,7 @@
         <v>6311.2504383791847</v>
       </c>
       <c r="N73">
-        <f t="shared" si="14"/>
+        <f t="shared" si="15"/>
         <v>1.6714910000000001</v>
       </c>
     </row>
@@ -45260,7 +45260,7 @@
         <v>73</v>
       </c>
       <c r="B74" s="1">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>49.758648490814927</v>
       </c>
       <c r="C74" s="1">
@@ -45268,11 +45268,11 @@
         <v>6128.3338757612855</v>
       </c>
       <c r="D74" s="1">
-        <f t="shared" si="10"/>
+        <f t="shared" si="11"/>
         <v>685.08648490814926</v>
       </c>
       <c r="E74" s="1">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v>39.647999999999996</v>
       </c>
       <c r="F74" s="1">
@@ -45280,11 +45280,11 @@
         <v>10968.724778046813</v>
       </c>
       <c r="G74">
-        <f t="shared" si="12"/>
+        <f t="shared" si="13"/>
         <v>59</v>
       </c>
       <c r="H74">
-        <f t="shared" si="13"/>
+        <f t="shared" si="14"/>
         <v>25</v>
       </c>
       <c r="J74" s="1">
@@ -45300,7 +45300,7 @@
         <v>6534.5226681715967</v>
       </c>
       <c r="N74">
-        <f t="shared" si="14"/>
+        <f t="shared" si="15"/>
         <v>1.678580875</v>
       </c>
     </row>
@@ -45309,7 +45309,7 @@
         <v>74</v>
       </c>
       <c r="B75" s="1">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>50.889701257893044</v>
       </c>
       <c r="C75" s="1">
@@ -45317,11 +45317,11 @@
         <v>6329.1730503177196</v>
       </c>
       <c r="D75" s="1">
-        <f t="shared" si="10"/>
+        <f t="shared" si="11"/>
         <v>698.89701257893046</v>
       </c>
       <c r="E75" s="1">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v>40.083333333333329</v>
       </c>
       <c r="F75" s="1">
@@ -45329,11 +45329,11 @@
         <v>11956.365904365906</v>
       </c>
       <c r="G75">
-        <f t="shared" si="12"/>
+        <f t="shared" si="13"/>
         <v>60</v>
       </c>
       <c r="H75">
-        <f t="shared" si="13"/>
+        <f t="shared" si="14"/>
         <v>25</v>
       </c>
       <c r="J75" s="1">
@@ -45349,7 +45349,7 @@
         <v>7093.3749954709074</v>
       </c>
       <c r="N75">
-        <f t="shared" si="14"/>
+        <f t="shared" si="15"/>
         <v>1.685568</v>
       </c>
     </row>
@@ -45358,7 +45358,7 @@
         <v>75</v>
       </c>
       <c r="B76" s="1">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>52.101933598375609</v>
       </c>
       <c r="C76" s="1">
@@ -45366,11 +45366,11 @@
         <v>6541.7030278294396</v>
       </c>
       <c r="D76" s="1">
-        <f t="shared" si="10"/>
+        <f t="shared" si="11"/>
         <v>713.51933598375604</v>
       </c>
       <c r="E76" s="1">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v>40.51466666666667</v>
       </c>
       <c r="F76" s="1">
@@ -45378,11 +45378,11 @@
         <v>12419.675179358914</v>
       </c>
       <c r="G76">
-        <f t="shared" si="12"/>
+        <f t="shared" si="13"/>
         <v>61</v>
       </c>
       <c r="H76">
-        <f t="shared" si="13"/>
+        <f t="shared" si="14"/>
         <v>26</v>
       </c>
       <c r="J76" s="1">
@@ -45398,7 +45398,7 @@
         <v>7338.2683371859503</v>
       </c>
       <c r="N76">
-        <f t="shared" si="14"/>
+        <f t="shared" si="15"/>
         <v>1.6924531249999999</v>
       </c>
     </row>
@@ -45407,7 +45407,7 @@
         <v>76</v>
       </c>
       <c r="B77" s="1">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>53.401172051333091</v>
       </c>
       <c r="C77" s="1">
@@ -45415,11 +45415,11 @@
         <v>6766.8847062618406</v>
       </c>
       <c r="D77" s="1">
-        <f t="shared" si="10"/>
+        <f t="shared" si="11"/>
         <v>729.01172051333094</v>
       </c>
       <c r="E77" s="1">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v>40.942</v>
       </c>
       <c r="F77" s="1">
@@ -45427,11 +45427,11 @@
         <v>13183.674466318205</v>
       </c>
       <c r="G77">
-        <f t="shared" si="12"/>
+        <f t="shared" si="13"/>
         <v>61</v>
       </c>
       <c r="H77">
-        <f t="shared" si="13"/>
+        <f t="shared" si="14"/>
         <v>26</v>
       </c>
       <c r="J77" s="1">
@@ -45447,7 +45447,7 @@
         <v>7758.5848626873158</v>
       </c>
       <c r="N77">
-        <f t="shared" si="14"/>
+        <f t="shared" si="15"/>
         <v>1.6992370000000001</v>
       </c>
     </row>
@@ -45456,7 +45456,7 @@
         <v>77</v>
       </c>
       <c r="B78" s="1">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>54.793661346719624</v>
       </c>
       <c r="C78" s="1">
@@ -45464,11 +45464,11 @@
         <v>7005.7566931763749</v>
       </c>
       <c r="D78" s="1">
-        <f t="shared" si="10"/>
+        <f t="shared" si="11"/>
         <v>745.43661346719625</v>
       </c>
       <c r="E78" s="1">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v>41.365333333333332</v>
       </c>
       <c r="F78" s="1">
@@ -45476,11 +45476,11 @@
         <v>13684.018824136154</v>
       </c>
       <c r="G78">
-        <f t="shared" si="12"/>
+        <f t="shared" si="13"/>
         <v>62</v>
       </c>
       <c r="H78">
-        <f t="shared" si="13"/>
+        <f t="shared" si="14"/>
         <v>26</v>
       </c>
       <c r="J78" s="1">
@@ -45496,7 +45496,7 @@
         <v>8021.4874179787857</v>
       </c>
       <c r="N78">
-        <f t="shared" si="14"/>
+        <f t="shared" si="15"/>
         <v>1.705920375</v>
       </c>
     </row>
@@ -45505,7 +45505,7 @@
         <v>78</v>
       </c>
       <c r="B79" s="1">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>56.286094420380778</v>
       </c>
       <c r="C79" s="1">
@@ -45513,11 +45513,11 @@
         <v>7259.4415107055802</v>
       </c>
       <c r="D79" s="1">
-        <f t="shared" si="10"/>
+        <f t="shared" si="11"/>
         <v>762.86094420380778</v>
       </c>
       <c r="E79" s="1">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v>41.784666666666666</v>
       </c>
       <c r="F79" s="1">
@@ -45525,11 +45525,11 @@
         <v>14731.121464013913</v>
       </c>
       <c r="G79">
-        <f t="shared" si="12"/>
+        <f t="shared" si="13"/>
         <v>63</v>
       </c>
       <c r="H79">
-        <f t="shared" si="13"/>
+        <f t="shared" si="14"/>
         <v>27</v>
       </c>
       <c r="J79" s="1">
@@ -45545,7 +45545,7 @@
         <v>8602.0946310279633</v>
       </c>
       <c r="N79">
-        <f t="shared" si="14"/>
+        <f t="shared" si="15"/>
         <v>1.712504</v>
       </c>
     </row>
@@ -45554,7 +45554,7 @@
         <v>79</v>
       </c>
       <c r="B80" s="1">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>57.885644583342263</v>
       </c>
       <c r="C80" s="1">
@@ -45562,11 +45562,11 @@
         <v>7529.1522909176538</v>
       </c>
       <c r="D80" s="1">
-        <f t="shared" si="10"/>
+        <f t="shared" si="11"/>
         <v>781.35644583342264</v>
       </c>
       <c r="E80" s="1">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v>42.2</v>
       </c>
       <c r="F80" s="1">
@@ -45574,11 +45574,11 @@
         <v>15277.654028436018</v>
       </c>
       <c r="G80">
-        <f t="shared" si="12"/>
+        <f t="shared" si="13"/>
         <v>64</v>
       </c>
       <c r="H80">
-        <f t="shared" si="13"/>
+        <f t="shared" si="14"/>
         <v>27</v>
       </c>
       <c r="J80" s="1">
@@ -45594,7 +45594,7 @@
         <v>8887.5829695708526</v>
       </c>
       <c r="N80">
-        <f t="shared" si="14"/>
+        <f t="shared" si="15"/>
         <v>1.7189886249999999</v>
       </c>
     </row>
@@ -45603,7 +45603,7 @@
         <v>80</v>
       </c>
       <c r="B81" s="1">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>73.599999999999994</v>
       </c>
       <c r="C81" s="1">
@@ -45611,11 +45611,11 @@
         <v>9384.1999999999989</v>
       </c>
       <c r="D81" s="1">
-        <f t="shared" si="10"/>
+        <f t="shared" si="11"/>
         <v>941</v>
       </c>
       <c r="E81" s="1">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v>42.611333333333334</v>
       </c>
       <c r="F81" s="1">
@@ -45623,11 +45623,11 @@
         <v>16749.393745013065</v>
       </c>
       <c r="G81">
-        <f t="shared" si="12"/>
+        <f t="shared" si="13"/>
         <v>65</v>
       </c>
       <c r="H81">
-        <f t="shared" si="13"/>
+        <f t="shared" si="14"/>
         <v>27</v>
       </c>
       <c r="J81" s="1">
@@ -45643,7 +45643,7 @@
         <v>9707.6831094765275</v>
       </c>
       <c r="N81">
-        <f t="shared" si="14"/>
+        <f t="shared" si="15"/>
         <v>1.7253749999999999</v>
       </c>
     </row>
@@ -45652,7 +45652,7 @@
         <v>81</v>
       </c>
       <c r="B82" s="1">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>75.437400640929098</v>
       </c>
       <c r="C82" s="1">
@@ -45660,11 +45660,11 @@
         <v>9709.6012326813598</v>
       </c>
       <c r="D82" s="1">
-        <f t="shared" si="10"/>
+        <f t="shared" si="11"/>
         <v>961.87400640929104</v>
       </c>
       <c r="E82" s="1">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v>43.018666666666668</v>
       </c>
       <c r="F82" s="1">
@@ -45672,11 +45672,11 @@
         <v>17774.35376890652</v>
       </c>
       <c r="G82">
-        <f t="shared" si="12"/>
+        <f t="shared" si="13"/>
         <v>65</v>
       </c>
       <c r="H82">
-        <f t="shared" si="13"/>
+        <f t="shared" si="14"/>
         <v>28</v>
       </c>
       <c r="J82" s="1">
@@ -45692,7 +45692,7 @@
         <v>10264.320937518271</v>
       </c>
       <c r="N82">
-        <f t="shared" si="14"/>
+        <f t="shared" si="15"/>
         <v>1.731663875</v>
       </c>
     </row>
@@ -45701,7 +45701,7 @@
         <v>82</v>
       </c>
       <c r="B83" s="1">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>77.406677887924062</v>
       </c>
       <c r="C83" s="1">
@@ -45709,11 +45709,11 @@
         <v>10055.286621533682</v>
       </c>
       <c r="D83" s="1">
-        <f t="shared" si="10"/>
+        <f t="shared" si="11"/>
         <v>984.06677887924059</v>
       </c>
       <c r="E83" s="1">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v>43.421999999999997</v>
       </c>
       <c r="F83" s="1">
@@ -45721,11 +45721,11 @@
         <v>19351.227488369954</v>
       </c>
       <c r="G83">
-        <f t="shared" si="12"/>
+        <f t="shared" si="13"/>
         <v>66</v>
       </c>
       <c r="H83">
-        <f t="shared" si="13"/>
+        <f t="shared" si="14"/>
         <v>28</v>
       </c>
       <c r="J83" s="1">
@@ -45741,7 +45741,7 @@
         <v>11135.11561853799</v>
       </c>
       <c r="N83">
-        <f t="shared" si="14"/>
+        <f t="shared" si="15"/>
         <v>1.7378559999999998</v>
       </c>
     </row>
@@ -45750,7 +45750,7 @@
         <v>83</v>
       </c>
       <c r="B84" s="1">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>79.517296981629883</v>
       </c>
       <c r="C84" s="1">
@@ -45758,11 +45758,11 @@
         <v>10422.909909265392</v>
       </c>
       <c r="D84" s="1">
-        <f t="shared" si="10"/>
+        <f t="shared" si="11"/>
         <v>1007.6729698162989</v>
       </c>
       <c r="E84" s="1">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v>43.821333333333328</v>
       </c>
       <c r="F84" s="1">
@@ -45770,11 +45770,11 @@
         <v>20472.950769792493</v>
       </c>
       <c r="G84">
-        <f t="shared" si="12"/>
+        <f t="shared" si="13"/>
         <v>67</v>
       </c>
       <c r="H84">
-        <f t="shared" si="13"/>
+        <f t="shared" si="14"/>
         <v>28</v>
       </c>
       <c r="J84" s="1">
@@ -45790,7 +45790,7 @@
         <v>11739.399537583346</v>
       </c>
       <c r="N84">
-        <f t="shared" si="14"/>
+        <f t="shared" si="15"/>
         <v>1.7439521250000001</v>
       </c>
     </row>
@@ -45799,7 +45799,7 @@
         <v>84</v>
       </c>
       <c r="B85" s="1">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>81.779402515786089</v>
       </c>
       <c r="C85" s="1">
@@ -45807,11 +45807,11 @@
         <v>10814.257735856443</v>
       </c>
       <c r="D85" s="1">
-        <f t="shared" si="10"/>
+        <f t="shared" si="11"/>
         <v>1032.7940251578609</v>
       </c>
       <c r="E85" s="1">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v>44.216666666666669</v>
       </c>
       <c r="F85" s="1">
@@ -45819,11 +45819,11 @@
         <v>22513.185073501696</v>
       </c>
       <c r="G85">
-        <f t="shared" si="12"/>
+        <f t="shared" si="13"/>
         <v>68</v>
       </c>
       <c r="H85">
-        <f t="shared" si="13"/>
+        <f t="shared" si="14"/>
         <v>29</v>
       </c>
       <c r="J85" s="1">
@@ -45839,7 +45839,7 @@
         <v>12865.022702610695</v>
       </c>
       <c r="N85">
-        <f t="shared" si="14"/>
+        <f t="shared" si="15"/>
         <v>1.7499530000000001</v>
       </c>
     </row>
@@ -45848,7 +45848,7 @@
         <v>85</v>
       </c>
       <c r="B86" s="1">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>84.203867196751233</v>
       </c>
       <c r="C86" s="1">
@@ -45856,11 +45856,11 @@
         <v>11231.260196413397</v>
       </c>
       <c r="D86" s="1">
-        <f t="shared" si="10"/>
+        <f t="shared" si="11"/>
         <v>1059.5386719675123</v>
       </c>
       <c r="E86" s="1">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v>44.608000000000004</v>
       </c>
       <c r="F86" s="1">
@@ -45868,11 +45868,11 @@
         <v>24151.093974175034</v>
       </c>
       <c r="G86">
-        <f t="shared" si="12"/>
+        <f t="shared" si="13"/>
         <v>69</v>
       </c>
       <c r="H86">
-        <f t="shared" si="13"/>
+        <f t="shared" si="14"/>
         <v>29</v>
       </c>
       <c r="J86" s="1">
@@ -45888,7 +45888,7 @@
         <v>13754.571874057416</v>
       </c>
       <c r="N86">
-        <f t="shared" si="14"/>
+        <f t="shared" si="15"/>
         <v>1.755859375</v>
       </c>
     </row>
@@ -45897,7 +45897,7 @@
         <v>86</v>
       </c>
       <c r="B87" s="1">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>86.802344102666183</v>
       </c>
       <c r="C87" s="1">
@@ -45905,11 +45905,11 @@
         <v>11676.002229961008</v>
       </c>
       <c r="D87" s="1">
-        <f t="shared" si="10"/>
+        <f t="shared" si="11"/>
         <v>1088.0234410266619</v>
       </c>
       <c r="E87" s="1">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v>44.995333333333335</v>
       </c>
       <c r="F87" s="1">
@@ -45917,11 +45917,11 @@
         <v>26350.15483087135</v>
       </c>
       <c r="G87">
-        <f t="shared" si="12"/>
+        <f t="shared" si="13"/>
         <v>69</v>
       </c>
       <c r="H87">
-        <f t="shared" si="13"/>
+        <f t="shared" si="14"/>
         <v>29</v>
       </c>
       <c r="J87" s="1">
@@ -45937,7 +45937,7 @@
         <v>14957.469285355817</v>
       </c>
       <c r="N87">
-        <f t="shared" si="14"/>
+        <f t="shared" si="15"/>
         <v>1.7616719999999999</v>
       </c>
     </row>
@@ -45946,7 +45946,7 @@
         <v>87</v>
       </c>
       <c r="B88" s="1">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>89.587322693439219</v>
       </c>
       <c r="C88" s="1">
@@ -45954,11 +45954,11 @@
         <v>12150.735904060897</v>
       </c>
       <c r="D88" s="1">
-        <f t="shared" si="10"/>
+        <f t="shared" si="11"/>
         <v>1118.3732269343923</v>
       </c>
       <c r="E88" s="1">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v>45.378666666666668</v>
       </c>
       <c r="F88" s="1">
@@ -45966,11 +45966,11 @@
         <v>28139.654463183873</v>
       </c>
       <c r="G88">
-        <f t="shared" si="12"/>
+        <f t="shared" si="13"/>
         <v>70</v>
       </c>
       <c r="H88">
-        <f t="shared" si="13"/>
+        <f t="shared" si="14"/>
         <v>30</v>
       </c>
       <c r="J88" s="1">
@@ -45986,7 +45986,7 @@
         <v>15921.572822426311</v>
       </c>
       <c r="N88">
-        <f t="shared" si="14"/>
+        <f t="shared" si="15"/>
         <v>1.7673916250000001</v>
       </c>
     </row>
@@ -45995,7 +45995,7 @@
         <v>88</v>
       </c>
       <c r="B89" s="1">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>92.572188840761555</v>
       </c>
       <c r="C89" s="1">
@@ -46003,11 +46003,11 @@
         <v>12657.893665181822</v>
       </c>
       <c r="D89" s="1">
-        <f t="shared" si="10"/>
+        <f t="shared" si="11"/>
         <v>1150.7218884076156</v>
       </c>
       <c r="E89" s="1">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v>45.757999999999996</v>
       </c>
       <c r="F89" s="1">
@@ -46015,11 +46015,11 @@
         <v>30846.474933344991</v>
       </c>
       <c r="G89">
-        <f t="shared" si="12"/>
+        <f t="shared" si="13"/>
         <v>71</v>
       </c>
       <c r="H89">
-        <f t="shared" si="13"/>
+        <f t="shared" si="14"/>
         <v>30</v>
       </c>
       <c r="J89" s="1">
@@ -46035,7 +46035,7 @@
         <v>17397.712564470541</v>
       </c>
       <c r="N89">
-        <f t="shared" si="14"/>
+        <f t="shared" si="15"/>
         <v>1.7730190000000001</v>
       </c>
     </row>
@@ -46044,7 +46044,7 @@
         <v>89</v>
       </c>
       <c r="B90" s="1">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>95.771289166684539</v>
       </c>
       <c r="C90" s="1">
@@ -46052,11 +46052,11 @@
         <v>13200.102630168893</v>
       </c>
       <c r="D90" s="1">
-        <f t="shared" si="10"/>
+        <f t="shared" si="11"/>
         <v>1185.2128916668453</v>
       </c>
       <c r="E90" s="1">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v>46.133333333333333</v>
       </c>
       <c r="F90" s="1">
@@ -46064,11 +46064,11 @@
         <v>33195.780346820808</v>
       </c>
       <c r="G90">
-        <f t="shared" si="12"/>
+        <f t="shared" si="13"/>
         <v>72</v>
       </c>
       <c r="H90">
-        <f t="shared" si="13"/>
+        <f t="shared" si="14"/>
         <v>30</v>
       </c>
       <c r="J90" s="1">
@@ -46084,7 +46084,7 @@
         <v>18664.467885378464</v>
       </c>
       <c r="N90">
-        <f t="shared" si="14"/>
+        <f t="shared" si="15"/>
         <v>1.778554875</v>
       </c>
     </row>
@@ -46093,19 +46093,19 @@
         <v>90</v>
       </c>
       <c r="B91" s="1">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>119.2</v>
       </c>
       <c r="C91" s="1">
-        <f t="shared" ref="C91:C100" si="15">(A91*20+A91*B91*2+30)*0.7</f>
+        <f t="shared" ref="C91:C100" si="16">(A91*20+A91*B91*2+30)*0.7</f>
         <v>16300.199999999999</v>
       </c>
       <c r="D91" s="1">
-        <f t="shared" si="10"/>
+        <f t="shared" si="11"/>
         <v>1422</v>
       </c>
       <c r="E91" s="1">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v>46.504666666666665</v>
       </c>
       <c r="F91" s="1">
@@ -46113,11 +46113,11 @@
         <v>37890.54145103717</v>
       </c>
       <c r="G91">
-        <f t="shared" si="12"/>
+        <f t="shared" si="13"/>
         <v>73</v>
       </c>
       <c r="H91">
-        <f t="shared" si="13"/>
+        <f t="shared" si="14"/>
         <v>31</v>
       </c>
       <c r="J91" s="1">
@@ -46133,7 +46133,7 @@
         <v>21239.092741612763</v>
       </c>
       <c r="N91">
-        <f t="shared" si="14"/>
+        <f t="shared" si="15"/>
         <v>1.784</v>
       </c>
     </row>
@@ -46142,19 +46142,19 @@
         <v>91</v>
       </c>
       <c r="B92" s="1">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>122.87480128185821</v>
       </c>
       <c r="C92" s="1">
-        <f t="shared" si="15"/>
+        <f t="shared" si="16"/>
         <v>16949.249683308735</v>
       </c>
       <c r="D92" s="1">
-        <f t="shared" si="10"/>
+        <f t="shared" si="11"/>
         <v>1461.2480128185821</v>
       </c>
       <c r="E92" s="1">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v>46.872</v>
       </c>
       <c r="F92" s="1">
@@ -46162,11 +46162,11 @@
         <v>40589.84041645332</v>
       </c>
       <c r="G92">
-        <f t="shared" si="12"/>
+        <f t="shared" si="13"/>
         <v>73</v>
       </c>
       <c r="H92">
-        <f t="shared" si="13"/>
+        <f t="shared" si="14"/>
         <v>31</v>
       </c>
       <c r="J92" s="1">
@@ -46182,7 +46182,7 @@
         <v>22684.060782206838</v>
       </c>
       <c r="N92">
-        <f t="shared" si="14"/>
+        <f t="shared" si="15"/>
         <v>1.7893551250000002</v>
       </c>
     </row>
@@ -46191,19 +46191,19 @@
         <v>92</v>
       </c>
       <c r="B93" s="1">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>126.81335577584814</v>
       </c>
       <c r="C93" s="1">
-        <f t="shared" si="15"/>
+        <f t="shared" si="16"/>
         <v>17642.560223929238</v>
       </c>
       <c r="D93" s="1">
-        <f t="shared" si="10"/>
+        <f t="shared" si="11"/>
         <v>1503.1335577584814</v>
       </c>
       <c r="E93" s="1">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v>47.23533333333333</v>
       </c>
       <c r="F93" s="1">
@@ -46211,11 +46211,11 @@
         <v>44216.412854783848</v>
       </c>
       <c r="G93">
-        <f t="shared" si="12"/>
+        <f t="shared" si="13"/>
         <v>74</v>
       </c>
       <c r="H93">
-        <f t="shared" si="13"/>
+        <f t="shared" si="14"/>
         <v>31</v>
       </c>
       <c r="J93" s="1">
@@ -46231,7 +46231,7 @@
         <v>24638.30126516064</v>
       </c>
       <c r="N93">
-        <f t="shared" si="14"/>
+        <f t="shared" si="15"/>
         <v>1.7946209999999998</v>
       </c>
     </row>
@@ -46240,19 +46240,19 @@
         <v>93</v>
       </c>
       <c r="B94" s="1">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>131.03459396325971</v>
       </c>
       <c r="C94" s="1">
-        <f t="shared" si="15"/>
+        <f t="shared" si="16"/>
         <v>18383.704134016414</v>
       </c>
       <c r="D94" s="1">
-        <f t="shared" si="10"/>
+        <f t="shared" si="11"/>
         <v>1547.845939632597</v>
       </c>
       <c r="E94" s="1">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v>47.594666666666669</v>
       </c>
       <c r="F94" s="1">
@@ -46260,11 +46260,11 @@
         <v>47537.006947557151</v>
       </c>
       <c r="G94">
-        <f t="shared" si="12"/>
+        <f t="shared" si="13"/>
         <v>75</v>
       </c>
       <c r="H94">
-        <f t="shared" si="13"/>
+        <f t="shared" si="14"/>
         <v>32</v>
       </c>
       <c r="J94" s="1">
@@ -46280,7 +46280,7 @@
         <v>26412.406860605788</v>
       </c>
       <c r="N94">
-        <f t="shared" si="14"/>
+        <f t="shared" si="15"/>
         <v>1.799798375</v>
       </c>
     </row>
@@ -46289,19 +46289,19 @@
         <v>94</v>
       </c>
       <c r="B95" s="1">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>135.55880503157218</v>
       </c>
       <c r="C95" s="1">
-        <f t="shared" si="15"/>
+        <f t="shared" si="16"/>
         <v>19176.538742154899</v>
       </c>
       <c r="D95" s="1">
-        <f t="shared" si="10"/>
+        <f t="shared" si="11"/>
         <v>1595.5880503157218</v>
       </c>
       <c r="E95" s="1">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v>47.95</v>
       </c>
       <c r="F95" s="1">
@@ -46309,11 +46309,11 @@
         <v>53172.888425443169</v>
       </c>
       <c r="G95">
-        <f t="shared" si="12"/>
+        <f t="shared" si="13"/>
         <v>76</v>
       </c>
       <c r="H95">
-        <f t="shared" si="13"/>
+        <f t="shared" si="14"/>
         <v>32</v>
       </c>
       <c r="J95" s="1">
@@ -46329,7 +46329,7 @@
         <v>29460.491967060094</v>
       </c>
       <c r="N95">
-        <f t="shared" si="14"/>
+        <f t="shared" si="15"/>
         <v>1.804888</v>
       </c>
     </row>
@@ -46338,19 +46338,19 @@
         <v>95</v>
       </c>
       <c r="B96" s="1">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>140.40773439350247</v>
       </c>
       <c r="C96" s="1">
-        <f t="shared" si="15"/>
+        <f t="shared" si="16"/>
         <v>20025.228674335827</v>
       </c>
       <c r="D96" s="1">
-        <f t="shared" si="10"/>
+        <f t="shared" si="11"/>
         <v>1646.5773439350246</v>
       </c>
       <c r="E96" s="1">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v>48.301333333333332</v>
       </c>
       <c r="F96" s="1">
@@ -46358,11 +46358,11 @@
         <v>56916.461933417988</v>
       </c>
       <c r="G96">
-        <f t="shared" si="12"/>
+        <f t="shared" si="13"/>
         <v>77</v>
       </c>
       <c r="H96">
-        <f t="shared" si="13"/>
+        <f t="shared" si="14"/>
         <v>32</v>
       </c>
       <c r="J96" s="1">
@@ -46378,7 +46378,7 @@
         <v>31447.459391872362</v>
       </c>
       <c r="N96">
-        <f t="shared" si="14"/>
+        <f t="shared" si="15"/>
         <v>1.809890625</v>
       </c>
     </row>
@@ -46387,19 +46387,19 @@
         <v>96</v>
       </c>
       <c r="B97" s="1">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>145.60468820533237</v>
       </c>
       <c r="C97" s="1">
-        <f t="shared" si="15"/>
+        <f t="shared" si="16"/>
         <v>20934.27009479667</v>
       </c>
       <c r="D97" s="1">
-        <f t="shared" si="10"/>
+        <f t="shared" si="11"/>
         <v>1701.0468820533238</v>
       </c>
       <c r="E97" s="1">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v>48.648666666666671</v>
       </c>
       <c r="F97" s="1">
@@ -46407,11 +46407,11 @@
         <v>61603.024406287252</v>
       </c>
       <c r="G97">
-        <f t="shared" si="12"/>
+        <f t="shared" si="13"/>
         <v>77</v>
       </c>
       <c r="H97">
-        <f t="shared" si="13"/>
+        <f t="shared" si="14"/>
         <v>33</v>
       </c>
       <c r="J97" s="1">
@@ -46427,7 +46427,7 @@
         <v>33944.66982234874</v>
       </c>
       <c r="N97">
-        <f t="shared" si="14"/>
+        <f t="shared" si="15"/>
         <v>1.8148070000000001</v>
       </c>
     </row>
@@ -46436,19 +46436,19 @@
         <v>97</v>
       </c>
       <c r="B98" s="1">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>151.17464538687844</v>
       </c>
       <c r="C98" s="1">
-        <f t="shared" si="15"/>
+        <f t="shared" si="16"/>
         <v>21908.516843538091</v>
       </c>
       <c r="D98" s="1">
-        <f t="shared" si="10"/>
+        <f t="shared" si="11"/>
         <v>1759.2464538687843</v>
       </c>
       <c r="E98" s="1">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v>48.992000000000004</v>
       </c>
       <c r="F98" s="1">
@@ -46456,11 +46456,11 @@
         <v>66036.475342913123</v>
       </c>
       <c r="G98">
-        <f t="shared" si="12"/>
+        <f t="shared" si="13"/>
         <v>78</v>
       </c>
       <c r="H98">
-        <f t="shared" si="13"/>
+        <f t="shared" si="14"/>
         <v>33</v>
       </c>
       <c r="J98" s="1">
@@ -46476,7 +46476,7 @@
         <v>36290.998472931387</v>
       </c>
       <c r="N98">
-        <f t="shared" si="14"/>
+        <f t="shared" si="15"/>
         <v>1.8196378750000002</v>
       </c>
     </row>
@@ -46485,19 +46485,19 @@
         <v>98</v>
       </c>
       <c r="B99" s="1">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>157.14437768152311</v>
       </c>
       <c r="C99" s="1">
-        <f t="shared" si="15"/>
+        <f t="shared" si="16"/>
         <v>22953.208617904969</v>
       </c>
       <c r="D99" s="1">
-        <f t="shared" si="10"/>
+        <f t="shared" si="11"/>
         <v>1821.4437768152311</v>
       </c>
       <c r="E99" s="1">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v>49.331333333333333</v>
       </c>
       <c r="F99" s="1">
@@ -46505,11 +46505,11 @@
         <v>72765.132370231222</v>
       </c>
       <c r="G99">
-        <f t="shared" si="12"/>
+        <f t="shared" si="13"/>
         <v>79</v>
       </c>
       <c r="H99">
-        <f t="shared" si="13"/>
+        <f t="shared" si="14"/>
         <v>33</v>
       </c>
       <c r="J99" s="1">
@@ -46525,7 +46525,7 @@
         <v>39884.767883423243</v>
       </c>
       <c r="N99">
-        <f t="shared" si="14"/>
+        <f t="shared" si="15"/>
         <v>1.824384</v>
       </c>
     </row>
@@ -46534,19 +46534,19 @@
         <v>99</v>
       </c>
       <c r="B100" s="1">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>163.54257833336908</v>
       </c>
       <c r="C100" s="1">
-        <f t="shared" si="15"/>
+        <f t="shared" si="16"/>
         <v>24074.001357004952</v>
       </c>
       <c r="D100" s="1">
-        <f t="shared" si="10"/>
+        <f t="shared" si="11"/>
         <v>1887.9257833336908</v>
       </c>
       <c r="E100" s="1">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v>49.666666666666671</v>
       </c>
       <c r="F100" s="1">
@@ -46554,11 +46554,11 @@
         <v>77701.288590604017</v>
       </c>
       <c r="G100">
-        <f t="shared" si="12"/>
+        <f t="shared" si="13"/>
         <v>80</v>
       </c>
       <c r="H100">
-        <f t="shared" si="13"/>
+        <f t="shared" si="14"/>
         <v>34</v>
       </c>
       <c r="J100" s="1">
@@ -46574,7 +46574,7 @@
         <v>42481.863922706711</v>
       </c>
       <c r="N100">
-        <f t="shared" si="14"/>
+        <f t="shared" si="15"/>
         <v>1.8290461250000001</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Cart, stun, firewall, knockback, screen shake, and a big rework of how sprites are stored.
</commit_message>
<xml_diff>
--- a/Other/RoStatProcessing.xlsx
+++ b/Other/RoStatProcessing.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27830"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27928"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\ProjectsSSD\RagnarokRebuildTcp\Other\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{33C7F4F3-E3C7-4A60-AE9F-9F1FBD7698F1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E611A139-DC73-4FEA-B8E6-9B55D33AE1F6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4106" yWindow="3300" windowWidth="20700" windowHeight="13123" xr2:uid="{1C41742B-2950-4FF8-AA39-6557869B44EA}"/>
+    <workbookView xWindow="4106" yWindow="3300" windowWidth="27085" windowHeight="14100" activeTab="1" xr2:uid="{1C41742B-2950-4FF8-AA39-6557869B44EA}"/>
   </bookViews>
   <sheets>
     <sheet name="StatDef" sheetId="3" r:id="rId1"/>
@@ -31,7 +31,6 @@
     <definedName name="MonsterStatChart">StatDef!$A:$R</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
-  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -52,7 +51,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2998" uniqueCount="1118">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2999" uniqueCount="1120">
   <si>
     <t>Id</t>
   </si>
@@ -2310,9 +2309,6 @@
     <t>Evil Druid</t>
   </si>
   <si>
-    <t>Strong,Undead</t>
-  </si>
-  <si>
     <t>evil_druid.spr</t>
   </si>
   <si>
@@ -3406,6 +3402,15 @@
   </si>
   <si>
     <t>Brute,WorldBoss</t>
+  </si>
+  <si>
+    <t>Buff,Undead</t>
+  </si>
+  <si>
+    <t>Magic</t>
+  </si>
+  <si>
+    <t>Elite,Magic,Undead</t>
   </si>
 </sst>
 </file>
@@ -3847,11 +3852,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{811A97A5-94A7-4FFA-A162-65D076B52481}">
   <dimension ref="A1:AJ303"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <pane xSplit="3" ySplit="1" topLeftCell="D33" activePane="bottomRight" state="frozen"/>
+    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <pane xSplit="3" ySplit="1" topLeftCell="D216" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="D51" sqref="D51"/>
+      <selection pane="bottomRight" activeCell="E225" sqref="E225"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
@@ -5050,7 +5055,7 @@
         <v>41</v>
       </c>
       <c r="AC11" t="s">
-        <v>1099</v>
+        <v>1098</v>
       </c>
       <c r="AD11" t="s">
         <v>59</v>
@@ -10293,7 +10298,7 @@
         <v>41</v>
       </c>
       <c r="AC60" t="s">
-        <v>1108</v>
+        <v>1107</v>
       </c>
       <c r="AD60" t="s">
         <v>42</v>
@@ -11149,7 +11154,7 @@
         <v>41</v>
       </c>
       <c r="AC68" t="s">
-        <v>1098</v>
+        <v>1097</v>
       </c>
       <c r="AD68" t="s">
         <v>99</v>
@@ -11473,7 +11478,7 @@
         <v>48</v>
       </c>
       <c r="AD71" t="s">
-        <v>1107</v>
+        <v>1106</v>
       </c>
       <c r="AE71">
         <v>384</v>
@@ -21742,7 +21747,7 @@
         <v>41</v>
       </c>
       <c r="AC167" t="s">
-        <v>1093</v>
+        <v>1092</v>
       </c>
       <c r="AD167" t="s">
         <v>99</v>
@@ -26664,7 +26669,7 @@
         <v>41</v>
       </c>
       <c r="AC213" t="s">
-        <v>752</v>
+        <v>1119</v>
       </c>
       <c r="AD213" t="s">
         <v>99</v>
@@ -26673,7 +26678,7 @@
         <v>168</v>
       </c>
       <c r="AF213" t="s">
-        <v>753</v>
+        <v>752</v>
       </c>
       <c r="AG213">
         <v>0</v>
@@ -26690,10 +26695,10 @@
         <v>4211</v>
       </c>
       <c r="B214" t="s">
+        <v>753</v>
+      </c>
+      <c r="C214" t="s">
         <v>754</v>
-      </c>
-      <c r="C214" t="s">
-        <v>755</v>
       </c>
       <c r="D214">
         <v>79</v>
@@ -26771,7 +26776,7 @@
         <v>41</v>
       </c>
       <c r="AC214" t="s">
-        <v>756</v>
+        <v>755</v>
       </c>
       <c r="AD214" t="s">
         <v>99</v>
@@ -26780,7 +26785,7 @@
         <v>720</v>
       </c>
       <c r="AF214" t="s">
-        <v>757</v>
+        <v>756</v>
       </c>
       <c r="AG214">
         <v>0</v>
@@ -26797,10 +26802,10 @@
         <v>4212</v>
       </c>
       <c r="B215" t="s">
+        <v>757</v>
+      </c>
+      <c r="C215" t="s">
         <v>758</v>
-      </c>
-      <c r="C215" t="s">
-        <v>759</v>
       </c>
       <c r="D215">
         <v>65</v>
@@ -26887,7 +26892,7 @@
         <v>240</v>
       </c>
       <c r="AF215" t="s">
-        <v>760</v>
+        <v>759</v>
       </c>
       <c r="AG215">
         <v>0</v>
@@ -26904,10 +26909,10 @@
         <v>4213</v>
       </c>
       <c r="B216" t="s">
+        <v>760</v>
+      </c>
+      <c r="C216" t="s">
         <v>761</v>
-      </c>
-      <c r="C216" t="s">
-        <v>762</v>
       </c>
       <c r="D216">
         <v>53</v>
@@ -26994,7 +26999,7 @@
         <v>384</v>
       </c>
       <c r="AF216" t="s">
-        <v>763</v>
+        <v>762</v>
       </c>
       <c r="AG216">
         <v>0</v>
@@ -27011,10 +27016,10 @@
         <v>4214</v>
       </c>
       <c r="B217" t="s">
+        <v>763</v>
+      </c>
+      <c r="C217" t="s">
         <v>764</v>
-      </c>
-      <c r="C217" t="s">
-        <v>765</v>
       </c>
       <c r="D217">
         <v>77</v>
@@ -27092,7 +27097,7 @@
         <v>119</v>
       </c>
       <c r="AC217" t="s">
-        <v>766</v>
+        <v>765</v>
       </c>
       <c r="AD217" t="s">
         <v>99</v>
@@ -27101,7 +27106,7 @@
         <v>269</v>
       </c>
       <c r="AF217" t="s">
-        <v>767</v>
+        <v>766</v>
       </c>
       <c r="AG217">
         <v>0</v>
@@ -27118,10 +27123,10 @@
         <v>4215</v>
       </c>
       <c r="B218" t="s">
+        <v>767</v>
+      </c>
+      <c r="C218" t="s">
         <v>768</v>
-      </c>
-      <c r="C218" t="s">
-        <v>769</v>
       </c>
       <c r="D218">
         <v>80</v>
@@ -27208,7 +27213,7 @@
         <v>408</v>
       </c>
       <c r="AF218" t="s">
-        <v>770</v>
+        <v>769</v>
       </c>
       <c r="AG218">
         <v>0</v>
@@ -27225,10 +27230,10 @@
         <v>4216</v>
       </c>
       <c r="B219" t="s">
+        <v>770</v>
+      </c>
+      <c r="C219" t="s">
         <v>771</v>
-      </c>
-      <c r="C219" t="s">
-        <v>772</v>
       </c>
       <c r="D219">
         <v>52</v>
@@ -27288,7 +27293,7 @@
         <v>469</v>
       </c>
       <c r="W219" t="s">
-        <v>773</v>
+        <v>772</v>
       </c>
       <c r="X219">
         <v>1848</v>
@@ -27306,7 +27311,7 @@
         <v>41</v>
       </c>
       <c r="AC219" t="s">
-        <v>469</v>
+        <v>1117</v>
       </c>
       <c r="AD219" t="s">
         <v>99</v>
@@ -27315,7 +27320,7 @@
         <v>864</v>
       </c>
       <c r="AF219" t="s">
-        <v>774</v>
+        <v>773</v>
       </c>
       <c r="AG219">
         <v>0</v>
@@ -27332,10 +27337,10 @@
         <v>4217</v>
       </c>
       <c r="B220" t="s">
+        <v>774</v>
+      </c>
+      <c r="C220" t="s">
         <v>775</v>
-      </c>
-      <c r="C220" t="s">
-        <v>776</v>
       </c>
       <c r="D220">
         <v>53</v>
@@ -27395,7 +27400,7 @@
         <v>469</v>
       </c>
       <c r="W220" t="s">
-        <v>773</v>
+        <v>772</v>
       </c>
       <c r="X220">
         <v>1768</v>
@@ -27413,7 +27418,7 @@
         <v>41</v>
       </c>
       <c r="AC220" t="s">
-        <v>469</v>
+        <v>1117</v>
       </c>
       <c r="AD220" t="s">
         <v>99</v>
@@ -27422,7 +27427,7 @@
         <v>480</v>
       </c>
       <c r="AF220" t="s">
-        <v>777</v>
+        <v>776</v>
       </c>
       <c r="AG220">
         <v>0</v>
@@ -27439,10 +27444,10 @@
         <v>4218</v>
       </c>
       <c r="B221" t="s">
+        <v>777</v>
+      </c>
+      <c r="C221" t="s">
         <v>778</v>
-      </c>
-      <c r="C221" t="s">
-        <v>779</v>
       </c>
       <c r="D221">
         <v>61</v>
@@ -27529,7 +27534,7 @@
         <v>336</v>
       </c>
       <c r="AF221" t="s">
-        <v>780</v>
+        <v>779</v>
       </c>
       <c r="AG221">
         <v>0</v>
@@ -27546,10 +27551,10 @@
         <v>4219</v>
       </c>
       <c r="B222" t="s">
+        <v>780</v>
+      </c>
+      <c r="C222" t="s">
         <v>781</v>
-      </c>
-      <c r="C222" t="s">
-        <v>782</v>
       </c>
       <c r="D222">
         <v>66</v>
@@ -27627,7 +27632,7 @@
         <v>41</v>
       </c>
       <c r="AC222" t="s">
-        <v>783</v>
+        <v>782</v>
       </c>
       <c r="AD222" t="s">
         <v>99</v>
@@ -27636,7 +27641,7 @@
         <v>660</v>
       </c>
       <c r="AF222" t="s">
-        <v>784</v>
+        <v>783</v>
       </c>
       <c r="AG222">
         <v>0</v>
@@ -27653,10 +27658,10 @@
         <v>4220</v>
       </c>
       <c r="B223" t="s">
+        <v>784</v>
+      </c>
+      <c r="C223" t="s">
         <v>785</v>
-      </c>
-      <c r="C223" t="s">
-        <v>786</v>
       </c>
       <c r="D223">
         <v>48</v>
@@ -27716,7 +27721,7 @@
         <v>219</v>
       </c>
       <c r="W223" t="s">
-        <v>787</v>
+        <v>786</v>
       </c>
       <c r="X223">
         <v>1020</v>
@@ -27743,7 +27748,7 @@
         <v>600</v>
       </c>
       <c r="AF223" t="s">
-        <v>788</v>
+        <v>787</v>
       </c>
       <c r="AG223">
         <v>0</v>
@@ -27760,10 +27765,10 @@
         <v>4221</v>
       </c>
       <c r="B224" t="s">
+        <v>788</v>
+      </c>
+      <c r="C224" t="s">
         <v>789</v>
-      </c>
-      <c r="C224" t="s">
-        <v>790</v>
       </c>
       <c r="D224">
         <v>82</v>
@@ -27850,7 +27855,7 @@
         <v>288</v>
       </c>
       <c r="AF224" t="s">
-        <v>791</v>
+        <v>790</v>
       </c>
       <c r="AG224">
         <v>0</v>
@@ -27867,10 +27872,10 @@
         <v>4222</v>
       </c>
       <c r="B225" t="s">
+        <v>791</v>
+      </c>
+      <c r="C225" t="s">
         <v>792</v>
-      </c>
-      <c r="C225" t="s">
-        <v>793</v>
       </c>
       <c r="D225">
         <v>51</v>
@@ -27897,7 +27902,7 @@
         <v>100</v>
       </c>
       <c r="L225">
-        <v>100</v>
+        <v>120</v>
       </c>
       <c r="M225">
         <v>5</v>
@@ -27948,7 +27953,7 @@
         <v>41</v>
       </c>
       <c r="AC225" t="s">
-        <v>41</v>
+        <v>286</v>
       </c>
       <c r="AD225" t="s">
         <v>99</v>
@@ -27957,7 +27962,7 @@
         <v>540</v>
       </c>
       <c r="AF225" t="s">
-        <v>794</v>
+        <v>793</v>
       </c>
       <c r="AG225">
         <v>0</v>
@@ -27974,10 +27979,10 @@
         <v>4223</v>
       </c>
       <c r="B226" t="s">
+        <v>794</v>
+      </c>
+      <c r="C226" t="s">
         <v>795</v>
-      </c>
-      <c r="C226" t="s">
-        <v>796</v>
       </c>
       <c r="D226">
         <v>71</v>
@@ -28004,7 +28009,7 @@
         <v>100</v>
       </c>
       <c r="L226">
-        <v>100</v>
+        <v>120</v>
       </c>
       <c r="M226">
         <v>5</v>
@@ -28037,7 +28042,7 @@
         <v>219</v>
       </c>
       <c r="W226" t="s">
-        <v>797</v>
+        <v>796</v>
       </c>
       <c r="X226">
         <v>1790</v>
@@ -28064,7 +28069,7 @@
         <v>900</v>
       </c>
       <c r="AF226" t="s">
-        <v>798</v>
+        <v>797</v>
       </c>
       <c r="AG226">
         <v>0</v>
@@ -28081,10 +28086,10 @@
         <v>4224</v>
       </c>
       <c r="B227" t="s">
+        <v>798</v>
+      </c>
+      <c r="C227" t="s">
         <v>799</v>
-      </c>
-      <c r="C227" t="s">
-        <v>800</v>
       </c>
       <c r="D227">
         <v>73</v>
@@ -28171,7 +28176,7 @@
         <v>1920</v>
       </c>
       <c r="AF227" t="s">
-        <v>801</v>
+        <v>800</v>
       </c>
       <c r="AG227">
         <v>0</v>
@@ -28188,10 +28193,10 @@
         <v>4225</v>
       </c>
       <c r="B228" t="s">
+        <v>801</v>
+      </c>
+      <c r="C228" t="s">
         <v>802</v>
-      </c>
-      <c r="C228" t="s">
-        <v>803</v>
       </c>
       <c r="D228">
         <v>73</v>
@@ -28251,7 +28256,7 @@
         <v>160</v>
       </c>
       <c r="W228" t="s">
-        <v>797</v>
+        <v>796</v>
       </c>
       <c r="X228">
         <v>1744</v>
@@ -28278,7 +28283,7 @@
         <v>960</v>
       </c>
       <c r="AF228" t="s">
-        <v>804</v>
+        <v>803</v>
       </c>
       <c r="AG228">
         <v>0</v>
@@ -28295,10 +28300,10 @@
         <v>4226</v>
       </c>
       <c r="B229" t="s">
+        <v>804</v>
+      </c>
+      <c r="C229" t="s">
         <v>805</v>
-      </c>
-      <c r="C229" t="s">
-        <v>806</v>
       </c>
       <c r="D229">
         <v>61</v>
@@ -28385,7 +28390,7 @@
         <v>660</v>
       </c>
       <c r="AF229" t="s">
-        <v>807</v>
+        <v>806</v>
       </c>
       <c r="AG229">
         <v>0</v>
@@ -28402,10 +28407,10 @@
         <v>4227</v>
       </c>
       <c r="B230" t="s">
+        <v>807</v>
+      </c>
+      <c r="C230" t="s">
         <v>808</v>
-      </c>
-      <c r="C230" t="s">
-        <v>809</v>
       </c>
       <c r="D230">
         <v>51</v>
@@ -28465,7 +28470,7 @@
         <v>219</v>
       </c>
       <c r="W230" t="s">
-        <v>787</v>
+        <v>786</v>
       </c>
       <c r="X230">
         <v>1056</v>
@@ -28483,7 +28488,7 @@
         <v>41</v>
       </c>
       <c r="AC230" t="s">
-        <v>810</v>
+        <v>809</v>
       </c>
       <c r="AD230" t="s">
         <v>99</v>
@@ -28492,7 +28497,7 @@
         <v>720</v>
       </c>
       <c r="AF230" t="s">
-        <v>811</v>
+        <v>810</v>
       </c>
       <c r="AG230">
         <v>0</v>
@@ -28509,10 +28514,10 @@
         <v>4228</v>
       </c>
       <c r="B231" t="s">
+        <v>811</v>
+      </c>
+      <c r="C231" t="s">
         <v>812</v>
-      </c>
-      <c r="C231" t="s">
-        <v>813</v>
       </c>
       <c r="D231">
         <v>40</v>
@@ -28590,7 +28595,7 @@
         <v>41</v>
       </c>
       <c r="AC231" t="s">
-        <v>1094</v>
+        <v>1093</v>
       </c>
       <c r="AD231" t="s">
         <v>99</v>
@@ -28599,7 +28604,7 @@
         <v>432</v>
       </c>
       <c r="AF231" t="s">
-        <v>814</v>
+        <v>813</v>
       </c>
       <c r="AG231">
         <v>0</v>
@@ -28616,10 +28621,10 @@
         <v>4229</v>
       </c>
       <c r="B232" t="s">
+        <v>814</v>
+      </c>
+      <c r="C232" t="s">
         <v>815</v>
-      </c>
-      <c r="C232" t="s">
-        <v>816</v>
       </c>
       <c r="D232">
         <v>48</v>
@@ -28706,7 +28711,7 @@
         <v>336</v>
       </c>
       <c r="AF232" t="s">
-        <v>817</v>
+        <v>816</v>
       </c>
       <c r="AG232">
         <v>0</v>
@@ -28723,10 +28728,10 @@
         <v>4230</v>
       </c>
       <c r="B233" t="s">
+        <v>817</v>
+      </c>
+      <c r="C233" t="s">
         <v>818</v>
-      </c>
-      <c r="C233" t="s">
-        <v>819</v>
       </c>
       <c r="D233">
         <v>35</v>
@@ -28813,7 +28818,7 @@
         <v>360</v>
       </c>
       <c r="AF233" t="s">
-        <v>820</v>
+        <v>819</v>
       </c>
       <c r="AG233">
         <v>0</v>
@@ -28830,10 +28835,10 @@
         <v>4231</v>
       </c>
       <c r="B234" t="s">
+        <v>820</v>
+      </c>
+      <c r="C234" t="s">
         <v>821</v>
-      </c>
-      <c r="C234" t="s">
-        <v>822</v>
       </c>
       <c r="D234">
         <v>70</v>
@@ -28920,7 +28925,7 @@
         <v>108</v>
       </c>
       <c r="AF234" t="s">
-        <v>823</v>
+        <v>822</v>
       </c>
       <c r="AG234">
         <v>0</v>
@@ -28937,10 +28942,10 @@
         <v>4232</v>
       </c>
       <c r="B235" t="s">
+        <v>823</v>
+      </c>
+      <c r="C235" t="s">
         <v>824</v>
-      </c>
-      <c r="C235" t="s">
-        <v>825</v>
       </c>
       <c r="D235">
         <v>58</v>
@@ -29027,7 +29032,7 @@
         <v>756</v>
       </c>
       <c r="AF235" t="s">
-        <v>826</v>
+        <v>825</v>
       </c>
       <c r="AG235">
         <v>0</v>
@@ -29044,10 +29049,10 @@
         <v>4233</v>
       </c>
       <c r="B236" t="s">
+        <v>826</v>
+      </c>
+      <c r="C236" t="s">
         <v>827</v>
-      </c>
-      <c r="C236" t="s">
-        <v>828</v>
       </c>
       <c r="D236">
         <v>49</v>
@@ -29134,7 +29139,7 @@
         <v>396</v>
       </c>
       <c r="AF236" t="s">
-        <v>829</v>
+        <v>828</v>
       </c>
       <c r="AG236">
         <v>0</v>
@@ -29151,10 +29156,10 @@
         <v>4234</v>
       </c>
       <c r="B237" t="s">
+        <v>829</v>
+      </c>
+      <c r="C237" t="s">
         <v>830</v>
-      </c>
-      <c r="C237" t="s">
-        <v>831</v>
       </c>
       <c r="D237">
         <v>63</v>
@@ -29214,7 +29219,7 @@
         <v>53</v>
       </c>
       <c r="W237" t="s">
-        <v>797</v>
+        <v>796</v>
       </c>
       <c r="X237">
         <v>1100</v>
@@ -29232,7 +29237,7 @@
         <v>41</v>
       </c>
       <c r="AC237" t="s">
-        <v>832</v>
+        <v>831</v>
       </c>
       <c r="AD237" t="s">
         <v>42</v>
@@ -29241,7 +29246,7 @@
         <v>720</v>
       </c>
       <c r="AF237" t="s">
-        <v>833</v>
+        <v>832</v>
       </c>
       <c r="AG237">
         <v>0</v>
@@ -29258,10 +29263,10 @@
         <v>4235</v>
       </c>
       <c r="B238" t="s">
+        <v>833</v>
+      </c>
+      <c r="C238" t="s">
         <v>834</v>
-      </c>
-      <c r="C238" t="s">
-        <v>835</v>
       </c>
       <c r="D238">
         <v>70</v>
@@ -29339,7 +29344,7 @@
         <v>41</v>
       </c>
       <c r="AC238" t="s">
-        <v>832</v>
+        <v>831</v>
       </c>
       <c r="AD238" t="s">
         <v>42</v>
@@ -29348,7 +29353,7 @@
         <v>1248</v>
       </c>
       <c r="AF238" t="s">
-        <v>836</v>
+        <v>835</v>
       </c>
       <c r="AG238">
         <v>0</v>
@@ -29365,10 +29370,10 @@
         <v>4236</v>
       </c>
       <c r="B239" t="s">
+        <v>836</v>
+      </c>
+      <c r="C239" t="s">
         <v>837</v>
-      </c>
-      <c r="C239" t="s">
-        <v>838</v>
       </c>
       <c r="D239">
         <v>72</v>
@@ -29446,7 +29451,7 @@
         <v>41</v>
       </c>
       <c r="AC239" t="s">
-        <v>832</v>
+        <v>831</v>
       </c>
       <c r="AD239" t="s">
         <v>99</v>
@@ -29455,7 +29460,7 @@
         <v>522</v>
       </c>
       <c r="AF239" t="s">
-        <v>839</v>
+        <v>838</v>
       </c>
       <c r="AG239">
         <v>0</v>
@@ -29472,10 +29477,10 @@
         <v>4237</v>
       </c>
       <c r="B240" t="s">
+        <v>839</v>
+      </c>
+      <c r="C240" t="s">
         <v>840</v>
-      </c>
-      <c r="C240" t="s">
-        <v>841</v>
       </c>
       <c r="D240">
         <v>68</v>
@@ -29553,7 +29558,7 @@
         <v>41</v>
       </c>
       <c r="AC240" t="s">
-        <v>832</v>
+        <v>831</v>
       </c>
       <c r="AD240" t="s">
         <v>99</v>
@@ -29562,7 +29567,7 @@
         <v>1200</v>
       </c>
       <c r="AF240" t="s">
-        <v>842</v>
+        <v>841</v>
       </c>
       <c r="AG240">
         <v>0</v>
@@ -29579,10 +29584,10 @@
         <v>4238</v>
       </c>
       <c r="B241" t="s">
+        <v>842</v>
+      </c>
+      <c r="C241" t="s">
         <v>843</v>
-      </c>
-      <c r="C241" t="s">
-        <v>844</v>
       </c>
       <c r="D241">
         <v>71</v>
@@ -29660,7 +29665,7 @@
         <v>41</v>
       </c>
       <c r="AC241" t="s">
-        <v>845</v>
+        <v>844</v>
       </c>
       <c r="AD241" t="s">
         <v>99</v>
@@ -29669,7 +29674,7 @@
         <v>540</v>
       </c>
       <c r="AF241" t="s">
-        <v>846</v>
+        <v>845</v>
       </c>
       <c r="AG241">
         <v>0</v>
@@ -29686,10 +29691,10 @@
         <v>4239</v>
       </c>
       <c r="B242" t="s">
+        <v>846</v>
+      </c>
+      <c r="C242" t="s">
         <v>847</v>
-      </c>
-      <c r="C242" t="s">
-        <v>848</v>
       </c>
       <c r="D242">
         <v>84</v>
@@ -29767,7 +29772,7 @@
         <v>119</v>
       </c>
       <c r="AC242" t="s">
-        <v>849</v>
+        <v>848</v>
       </c>
       <c r="AD242" t="s">
         <v>99</v>
@@ -29776,7 +29781,7 @@
         <v>624</v>
       </c>
       <c r="AF242" t="s">
-        <v>850</v>
+        <v>849</v>
       </c>
       <c r="AG242">
         <v>0</v>
@@ -29793,10 +29798,10 @@
         <v>4240</v>
       </c>
       <c r="B243" t="s">
+        <v>850</v>
+      </c>
+      <c r="C243" t="s">
         <v>851</v>
-      </c>
-      <c r="C243" t="s">
-        <v>852</v>
       </c>
       <c r="D243">
         <v>58</v>
@@ -29883,7 +29888,7 @@
         <v>432</v>
       </c>
       <c r="AF243" t="s">
-        <v>853</v>
+        <v>852</v>
       </c>
       <c r="AG243">
         <v>0</v>
@@ -29900,10 +29905,10 @@
         <v>4241</v>
       </c>
       <c r="B244" t="s">
+        <v>853</v>
+      </c>
+      <c r="C244" t="s">
         <v>854</v>
-      </c>
-      <c r="C244" t="s">
-        <v>855</v>
       </c>
       <c r="D244">
         <v>34</v>
@@ -29990,7 +29995,7 @@
         <v>240</v>
       </c>
       <c r="AF244" t="s">
-        <v>856</v>
+        <v>855</v>
       </c>
       <c r="AG244">
         <v>0</v>
@@ -30007,10 +30012,10 @@
         <v>4242</v>
       </c>
       <c r="B245" t="s">
+        <v>856</v>
+      </c>
+      <c r="C245" t="s">
         <v>857</v>
-      </c>
-      <c r="C245" t="s">
-        <v>858</v>
       </c>
       <c r="D245">
         <v>66</v>
@@ -30097,7 +30102,7 @@
         <v>336</v>
       </c>
       <c r="AF245" t="s">
-        <v>859</v>
+        <v>858</v>
       </c>
       <c r="AG245">
         <v>0</v>
@@ -30114,10 +30119,10 @@
         <v>4243</v>
       </c>
       <c r="B246" t="s">
-        <v>860</v>
+        <v>859</v>
       </c>
       <c r="C246" t="s">
-        <v>858</v>
+        <v>857</v>
       </c>
       <c r="D246">
         <v>65</v>
@@ -30204,7 +30209,7 @@
         <v>336</v>
       </c>
       <c r="AF246" t="s">
-        <v>861</v>
+        <v>860</v>
       </c>
       <c r="AG246">
         <v>0</v>
@@ -30221,10 +30226,10 @@
         <v>4244</v>
       </c>
       <c r="B247" t="s">
+        <v>861</v>
+      </c>
+      <c r="C247" t="s">
         <v>862</v>
-      </c>
-      <c r="C247" t="s">
-        <v>863</v>
       </c>
       <c r="D247">
         <v>56</v>
@@ -30302,7 +30307,7 @@
         <v>41</v>
       </c>
       <c r="AC247" t="s">
-        <v>1105</v>
+        <v>1104</v>
       </c>
       <c r="AD247" t="s">
         <v>115</v>
@@ -30311,7 +30316,7 @@
         <v>480</v>
       </c>
       <c r="AF247" t="s">
-        <v>864</v>
+        <v>863</v>
       </c>
       <c r="AG247">
         <v>0</v>
@@ -30328,10 +30333,10 @@
         <v>4245</v>
       </c>
       <c r="B248" t="s">
+        <v>864</v>
+      </c>
+      <c r="C248" t="s">
         <v>865</v>
-      </c>
-      <c r="C248" t="s">
-        <v>866</v>
       </c>
       <c r="D248">
         <v>37</v>
@@ -30418,7 +30423,7 @@
         <v>432</v>
       </c>
       <c r="AF248" t="s">
-        <v>867</v>
+        <v>866</v>
       </c>
       <c r="AG248">
         <v>0</v>
@@ -30435,10 +30440,10 @@
         <v>4246</v>
       </c>
       <c r="B249" t="s">
+        <v>867</v>
+      </c>
+      <c r="C249" t="s">
         <v>868</v>
-      </c>
-      <c r="C249" t="s">
-        <v>869</v>
       </c>
       <c r="D249">
         <v>60</v>
@@ -30498,7 +30503,7 @@
         <v>229</v>
       </c>
       <c r="W249" t="s">
-        <v>870</v>
+        <v>869</v>
       </c>
       <c r="X249">
         <v>1072</v>
@@ -30525,7 +30530,7 @@
         <v>312</v>
       </c>
       <c r="AF249" t="s">
-        <v>871</v>
+        <v>870</v>
       </c>
       <c r="AG249">
         <v>0</v>
@@ -30542,10 +30547,10 @@
         <v>4247</v>
       </c>
       <c r="B250" t="s">
+        <v>871</v>
+      </c>
+      <c r="C250" t="s">
         <v>872</v>
-      </c>
-      <c r="C250" t="s">
-        <v>873</v>
       </c>
       <c r="D250">
         <v>67</v>
@@ -30632,7 +30637,7 @@
         <v>720</v>
       </c>
       <c r="AF250" t="s">
-        <v>874</v>
+        <v>873</v>
       </c>
       <c r="AG250">
         <v>0</v>
@@ -30649,10 +30654,10 @@
         <v>4248</v>
       </c>
       <c r="B251" t="s">
+        <v>874</v>
+      </c>
+      <c r="C251" t="s">
         <v>875</v>
-      </c>
-      <c r="C251" t="s">
-        <v>876</v>
       </c>
       <c r="D251">
         <v>69</v>
@@ -30739,7 +30744,7 @@
         <v>720</v>
       </c>
       <c r="AF251" t="s">
-        <v>877</v>
+        <v>876</v>
       </c>
       <c r="AG251">
         <v>0</v>
@@ -30756,10 +30761,10 @@
         <v>4249</v>
       </c>
       <c r="B252" t="s">
+        <v>877</v>
+      </c>
+      <c r="C252" t="s">
         <v>878</v>
-      </c>
-      <c r="C252" t="s">
-        <v>879</v>
       </c>
       <c r="D252">
         <v>56</v>
@@ -30819,7 +30824,7 @@
         <v>219</v>
       </c>
       <c r="W252" t="s">
-        <v>880</v>
+        <v>879</v>
       </c>
       <c r="X252">
         <v>1260</v>
@@ -30846,7 +30851,7 @@
         <v>672</v>
       </c>
       <c r="AF252" t="s">
-        <v>881</v>
+        <v>880</v>
       </c>
       <c r="AG252">
         <v>0</v>
@@ -30863,10 +30868,10 @@
         <v>4250</v>
       </c>
       <c r="B253" t="s">
+        <v>881</v>
+      </c>
+      <c r="C253" t="s">
         <v>882</v>
-      </c>
-      <c r="C253" t="s">
-        <v>883</v>
       </c>
       <c r="D253">
         <v>52</v>
@@ -30953,7 +30958,7 @@
         <v>540</v>
       </c>
       <c r="AF253" t="s">
-        <v>884</v>
+        <v>883</v>
       </c>
       <c r="AG253">
         <v>0</v>
@@ -30970,10 +30975,10 @@
         <v>4251</v>
       </c>
       <c r="B254" t="s">
+        <v>884</v>
+      </c>
+      <c r="C254" t="s">
         <v>885</v>
-      </c>
-      <c r="C254" t="s">
-        <v>886</v>
       </c>
       <c r="D254">
         <v>70</v>
@@ -31033,7 +31038,7 @@
         <v>219</v>
       </c>
       <c r="W254" t="s">
-        <v>787</v>
+        <v>786</v>
       </c>
       <c r="X254">
         <v>972</v>
@@ -31060,7 +31065,7 @@
         <v>384</v>
       </c>
       <c r="AF254" t="s">
-        <v>887</v>
+        <v>886</v>
       </c>
       <c r="AG254">
         <v>0</v>
@@ -31077,10 +31082,10 @@
         <v>4252</v>
       </c>
       <c r="B255" t="s">
+        <v>887</v>
+      </c>
+      <c r="C255" t="s">
         <v>888</v>
-      </c>
-      <c r="C255" t="s">
-        <v>889</v>
       </c>
       <c r="D255">
         <v>72</v>
@@ -31140,7 +31145,7 @@
         <v>140</v>
       </c>
       <c r="W255" t="s">
-        <v>797</v>
+        <v>796</v>
       </c>
       <c r="X255">
         <v>504</v>
@@ -31167,7 +31172,7 @@
         <v>420</v>
       </c>
       <c r="AF255" t="s">
-        <v>890</v>
+        <v>889</v>
       </c>
       <c r="AG255">
         <v>0</v>
@@ -31184,10 +31189,10 @@
         <v>4253</v>
       </c>
       <c r="B256" t="s">
-        <v>891</v>
+        <v>890</v>
       </c>
       <c r="C256" t="s">
-        <v>889</v>
+        <v>888</v>
       </c>
       <c r="D256">
         <v>80</v>
@@ -31274,7 +31279,7 @@
         <v>420</v>
       </c>
       <c r="AF256" t="s">
-        <v>892</v>
+        <v>891</v>
       </c>
       <c r="AG256">
         <v>0</v>
@@ -31291,10 +31296,10 @@
         <v>4254</v>
       </c>
       <c r="B257" t="s">
-        <v>893</v>
+        <v>892</v>
       </c>
       <c r="C257" t="s">
-        <v>889</v>
+        <v>888</v>
       </c>
       <c r="D257">
         <v>78</v>
@@ -31381,7 +31386,7 @@
         <v>420</v>
       </c>
       <c r="AF257" t="s">
-        <v>894</v>
+        <v>893</v>
       </c>
       <c r="AG257">
         <v>0</v>
@@ -31398,10 +31403,10 @@
         <v>4255</v>
       </c>
       <c r="B258" t="s">
-        <v>895</v>
+        <v>894</v>
       </c>
       <c r="C258" t="s">
-        <v>889</v>
+        <v>888</v>
       </c>
       <c r="D258">
         <v>75</v>
@@ -31488,7 +31493,7 @@
         <v>420</v>
       </c>
       <c r="AF258" t="s">
-        <v>896</v>
+        <v>895</v>
       </c>
       <c r="AG258">
         <v>0</v>
@@ -31505,10 +31510,10 @@
         <v>4256</v>
       </c>
       <c r="B259" t="s">
+        <v>896</v>
+      </c>
+      <c r="C259" t="s">
         <v>897</v>
-      </c>
-      <c r="C259" t="s">
-        <v>898</v>
       </c>
       <c r="D259">
         <v>25</v>
@@ -31595,7 +31600,7 @@
         <v>108</v>
       </c>
       <c r="AF259" t="s">
-        <v>899</v>
+        <v>898</v>
       </c>
       <c r="AG259">
         <v>0</v>
@@ -31612,10 +31617,10 @@
         <v>4257</v>
       </c>
       <c r="B260" t="s">
-        <v>900</v>
+        <v>899</v>
       </c>
       <c r="C260" t="s">
-        <v>898</v>
+        <v>897</v>
       </c>
       <c r="D260">
         <v>28</v>
@@ -31675,7 +31680,7 @@
         <v>160</v>
       </c>
       <c r="W260" t="s">
-        <v>901</v>
+        <v>900</v>
       </c>
       <c r="X260">
         <v>1248</v>
@@ -31702,7 +31707,7 @@
         <v>336</v>
       </c>
       <c r="AF260" t="s">
-        <v>902</v>
+        <v>901</v>
       </c>
       <c r="AG260">
         <v>0</v>
@@ -31719,10 +31724,10 @@
         <v>4258</v>
       </c>
       <c r="B261" t="s">
+        <v>902</v>
+      </c>
+      <c r="C261" t="s">
         <v>903</v>
-      </c>
-      <c r="C261" t="s">
-        <v>904</v>
       </c>
       <c r="D261">
         <v>35</v>
@@ -31809,7 +31814,7 @@
         <v>1224</v>
       </c>
       <c r="AF261" t="s">
-        <v>905</v>
+        <v>904</v>
       </c>
       <c r="AG261">
         <v>0</v>
@@ -31826,10 +31831,10 @@
         <v>4259</v>
       </c>
       <c r="B262" t="s">
+        <v>905</v>
+      </c>
+      <c r="C262" t="s">
         <v>906</v>
-      </c>
-      <c r="C262" t="s">
-        <v>907</v>
       </c>
       <c r="D262">
         <v>42</v>
@@ -31916,7 +31921,7 @@
         <v>336</v>
       </c>
       <c r="AF262" t="s">
-        <v>908</v>
+        <v>907</v>
       </c>
       <c r="AG262">
         <v>0</v>
@@ -31933,10 +31938,10 @@
         <v>4260</v>
       </c>
       <c r="B263" t="s">
+        <v>908</v>
+      </c>
+      <c r="C263" t="s">
         <v>909</v>
-      </c>
-      <c r="C263" t="s">
-        <v>910</v>
       </c>
       <c r="D263">
         <v>25</v>
@@ -32023,7 +32028,7 @@
         <v>384</v>
       </c>
       <c r="AF263" t="s">
-        <v>911</v>
+        <v>910</v>
       </c>
       <c r="AG263">
         <v>0</v>
@@ -32040,10 +32045,10 @@
         <v>4261</v>
       </c>
       <c r="B264" t="s">
+        <v>911</v>
+      </c>
+      <c r="C264" t="s">
         <v>912</v>
-      </c>
-      <c r="C264" t="s">
-        <v>913</v>
       </c>
       <c r="D264">
         <v>73</v>
@@ -32121,7 +32126,7 @@
         <v>119</v>
       </c>
       <c r="AC264" t="s">
-        <v>1117</v>
+        <v>1116</v>
       </c>
       <c r="AD264" t="s">
         <v>99</v>
@@ -32130,7 +32135,7 @@
         <v>312</v>
       </c>
       <c r="AF264" t="s">
-        <v>914</v>
+        <v>913</v>
       </c>
       <c r="AG264">
         <v>0</v>
@@ -32147,10 +32152,10 @@
         <v>4262</v>
       </c>
       <c r="B265" t="s">
+        <v>914</v>
+      </c>
+      <c r="C265" t="s">
         <v>915</v>
-      </c>
-      <c r="C265" t="s">
-        <v>916</v>
       </c>
       <c r="D265">
         <v>61</v>
@@ -32237,7 +32242,7 @@
         <v>288</v>
       </c>
       <c r="AF265" t="s">
-        <v>917</v>
+        <v>916</v>
       </c>
       <c r="AG265">
         <v>0</v>
@@ -32254,10 +32259,10 @@
         <v>4263</v>
       </c>
       <c r="B266" t="s">
+        <v>917</v>
+      </c>
+      <c r="C266" t="s">
         <v>918</v>
-      </c>
-      <c r="C266" t="s">
-        <v>919</v>
       </c>
       <c r="D266">
         <v>77</v>
@@ -32344,7 +32349,7 @@
         <v>252</v>
       </c>
       <c r="AF266" t="s">
-        <v>920</v>
+        <v>919</v>
       </c>
       <c r="AG266">
         <v>0</v>
@@ -32361,10 +32366,10 @@
         <v>4264</v>
       </c>
       <c r="B267" t="s">
+        <v>920</v>
+      </c>
+      <c r="C267" t="s">
         <v>921</v>
-      </c>
-      <c r="C267" t="s">
-        <v>922</v>
       </c>
       <c r="D267">
         <v>38</v>
@@ -32451,7 +32456,7 @@
         <v>432</v>
       </c>
       <c r="AF267" t="s">
-        <v>923</v>
+        <v>922</v>
       </c>
       <c r="AG267">
         <v>0</v>
@@ -32468,10 +32473,10 @@
         <v>4265</v>
       </c>
       <c r="B268" t="s">
+        <v>923</v>
+      </c>
+      <c r="C268" t="s">
         <v>924</v>
-      </c>
-      <c r="C268" t="s">
-        <v>925</v>
       </c>
       <c r="D268">
         <v>74</v>
@@ -32549,7 +32554,7 @@
         <v>41</v>
       </c>
       <c r="AC268" t="s">
-        <v>926</v>
+        <v>925</v>
       </c>
       <c r="AD268" t="s">
         <v>99</v>
@@ -32558,7 +32563,7 @@
         <v>720</v>
       </c>
       <c r="AF268" t="s">
-        <v>927</v>
+        <v>926</v>
       </c>
       <c r="AG268">
         <v>0</v>
@@ -32575,10 +32580,10 @@
         <v>4266</v>
       </c>
       <c r="B269" t="s">
+        <v>927</v>
+      </c>
+      <c r="C269" t="s">
         <v>928</v>
-      </c>
-      <c r="C269" t="s">
-        <v>929</v>
       </c>
       <c r="D269">
         <v>15</v>
@@ -32665,7 +32670,7 @@
         <v>468</v>
       </c>
       <c r="AF269" t="s">
-        <v>930</v>
+        <v>929</v>
       </c>
       <c r="AG269">
         <v>0</v>
@@ -32682,10 +32687,10 @@
         <v>4267</v>
       </c>
       <c r="B270" t="s">
+        <v>930</v>
+      </c>
+      <c r="C270" t="s">
         <v>931</v>
-      </c>
-      <c r="C270" t="s">
-        <v>932</v>
       </c>
       <c r="D270">
         <v>42</v>
@@ -32772,7 +32777,7 @@
         <v>540</v>
       </c>
       <c r="AF270" t="s">
-        <v>933</v>
+        <v>932</v>
       </c>
       <c r="AG270">
         <v>0</v>
@@ -32789,10 +32794,10 @@
         <v>4268</v>
       </c>
       <c r="B271" t="s">
+        <v>933</v>
+      </c>
+      <c r="C271" t="s">
         <v>934</v>
-      </c>
-      <c r="C271" t="s">
-        <v>935</v>
       </c>
       <c r="D271">
         <v>18</v>
@@ -32879,7 +32884,7 @@
         <v>336</v>
       </c>
       <c r="AF271" t="s">
-        <v>936</v>
+        <v>935</v>
       </c>
       <c r="AG271">
         <v>0</v>
@@ -32896,10 +32901,10 @@
         <v>4269</v>
       </c>
       <c r="B272" t="s">
+        <v>936</v>
+      </c>
+      <c r="C272" t="s">
         <v>937</v>
-      </c>
-      <c r="C272" t="s">
-        <v>938</v>
       </c>
       <c r="D272">
         <v>20</v>
@@ -32986,7 +32991,7 @@
         <v>288</v>
       </c>
       <c r="AF272" t="s">
-        <v>939</v>
+        <v>938</v>
       </c>
       <c r="AG272">
         <v>0</v>
@@ -33003,10 +33008,10 @@
         <v>4270</v>
       </c>
       <c r="B273" t="s">
+        <v>939</v>
+      </c>
+      <c r="C273" t="s">
         <v>940</v>
-      </c>
-      <c r="C273" t="s">
-        <v>941</v>
       </c>
       <c r="D273">
         <v>21</v>
@@ -33093,7 +33098,7 @@
         <v>252</v>
       </c>
       <c r="AF273" t="s">
-        <v>942</v>
+        <v>941</v>
       </c>
       <c r="AG273">
         <v>0</v>
@@ -33110,10 +33115,10 @@
         <v>4271</v>
       </c>
       <c r="B274" t="s">
+        <v>942</v>
+      </c>
+      <c r="C274" t="s">
         <v>943</v>
-      </c>
-      <c r="C274" t="s">
-        <v>944</v>
       </c>
       <c r="D274">
         <v>61</v>
@@ -33173,7 +33178,7 @@
         <v>160</v>
       </c>
       <c r="W274" t="s">
-        <v>945</v>
+        <v>944</v>
       </c>
       <c r="X274">
         <v>1100</v>
@@ -33200,7 +33205,7 @@
         <v>576</v>
       </c>
       <c r="AF274" t="s">
-        <v>946</v>
+        <v>945</v>
       </c>
       <c r="AG274">
         <v>0</v>
@@ -33217,10 +33222,10 @@
         <v>4272</v>
       </c>
       <c r="B275" t="s">
+        <v>946</v>
+      </c>
+      <c r="C275" t="s">
         <v>947</v>
-      </c>
-      <c r="C275" t="s">
-        <v>948</v>
       </c>
       <c r="D275">
         <v>63</v>
@@ -33307,7 +33312,7 @@
         <v>576</v>
       </c>
       <c r="AF275" t="s">
-        <v>949</v>
+        <v>948</v>
       </c>
       <c r="AG275">
         <v>0</v>
@@ -33324,10 +33329,10 @@
         <v>4273</v>
       </c>
       <c r="B276" t="s">
+        <v>949</v>
+      </c>
+      <c r="C276" t="s">
         <v>950</v>
-      </c>
-      <c r="C276" t="s">
-        <v>951</v>
       </c>
       <c r="D276">
         <v>61</v>
@@ -33414,7 +33419,7 @@
         <v>480</v>
       </c>
       <c r="AF276" t="s">
-        <v>952</v>
+        <v>951</v>
       </c>
       <c r="AG276">
         <v>0</v>
@@ -33431,10 +33436,10 @@
         <v>4274</v>
       </c>
       <c r="B277" t="s">
+        <v>952</v>
+      </c>
+      <c r="C277" t="s">
         <v>953</v>
-      </c>
-      <c r="C277" t="s">
-        <v>954</v>
       </c>
       <c r="D277">
         <v>65</v>
@@ -33521,7 +33526,7 @@
         <v>900</v>
       </c>
       <c r="AF277" t="s">
-        <v>955</v>
+        <v>954</v>
       </c>
       <c r="AG277">
         <v>0</v>
@@ -33538,10 +33543,10 @@
         <v>4275</v>
       </c>
       <c r="B278" t="s">
+        <v>955</v>
+      </c>
+      <c r="C278" t="s">
         <v>956</v>
-      </c>
-      <c r="C278" t="s">
-        <v>957</v>
       </c>
       <c r="D278">
         <v>59</v>
@@ -33628,7 +33633,7 @@
         <v>432</v>
       </c>
       <c r="AF278" t="s">
-        <v>958</v>
+        <v>957</v>
       </c>
       <c r="AG278">
         <v>0</v>
@@ -33645,10 +33650,10 @@
         <v>4276</v>
       </c>
       <c r="B279" t="s">
+        <v>958</v>
+      </c>
+      <c r="C279" t="s">
         <v>959</v>
-      </c>
-      <c r="C279" t="s">
-        <v>960</v>
       </c>
       <c r="D279">
         <v>72</v>
@@ -33735,7 +33740,7 @@
         <v>288</v>
       </c>
       <c r="AF279" t="s">
-        <v>961</v>
+        <v>960</v>
       </c>
       <c r="AG279">
         <v>0</v>
@@ -33752,10 +33757,10 @@
         <v>4277</v>
       </c>
       <c r="B280" t="s">
+        <v>961</v>
+      </c>
+      <c r="C280" t="s">
         <v>962</v>
-      </c>
-      <c r="C280" t="s">
-        <v>963</v>
       </c>
       <c r="D280">
         <v>79</v>
@@ -33815,7 +33820,7 @@
         <v>219</v>
       </c>
       <c r="W280" t="s">
-        <v>797</v>
+        <v>796</v>
       </c>
       <c r="X280">
         <v>1720</v>
@@ -33833,7 +33838,7 @@
         <v>41</v>
       </c>
       <c r="AC280" t="s">
-        <v>964</v>
+        <v>963</v>
       </c>
       <c r="AD280" t="s">
         <v>99</v>
@@ -33842,7 +33847,7 @@
         <v>1080</v>
       </c>
       <c r="AF280" t="s">
-        <v>965</v>
+        <v>964</v>
       </c>
       <c r="AG280">
         <v>0</v>
@@ -33859,10 +33864,10 @@
         <v>4278</v>
       </c>
       <c r="B281" t="s">
+        <v>965</v>
+      </c>
+      <c r="C281" t="s">
         <v>966</v>
-      </c>
-      <c r="C281" t="s">
-        <v>967</v>
       </c>
       <c r="D281">
         <v>40</v>
@@ -33949,7 +33954,7 @@
         <v>384</v>
       </c>
       <c r="AF281" t="s">
-        <v>968</v>
+        <v>967</v>
       </c>
       <c r="AG281">
         <v>0</v>
@@ -33966,10 +33971,10 @@
         <v>4279</v>
       </c>
       <c r="B282" t="s">
+        <v>968</v>
+      </c>
+      <c r="C282" t="s">
         <v>969</v>
-      </c>
-      <c r="C282" t="s">
-        <v>970</v>
       </c>
       <c r="D282">
         <v>32</v>
@@ -34056,7 +34061,7 @@
         <v>540</v>
       </c>
       <c r="AF282" t="s">
-        <v>971</v>
+        <v>970</v>
       </c>
       <c r="AG282">
         <v>0</v>
@@ -34073,10 +34078,10 @@
         <v>4280</v>
       </c>
       <c r="B283" t="s">
+        <v>971</v>
+      </c>
+      <c r="C283" t="s">
         <v>972</v>
-      </c>
-      <c r="C283" t="s">
-        <v>973</v>
       </c>
       <c r="D283">
         <v>60</v>
@@ -34163,7 +34168,7 @@
         <v>720</v>
       </c>
       <c r="AF283" t="s">
-        <v>974</v>
+        <v>973</v>
       </c>
       <c r="AG283">
         <v>0</v>
@@ -34180,10 +34185,10 @@
         <v>4281</v>
       </c>
       <c r="B284" t="s">
+        <v>974</v>
+      </c>
+      <c r="C284" t="s">
         <v>975</v>
-      </c>
-      <c r="C284" t="s">
-        <v>976</v>
       </c>
       <c r="D284">
         <v>34</v>
@@ -34270,7 +34275,7 @@
         <v>696</v>
       </c>
       <c r="AF284" t="s">
-        <v>977</v>
+        <v>976</v>
       </c>
       <c r="AG284">
         <v>0</v>
@@ -34287,10 +34292,10 @@
         <v>4282</v>
       </c>
       <c r="B285" t="s">
+        <v>977</v>
+      </c>
+      <c r="C285" t="s">
         <v>978</v>
-      </c>
-      <c r="C285" t="s">
-        <v>979</v>
       </c>
       <c r="D285">
         <v>45</v>
@@ -34368,7 +34373,7 @@
         <v>41</v>
       </c>
       <c r="AC285" t="s">
-        <v>1102</v>
+        <v>1101</v>
       </c>
       <c r="AD285" t="s">
         <v>115</v>
@@ -34377,7 +34382,7 @@
         <v>936</v>
       </c>
       <c r="AF285" t="s">
-        <v>980</v>
+        <v>979</v>
       </c>
       <c r="AG285">
         <v>0</v>
@@ -34394,10 +34399,10 @@
         <v>4283</v>
       </c>
       <c r="B286" t="s">
+        <v>980</v>
+      </c>
+      <c r="C286" t="s">
         <v>981</v>
-      </c>
-      <c r="C286" t="s">
-        <v>982</v>
       </c>
       <c r="D286">
         <v>70</v>
@@ -34475,7 +34480,7 @@
         <v>119</v>
       </c>
       <c r="AC286" t="s">
-        <v>983</v>
+        <v>982</v>
       </c>
       <c r="AD286" t="s">
         <v>99</v>
@@ -34484,7 +34489,7 @@
         <v>384</v>
       </c>
       <c r="AF286" t="s">
-        <v>984</v>
+        <v>983</v>
       </c>
       <c r="AG286">
         <v>0</v>
@@ -34501,10 +34506,10 @@
         <v>4284</v>
       </c>
       <c r="B287" t="s">
+        <v>984</v>
+      </c>
+      <c r="C287" t="s">
         <v>985</v>
-      </c>
-      <c r="C287" t="s">
-        <v>986</v>
       </c>
       <c r="D287">
         <v>50</v>
@@ -34591,7 +34596,7 @@
         <v>0</v>
       </c>
       <c r="AF287" t="s">
-        <v>987</v>
+        <v>986</v>
       </c>
       <c r="AG287">
         <v>0</v>
@@ -34603,7 +34608,7 @@
         <v>1</v>
       </c>
       <c r="AJ287" t="s">
-        <v>988</v>
+        <v>987</v>
       </c>
     </row>
     <row r="288" spans="1:36" x14ac:dyDescent="0.4">
@@ -34611,10 +34616,10 @@
         <v>4285</v>
       </c>
       <c r="B288" t="s">
+        <v>988</v>
+      </c>
+      <c r="C288" t="s">
         <v>989</v>
-      </c>
-      <c r="C288" t="s">
-        <v>990</v>
       </c>
       <c r="D288">
         <v>50</v>
@@ -34695,13 +34700,13 @@
         <v>41</v>
       </c>
       <c r="AD288" t="s">
-        <v>991</v>
+        <v>990</v>
       </c>
       <c r="AE288">
         <v>216</v>
       </c>
       <c r="AF288" t="s">
-        <v>992</v>
+        <v>991</v>
       </c>
       <c r="AG288">
         <v>0</v>
@@ -34713,7 +34718,7 @@
         <v>1</v>
       </c>
       <c r="AJ288" t="s">
-        <v>988</v>
+        <v>987</v>
       </c>
     </row>
     <row r="289" spans="1:36" x14ac:dyDescent="0.4">
@@ -34721,10 +34726,10 @@
         <v>4286</v>
       </c>
       <c r="B289" t="s">
+        <v>992</v>
+      </c>
+      <c r="C289" t="s">
         <v>993</v>
-      </c>
-      <c r="C289" t="s">
-        <v>994</v>
       </c>
       <c r="D289">
         <v>99</v>
@@ -34802,7 +34807,7 @@
         <v>119</v>
       </c>
       <c r="AC289" t="s">
-        <v>995</v>
+        <v>994</v>
       </c>
       <c r="AD289" t="s">
         <v>99</v>
@@ -34811,7 +34816,7 @@
         <v>504</v>
       </c>
       <c r="AF289" t="s">
-        <v>996</v>
+        <v>995</v>
       </c>
       <c r="AG289">
         <v>0</v>
@@ -34828,10 +34833,10 @@
         <v>4287</v>
       </c>
       <c r="B290" t="s">
+        <v>996</v>
+      </c>
+      <c r="C290" t="s">
         <v>997</v>
-      </c>
-      <c r="C290" t="s">
-        <v>998</v>
       </c>
       <c r="D290">
         <v>99</v>
@@ -34909,7 +34914,7 @@
         <v>119</v>
       </c>
       <c r="AC290" t="s">
-        <v>999</v>
+        <v>998</v>
       </c>
       <c r="AD290" t="s">
         <v>99</v>
@@ -34918,7 +34923,7 @@
         <v>504</v>
       </c>
       <c r="AF290" t="s">
-        <v>1000</v>
+        <v>999</v>
       </c>
       <c r="AG290">
         <v>0</v>
@@ -34935,10 +34940,10 @@
         <v>4288</v>
       </c>
       <c r="B291" t="s">
+        <v>1000</v>
+      </c>
+      <c r="C291" t="s">
         <v>1001</v>
-      </c>
-      <c r="C291" t="s">
-        <v>1002</v>
       </c>
       <c r="D291">
         <v>43</v>
@@ -35019,13 +35024,13 @@
         <v>48</v>
       </c>
       <c r="AD291" t="s">
-        <v>1107</v>
+        <v>1106</v>
       </c>
       <c r="AE291">
         <v>384</v>
       </c>
       <c r="AF291" t="s">
-        <v>1003</v>
+        <v>1002</v>
       </c>
       <c r="AG291">
         <v>0</v>
@@ -35042,10 +35047,10 @@
         <v>4289</v>
       </c>
       <c r="B292" t="s">
+        <v>1003</v>
+      </c>
+      <c r="C292" t="s">
         <v>1004</v>
-      </c>
-      <c r="C292" t="s">
-        <v>1005</v>
       </c>
       <c r="D292">
         <v>69</v>
@@ -35132,7 +35137,7 @@
         <v>480</v>
       </c>
       <c r="AF292" t="s">
-        <v>1006</v>
+        <v>1005</v>
       </c>
       <c r="AG292">
         <v>0</v>
@@ -35149,10 +35154,10 @@
         <v>4290</v>
       </c>
       <c r="B293" t="s">
+        <v>1006</v>
+      </c>
+      <c r="C293" t="s">
         <v>1007</v>
-      </c>
-      <c r="C293" t="s">
-        <v>1008</v>
       </c>
       <c r="D293">
         <v>41</v>
@@ -35239,7 +35244,7 @@
         <v>576</v>
       </c>
       <c r="AF293" t="s">
-        <v>1009</v>
+        <v>1008</v>
       </c>
       <c r="AG293">
         <v>0</v>
@@ -35256,10 +35261,10 @@
         <v>4291</v>
       </c>
       <c r="B294" t="s">
+        <v>1009</v>
+      </c>
+      <c r="C294" t="s">
         <v>1010</v>
-      </c>
-      <c r="C294" t="s">
-        <v>1011</v>
       </c>
       <c r="D294">
         <v>30</v>
@@ -35346,7 +35351,7 @@
         <v>432</v>
       </c>
       <c r="AF294" t="s">
-        <v>1012</v>
+        <v>1011</v>
       </c>
       <c r="AG294">
         <v>0</v>
@@ -35363,10 +35368,10 @@
         <v>4292</v>
       </c>
       <c r="B295" t="s">
+        <v>1012</v>
+      </c>
+      <c r="C295" t="s">
         <v>1013</v>
-      </c>
-      <c r="C295" t="s">
-        <v>1014</v>
       </c>
       <c r="D295">
         <v>65</v>
@@ -35453,7 +35458,7 @@
         <v>624</v>
       </c>
       <c r="AF295" t="s">
-        <v>1015</v>
+        <v>1014</v>
       </c>
       <c r="AG295">
         <v>0</v>
@@ -35470,10 +35475,10 @@
         <v>4293</v>
       </c>
       <c r="B296" t="s">
+        <v>1015</v>
+      </c>
+      <c r="C296" t="s">
         <v>1016</v>
-      </c>
-      <c r="C296" t="s">
-        <v>1017</v>
       </c>
       <c r="D296">
         <v>47</v>
@@ -35560,7 +35565,7 @@
         <v>480</v>
       </c>
       <c r="AF296" t="s">
-        <v>1018</v>
+        <v>1017</v>
       </c>
       <c r="AG296">
         <v>0</v>
@@ -35577,10 +35582,10 @@
         <v>4294</v>
       </c>
       <c r="B297" t="s">
+        <v>1018</v>
+      </c>
+      <c r="C297" t="s">
         <v>1019</v>
-      </c>
-      <c r="C297" t="s">
-        <v>1020</v>
       </c>
       <c r="D297">
         <v>71</v>
@@ -35667,7 +35672,7 @@
         <v>425</v>
       </c>
       <c r="AF297" t="s">
-        <v>1021</v>
+        <v>1020</v>
       </c>
       <c r="AG297">
         <v>0</v>
@@ -35684,10 +35689,10 @@
         <v>4295</v>
       </c>
       <c r="B298" t="s">
+        <v>1021</v>
+      </c>
+      <c r="C298" t="s">
         <v>1022</v>
-      </c>
-      <c r="C298" t="s">
-        <v>1023</v>
       </c>
       <c r="D298">
         <v>33</v>
@@ -35774,7 +35779,7 @@
         <v>672</v>
       </c>
       <c r="AF298" t="s">
-        <v>1024</v>
+        <v>1023</v>
       </c>
       <c r="AG298">
         <v>0</v>
@@ -35791,10 +35796,10 @@
         <v>4296</v>
       </c>
       <c r="B299" t="s">
-        <v>1025</v>
+        <v>1024</v>
       </c>
       <c r="C299" t="s">
-        <v>1106</v>
+        <v>1105</v>
       </c>
       <c r="D299">
         <v>56</v>
@@ -35881,7 +35886,7 @@
         <v>540</v>
       </c>
       <c r="AF299" t="s">
-        <v>1026</v>
+        <v>1025</v>
       </c>
       <c r="AG299">
         <v>0</v>
@@ -35898,10 +35903,10 @@
         <v>4297</v>
       </c>
       <c r="B300" t="s">
+        <v>1026</v>
+      </c>
+      <c r="C300" t="s">
         <v>1027</v>
-      </c>
-      <c r="C300" t="s">
-        <v>1028</v>
       </c>
       <c r="D300">
         <v>46</v>
@@ -35988,7 +35993,7 @@
         <v>624</v>
       </c>
       <c r="AF300" t="s">
-        <v>1029</v>
+        <v>1028</v>
       </c>
       <c r="AG300">
         <v>0</v>
@@ -36005,7 +36010,7 @@
         <v>4298</v>
       </c>
       <c r="B301" t="s">
-        <v>1103</v>
+        <v>1102</v>
       </c>
       <c r="C301" t="s">
         <v>565</v>
@@ -36107,7 +36112,7 @@
         <v>1</v>
       </c>
       <c r="AJ301" t="s">
-        <v>1104</v>
+        <v>1103</v>
       </c>
     </row>
     <row r="302" spans="1:36" x14ac:dyDescent="0.4">
@@ -36115,7 +36120,7 @@
         <v>4299</v>
       </c>
       <c r="B302" t="s">
-        <v>1112</v>
+        <v>1111</v>
       </c>
       <c r="C302" t="s">
         <v>77</v>
@@ -36196,7 +36201,7 @@
         <v>41</v>
       </c>
       <c r="AC302" t="s">
-        <v>1099</v>
+        <v>1098</v>
       </c>
       <c r="AD302" t="s">
         <v>59</v>
@@ -36222,10 +36227,10 @@
         <v>4300</v>
       </c>
       <c r="B303" t="s">
+        <v>1112</v>
+      </c>
+      <c r="C303" t="s">
         <v>1113</v>
-      </c>
-      <c r="C303" t="s">
-        <v>1114</v>
       </c>
       <c r="D303">
         <v>31</v>
@@ -36303,7 +36308,7 @@
         <v>41</v>
       </c>
       <c r="AC303" t="s">
-        <v>1115</v>
+        <v>1114</v>
       </c>
       <c r="AD303" t="s">
         <v>99</v>
@@ -36324,7 +36329,7 @@
         <v>0.7</v>
       </c>
       <c r="AJ303" t="s">
-        <v>1116</v>
+        <v>1115</v>
       </c>
     </row>
   </sheetData>
@@ -36358,30 +36363,30 @@
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A1" t="s">
-        <v>1031</v>
+        <v>1030</v>
       </c>
       <c r="B1" t="s">
         <v>28</v>
       </c>
       <c r="C1" t="s">
+        <v>1084</v>
+      </c>
+      <c r="D1" t="s">
         <v>1085</v>
       </c>
-      <c r="D1" t="s">
-        <v>1086</v>
-      </c>
       <c r="E1" t="s">
+        <v>1044</v>
+      </c>
+      <c r="F1" t="s">
         <v>1045</v>
-      </c>
-      <c r="F1" t="s">
-        <v>1046</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A2" t="s">
-        <v>1060</v>
+        <v>1059</v>
       </c>
       <c r="B2" t="s">
-        <v>1047</v>
+        <v>1046</v>
       </c>
       <c r="C2">
         <v>0</v>
@@ -36392,10 +36397,10 @@
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A3" t="s">
-        <v>1060</v>
+        <v>1059</v>
       </c>
       <c r="B3" t="s">
-        <v>1048</v>
+        <v>1047</v>
       </c>
       <c r="C3">
         <v>0</v>
@@ -36404,18 +36409,18 @@
         <v>2</v>
       </c>
       <c r="E3" t="s">
+        <v>1086</v>
+      </c>
+      <c r="F3" t="s">
         <v>1087</v>
-      </c>
-      <c r="F3" t="s">
-        <v>1088</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A4" t="s">
-        <v>1060</v>
+        <v>1059</v>
       </c>
       <c r="B4" t="s">
-        <v>1049</v>
+        <v>1048</v>
       </c>
       <c r="C4">
         <v>0</v>
@@ -36424,18 +36429,18 @@
         <v>2</v>
       </c>
       <c r="E4" t="s">
+        <v>1088</v>
+      </c>
+      <c r="F4" t="s">
         <v>1089</v>
-      </c>
-      <c r="F4" t="s">
-        <v>1090</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A5" t="s">
-        <v>1063</v>
+        <v>1062</v>
       </c>
       <c r="B5" t="s">
-        <v>1047</v>
+        <v>1046</v>
       </c>
       <c r="C5">
         <v>0</v>
@@ -36446,10 +36451,10 @@
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A6" t="s">
-        <v>1063</v>
+        <v>1062</v>
       </c>
       <c r="B6" t="s">
-        <v>1048</v>
+        <v>1047</v>
       </c>
       <c r="C6">
         <v>0</v>
@@ -36458,10 +36463,10 @@
         <v>2</v>
       </c>
       <c r="E6" t="s">
+        <v>1090</v>
+      </c>
+      <c r="F6" t="s">
         <v>1091</v>
-      </c>
-      <c r="F6" t="s">
-        <v>1092</v>
       </c>
     </row>
   </sheetData>
@@ -36485,7 +36490,7 @@
         <v>3</v>
       </c>
       <c r="B1" t="s">
-        <v>1036</v>
+        <v>1035</v>
       </c>
       <c r="C1" t="s">
         <v>4</v>
@@ -37711,7 +37716,7 @@
         <v>3</v>
       </c>
       <c r="B1" s="7" t="s">
-        <v>1036</v>
+        <v>1035</v>
       </c>
       <c r="C1" s="7" t="s">
         <v>4</v>
@@ -37720,13 +37725,13 @@
         <v>11</v>
       </c>
       <c r="E1" s="7" t="s">
-        <v>1037</v>
+        <v>1036</v>
       </c>
       <c r="F1" s="7" t="s">
         <v>16</v>
       </c>
       <c r="G1" s="6" t="s">
-        <v>1038</v>
+        <v>1037</v>
       </c>
       <c r="H1" s="6" t="s">
         <v>14</v>
@@ -38432,11 +38437,11 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0E19C42E-4D03-4797-B846-FB5E09BB39D3}">
-  <dimension ref="A1:N24"/>
+  <dimension ref="A1:N25"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="P18" sqref="P18"/>
+      <selection pane="bottomLeft" activeCell="K9" sqref="K9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
@@ -38476,21 +38481,21 @@
         <v>14</v>
       </c>
       <c r="K1" t="s">
-        <v>1030</v>
+        <v>1029</v>
       </c>
       <c r="L1" t="s">
         <v>16</v>
       </c>
       <c r="M1" t="s">
+        <v>1030</v>
+      </c>
+      <c r="N1" t="s">
         <v>1031</v>
-      </c>
-      <c r="N1" t="s">
-        <v>1032</v>
       </c>
     </row>
     <row r="2" spans="1:14" x14ac:dyDescent="0.4">
       <c r="A2" t="s">
-        <v>1033</v>
+        <v>1032</v>
       </c>
       <c r="B2">
         <v>0</v>
@@ -38710,7 +38715,7 @@
     </row>
     <row r="7" spans="1:14" x14ac:dyDescent="0.4">
       <c r="A7" t="s">
-        <v>1034</v>
+        <v>1033</v>
       </c>
       <c r="B7">
         <v>100</v>
@@ -38798,13 +38803,13 @@
     </row>
     <row r="9" spans="1:14" x14ac:dyDescent="0.4">
       <c r="A9" t="s">
-        <v>39</v>
+        <v>1118</v>
       </c>
       <c r="B9">
-        <v>120</v>
+        <v>100</v>
       </c>
       <c r="C9">
-        <v>90</v>
+        <v>100</v>
       </c>
       <c r="D9">
         <v>70</v>
@@ -38813,28 +38818,28 @@
         <v>80</v>
       </c>
       <c r="F9">
-        <v>112</v>
+        <v>90</v>
       </c>
       <c r="G9">
-        <v>100</v>
+        <v>150</v>
       </c>
       <c r="H9">
+        <v>120</v>
+      </c>
+      <c r="I9">
+        <v>100</v>
+      </c>
+      <c r="J9">
         <v>80</v>
       </c>
-      <c r="I9">
-        <v>100</v>
-      </c>
-      <c r="J9">
+      <c r="K9">
+        <v>200</v>
+      </c>
+      <c r="L9">
+        <v>110</v>
+      </c>
+      <c r="M9">
         <v>120</v>
-      </c>
-      <c r="K9">
-        <v>120</v>
-      </c>
-      <c r="L9">
-        <v>90</v>
-      </c>
-      <c r="M9">
-        <v>90</v>
       </c>
       <c r="N9">
         <v>1</v>
@@ -38842,43 +38847,43 @@
     </row>
     <row r="10" spans="1:14" x14ac:dyDescent="0.4">
       <c r="A10" t="s">
-        <v>48</v>
+        <v>39</v>
       </c>
       <c r="B10">
+        <v>120</v>
+      </c>
+      <c r="C10">
+        <v>90</v>
+      </c>
+      <c r="D10">
+        <v>70</v>
+      </c>
+      <c r="E10">
         <v>80</v>
       </c>
-      <c r="C10">
-        <v>105</v>
-      </c>
-      <c r="D10">
+      <c r="F10">
+        <v>112</v>
+      </c>
+      <c r="G10">
+        <v>100</v>
+      </c>
+      <c r="H10">
         <v>80</v>
       </c>
-      <c r="E10">
-        <v>130</v>
-      </c>
-      <c r="F10">
-        <v>85</v>
-      </c>
-      <c r="G10">
-        <v>85</v>
-      </c>
-      <c r="H10">
+      <c r="I10">
+        <v>100</v>
+      </c>
+      <c r="J10">
         <v>120</v>
       </c>
-      <c r="I10">
-        <v>72</v>
-      </c>
-      <c r="J10">
-        <v>110</v>
-      </c>
       <c r="K10">
+        <v>120</v>
+      </c>
+      <c r="L10">
         <v>90</v>
       </c>
-      <c r="L10">
-        <v>94</v>
-      </c>
       <c r="M10">
-        <v>106</v>
+        <v>90</v>
       </c>
       <c r="N10">
         <v>1</v>
@@ -38886,43 +38891,43 @@
     </row>
     <row r="11" spans="1:14" x14ac:dyDescent="0.4">
       <c r="A11" t="s">
-        <v>219</v>
+        <v>48</v>
       </c>
       <c r="B11">
-        <v>92</v>
+        <v>80</v>
       </c>
       <c r="C11">
+        <v>105</v>
+      </c>
+      <c r="D11">
+        <v>80</v>
+      </c>
+      <c r="E11">
+        <v>130</v>
+      </c>
+      <c r="F11">
+        <v>85</v>
+      </c>
+      <c r="G11">
+        <v>85</v>
+      </c>
+      <c r="H11">
+        <v>120</v>
+      </c>
+      <c r="I11">
+        <v>72</v>
+      </c>
+      <c r="J11">
         <v>110</v>
       </c>
-      <c r="D11">
-        <v>110</v>
-      </c>
-      <c r="E11">
-        <v>98</v>
-      </c>
-      <c r="F11">
+      <c r="K11">
         <v>90</v>
       </c>
-      <c r="G11">
-        <v>120</v>
-      </c>
-      <c r="H11">
-        <v>102</v>
-      </c>
-      <c r="I11">
-        <v>95</v>
-      </c>
-      <c r="J11">
-        <v>95</v>
-      </c>
-      <c r="K11">
-        <v>95</v>
-      </c>
       <c r="L11">
-        <v>105</v>
+        <v>94</v>
       </c>
       <c r="M11">
-        <v>95</v>
+        <v>106</v>
       </c>
       <c r="N11">
         <v>1</v>
@@ -38930,43 +38935,43 @@
     </row>
     <row r="12" spans="1:14" x14ac:dyDescent="0.4">
       <c r="A12" t="s">
-        <v>547</v>
+        <v>219</v>
       </c>
       <c r="B12">
-        <v>60</v>
+        <v>92</v>
       </c>
       <c r="C12">
-        <v>100</v>
+        <v>110</v>
       </c>
       <c r="D12">
-        <v>60</v>
+        <v>110</v>
       </c>
       <c r="E12">
+        <v>98</v>
+      </c>
+      <c r="F12">
+        <v>90</v>
+      </c>
+      <c r="G12">
         <v>120</v>
       </c>
-      <c r="F12">
-        <v>50</v>
-      </c>
-      <c r="G12">
-        <v>150</v>
-      </c>
       <c r="H12">
-        <v>130</v>
+        <v>102</v>
       </c>
       <c r="I12">
-        <v>60</v>
+        <v>95</v>
       </c>
       <c r="J12">
-        <v>50</v>
+        <v>95</v>
       </c>
       <c r="K12">
-        <v>130</v>
+        <v>95</v>
       </c>
       <c r="L12">
-        <v>100</v>
+        <v>105</v>
       </c>
       <c r="M12">
-        <v>100</v>
+        <v>95</v>
       </c>
       <c r="N12">
         <v>1</v>
@@ -38974,43 +38979,43 @@
     </row>
     <row r="13" spans="1:14" x14ac:dyDescent="0.4">
       <c r="A13" t="s">
-        <v>469</v>
+        <v>547</v>
       </c>
       <c r="B13">
-        <v>140</v>
+        <v>60</v>
       </c>
       <c r="C13">
-        <v>90</v>
+        <v>100</v>
       </c>
       <c r="D13">
-        <v>70</v>
+        <v>60</v>
       </c>
       <c r="E13">
-        <v>90</v>
+        <v>120</v>
       </c>
       <c r="F13">
-        <v>70</v>
+        <v>50</v>
       </c>
       <c r="G13">
-        <v>90</v>
+        <v>150</v>
       </c>
       <c r="H13">
-        <v>100</v>
+        <v>130</v>
       </c>
       <c r="I13">
-        <v>0</v>
+        <v>60</v>
       </c>
       <c r="J13">
-        <v>70</v>
+        <v>50</v>
       </c>
       <c r="K13">
-        <v>70</v>
+        <v>130</v>
       </c>
       <c r="L13">
-        <v>82</v>
+        <v>100</v>
       </c>
       <c r="M13">
-        <v>85</v>
+        <v>100</v>
       </c>
       <c r="N13">
         <v>1</v>
@@ -39018,43 +39023,43 @@
     </row>
     <row r="14" spans="1:14" x14ac:dyDescent="0.4">
       <c r="A14" t="s">
-        <v>229</v>
+        <v>469</v>
       </c>
       <c r="B14">
-        <v>120</v>
+        <v>140</v>
       </c>
       <c r="C14">
-        <v>120</v>
+        <v>90</v>
       </c>
       <c r="D14">
+        <v>70</v>
+      </c>
+      <c r="E14">
         <v>90</v>
       </c>
-      <c r="E14">
-        <v>100</v>
-      </c>
       <c r="F14">
-        <v>110</v>
+        <v>70</v>
       </c>
       <c r="G14">
-        <v>130</v>
+        <v>90</v>
       </c>
       <c r="H14">
-        <v>110</v>
+        <v>100</v>
       </c>
       <c r="I14">
-        <v>130</v>
+        <v>0</v>
       </c>
       <c r="J14">
-        <v>90</v>
+        <v>70</v>
       </c>
       <c r="K14">
         <v>110</v>
       </c>
       <c r="L14">
-        <v>105</v>
+        <v>82</v>
       </c>
       <c r="M14">
-        <v>110</v>
+        <v>85</v>
       </c>
       <c r="N14">
         <v>1</v>
@@ -39062,43 +39067,43 @@
     </row>
     <row r="15" spans="1:14" x14ac:dyDescent="0.4">
       <c r="A15" t="s">
-        <v>275</v>
+        <v>229</v>
       </c>
       <c r="B15">
+        <v>120</v>
+      </c>
+      <c r="C15">
+        <v>120</v>
+      </c>
+      <c r="D15">
+        <v>90</v>
+      </c>
+      <c r="E15">
+        <v>100</v>
+      </c>
+      <c r="F15">
+        <v>110</v>
+      </c>
+      <c r="G15">
         <v>130</v>
       </c>
-      <c r="C15">
+      <c r="H15">
         <v>110</v>
       </c>
-      <c r="D15">
+      <c r="I15">
         <v>130</v>
       </c>
-      <c r="E15">
-        <v>100</v>
-      </c>
-      <c r="F15">
-        <v>120</v>
-      </c>
-      <c r="G15">
-        <v>70</v>
-      </c>
-      <c r="H15">
+      <c r="J15">
         <v>90</v>
       </c>
-      <c r="I15">
-        <v>80</v>
-      </c>
-      <c r="J15">
-        <v>80</v>
-      </c>
       <c r="K15">
-        <v>80</v>
+        <v>110</v>
       </c>
       <c r="L15">
+        <v>105</v>
+      </c>
+      <c r="M15">
         <v>110</v>
-      </c>
-      <c r="M15">
-        <v>90</v>
       </c>
       <c r="N15">
         <v>1</v>
@@ -39106,43 +39111,43 @@
     </row>
     <row r="16" spans="1:14" x14ac:dyDescent="0.4">
       <c r="A16" t="s">
-        <v>379</v>
+        <v>275</v>
       </c>
       <c r="B16">
-        <v>125</v>
+        <v>130</v>
       </c>
       <c r="C16">
+        <v>110</v>
+      </c>
+      <c r="D16">
+        <v>130</v>
+      </c>
+      <c r="E16">
+        <v>100</v>
+      </c>
+      <c r="F16">
         <v>120</v>
       </c>
-      <c r="D16">
-        <v>120</v>
-      </c>
-      <c r="E16">
+      <c r="G16">
+        <v>70</v>
+      </c>
+      <c r="H16">
+        <v>90</v>
+      </c>
+      <c r="I16">
+        <v>80</v>
+      </c>
+      <c r="J16">
+        <v>80</v>
+      </c>
+      <c r="K16">
+        <v>80</v>
+      </c>
+      <c r="L16">
         <v>110</v>
       </c>
-      <c r="F16">
-        <v>110</v>
-      </c>
-      <c r="G16">
+      <c r="M16">
         <v>90</v>
-      </c>
-      <c r="H16">
-        <v>100</v>
-      </c>
-      <c r="I16">
-        <v>100</v>
-      </c>
-      <c r="J16">
-        <v>100</v>
-      </c>
-      <c r="K16">
-        <v>100</v>
-      </c>
-      <c r="L16">
-        <v>115</v>
-      </c>
-      <c r="M16">
-        <v>105</v>
       </c>
       <c r="N16">
         <v>1</v>
@@ -39150,43 +39155,43 @@
     </row>
     <row r="17" spans="1:14" x14ac:dyDescent="0.4">
       <c r="A17" t="s">
-        <v>832</v>
+        <v>379</v>
       </c>
       <c r="B17">
-        <v>150</v>
+        <v>125</v>
       </c>
       <c r="C17">
         <v>120</v>
       </c>
       <c r="D17">
+        <v>120</v>
+      </c>
+      <c r="E17">
         <v>110</v>
       </c>
-      <c r="E17">
-        <v>70</v>
-      </c>
       <c r="F17">
-        <v>130</v>
+        <v>110</v>
       </c>
       <c r="G17">
         <v>90</v>
       </c>
       <c r="H17">
-        <v>90</v>
+        <v>100</v>
       </c>
       <c r="I17">
-        <v>90</v>
+        <v>100</v>
       </c>
       <c r="J17">
-        <v>130</v>
+        <v>100</v>
       </c>
       <c r="K17">
-        <v>110</v>
+        <v>100</v>
       </c>
       <c r="L17">
-        <v>135</v>
+        <v>115</v>
       </c>
       <c r="M17">
-        <v>125</v>
+        <v>105</v>
       </c>
       <c r="N17">
         <v>1</v>
@@ -39194,25 +39199,25 @@
     </row>
     <row r="18" spans="1:14" x14ac:dyDescent="0.4">
       <c r="A18" t="s">
-        <v>327</v>
+        <v>831</v>
       </c>
       <c r="B18">
+        <v>150</v>
+      </c>
+      <c r="C18">
+        <v>120</v>
+      </c>
+      <c r="D18">
+        <v>110</v>
+      </c>
+      <c r="E18">
+        <v>70</v>
+      </c>
+      <c r="F18">
         <v>130</v>
       </c>
-      <c r="C18">
-        <v>110</v>
-      </c>
-      <c r="D18">
-        <v>120</v>
-      </c>
-      <c r="E18">
-        <v>60</v>
-      </c>
-      <c r="F18">
-        <v>150</v>
-      </c>
       <c r="G18">
-        <v>80</v>
+        <v>90</v>
       </c>
       <c r="H18">
         <v>90</v>
@@ -39224,13 +39229,13 @@
         <v>150</v>
       </c>
       <c r="K18">
-        <v>105</v>
+        <v>110</v>
       </c>
       <c r="L18">
+        <v>135</v>
+      </c>
+      <c r="M18">
         <v>125</v>
-      </c>
-      <c r="M18">
-        <v>135</v>
       </c>
       <c r="N18">
         <v>1</v>
@@ -39238,43 +39243,43 @@
     </row>
     <row r="19" spans="1:14" x14ac:dyDescent="0.4">
       <c r="A19" t="s">
-        <v>286</v>
+        <v>327</v>
       </c>
       <c r="B19">
-        <v>160</v>
+        <v>130</v>
       </c>
       <c r="C19">
-        <v>130</v>
+        <v>110</v>
       </c>
       <c r="D19">
-        <v>110</v>
+        <v>120</v>
       </c>
       <c r="E19">
-        <v>100</v>
+        <v>60</v>
       </c>
       <c r="F19">
-        <v>110</v>
+        <v>150</v>
       </c>
       <c r="G19">
-        <v>95</v>
+        <v>80</v>
       </c>
       <c r="H19">
-        <v>100</v>
+        <v>90</v>
       </c>
       <c r="I19">
-        <v>100</v>
+        <v>90</v>
       </c>
       <c r="J19">
+        <v>150</v>
+      </c>
+      <c r="K19">
         <v>105</v>
       </c>
-      <c r="K19">
-        <v>95</v>
-      </c>
       <c r="L19">
+        <v>125</v>
+      </c>
+      <c r="M19">
         <v>135</v>
-      </c>
-      <c r="M19">
-        <v>125</v>
       </c>
       <c r="N19">
         <v>1</v>
@@ -39282,10 +39287,10 @@
     </row>
     <row r="20" spans="1:14" x14ac:dyDescent="0.4">
       <c r="A20" t="s">
-        <v>456</v>
+        <v>286</v>
       </c>
       <c r="B20">
-        <v>250</v>
+        <v>160</v>
       </c>
       <c r="C20">
         <v>130</v>
@@ -39294,75 +39299,75 @@
         <v>110</v>
       </c>
       <c r="E20">
-        <v>110</v>
+        <v>100</v>
       </c>
       <c r="F20">
         <v>110</v>
       </c>
       <c r="G20">
-        <v>110</v>
+        <v>95</v>
       </c>
       <c r="H20">
-        <v>110</v>
+        <v>100</v>
       </c>
       <c r="I20">
-        <v>110</v>
+        <v>100</v>
       </c>
       <c r="J20">
-        <v>110</v>
+        <v>105</v>
       </c>
       <c r="K20">
-        <v>110</v>
+        <v>95</v>
       </c>
       <c r="L20">
-        <v>180</v>
+        <v>135</v>
       </c>
       <c r="M20">
-        <v>180</v>
+        <v>125</v>
       </c>
       <c r="N20">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="21" spans="1:14" x14ac:dyDescent="0.4">
       <c r="A21" t="s">
-        <v>181</v>
+        <v>456</v>
       </c>
       <c r="B21">
-        <v>350</v>
+        <v>250</v>
       </c>
       <c r="C21">
-        <v>160</v>
+        <v>130</v>
       </c>
       <c r="D21">
-        <v>120</v>
+        <v>110</v>
       </c>
       <c r="E21">
-        <v>120</v>
+        <v>110</v>
       </c>
       <c r="F21">
-        <v>120</v>
+        <v>110</v>
       </c>
       <c r="G21">
-        <v>120</v>
+        <v>110</v>
       </c>
       <c r="H21">
-        <v>120</v>
+        <v>110</v>
       </c>
       <c r="I21">
-        <v>120</v>
+        <v>110</v>
       </c>
       <c r="J21">
-        <v>120</v>
+        <v>110</v>
       </c>
       <c r="K21">
-        <v>120</v>
+        <v>110</v>
       </c>
       <c r="L21">
-        <v>250</v>
+        <v>180</v>
       </c>
       <c r="M21">
-        <v>200</v>
+        <v>180</v>
       </c>
       <c r="N21">
         <v>2</v>
@@ -39370,75 +39375,75 @@
     </row>
     <row r="22" spans="1:14" x14ac:dyDescent="0.4">
       <c r="A22" t="s">
-        <v>756</v>
+        <v>181</v>
       </c>
       <c r="B22">
-        <v>700</v>
+        <v>350</v>
       </c>
       <c r="C22">
-        <v>175</v>
+        <v>160</v>
       </c>
       <c r="D22">
-        <v>130</v>
+        <v>120</v>
       </c>
       <c r="E22">
-        <v>130</v>
+        <v>120</v>
       </c>
       <c r="F22">
-        <v>130</v>
+        <v>120</v>
       </c>
       <c r="G22">
-        <v>130</v>
+        <v>120</v>
       </c>
       <c r="H22">
-        <v>130</v>
+        <v>120</v>
       </c>
       <c r="I22">
-        <v>130</v>
+        <v>120</v>
       </c>
       <c r="J22">
-        <v>130</v>
+        <v>120</v>
       </c>
       <c r="K22">
-        <v>130</v>
+        <v>120</v>
       </c>
       <c r="L22">
-        <v>450</v>
+        <v>250</v>
       </c>
       <c r="M22">
-        <v>400</v>
+        <v>200</v>
       </c>
       <c r="N22">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="23" spans="1:14" x14ac:dyDescent="0.4">
       <c r="A23" t="s">
-        <v>192</v>
+        <v>755</v>
       </c>
       <c r="B23">
-        <v>1000</v>
+        <v>700</v>
       </c>
       <c r="C23">
-        <v>190</v>
+        <v>175</v>
       </c>
       <c r="D23">
-        <v>140</v>
+        <v>130</v>
       </c>
       <c r="E23">
-        <v>140</v>
+        <v>130</v>
       </c>
       <c r="F23">
-        <v>140</v>
+        <v>130</v>
       </c>
       <c r="G23">
-        <v>140</v>
+        <v>130</v>
       </c>
       <c r="H23">
-        <v>140</v>
+        <v>130</v>
       </c>
       <c r="I23">
-        <v>140</v>
+        <v>130</v>
       </c>
       <c r="J23">
         <v>130</v>
@@ -39447,56 +39452,100 @@
         <v>130</v>
       </c>
       <c r="L23">
-        <v>900</v>
+        <v>450</v>
       </c>
       <c r="M23">
-        <v>800</v>
+        <v>400</v>
       </c>
       <c r="N23">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="24" spans="1:14" x14ac:dyDescent="0.4">
       <c r="A24" t="s">
+        <v>192</v>
+      </c>
+      <c r="B24">
+        <v>1000</v>
+      </c>
+      <c r="C24">
+        <v>190</v>
+      </c>
+      <c r="D24">
+        <v>140</v>
+      </c>
+      <c r="E24">
+        <v>140</v>
+      </c>
+      <c r="F24">
+        <v>140</v>
+      </c>
+      <c r="G24">
+        <v>140</v>
+      </c>
+      <c r="H24">
+        <v>140</v>
+      </c>
+      <c r="I24">
+        <v>140</v>
+      </c>
+      <c r="J24">
+        <v>130</v>
+      </c>
+      <c r="K24">
+        <v>130</v>
+      </c>
+      <c r="L24">
+        <v>900</v>
+      </c>
+      <c r="M24">
+        <v>800</v>
+      </c>
+      <c r="N24">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="25" spans="1:14" x14ac:dyDescent="0.4">
+      <c r="A25" t="s">
         <v>682</v>
       </c>
-      <c r="B24">
+      <c r="B25">
         <v>3000</v>
       </c>
-      <c r="C24">
+      <c r="C25">
         <v>200</v>
       </c>
-      <c r="D24">
+      <c r="D25">
         <v>180</v>
       </c>
-      <c r="E24">
+      <c r="E25">
         <v>180</v>
       </c>
-      <c r="F24">
+      <c r="F25">
         <v>180</v>
       </c>
-      <c r="G24">
+      <c r="G25">
         <v>180</v>
       </c>
-      <c r="H24">
+      <c r="H25">
         <v>180</v>
       </c>
-      <c r="I24">
+      <c r="I25">
         <v>180</v>
       </c>
-      <c r="J24">
+      <c r="J25">
         <v>140</v>
       </c>
-      <c r="K24">
+      <c r="K25">
         <v>140</v>
       </c>
-      <c r="L24">
+      <c r="L25">
         <v>1600</v>
       </c>
-      <c r="M24">
+      <c r="M25">
         <v>1600</v>
       </c>
-      <c r="N24">
+      <c r="N25">
         <v>5</v>
       </c>
     </row>
@@ -39510,8 +39559,8 @@
   <dimension ref="A1:M41"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="Q27" sqref="Q27"/>
+      <pane ySplit="1" topLeftCell="A5" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="K33" sqref="K33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
@@ -39548,18 +39597,18 @@
         <v>14</v>
       </c>
       <c r="K1" t="s">
-        <v>1030</v>
+        <v>1029</v>
       </c>
       <c r="L1" t="s">
         <v>16</v>
       </c>
       <c r="M1" t="s">
-        <v>1031</v>
+        <v>1030</v>
       </c>
     </row>
     <row r="2" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A2" s="2" t="s">
-        <v>945</v>
+        <v>944</v>
       </c>
       <c r="B2" s="2">
         <v>100</v>
@@ -39600,7 +39649,7 @@
     </row>
     <row r="3" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A3" s="2" t="s">
-        <v>797</v>
+        <v>796</v>
       </c>
       <c r="B3" s="2">
         <v>101</v>
@@ -40297,7 +40346,7 @@
     </row>
     <row r="20" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A20" s="2" t="s">
-        <v>787</v>
+        <v>786</v>
       </c>
       <c r="B20" s="2">
         <v>97</v>
@@ -40461,7 +40510,7 @@
     </row>
     <row r="24" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A24" t="s">
-        <v>880</v>
+        <v>879</v>
       </c>
       <c r="B24">
         <v>100</v>
@@ -40502,7 +40551,7 @@
     </row>
     <row r="25" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A25" t="s">
-        <v>1035</v>
+        <v>1034</v>
       </c>
       <c r="B25">
         <v>100</v>
@@ -40737,7 +40786,7 @@
         <v>99</v>
       </c>
       <c r="K30" s="3">
-        <v>99</v>
+        <v>110</v>
       </c>
       <c r="L30" s="3">
         <v>100</v>
@@ -40778,7 +40827,7 @@
         <v>98</v>
       </c>
       <c r="K31" s="3">
-        <v>98</v>
+        <v>120</v>
       </c>
       <c r="L31" s="3">
         <v>102</v>
@@ -40789,7 +40838,7 @@
     </row>
     <row r="32" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A32" s="3" t="s">
-        <v>773</v>
+        <v>772</v>
       </c>
       <c r="B32" s="3">
         <v>115</v>
@@ -40819,7 +40868,7 @@
         <v>97</v>
       </c>
       <c r="K32" s="3">
-        <v>97</v>
+        <v>135</v>
       </c>
       <c r="L32" s="3">
         <v>104</v>
@@ -40860,7 +40909,7 @@
         <v>96</v>
       </c>
       <c r="K33" s="3">
-        <v>96</v>
+        <v>150</v>
       </c>
       <c r="L33" s="3">
         <v>106</v>
@@ -41076,7 +41125,7 @@
     </row>
     <row r="39" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A39" s="3" t="s">
-        <v>901</v>
+        <v>900</v>
       </c>
       <c r="B39" s="3">
         <v>104</v>
@@ -41117,7 +41166,7 @@
     </row>
     <row r="40" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A40" s="3" t="s">
-        <v>870</v>
+        <v>869</v>
       </c>
       <c r="B40" s="3">
         <v>106</v>
@@ -41248,13 +41297,13 @@
         <v>14</v>
       </c>
       <c r="K1" t="s">
-        <v>1030</v>
+        <v>1029</v>
       </c>
       <c r="L1" t="s">
         <v>16</v>
       </c>
       <c r="M1" t="s">
-        <v>1031</v>
+        <v>1030</v>
       </c>
     </row>
     <row r="2" spans="1:13" x14ac:dyDescent="0.4">
@@ -41697,7 +41746,7 @@
         <v>3</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>1036</v>
+        <v>1035</v>
       </c>
       <c r="C1" s="1" t="s">
         <v>4</v>
@@ -41706,13 +41755,13 @@
         <v>11</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>1037</v>
+        <v>1036</v>
       </c>
       <c r="F1" s="1" t="s">
         <v>16</v>
       </c>
       <c r="G1" t="s">
-        <v>1038</v>
+        <v>1037</v>
       </c>
       <c r="H1" t="s">
         <v>14</v>
@@ -41721,10 +41770,10 @@
         <v>16</v>
       </c>
       <c r="K1" s="1" t="s">
+        <v>1109</v>
+      </c>
+      <c r="L1" t="s">
         <v>1110</v>
-      </c>
-      <c r="L1" t="s">
-        <v>1111</v>
       </c>
     </row>
     <row r="2" spans="1:14" x14ac:dyDescent="0.4">
@@ -43063,7 +43112,7 @@
         <v>518.70046566496637</v>
       </c>
       <c r="D29" s="1">
-        <f t="shared" ref="D3:D34" si="8">(5+A29*2.5+10*B29)</f>
+        <f t="shared" ref="D29:D34" si="8">(5+A29*2.5+10*B29)</f>
         <v>101.96440450636899</v>
       </c>
       <c r="E29" s="1">
@@ -46599,21 +46648,21 @@
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A1" t="s">
+        <v>1038</v>
+      </c>
+      <c r="B1" t="s">
         <v>1039</v>
       </c>
-      <c r="B1" t="s">
+      <c r="C1" t="s">
         <v>1040</v>
       </c>
-      <c r="C1" t="s">
-        <v>1041</v>
-      </c>
       <c r="E1" t="s">
-        <v>1100</v>
+        <v>1099</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A2" t="s">
-        <v>1042</v>
+        <v>1041</v>
       </c>
       <c r="B2">
         <v>0.05</v>
@@ -46748,7 +46797,7 @@
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A11" t="s">
-        <v>1030</v>
+        <v>1029</v>
       </c>
       <c r="B11">
         <v>7.4999999999999997E-2</v>
@@ -46787,25 +46836,25 @@
         <v>16</v>
       </c>
       <c r="E1" t="s">
-        <v>1109</v>
+        <v>1108</v>
       </c>
       <c r="M1" t="s">
         <v>3</v>
       </c>
       <c r="N1" t="s">
-        <v>1097</v>
+        <v>1096</v>
       </c>
       <c r="O1" t="s">
         <v>3</v>
       </c>
       <c r="P1" t="s">
-        <v>1096</v>
+        <v>1095</v>
       </c>
       <c r="Q1" t="s">
         <v>3</v>
       </c>
       <c r="R1" t="s">
-        <v>1101</v>
+        <v>1100</v>
       </c>
     </row>
     <row r="2" spans="1:20" x14ac:dyDescent="0.4">
@@ -53146,7 +53195,7 @@
     </row>
     <row r="106" spans="1:20" x14ac:dyDescent="0.4">
       <c r="L106" t="s">
-        <v>1095</v>
+        <v>1094</v>
       </c>
     </row>
   </sheetData>
@@ -53169,7 +53218,7 @@
   <sheetData>
     <row r="1" spans="1:19" x14ac:dyDescent="0.4">
       <c r="G1" s="8" t="s">
-        <v>1043</v>
+        <v>1042</v>
       </c>
       <c r="H1" s="8"/>
       <c r="I1" s="8"/>
@@ -53195,52 +53244,52 @@
         <v>4</v>
       </c>
       <c r="D2" s="5" t="s">
+        <v>1043</v>
+      </c>
+      <c r="E2" s="5" t="s">
         <v>1044</v>
       </c>
-      <c r="E2" s="5" t="s">
+      <c r="F2" s="5" t="s">
         <v>1045</v>
       </c>
-      <c r="F2" s="5" t="s">
+      <c r="G2" s="4" t="s">
         <v>1046</v>
       </c>
-      <c r="G2" s="4" t="s">
+      <c r="H2" s="4" t="s">
         <v>1047</v>
       </c>
-      <c r="H2" s="4" t="s">
+      <c r="I2" s="4" t="s">
         <v>1048</v>
       </c>
-      <c r="I2" s="4" t="s">
+      <c r="J2" s="4" t="s">
         <v>1049</v>
       </c>
-      <c r="J2" s="4" t="s">
+      <c r="K2" s="4" t="s">
         <v>1050</v>
       </c>
-      <c r="K2" s="4" t="s">
+      <c r="L2" s="4" t="s">
         <v>1051</v>
       </c>
-      <c r="L2" s="4" t="s">
+      <c r="M2" s="4" t="s">
         <v>1052</v>
       </c>
-      <c r="M2" s="4" t="s">
+      <c r="N2" s="4" t="s">
         <v>1053</v>
       </c>
-      <c r="N2" s="4" t="s">
+      <c r="O2" s="4" t="s">
         <v>1054</v>
       </c>
-      <c r="O2" s="4" t="s">
+      <c r="P2" s="4" t="s">
         <v>1055</v>
       </c>
-      <c r="P2" s="4" t="s">
+      <c r="Q2" s="4" t="s">
         <v>1056</v>
       </c>
-      <c r="Q2" s="4" t="s">
+      <c r="R2" s="4" t="s">
         <v>1057</v>
       </c>
-      <c r="R2" s="4" t="s">
+      <c r="S2" s="4" t="s">
         <v>1058</v>
-      </c>
-      <c r="S2" s="4" t="s">
-        <v>1059</v>
       </c>
     </row>
     <row r="3" spans="1:19" x14ac:dyDescent="0.4">
@@ -53248,19 +53297,19 @@
         <v>0</v>
       </c>
       <c r="B3" t="s">
+        <v>1059</v>
+      </c>
+      <c r="C3">
+        <v>1</v>
+      </c>
+      <c r="D3">
+        <v>1</v>
+      </c>
+      <c r="E3" t="s">
         <v>1060</v>
       </c>
-      <c r="C3">
-        <v>1</v>
-      </c>
-      <c r="D3">
-        <v>1</v>
-      </c>
-      <c r="E3" t="s">
+      <c r="F3" t="s">
         <v>1061</v>
-      </c>
-      <c r="F3" t="s">
-        <v>1062</v>
       </c>
       <c r="G3">
         <v>1</v>
@@ -53307,7 +53356,7 @@
         <v>1</v>
       </c>
       <c r="B4" t="s">
-        <v>1063</v>
+        <v>1062</v>
       </c>
       <c r="C4">
         <v>1.6</v>
@@ -53316,10 +53365,10 @@
         <v>1</v>
       </c>
       <c r="E4" t="s">
+        <v>1063</v>
+      </c>
+      <c r="F4" t="s">
         <v>1064</v>
-      </c>
-      <c r="F4" t="s">
-        <v>1065</v>
       </c>
       <c r="G4">
         <v>1</v>
@@ -53366,7 +53415,7 @@
         <v>2</v>
       </c>
       <c r="B5" t="s">
-        <v>1066</v>
+        <v>1065</v>
       </c>
       <c r="C5">
         <v>1.1499999999999999</v>
@@ -53375,10 +53424,10 @@
         <v>1.5</v>
       </c>
       <c r="E5" t="s">
+        <v>1066</v>
+      </c>
+      <c r="F5" t="s">
         <v>1067</v>
-      </c>
-      <c r="F5" t="s">
-        <v>1068</v>
       </c>
       <c r="G5">
         <v>1</v>
@@ -53425,7 +53474,7 @@
         <v>3</v>
       </c>
       <c r="B6" t="s">
-        <v>1069</v>
+        <v>1068</v>
       </c>
       <c r="C6">
         <v>1.1000000000000001</v>
@@ -53434,10 +53483,10 @@
         <v>1.8</v>
       </c>
       <c r="E6" t="s">
+        <v>1069</v>
+      </c>
+      <c r="F6" t="s">
         <v>1070</v>
-      </c>
-      <c r="F6" t="s">
-        <v>1071</v>
       </c>
       <c r="G6">
         <v>1</v>
@@ -53484,7 +53533,7 @@
         <v>4</v>
       </c>
       <c r="B7" t="s">
-        <v>1072</v>
+        <v>1071</v>
       </c>
       <c r="C7">
         <v>1.2</v>
@@ -53493,10 +53542,10 @@
         <v>1.6</v>
       </c>
       <c r="E7" t="s">
+        <v>1072</v>
+      </c>
+      <c r="F7" t="s">
         <v>1073</v>
-      </c>
-      <c r="F7" t="s">
-        <v>1074</v>
       </c>
       <c r="G7">
         <v>1</v>
@@ -53543,7 +53592,7 @@
         <v>5</v>
       </c>
       <c r="B8" t="s">
-        <v>1075</v>
+        <v>1074</v>
       </c>
       <c r="C8">
         <v>1.3</v>
@@ -53552,10 +53601,10 @@
         <v>1.3</v>
       </c>
       <c r="E8" t="s">
+        <v>1075</v>
+      </c>
+      <c r="F8" t="s">
         <v>1076</v>
-      </c>
-      <c r="F8" t="s">
-        <v>1077</v>
       </c>
       <c r="G8">
         <v>1</v>
@@ -53602,7 +53651,7 @@
         <v>6</v>
       </c>
       <c r="B9" t="s">
-        <v>1078</v>
+        <v>1077</v>
       </c>
       <c r="C9">
         <v>1.4</v>
@@ -53611,10 +53660,10 @@
         <v>1.4</v>
       </c>
       <c r="E9" t="s">
+        <v>1078</v>
+      </c>
+      <c r="F9" t="s">
         <v>1079</v>
-      </c>
-      <c r="F9" t="s">
-        <v>1080</v>
       </c>
       <c r="G9">
         <v>1</v>
@@ -53661,19 +53710,19 @@
         <v>200</v>
       </c>
       <c r="B10" t="s">
+        <v>1080</v>
+      </c>
+      <c r="C10">
+        <v>1</v>
+      </c>
+      <c r="D10">
+        <v>1</v>
+      </c>
+      <c r="E10" t="s">
         <v>1081</v>
       </c>
-      <c r="C10">
-        <v>1</v>
-      </c>
-      <c r="D10">
-        <v>1</v>
-      </c>
-      <c r="E10" t="s">
+      <c r="F10" t="s">
         <v>1082</v>
-      </c>
-      <c r="F10" t="s">
-        <v>1083</v>
       </c>
       <c r="G10">
         <v>1</v>
@@ -53742,7 +53791,7 @@
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>1084</v>
+        <v>1083</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.4">
@@ -53750,7 +53799,7 @@
         <v>0</v>
       </c>
       <c r="B2" t="s">
-        <v>1047</v>
+        <v>1046</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.4">
@@ -53758,7 +53807,7 @@
         <v>1</v>
       </c>
       <c r="B3" t="s">
-        <v>1048</v>
+        <v>1047</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.4">
@@ -53766,7 +53815,7 @@
         <v>2</v>
       </c>
       <c r="B4" t="s">
-        <v>1049</v>
+        <v>1048</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.4">
@@ -53774,7 +53823,7 @@
         <v>3</v>
       </c>
       <c r="B5" t="s">
-        <v>1050</v>
+        <v>1049</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.4">
@@ -53782,7 +53831,7 @@
         <v>4</v>
       </c>
       <c r="B6" t="s">
-        <v>1051</v>
+        <v>1050</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.4">
@@ -53790,7 +53839,7 @@
         <v>5</v>
       </c>
       <c r="B7" t="s">
-        <v>1052</v>
+        <v>1051</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.4">
@@ -53798,7 +53847,7 @@
         <v>6</v>
       </c>
       <c r="B8" t="s">
-        <v>1053</v>
+        <v>1052</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.4">
@@ -53806,7 +53855,7 @@
         <v>7</v>
       </c>
       <c r="B9" t="s">
-        <v>1054</v>
+        <v>1053</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.4">
@@ -53814,7 +53863,7 @@
         <v>8</v>
       </c>
       <c r="B10" t="s">
-        <v>1055</v>
+        <v>1054</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.4">
@@ -53822,7 +53871,7 @@
         <v>9</v>
       </c>
       <c r="B11" t="s">
-        <v>1056</v>
+        <v>1055</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.4">
@@ -53830,7 +53879,7 @@
         <v>10</v>
       </c>
       <c r="B12" t="s">
-        <v>1057</v>
+        <v>1056</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.4">
@@ -53838,7 +53887,7 @@
         <v>11</v>
       </c>
       <c r="B13" t="s">
-        <v>1058</v>
+        <v>1057</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.4">
@@ -53846,7 +53895,7 @@
         <v>12</v>
       </c>
       <c r="B14" t="s">
-        <v>1059</v>
+        <v>1058</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Provoke, Endure (without visual), status effect changes, cast sense AI, and more.
</commit_message>
<xml_diff>
--- a/Other/RoStatProcessing.xlsx
+++ b/Other/RoStatProcessing.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\ProjectsSSD\RagnarokRebuildTcp\Other\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E8645FF7-8102-4F90-8EEE-24DACEBBD760}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B4A0ED1C-D6E2-4EE7-9C49-D65CC594FFCA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="4106" yWindow="3300" windowWidth="27085" windowHeight="14100" xr2:uid="{1C41742B-2950-4FF8-AA39-6557869B44EA}"/>
   </bookViews>
@@ -51,7 +51,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3008" uniqueCount="1122">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3008" uniqueCount="1123">
   <si>
     <t>Id</t>
   </si>
@@ -3417,6 +3417,9 @@
   </si>
   <si>
     <t>Effect</t>
+  </si>
+  <si>
+    <t>AiPassiveSense</t>
   </si>
 </sst>
 </file>
@@ -3859,10 +3862,10 @@
   <dimension ref="A1:AJ304"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <pane xSplit="3" ySplit="1" topLeftCell="D2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="3" ySplit="1" topLeftCell="O68" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="A3" sqref="A3"/>
+      <selection pane="bottomRight" activeCell="Z84" sqref="Z84"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
@@ -5920,7 +5923,7 @@
         <v>41</v>
       </c>
       <c r="AD19" t="s">
-        <v>42</v>
+        <v>1122</v>
       </c>
       <c r="AE19">
         <v>252</v>
@@ -6562,7 +6565,7 @@
         <v>275</v>
       </c>
       <c r="AD25" t="s">
-        <v>42</v>
+        <v>1122</v>
       </c>
       <c r="AE25">
         <v>432</v>
@@ -8381,7 +8384,7 @@
         <v>41</v>
       </c>
       <c r="AD42" t="s">
-        <v>99</v>
+        <v>1122</v>
       </c>
       <c r="AE42">
         <v>324</v>
@@ -8488,7 +8491,7 @@
         <v>188</v>
       </c>
       <c r="AD43" t="s">
-        <v>42</v>
+        <v>99</v>
       </c>
       <c r="AE43">
         <v>1008</v>
@@ -8809,7 +8812,7 @@
         <v>275</v>
       </c>
       <c r="AD46" t="s">
-        <v>42</v>
+        <v>1122</v>
       </c>
       <c r="AE46">
         <v>192</v>
@@ -10093,7 +10096,7 @@
         <v>39</v>
       </c>
       <c r="AD58" t="s">
-        <v>42</v>
+        <v>1122</v>
       </c>
       <c r="AE58">
         <v>288</v>
@@ -10307,7 +10310,7 @@
         <v>547</v>
       </c>
       <c r="AD60" t="s">
-        <v>42</v>
+        <v>1122</v>
       </c>
       <c r="AE60">
         <v>480</v>
@@ -10414,7 +10417,7 @@
         <v>1107</v>
       </c>
       <c r="AD61" t="s">
-        <v>42</v>
+        <v>1122</v>
       </c>
       <c r="AE61">
         <v>840</v>
@@ -10521,7 +10524,7 @@
         <v>219</v>
       </c>
       <c r="AD62" t="s">
-        <v>42</v>
+        <v>1122</v>
       </c>
       <c r="AE62">
         <v>324</v>
@@ -12233,7 +12236,7 @@
         <v>48</v>
       </c>
       <c r="AD78" t="s">
-        <v>42</v>
+        <v>1122</v>
       </c>
       <c r="AE78">
         <v>576</v>
@@ -12340,7 +12343,7 @@
         <v>41</v>
       </c>
       <c r="AD79" t="s">
-        <v>42</v>
+        <v>1122</v>
       </c>
       <c r="AE79">
         <v>480</v>
@@ -12661,7 +12664,7 @@
         <v>327</v>
       </c>
       <c r="AD82" t="s">
-        <v>42</v>
+        <v>1122</v>
       </c>
       <c r="AE82">
         <v>576</v>
@@ -12982,7 +12985,7 @@
         <v>41</v>
       </c>
       <c r="AD85" t="s">
-        <v>42</v>
+        <v>1122</v>
       </c>
       <c r="AE85">
         <v>288</v>
@@ -14159,7 +14162,7 @@
         <v>41</v>
       </c>
       <c r="AD96" t="s">
-        <v>42</v>
+        <v>1122</v>
       </c>
       <c r="AE96">
         <v>216</v>
@@ -14266,7 +14269,7 @@
         <v>48</v>
       </c>
       <c r="AD97" t="s">
-        <v>42</v>
+        <v>1122</v>
       </c>
       <c r="AE97">
         <v>336</v>
@@ -14373,7 +14376,7 @@
         <v>48</v>
       </c>
       <c r="AD98" t="s">
-        <v>42</v>
+        <v>1122</v>
       </c>
       <c r="AE98">
         <v>720</v>
@@ -15229,7 +15232,7 @@
         <v>48</v>
       </c>
       <c r="AD106" t="s">
-        <v>42</v>
+        <v>1122</v>
       </c>
       <c r="AE106">
         <v>312</v>
@@ -15443,7 +15446,7 @@
         <v>48</v>
       </c>
       <c r="AD108" t="s">
-        <v>42</v>
+        <v>1122</v>
       </c>
       <c r="AE108">
         <v>252</v>
@@ -15550,7 +15553,7 @@
         <v>41</v>
       </c>
       <c r="AD109" t="s">
-        <v>42</v>
+        <v>1122</v>
       </c>
       <c r="AE109">
         <v>504</v>
@@ -19295,7 +19298,7 @@
         <v>469</v>
       </c>
       <c r="AD144" t="s">
-        <v>42</v>
+        <v>1122</v>
       </c>
       <c r="AE144">
         <v>336</v>
@@ -20151,7 +20154,7 @@
         <v>219</v>
       </c>
       <c r="AD152" t="s">
-        <v>42</v>
+        <v>1122</v>
       </c>
       <c r="AE152">
         <v>288</v>
@@ -21114,7 +21117,7 @@
         <v>181</v>
       </c>
       <c r="AD161" t="s">
-        <v>42</v>
+        <v>1122</v>
       </c>
       <c r="AE161">
         <v>384</v>
@@ -21756,7 +21759,7 @@
         <v>41</v>
       </c>
       <c r="AD167" t="s">
-        <v>42</v>
+        <v>1122</v>
       </c>
       <c r="AE167">
         <v>432</v>
@@ -24859,7 +24862,7 @@
         <v>41</v>
       </c>
       <c r="AD196" t="s">
-        <v>42</v>
+        <v>1122</v>
       </c>
       <c r="AE196">
         <v>420</v>
@@ -24966,7 +24969,7 @@
         <v>41</v>
       </c>
       <c r="AD197" t="s">
-        <v>42</v>
+        <v>1122</v>
       </c>
       <c r="AE197">
         <v>192</v>
@@ -25073,7 +25076,7 @@
         <v>41</v>
       </c>
       <c r="AD198" t="s">
-        <v>42</v>
+        <v>1122</v>
       </c>
       <c r="AE198">
         <v>468</v>
@@ -25394,7 +25397,7 @@
         <v>41</v>
       </c>
       <c r="AD201" t="s">
-        <v>42</v>
+        <v>1122</v>
       </c>
       <c r="AE201">
         <v>432</v>
@@ -25929,7 +25932,7 @@
         <v>192</v>
       </c>
       <c r="AD206" t="s">
-        <v>42</v>
+        <v>1122</v>
       </c>
       <c r="AE206">
         <v>288</v>
@@ -26036,7 +26039,7 @@
         <v>41</v>
       </c>
       <c r="AD207" t="s">
-        <v>42</v>
+        <v>1122</v>
       </c>
       <c r="AE207">
         <v>504</v>
@@ -26357,7 +26360,7 @@
         <v>286</v>
       </c>
       <c r="AD210" t="s">
-        <v>42</v>
+        <v>1122</v>
       </c>
       <c r="AE210">
         <v>2112</v>
@@ -29353,7 +29356,7 @@
         <v>831</v>
       </c>
       <c r="AD238" t="s">
-        <v>42</v>
+        <v>1122</v>
       </c>
       <c r="AE238">
         <v>720</v>
@@ -29460,7 +29463,7 @@
         <v>831</v>
       </c>
       <c r="AD239" t="s">
-        <v>42</v>
+        <v>1122</v>
       </c>
       <c r="AE239">
         <v>1248</v>
@@ -31707,7 +31710,7 @@
         <v>41</v>
       </c>
       <c r="AD260" t="s">
-        <v>42</v>
+        <v>1122</v>
       </c>
       <c r="AE260">
         <v>108</v>
@@ -31814,7 +31817,7 @@
         <v>41</v>
       </c>
       <c r="AD261" t="s">
-        <v>42</v>
+        <v>1122</v>
       </c>
       <c r="AE261">
         <v>336</v>
@@ -32563,7 +32566,7 @@
         <v>41</v>
       </c>
       <c r="AD268" t="s">
-        <v>42</v>
+        <v>1122</v>
       </c>
       <c r="AE268">
         <v>432</v>
@@ -32777,7 +32780,7 @@
         <v>41</v>
       </c>
       <c r="AD270" t="s">
-        <v>42</v>
+        <v>1122</v>
       </c>
       <c r="AE270">
         <v>468</v>
@@ -32884,7 +32887,7 @@
         <v>275</v>
       </c>
       <c r="AD271" t="s">
-        <v>42</v>
+        <v>1122</v>
       </c>
       <c r="AE271">
         <v>540</v>
@@ -32991,7 +32994,7 @@
         <v>41</v>
       </c>
       <c r="AD272" t="s">
-        <v>42</v>
+        <v>1122</v>
       </c>
       <c r="AE272">
         <v>336</v>
@@ -34275,7 +34278,7 @@
         <v>327</v>
       </c>
       <c r="AD284" t="s">
-        <v>42</v>
+        <v>1122</v>
       </c>
       <c r="AE284">
         <v>720</v>
@@ -35886,7 +35889,7 @@
         <v>41</v>
       </c>
       <c r="AD299" t="s">
-        <v>42</v>
+        <v>1122</v>
       </c>
       <c r="AE299">
         <v>672</v>

</xml_diff>

<commit_message>
Item drops, item pickup, character inventory (no UI), looter monsters
</commit_message>
<xml_diff>
--- a/Other/RoStatProcessing.xlsx
+++ b/Other/RoStatProcessing.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\ProjectsSSD\RagnarokRebuildTcp\Other\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7CDD0B7D-9022-4243-9A79-B5886DE31F6F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{98CB16E1-E860-4E85-AC3B-A5B8F941D591}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4106" yWindow="3300" windowWidth="27085" windowHeight="14100" xr2:uid="{1C41742B-2950-4FF8-AA39-6557869B44EA}"/>
+    <workbookView xWindow="3566" yWindow="3626" windowWidth="29220" windowHeight="11443" xr2:uid="{1C41742B-2950-4FF8-AA39-6557869B44EA}"/>
   </bookViews>
   <sheets>
     <sheet name="StatDef" sheetId="3" r:id="rId1"/>
@@ -51,7 +51,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3008" uniqueCount="1124">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3008" uniqueCount="1130">
   <si>
     <t>Id</t>
   </si>
@@ -3423,6 +3423,24 @@
   </si>
   <si>
     <t>Buff,Brute</t>
+  </si>
+  <si>
+    <t>AiLooter</t>
+  </si>
+  <si>
+    <t>AiLooterAssist</t>
+  </si>
+  <si>
+    <t>AiAssistLooter</t>
+  </si>
+  <si>
+    <t>AiAggressiveSense</t>
+  </si>
+  <si>
+    <t>AiStandardBoss</t>
+  </si>
+  <si>
+    <t>AiAggressiveActiveSense</t>
   </si>
 </sst>
 </file>
@@ -3865,10 +3883,10 @@
   <dimension ref="A1:AJ304"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <pane xSplit="4" ySplit="1" topLeftCell="E151" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="4" ySplit="1" topLeftCell="E199" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="E1" sqref="E1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="K170" sqref="K170"/>
+      <selection pane="bottomRight" activeCell="S49" sqref="S49"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
@@ -3888,18 +3906,18 @@
     <col min="16" max="16" width="8.07421875" bestFit="1" customWidth="1"/>
     <col min="17" max="17" width="6.3828125" bestFit="1" customWidth="1"/>
     <col min="18" max="18" width="7.07421875" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="10.4609375" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="11.69140625" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="6.921875" customWidth="1"/>
+    <col min="20" max="20" width="7.921875" customWidth="1"/>
     <col min="21" max="21" width="7.765625" bestFit="1" customWidth="1"/>
     <col min="22" max="22" width="11" bestFit="1" customWidth="1"/>
     <col min="23" max="23" width="10.3046875" bestFit="1" customWidth="1"/>
-    <col min="24" max="24" width="15.07421875" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="9.921875" customWidth="1"/>
     <col min="25" max="25" width="9.921875" bestFit="1" customWidth="1"/>
     <col min="26" max="26" width="12.921875" bestFit="1" customWidth="1"/>
-    <col min="27" max="27" width="13.23046875" bestFit="1" customWidth="1"/>
+    <col min="27" max="27" width="9.765625" customWidth="1"/>
     <col min="28" max="28" width="9.15234375" bestFit="1" customWidth="1"/>
-    <col min="29" max="29" width="22.4609375" bestFit="1" customWidth="1"/>
-    <col min="30" max="30" width="19.15234375" bestFit="1" customWidth="1"/>
+    <col min="29" max="29" width="21.53515625" customWidth="1"/>
+    <col min="30" max="30" width="21.15234375" bestFit="1" customWidth="1"/>
     <col min="31" max="31" width="19.3828125" bestFit="1" customWidth="1"/>
     <col min="32" max="32" width="22" bestFit="1" customWidth="1"/>
     <col min="33" max="33" width="13.3828125" bestFit="1" customWidth="1"/>
@@ -4214,7 +4232,7 @@
         <v>39</v>
       </c>
       <c r="AD3" t="s">
-        <v>42</v>
+        <v>1124</v>
       </c>
       <c r="AE3">
         <v>288</v>
@@ -4321,7 +4339,7 @@
         <v>39</v>
       </c>
       <c r="AD4" t="s">
-        <v>42</v>
+        <v>1124</v>
       </c>
       <c r="AE4">
         <v>288</v>
@@ -4963,7 +4981,7 @@
         <v>39</v>
       </c>
       <c r="AD10" t="s">
-        <v>42</v>
+        <v>1124</v>
       </c>
       <c r="AE10">
         <v>288</v>
@@ -5070,7 +5088,7 @@
         <v>48</v>
       </c>
       <c r="AD11" t="s">
-        <v>74</v>
+        <v>1125</v>
       </c>
       <c r="AE11">
         <v>480</v>
@@ -5605,7 +5623,7 @@
         <v>39</v>
       </c>
       <c r="AD16" t="s">
-        <v>42</v>
+        <v>1124</v>
       </c>
       <c r="AE16">
         <v>288</v>
@@ -6033,7 +6051,7 @@
         <v>106</v>
       </c>
       <c r="AD20" t="s">
-        <v>99</v>
+        <v>1128</v>
       </c>
       <c r="AE20">
         <v>576</v>
@@ -6354,7 +6372,7 @@
         <v>120</v>
       </c>
       <c r="AD23" t="s">
-        <v>99</v>
+        <v>1128</v>
       </c>
       <c r="AE23">
         <v>264</v>
@@ -6461,7 +6479,7 @@
         <v>275</v>
       </c>
       <c r="AD24" t="s">
-        <v>74</v>
+        <v>1125</v>
       </c>
       <c r="AE24">
         <v>360</v>
@@ -6675,7 +6693,7 @@
         <v>130</v>
       </c>
       <c r="AD26" t="s">
-        <v>99</v>
+        <v>1127</v>
       </c>
       <c r="AE26">
         <v>360</v>
@@ -7638,7 +7656,7 @@
         <v>41</v>
       </c>
       <c r="AD35" t="s">
-        <v>99</v>
+        <v>1128</v>
       </c>
       <c r="AE35">
         <v>384</v>
@@ -7745,7 +7763,7 @@
         <v>41</v>
       </c>
       <c r="AD36" t="s">
-        <v>99</v>
+        <v>1127</v>
       </c>
       <c r="AE36">
         <v>384</v>
@@ -7852,7 +7870,7 @@
         <v>41</v>
       </c>
       <c r="AD37" t="s">
-        <v>99</v>
+        <v>1103</v>
       </c>
       <c r="AE37">
         <v>384</v>
@@ -7959,7 +7977,7 @@
         <v>41</v>
       </c>
       <c r="AD38" t="s">
-        <v>99</v>
+        <v>1103</v>
       </c>
       <c r="AE38">
         <v>384</v>
@@ -8066,7 +8084,7 @@
         <v>41</v>
       </c>
       <c r="AD39" t="s">
-        <v>99</v>
+        <v>1103</v>
       </c>
       <c r="AE39">
         <v>384</v>
@@ -8280,7 +8298,7 @@
         <v>181</v>
       </c>
       <c r="AD41" t="s">
-        <v>99</v>
+        <v>1128</v>
       </c>
       <c r="AE41">
         <v>324</v>
@@ -8601,7 +8619,7 @@
         <v>192</v>
       </c>
       <c r="AD44" t="s">
-        <v>99</v>
+        <v>1128</v>
       </c>
       <c r="AE44">
         <v>603</v>
@@ -9457,7 +9475,7 @@
         <v>221</v>
       </c>
       <c r="AD52" t="s">
-        <v>99</v>
+        <v>1128</v>
       </c>
       <c r="AE52">
         <v>336</v>
@@ -9564,7 +9582,7 @@
         <v>225</v>
       </c>
       <c r="AD53" t="s">
-        <v>99</v>
+        <v>1128</v>
       </c>
       <c r="AE53">
         <v>288</v>
@@ -9671,7 +9689,7 @@
         <v>231</v>
       </c>
       <c r="AD54" t="s">
-        <v>99</v>
+        <v>1128</v>
       </c>
       <c r="AE54">
         <v>312</v>
@@ -9778,7 +9796,7 @@
         <v>236</v>
       </c>
       <c r="AD55" t="s">
-        <v>99</v>
+        <v>1128</v>
       </c>
       <c r="AE55">
         <v>672</v>
@@ -9885,7 +9903,7 @@
         <v>1094</v>
       </c>
       <c r="AD56" t="s">
-        <v>99</v>
+        <v>1128</v>
       </c>
       <c r="AE56">
         <v>360</v>
@@ -10206,7 +10224,7 @@
         <v>39</v>
       </c>
       <c r="AD59" t="s">
-        <v>99</v>
+        <v>1127</v>
       </c>
       <c r="AE59">
         <v>288</v>
@@ -10634,7 +10652,7 @@
         <v>263</v>
       </c>
       <c r="AD63" t="s">
-        <v>99</v>
+        <v>1128</v>
       </c>
       <c r="AE63">
         <v>336</v>
@@ -10848,7 +10866,7 @@
         <v>41</v>
       </c>
       <c r="AD65" t="s">
-        <v>99</v>
+        <v>1103</v>
       </c>
       <c r="AE65">
         <v>552</v>
@@ -10955,7 +10973,7 @@
         <v>275</v>
       </c>
       <c r="AD66" t="s">
-        <v>99</v>
+        <v>1128</v>
       </c>
       <c r="AE66">
         <v>360</v>
@@ -11062,7 +11080,7 @@
         <v>279</v>
       </c>
       <c r="AD67" t="s">
-        <v>99</v>
+        <v>1128</v>
       </c>
       <c r="AE67">
         <v>408</v>
@@ -11169,7 +11187,7 @@
         <v>48</v>
       </c>
       <c r="AD68" t="s">
-        <v>74</v>
+        <v>1125</v>
       </c>
       <c r="AE68">
         <v>480</v>
@@ -11276,7 +11294,7 @@
         <v>1094</v>
       </c>
       <c r="AD69" t="s">
-        <v>99</v>
+        <v>1103</v>
       </c>
       <c r="AE69">
         <v>504</v>
@@ -11383,7 +11401,7 @@
         <v>290</v>
       </c>
       <c r="AD70" t="s">
-        <v>42</v>
+        <v>1126</v>
       </c>
       <c r="AE70">
         <v>720</v>
@@ -11490,7 +11508,7 @@
         <v>120</v>
       </c>
       <c r="AD71" t="s">
-        <v>99</v>
+        <v>1128</v>
       </c>
       <c r="AE71">
         <v>216</v>
@@ -11597,7 +11615,7 @@
         <v>48</v>
       </c>
       <c r="AD72" t="s">
-        <v>1103</v>
+        <v>1127</v>
       </c>
       <c r="AE72">
         <v>384</v>
@@ -11704,7 +11722,7 @@
         <v>48</v>
       </c>
       <c r="AD73" t="s">
-        <v>74</v>
+        <v>1125</v>
       </c>
       <c r="AE73">
         <v>432</v>
@@ -11811,7 +11829,7 @@
         <v>219</v>
       </c>
       <c r="AD74" t="s">
-        <v>42</v>
+        <v>1124</v>
       </c>
       <c r="AE74">
         <v>192</v>
@@ -11918,7 +11936,7 @@
         <v>48</v>
       </c>
       <c r="AD75" t="s">
-        <v>74</v>
+        <v>1125</v>
       </c>
       <c r="AE75">
         <v>180</v>
@@ -12025,7 +12043,7 @@
         <v>48</v>
       </c>
       <c r="AD76" t="s">
-        <v>74</v>
+        <v>1125</v>
       </c>
       <c r="AE76">
         <v>144</v>
@@ -12132,7 +12150,7 @@
         <v>48</v>
       </c>
       <c r="AD77" t="s">
-        <v>74</v>
+        <v>1125</v>
       </c>
       <c r="AE77">
         <v>144</v>
@@ -12453,7 +12471,7 @@
         <v>290</v>
       </c>
       <c r="AD80" t="s">
-        <v>99</v>
+        <v>1128</v>
       </c>
       <c r="AE80">
         <v>624</v>
@@ -12560,7 +12578,7 @@
         <v>106</v>
       </c>
       <c r="AD81" t="s">
-        <v>99</v>
+        <v>1128</v>
       </c>
       <c r="AE81">
         <v>624</v>
@@ -13202,7 +13220,7 @@
         <v>41</v>
       </c>
       <c r="AD87" t="s">
-        <v>99</v>
+        <v>1103</v>
       </c>
       <c r="AE87">
         <v>180</v>
@@ -13309,7 +13327,7 @@
         <v>41</v>
       </c>
       <c r="AD88" t="s">
-        <v>99</v>
+        <v>1127</v>
       </c>
       <c r="AE88">
         <v>288</v>
@@ -13523,7 +13541,7 @@
         <v>279</v>
       </c>
       <c r="AD90" t="s">
-        <v>99</v>
+        <v>1128</v>
       </c>
       <c r="AE90">
         <v>324</v>
@@ -13737,7 +13755,7 @@
         <v>48</v>
       </c>
       <c r="AD92" t="s">
-        <v>74</v>
+        <v>1125</v>
       </c>
       <c r="AE92">
         <v>288</v>
@@ -13844,7 +13862,7 @@
         <v>106</v>
       </c>
       <c r="AD93" t="s">
-        <v>99</v>
+        <v>1128</v>
       </c>
       <c r="AE93">
         <v>288</v>
@@ -14486,7 +14504,7 @@
         <v>379</v>
       </c>
       <c r="AD99" t="s">
-        <v>99</v>
+        <v>1127</v>
       </c>
       <c r="AE99">
         <v>336</v>
@@ -14593,7 +14611,7 @@
         <v>379</v>
       </c>
       <c r="AD100" t="s">
-        <v>99</v>
+        <v>1127</v>
       </c>
       <c r="AE100">
         <v>336</v>
@@ -14807,7 +14825,7 @@
         <v>48</v>
       </c>
       <c r="AD102" t="s">
-        <v>99</v>
+        <v>1127</v>
       </c>
       <c r="AE102">
         <v>336</v>
@@ -14914,7 +14932,7 @@
         <v>48</v>
       </c>
       <c r="AD103" t="s">
-        <v>99</v>
+        <v>1127</v>
       </c>
       <c r="AE103">
         <v>216</v>
@@ -15021,7 +15039,7 @@
         <v>395</v>
       </c>
       <c r="AD104" t="s">
-        <v>99</v>
+        <v>1128</v>
       </c>
       <c r="AE104">
         <v>576</v>
@@ -15128,7 +15146,7 @@
         <v>290</v>
       </c>
       <c r="AD105" t="s">
-        <v>99</v>
+        <v>1128</v>
       </c>
       <c r="AE105">
         <v>288</v>
@@ -15342,7 +15360,7 @@
         <v>39</v>
       </c>
       <c r="AD107" t="s">
-        <v>99</v>
+        <v>1127</v>
       </c>
       <c r="AE107">
         <v>288</v>
@@ -15984,7 +16002,7 @@
         <v>120</v>
       </c>
       <c r="AD113" t="s">
-        <v>99</v>
+        <v>1128</v>
       </c>
       <c r="AE113">
         <v>168</v>
@@ -16091,7 +16109,7 @@
         <v>41</v>
       </c>
       <c r="AD114" t="s">
-        <v>42</v>
+        <v>1124</v>
       </c>
       <c r="AE114">
         <v>562</v>
@@ -16305,7 +16323,7 @@
         <v>286</v>
       </c>
       <c r="AD116" t="s">
-        <v>99</v>
+        <v>1103</v>
       </c>
       <c r="AE116">
         <v>240</v>
@@ -16412,7 +16430,7 @@
         <v>286</v>
       </c>
       <c r="AD117" t="s">
-        <v>99</v>
+        <v>1103</v>
       </c>
       <c r="AE117">
         <v>240</v>
@@ -16519,7 +16537,7 @@
         <v>286</v>
       </c>
       <c r="AD118" t="s">
-        <v>99</v>
+        <v>1103</v>
       </c>
       <c r="AE118">
         <v>240</v>
@@ -16626,7 +16644,7 @@
         <v>120</v>
       </c>
       <c r="AD119" t="s">
-        <v>99</v>
+        <v>1128</v>
       </c>
       <c r="AE119">
         <v>240</v>
@@ -16840,7 +16858,7 @@
         <v>279</v>
       </c>
       <c r="AD121" t="s">
-        <v>99</v>
+        <v>1128</v>
       </c>
       <c r="AE121">
         <v>624</v>
@@ -16947,7 +16965,7 @@
         <v>275</v>
       </c>
       <c r="AD122" t="s">
-        <v>99</v>
+        <v>1128</v>
       </c>
       <c r="AE122">
         <v>540</v>
@@ -17161,7 +17179,7 @@
         <v>279</v>
       </c>
       <c r="AD124" t="s">
-        <v>99</v>
+        <v>1128</v>
       </c>
       <c r="AE124">
         <v>480</v>
@@ -17268,7 +17286,7 @@
         <v>188</v>
       </c>
       <c r="AD125" t="s">
-        <v>99</v>
+        <v>1127</v>
       </c>
       <c r="AE125">
         <v>864</v>
@@ -17375,7 +17393,7 @@
         <v>456</v>
       </c>
       <c r="AD126" t="s">
-        <v>99</v>
+        <v>1128</v>
       </c>
       <c r="AE126">
         <v>192</v>
@@ -17696,7 +17714,7 @@
         <v>469</v>
       </c>
       <c r="AD129" t="s">
-        <v>42</v>
+        <v>1124</v>
       </c>
       <c r="AE129">
         <v>288</v>
@@ -17803,7 +17821,7 @@
         <v>41</v>
       </c>
       <c r="AD130" t="s">
-        <v>99</v>
+        <v>1127</v>
       </c>
       <c r="AE130">
         <v>288</v>
@@ -18017,7 +18035,7 @@
         <v>219</v>
       </c>
       <c r="AD132" t="s">
-        <v>99</v>
+        <v>1127</v>
       </c>
       <c r="AE132">
         <v>480</v>
@@ -18338,7 +18356,7 @@
         <v>41</v>
       </c>
       <c r="AD135" t="s">
-        <v>99</v>
+        <v>1127</v>
       </c>
       <c r="AE135">
         <v>480</v>
@@ -18445,7 +18463,7 @@
         <v>275</v>
       </c>
       <c r="AD136" t="s">
-        <v>99</v>
+        <v>1127</v>
       </c>
       <c r="AE136">
         <v>144</v>
@@ -18552,7 +18570,7 @@
         <v>469</v>
       </c>
       <c r="AD137" t="s">
-        <v>42</v>
+        <v>1124</v>
       </c>
       <c r="AE137">
         <v>480</v>
@@ -18659,7 +18677,7 @@
         <v>507</v>
       </c>
       <c r="AD138" t="s">
-        <v>99</v>
+        <v>1128</v>
       </c>
       <c r="AE138">
         <v>288</v>
@@ -18766,7 +18784,7 @@
         <v>512</v>
       </c>
       <c r="AD139" t="s">
-        <v>99</v>
+        <v>1128</v>
       </c>
       <c r="AE139">
         <v>192</v>
@@ -18873,7 +18891,7 @@
         <v>516</v>
       </c>
       <c r="AD140" t="s">
-        <v>99</v>
+        <v>1127</v>
       </c>
       <c r="AE140">
         <v>576</v>
@@ -18980,7 +18998,7 @@
         <v>48</v>
       </c>
       <c r="AD141" t="s">
-        <v>99</v>
+        <v>1127</v>
       </c>
       <c r="AE141">
         <v>480</v>
@@ -19515,7 +19533,7 @@
         <v>469</v>
       </c>
       <c r="AD146" t="s">
-        <v>99</v>
+        <v>1127</v>
       </c>
       <c r="AE146">
         <v>672</v>
@@ -19836,7 +19854,7 @@
         <v>547</v>
       </c>
       <c r="AD149" t="s">
-        <v>99</v>
+        <v>1127</v>
       </c>
       <c r="AE149">
         <v>720</v>
@@ -20050,7 +20068,7 @@
         <v>547</v>
       </c>
       <c r="AD151" t="s">
-        <v>42</v>
+        <v>1128</v>
       </c>
       <c r="AE151">
         <v>1152</v>
@@ -20264,7 +20282,7 @@
         <v>558</v>
       </c>
       <c r="AD153" t="s">
-        <v>99</v>
+        <v>1128</v>
       </c>
       <c r="AE153">
         <v>288</v>
@@ -20371,7 +20389,7 @@
         <v>562</v>
       </c>
       <c r="AD154" t="s">
-        <v>99</v>
+        <v>1128</v>
       </c>
       <c r="AE154">
         <v>120</v>
@@ -20585,7 +20603,7 @@
         <v>507</v>
       </c>
       <c r="AD156" t="s">
-        <v>99</v>
+        <v>1128</v>
       </c>
       <c r="AE156">
         <v>216</v>
@@ -20799,7 +20817,7 @@
         <v>39</v>
       </c>
       <c r="AD158" t="s">
-        <v>99</v>
+        <v>1127</v>
       </c>
       <c r="AE158">
         <v>900</v>
@@ -20906,7 +20924,7 @@
         <v>41</v>
       </c>
       <c r="AD159" t="s">
-        <v>99</v>
+        <v>1128</v>
       </c>
       <c r="AE159">
         <v>468</v>
@@ -21013,7 +21031,7 @@
         <v>41</v>
       </c>
       <c r="AD160" t="s">
-        <v>99</v>
+        <v>1128</v>
       </c>
       <c r="AE160">
         <v>288</v>
@@ -21334,7 +21352,7 @@
         <v>286</v>
       </c>
       <c r="AD163" t="s">
-        <v>99</v>
+        <v>1128</v>
       </c>
       <c r="AE163">
         <v>540</v>
@@ -21441,7 +21459,7 @@
         <v>558</v>
       </c>
       <c r="AD164" t="s">
-        <v>99</v>
+        <v>1128</v>
       </c>
       <c r="AE164">
         <v>768</v>
@@ -21548,7 +21566,7 @@
         <v>558</v>
       </c>
       <c r="AD165" t="s">
-        <v>99</v>
+        <v>1128</v>
       </c>
       <c r="AE165">
         <v>768</v>
@@ -21655,7 +21673,7 @@
         <v>120</v>
       </c>
       <c r="AD166" t="s">
-        <v>99</v>
+        <v>1128</v>
       </c>
       <c r="AE166">
         <v>480</v>
@@ -21869,7 +21887,7 @@
         <v>1089</v>
       </c>
       <c r="AD168" t="s">
-        <v>99</v>
+        <v>1127</v>
       </c>
       <c r="AE168">
         <v>620</v>
@@ -21976,7 +21994,7 @@
         <v>41</v>
       </c>
       <c r="AD169" t="s">
-        <v>42</v>
+        <v>1128</v>
       </c>
       <c r="AE169">
         <v>312</v>
@@ -22083,7 +22101,7 @@
         <v>188</v>
       </c>
       <c r="AD170" t="s">
-        <v>99</v>
+        <v>1128</v>
       </c>
       <c r="AE170">
         <v>336</v>
@@ -22190,7 +22208,7 @@
         <v>120</v>
       </c>
       <c r="AD171" t="s">
-        <v>99</v>
+        <v>1128</v>
       </c>
       <c r="AE171">
         <v>768</v>
@@ -22297,7 +22315,7 @@
         <v>120</v>
       </c>
       <c r="AD172" t="s">
-        <v>99</v>
+        <v>1128</v>
       </c>
       <c r="AE172">
         <v>576</v>
@@ -22404,7 +22422,7 @@
         <v>48</v>
       </c>
       <c r="AD173" t="s">
-        <v>99</v>
+        <v>1127</v>
       </c>
       <c r="AE173">
         <v>720</v>
@@ -22618,7 +22636,7 @@
         <v>275</v>
       </c>
       <c r="AD175" t="s">
-        <v>99</v>
+        <v>1128</v>
       </c>
       <c r="AE175">
         <v>840</v>
@@ -22725,7 +22743,7 @@
         <v>130</v>
       </c>
       <c r="AD176" t="s">
-        <v>99</v>
+        <v>1128</v>
       </c>
       <c r="AE176">
         <v>1080</v>
@@ -22832,7 +22850,7 @@
         <v>181</v>
       </c>
       <c r="AD177" t="s">
-        <v>99</v>
+        <v>1128</v>
       </c>
       <c r="AE177">
         <v>240</v>
@@ -22939,7 +22957,7 @@
         <v>566</v>
       </c>
       <c r="AD178" t="s">
-        <v>99</v>
+        <v>1128</v>
       </c>
       <c r="AE178">
         <v>384</v>
@@ -23046,7 +23064,7 @@
         <v>641</v>
       </c>
       <c r="AD179" t="s">
-        <v>99</v>
+        <v>1128</v>
       </c>
       <c r="AE179">
         <v>216</v>
@@ -23153,7 +23171,7 @@
         <v>219</v>
       </c>
       <c r="AD180" t="s">
-        <v>99</v>
+        <v>1129</v>
       </c>
       <c r="AE180">
         <v>720</v>
@@ -23367,7 +23385,7 @@
         <v>41</v>
       </c>
       <c r="AD182" t="s">
-        <v>99</v>
+        <v>1128</v>
       </c>
       <c r="AE182">
         <v>192</v>
@@ -23581,7 +23599,7 @@
         <v>41</v>
       </c>
       <c r="AD184" t="s">
-        <v>99</v>
+        <v>1127</v>
       </c>
       <c r="AE184">
         <v>240</v>
@@ -23688,7 +23706,7 @@
         <v>41</v>
       </c>
       <c r="AD185" t="s">
-        <v>99</v>
+        <v>1128</v>
       </c>
       <c r="AE185">
         <v>288</v>
@@ -23795,7 +23813,7 @@
         <v>566</v>
       </c>
       <c r="AD186" t="s">
-        <v>99</v>
+        <v>1128</v>
       </c>
       <c r="AE186">
         <v>192</v>
@@ -23902,7 +23920,7 @@
         <v>507</v>
       </c>
       <c r="AD187" t="s">
-        <v>99</v>
+        <v>1128</v>
       </c>
       <c r="AE187">
         <v>480</v>
@@ -24223,7 +24241,7 @@
         <v>286</v>
       </c>
       <c r="AD190" t="s">
-        <v>99</v>
+        <v>1127</v>
       </c>
       <c r="AE190">
         <v>288</v>
@@ -24330,7 +24348,7 @@
         <v>41</v>
       </c>
       <c r="AD191" t="s">
-        <v>99</v>
+        <v>1127</v>
       </c>
       <c r="AE191">
         <v>432</v>
@@ -24437,7 +24455,7 @@
         <v>681</v>
       </c>
       <c r="AD192" t="s">
-        <v>99</v>
+        <v>1128</v>
       </c>
       <c r="AE192">
         <v>576</v>
@@ -24758,7 +24776,7 @@
         <v>41</v>
       </c>
       <c r="AD195" t="s">
-        <v>42</v>
+        <v>1124</v>
       </c>
       <c r="AE195">
         <v>480</v>
@@ -25186,7 +25204,7 @@
         <v>41</v>
       </c>
       <c r="AD199" t="s">
-        <v>99</v>
+        <v>1127</v>
       </c>
       <c r="AE199">
         <v>384</v>
@@ -25293,7 +25311,7 @@
         <v>286</v>
       </c>
       <c r="AD200" t="s">
-        <v>99</v>
+        <v>1128</v>
       </c>
       <c r="AE200">
         <v>384</v>
@@ -26149,7 +26167,7 @@
         <v>41</v>
       </c>
       <c r="AD208" t="s">
-        <v>99</v>
+        <v>1128</v>
       </c>
       <c r="AE208">
         <v>576</v>
@@ -26256,7 +26274,7 @@
         <v>456</v>
       </c>
       <c r="AD209" t="s">
-        <v>99</v>
+        <v>1128</v>
       </c>
       <c r="AE209">
         <v>360</v>
@@ -26470,7 +26488,7 @@
         <v>286</v>
       </c>
       <c r="AD211" t="s">
-        <v>99</v>
+        <v>1127</v>
       </c>
       <c r="AE211">
         <v>384</v>
@@ -26684,7 +26702,7 @@
         <v>746</v>
       </c>
       <c r="AD213" t="s">
-        <v>99</v>
+        <v>1128</v>
       </c>
       <c r="AE213">
         <v>384</v>
@@ -26791,7 +26809,7 @@
         <v>1116</v>
       </c>
       <c r="AD214" t="s">
-        <v>99</v>
+        <v>1128</v>
       </c>
       <c r="AE214">
         <v>168</v>
@@ -26898,7 +26916,7 @@
         <v>753</v>
       </c>
       <c r="AD215" t="s">
-        <v>99</v>
+        <v>1128</v>
       </c>
       <c r="AE215">
         <v>720</v>
@@ -27005,7 +27023,7 @@
         <v>507</v>
       </c>
       <c r="AD216" t="s">
-        <v>99</v>
+        <v>1128</v>
       </c>
       <c r="AE216">
         <v>240</v>
@@ -27112,7 +27130,7 @@
         <v>469</v>
       </c>
       <c r="AD217" t="s">
-        <v>99</v>
+        <v>1128</v>
       </c>
       <c r="AE217">
         <v>384</v>
@@ -27219,7 +27237,7 @@
         <v>763</v>
       </c>
       <c r="AD218" t="s">
-        <v>99</v>
+        <v>1128</v>
       </c>
       <c r="AE218">
         <v>269</v>
@@ -27326,7 +27344,7 @@
         <v>512</v>
       </c>
       <c r="AD219" t="s">
-        <v>99</v>
+        <v>1128</v>
       </c>
       <c r="AE219">
         <v>408</v>
@@ -27433,7 +27451,7 @@
         <v>1114</v>
       </c>
       <c r="AD220" t="s">
-        <v>99</v>
+        <v>1103</v>
       </c>
       <c r="AE220">
         <v>864</v>
@@ -27540,7 +27558,7 @@
         <v>1114</v>
       </c>
       <c r="AD221" t="s">
-        <v>99</v>
+        <v>1103</v>
       </c>
       <c r="AE221">
         <v>480</v>
@@ -27647,7 +27665,7 @@
         <v>286</v>
       </c>
       <c r="AD222" t="s">
-        <v>99</v>
+        <v>1128</v>
       </c>
       <c r="AE222">
         <v>336</v>
@@ -27754,7 +27772,7 @@
         <v>780</v>
       </c>
       <c r="AD223" t="s">
-        <v>99</v>
+        <v>1128</v>
       </c>
       <c r="AE223">
         <v>660</v>
@@ -27968,7 +27986,7 @@
         <v>192</v>
       </c>
       <c r="AD225" t="s">
-        <v>99</v>
+        <v>1128</v>
       </c>
       <c r="AE225">
         <v>288</v>
@@ -28075,7 +28093,7 @@
         <v>286</v>
       </c>
       <c r="AD226" t="s">
-        <v>99</v>
+        <v>1128</v>
       </c>
       <c r="AE226">
         <v>540</v>
@@ -28182,7 +28200,7 @@
         <v>286</v>
       </c>
       <c r="AD227" t="s">
-        <v>99</v>
+        <v>1103</v>
       </c>
       <c r="AE227">
         <v>900</v>
@@ -28289,7 +28307,7 @@
         <v>192</v>
       </c>
       <c r="AD228" t="s">
-        <v>99</v>
+        <v>1103</v>
       </c>
       <c r="AE228">
         <v>1920</v>
@@ -28396,7 +28414,7 @@
         <v>456</v>
       </c>
       <c r="AD229" t="s">
-        <v>99</v>
+        <v>1103</v>
       </c>
       <c r="AE229">
         <v>960</v>
@@ -28503,7 +28521,7 @@
         <v>516</v>
       </c>
       <c r="AD230" t="s">
-        <v>99</v>
+        <v>1128</v>
       </c>
       <c r="AE230">
         <v>660</v>
@@ -28610,7 +28628,7 @@
         <v>1122</v>
       </c>
       <c r="AD231" t="s">
-        <v>99</v>
+        <v>1128</v>
       </c>
       <c r="AE231">
         <v>720</v>
@@ -28824,7 +28842,7 @@
         <v>286</v>
       </c>
       <c r="AD233" t="s">
-        <v>99</v>
+        <v>1128</v>
       </c>
       <c r="AE233">
         <v>336</v>
@@ -29038,7 +29056,7 @@
         <v>512</v>
       </c>
       <c r="AD235" t="s">
-        <v>99</v>
+        <v>1128</v>
       </c>
       <c r="AE235">
         <v>108</v>
@@ -29145,7 +29163,7 @@
         <v>1123</v>
       </c>
       <c r="AD236" t="s">
-        <v>42</v>
+        <v>1124</v>
       </c>
       <c r="AE236">
         <v>756</v>
@@ -29252,7 +29270,7 @@
         <v>48</v>
       </c>
       <c r="AD237" t="s">
-        <v>99</v>
+        <v>1128</v>
       </c>
       <c r="AE237">
         <v>396</v>
@@ -29573,7 +29591,7 @@
         <v>828</v>
       </c>
       <c r="AD240" t="s">
-        <v>99</v>
+        <v>1128</v>
       </c>
       <c r="AE240">
         <v>522</v>
@@ -29680,7 +29698,7 @@
         <v>828</v>
       </c>
       <c r="AD241" t="s">
-        <v>99</v>
+        <v>1128</v>
       </c>
       <c r="AE241">
         <v>1200</v>
@@ -29787,7 +29805,7 @@
         <v>841</v>
       </c>
       <c r="AD242" t="s">
-        <v>99</v>
+        <v>1128</v>
       </c>
       <c r="AE242">
         <v>540</v>
@@ -29894,7 +29912,7 @@
         <v>845</v>
       </c>
       <c r="AD243" t="s">
-        <v>99</v>
+        <v>1128</v>
       </c>
       <c r="AE243">
         <v>624</v>
@@ -30215,7 +30233,7 @@
         <v>379</v>
       </c>
       <c r="AD246" t="s">
-        <v>99</v>
+        <v>1103</v>
       </c>
       <c r="AE246">
         <v>336</v>
@@ -30322,7 +30340,7 @@
         <v>379</v>
       </c>
       <c r="AD247" t="s">
-        <v>99</v>
+        <v>1103</v>
       </c>
       <c r="AE247">
         <v>336</v>
@@ -32034,7 +32052,7 @@
         <v>120</v>
       </c>
       <c r="AD263" t="s">
-        <v>99</v>
+        <v>1128</v>
       </c>
       <c r="AE263">
         <v>336</v>
@@ -32141,7 +32159,7 @@
         <v>41</v>
       </c>
       <c r="AD264" t="s">
-        <v>99</v>
+        <v>1128</v>
       </c>
       <c r="AE264">
         <v>384</v>
@@ -32248,7 +32266,7 @@
         <v>1113</v>
       </c>
       <c r="AD265" t="s">
-        <v>99</v>
+        <v>1128</v>
       </c>
       <c r="AE265">
         <v>312</v>
@@ -32462,7 +32480,7 @@
         <v>279</v>
       </c>
       <c r="AD267" t="s">
-        <v>99</v>
+        <v>1128</v>
       </c>
       <c r="AE267">
         <v>252</v>
@@ -32676,7 +32694,7 @@
         <v>922</v>
       </c>
       <c r="AD269" t="s">
-        <v>99</v>
+        <v>1128</v>
       </c>
       <c r="AE269">
         <v>720</v>
@@ -33211,7 +33229,7 @@
         <v>41</v>
       </c>
       <c r="AD274" t="s">
-        <v>99</v>
+        <v>1128</v>
       </c>
       <c r="AE274">
         <v>252</v>
@@ -33318,7 +33336,7 @@
         <v>181</v>
       </c>
       <c r="AD275" t="s">
-        <v>99</v>
+        <v>1128</v>
       </c>
       <c r="AE275">
         <v>576</v>
@@ -33425,7 +33443,7 @@
         <v>1104</v>
       </c>
       <c r="AD276" t="s">
-        <v>99</v>
+        <v>1127</v>
       </c>
       <c r="AE276">
         <v>576</v>
@@ -33532,7 +33550,7 @@
         <v>41</v>
       </c>
       <c r="AD277" t="s">
-        <v>42</v>
+        <v>1125</v>
       </c>
       <c r="AE277">
         <v>480</v>
@@ -33639,7 +33657,7 @@
         <v>746</v>
       </c>
       <c r="AD278" t="s">
-        <v>42</v>
+        <v>1128</v>
       </c>
       <c r="AE278">
         <v>900</v>
@@ -33746,7 +33764,7 @@
         <v>1104</v>
       </c>
       <c r="AD279" t="s">
-        <v>99</v>
+        <v>1127</v>
       </c>
       <c r="AE279">
         <v>432</v>
@@ -33853,7 +33871,7 @@
         <v>746</v>
       </c>
       <c r="AD280" t="s">
-        <v>99</v>
+        <v>1128</v>
       </c>
       <c r="AE280">
         <v>288</v>
@@ -33960,7 +33978,7 @@
         <v>960</v>
       </c>
       <c r="AD281" t="s">
-        <v>99</v>
+        <v>1128</v>
       </c>
       <c r="AE281">
         <v>1080</v>
@@ -34067,7 +34085,7 @@
         <v>41</v>
       </c>
       <c r="AD282" t="s">
-        <v>99</v>
+        <v>1128</v>
       </c>
       <c r="AE282">
         <v>384</v>
@@ -34174,7 +34192,7 @@
         <v>48</v>
       </c>
       <c r="AD283" t="s">
-        <v>42</v>
+        <v>1128</v>
       </c>
       <c r="AE283">
         <v>540</v>
@@ -35143,7 +35161,7 @@
         <v>48</v>
       </c>
       <c r="AD292" t="s">
-        <v>1103</v>
+        <v>1127</v>
       </c>
       <c r="AE292">
         <v>384</v>
@@ -36213,7 +36231,7 @@
         <v>566</v>
       </c>
       <c r="AD302" t="s">
-        <v>99</v>
+        <v>1128</v>
       </c>
       <c r="AE302">
         <v>180</v>
@@ -36430,7 +36448,7 @@
         <v>1111</v>
       </c>
       <c r="AD304" t="s">
-        <v>99</v>
+        <v>1128</v>
       </c>
       <c r="AE304">
         <v>504</v>

</xml_diff>

<commit_message>
User accounts, logins, character select, item fixes, and more.
</commit_message>
<xml_diff>
--- a/Other/RoStatProcessing.xlsx
+++ b/Other/RoStatProcessing.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\ProjectsSSD\RagnarokRebuildTcp\Other\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DD694717-FB7E-44FB-9CC7-D583816F4BEC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A099BD5A-BDE1-43FB-9610-C7C24588F3DE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3566" yWindow="3626" windowWidth="29220" windowHeight="11443" xr2:uid="{1C41742B-2950-4FF8-AA39-6557869B44EA}"/>
+    <workbookView xWindow="883" yWindow="2889" windowWidth="29220" windowHeight="11442" xr2:uid="{1C41742B-2950-4FF8-AA39-6557869B44EA}"/>
   </bookViews>
   <sheets>
     <sheet name="StatDef" sheetId="3" r:id="rId1"/>
@@ -51,7 +51,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3008" uniqueCount="1130">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3026" uniqueCount="1135">
   <si>
     <t>Id</t>
   </si>
@@ -3441,6 +3441,21 @@
   </si>
   <si>
     <t>AiAggressiveActiveSense</t>
+  </si>
+  <si>
+    <t>WERE_WOLF</t>
+  </si>
+  <si>
+    <t>Werewolf</t>
+  </si>
+  <si>
+    <t>were_wolf.spr</t>
+  </si>
+  <si>
+    <t>RAPTICE</t>
+  </si>
+  <si>
+    <t>Raptice</t>
   </si>
 </sst>
 </file>
@@ -3880,19 +3895,19 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{811A97A5-94A7-4FFA-A162-65D076B52481}">
-  <dimension ref="A1:AJ304"/>
+  <dimension ref="A1:AJ306"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <pane xSplit="4" ySplit="1" topLeftCell="E235" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="4" ySplit="1" topLeftCell="E284" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="E1" sqref="E1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="G249" sqref="G249"/>
+      <selection pane="bottomRight" activeCell="U295" sqref="U295"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
   <cols>
     <col min="1" max="1" width="5.07421875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="17.84375" customWidth="1"/>
+    <col min="2" max="2" width="22.61328125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="15.921875" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="7.61328125" bestFit="1" customWidth="1"/>
     <col min="5" max="8" width="5.765625" bestFit="1" customWidth="1"/>
@@ -36469,6 +36484,220 @@
         <v>1112</v>
       </c>
     </row>
+    <row r="305" spans="1:35" x14ac:dyDescent="0.4">
+      <c r="A305">
+        <v>4301</v>
+      </c>
+      <c r="B305" t="s">
+        <v>1130</v>
+      </c>
+      <c r="C305" t="s">
+        <v>1131</v>
+      </c>
+      <c r="D305">
+        <v>48</v>
+      </c>
+      <c r="E305">
+        <v>100</v>
+      </c>
+      <c r="F305">
+        <v>100</v>
+      </c>
+      <c r="G305">
+        <v>100</v>
+      </c>
+      <c r="H305">
+        <v>100</v>
+      </c>
+      <c r="I305">
+        <v>100</v>
+      </c>
+      <c r="J305">
+        <v>100</v>
+      </c>
+      <c r="K305">
+        <v>100</v>
+      </c>
+      <c r="L305">
+        <v>100</v>
+      </c>
+      <c r="M305">
+        <v>10</v>
+      </c>
+      <c r="N305">
+        <v>1</v>
+      </c>
+      <c r="O305">
+        <v>100</v>
+      </c>
+      <c r="P305">
+        <v>100</v>
+      </c>
+      <c r="Q305">
+        <v>100</v>
+      </c>
+      <c r="R305">
+        <v>100</v>
+      </c>
+      <c r="S305">
+        <v>10</v>
+      </c>
+      <c r="T305">
+        <v>12</v>
+      </c>
+      <c r="U305" t="s">
+        <v>38</v>
+      </c>
+      <c r="V305" t="s">
+        <v>53</v>
+      </c>
+      <c r="W305" t="s">
+        <v>619</v>
+      </c>
+      <c r="X305">
+        <v>748</v>
+      </c>
+      <c r="Y305">
+        <v>432</v>
+      </c>
+      <c r="Z305">
+        <v>648</v>
+      </c>
+      <c r="AA305">
+        <v>150</v>
+      </c>
+      <c r="AB305" t="s">
+        <v>119</v>
+      </c>
+      <c r="AC305" t="s">
+        <v>120</v>
+      </c>
+      <c r="AD305" t="s">
+        <v>1128</v>
+      </c>
+      <c r="AE305">
+        <v>216</v>
+      </c>
+      <c r="AF305" t="s">
+        <v>1132</v>
+      </c>
+      <c r="AG305">
+        <v>0</v>
+      </c>
+      <c r="AH305">
+        <v>0.5</v>
+      </c>
+      <c r="AI305">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="306" spans="1:35" x14ac:dyDescent="0.4">
+      <c r="A306">
+        <v>4302</v>
+      </c>
+      <c r="B306" t="s">
+        <v>1133</v>
+      </c>
+      <c r="C306" t="s">
+        <v>1134</v>
+      </c>
+      <c r="D306">
+        <v>38</v>
+      </c>
+      <c r="E306">
+        <v>100</v>
+      </c>
+      <c r="F306">
+        <v>100</v>
+      </c>
+      <c r="G306">
+        <v>100</v>
+      </c>
+      <c r="H306">
+        <v>100</v>
+      </c>
+      <c r="I306">
+        <v>100</v>
+      </c>
+      <c r="J306">
+        <v>100</v>
+      </c>
+      <c r="K306">
+        <v>100</v>
+      </c>
+      <c r="L306">
+        <v>100</v>
+      </c>
+      <c r="M306">
+        <v>10</v>
+      </c>
+      <c r="N306">
+        <v>3</v>
+      </c>
+      <c r="O306">
+        <v>100</v>
+      </c>
+      <c r="P306">
+        <v>100</v>
+      </c>
+      <c r="Q306">
+        <v>100</v>
+      </c>
+      <c r="R306">
+        <v>100</v>
+      </c>
+      <c r="S306">
+        <v>10</v>
+      </c>
+      <c r="T306">
+        <v>12</v>
+      </c>
+      <c r="U306" t="s">
+        <v>38</v>
+      </c>
+      <c r="V306" t="s">
+        <v>53</v>
+      </c>
+      <c r="W306" t="s">
+        <v>40</v>
+      </c>
+      <c r="X306">
+        <v>1540</v>
+      </c>
+      <c r="Y306">
+        <v>432</v>
+      </c>
+      <c r="Z306">
+        <v>720</v>
+      </c>
+      <c r="AA306">
+        <v>300</v>
+      </c>
+      <c r="AB306" t="s">
+        <v>41</v>
+      </c>
+      <c r="AC306" t="s">
+        <v>41</v>
+      </c>
+      <c r="AD306" t="s">
+        <v>1119</v>
+      </c>
+      <c r="AE306">
+        <v>324</v>
+      </c>
+      <c r="AF306" t="s">
+        <v>340</v>
+      </c>
+      <c r="AG306">
+        <v>0</v>
+      </c>
+      <c r="AH306">
+        <v>0.5</v>
+      </c>
+      <c r="AI306">
+        <v>1</v>
+      </c>
+    </row>
   </sheetData>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A3:AI180">
     <sortCondition ref="D3:D180"/>
@@ -37888,7 +38117,7 @@
       </c>
       <c r="D2" s="1">
         <f ca="1">OFFSET(StatCharts!D$2,Sheet2!$A2-1,0)</f>
-        <v>6.9859953719670784</v>
+        <v>6.5784953719670787</v>
       </c>
       <c r="E2" s="1">
         <f ca="1">OFFSET(StatCharts!E$2,Sheet2!$A2-1,0)</f>
@@ -37921,7 +38150,7 @@
       </c>
       <c r="D3" s="1">
         <f ca="1">OFFSET(StatCharts!D$2,Sheet2!$A3-1,0)</f>
-        <v>16.549936867076458</v>
+        <v>14.362436867076459</v>
       </c>
       <c r="E3" s="1">
         <f ca="1">OFFSET(StatCharts!E$2,Sheet2!$A3-1,0)</f>
@@ -37954,7 +38183,7 @@
       </c>
       <c r="D4" s="1">
         <f ca="1">OFFSET(StatCharts!D$2,Sheet2!$A4-1,0)</f>
-        <v>30.400000000000002</v>
+        <v>25.650000000000002</v>
       </c>
       <c r="E4" s="1">
         <f ca="1">OFFSET(StatCharts!E$2,Sheet2!$A4-1,0)</f>
@@ -37987,7 +38216,7 @@
       </c>
       <c r="D5" s="1">
         <f ca="1">OFFSET(StatCharts!D$2,Sheet2!$A5-1,0)</f>
-        <v>45.328427124746192</v>
+        <v>37.828427124746192</v>
       </c>
       <c r="E5" s="1">
         <f ca="1">OFFSET(StatCharts!E$2,Sheet2!$A5-1,0)</f>
@@ -38012,15 +38241,15 @@
       </c>
       <c r="B6" s="1">
         <f ca="1">OFFSET(StatCharts!B$2,Sheet2!$A6-1,0)</f>
-        <v>2.4</v>
+        <v>1.0666666666666667</v>
       </c>
       <c r="C6" s="1">
         <f ca="1">OFFSET(StatCharts!C$2,Sheet2!$A6-1,0)</f>
-        <v>368.2</v>
+        <v>330.86666666666667</v>
       </c>
       <c r="D6" s="1">
         <f ca="1">OFFSET(StatCharts!D$2,Sheet2!$A6-1,0)</f>
-        <v>79</v>
+        <v>55.666666666666664</v>
       </c>
       <c r="E6" s="1">
         <f ca="1">OFFSET(StatCharts!E$2,Sheet2!$A6-1,0)</f>
@@ -38045,15 +38274,15 @@
       </c>
       <c r="B7" s="1">
         <f ca="1">OFFSET(StatCharts!B$2,Sheet2!$A7-1,0)</f>
-        <v>2.5656854249492378</v>
+        <v>1.3990187582825713</v>
       </c>
       <c r="C7" s="1">
         <f ca="1">OFFSET(StatCharts!C$2,Sheet2!$A7-1,0)</f>
-        <v>635.79898987322326</v>
+        <v>594.96565653988989</v>
       </c>
       <c r="D7" s="1">
         <f ca="1">OFFSET(StatCharts!D$2,Sheet2!$A7-1,0)</f>
-        <v>93.156854249492369</v>
+        <v>68.990187582825712</v>
       </c>
       <c r="E7" s="1">
         <f ca="1">OFFSET(StatCharts!E$2,Sheet2!$A7-1,0)</f>
@@ -38086,7 +38315,7 @@
       </c>
       <c r="D8" s="1">
         <f ca="1">OFFSET(StatCharts!D$2,Sheet2!$A8-1,0)</f>
-        <v>148</v>
+        <v>133</v>
       </c>
       <c r="E8" s="1">
         <f ca="1">OFFSET(StatCharts!E$2,Sheet2!$A8-1,0)</f>
@@ -38111,15 +38340,15 @@
       </c>
       <c r="B9" s="1">
         <f ca="1">OFFSET(StatCharts!B$2,Sheet2!$A9-1,0)</f>
-        <v>7.1313708498984756</v>
+        <v>7.2980375165651434</v>
       </c>
       <c r="C9" s="1">
         <f ca="1">OFFSET(StatCharts!C$2,Sheet2!$A9-1,0)</f>
-        <v>1385.4371716450253</v>
+        <v>1393.603838311692</v>
       </c>
       <c r="D9" s="1">
         <f ca="1">OFFSET(StatCharts!D$2,Sheet2!$A9-1,0)</f>
-        <v>163.81370849898474</v>
+        <v>147.98037516565142</v>
       </c>
       <c r="E9" s="1">
         <f ca="1">OFFSET(StatCharts!E$2,Sheet2!$A9-1,0)</f>
@@ -38144,15 +38373,15 @@
       </c>
       <c r="B10" s="1">
         <f ca="1">OFFSET(StatCharts!B$2,Sheet2!$A10-1,0)</f>
-        <v>13.6</v>
+        <v>11.933333333333332</v>
       </c>
       <c r="C10" s="1">
         <f ca="1">OFFSET(StatCharts!C$2,Sheet2!$A10-1,0)</f>
-        <v>2042.6</v>
+        <v>1949.2666666666664</v>
       </c>
       <c r="D10" s="1">
         <f ca="1">OFFSET(StatCharts!D$2,Sheet2!$A10-1,0)</f>
-        <v>241</v>
+        <v>204.33333333333331</v>
       </c>
       <c r="E10" s="1">
         <f ca="1">OFFSET(StatCharts!E$2,Sheet2!$A10-1,0)</f>
@@ -38177,15 +38406,15 @@
       </c>
       <c r="B11" s="1">
         <f ca="1">OFFSET(StatCharts!B$2,Sheet2!$A11-1,0)</f>
-        <v>14.262741699796951</v>
+        <v>13.262741699796951</v>
       </c>
       <c r="C11" s="1">
         <f ca="1">OFFSET(StatCharts!C$2,Sheet2!$A11-1,0)</f>
-        <v>2424.5527270872076</v>
+        <v>2361.5527270872076</v>
       </c>
       <c r="D11" s="1">
         <f ca="1">OFFSET(StatCharts!D$2,Sheet2!$A11-1,0)</f>
-        <v>260.12741699796948</v>
+        <v>227.6274169979695</v>
       </c>
       <c r="E11" s="1">
         <f ca="1">OFFSET(StatCharts!E$2,Sheet2!$A11-1,0)</f>
@@ -38210,15 +38439,15 @@
       </c>
       <c r="B12" s="1">
         <f ca="1">OFFSET(StatCharts!B$2,Sheet2!$A12-1,0)</f>
-        <v>15.2</v>
+        <v>14.866666666666667</v>
       </c>
       <c r="C12" s="1">
         <f ca="1">OFFSET(StatCharts!C$2,Sheet2!$A12-1,0)</f>
-        <v>2835</v>
+        <v>2811.6666666666665</v>
       </c>
       <c r="D12" s="1">
         <f ca="1">OFFSET(StatCharts!D$2,Sheet2!$A12-1,0)</f>
-        <v>282</v>
+        <v>253.66666666666669</v>
       </c>
       <c r="E12" s="1">
         <f ca="1">OFFSET(StatCharts!E$2,Sheet2!$A12-1,0)</f>
@@ -38243,15 +38472,15 @@
       </c>
       <c r="B13" s="1">
         <f ca="1">OFFSET(StatCharts!B$2,Sheet2!$A13-1,0)</f>
-        <v>16.525483399593902</v>
+        <v>16.858816732927238</v>
       </c>
       <c r="C13" s="1">
         <f ca="1">OFFSET(StatCharts!C$2,Sheet2!$A13-1,0)</f>
-        <v>3288.4622217687302</v>
+        <v>3314.1288884353971</v>
       </c>
       <c r="D13" s="1">
         <f ca="1">OFFSET(StatCharts!D$2,Sheet2!$A13-1,0)</f>
-        <v>307.75483399593901</v>
+        <v>283.58816732927238</v>
       </c>
       <c r="E13" s="1">
         <f ca="1">OFFSET(StatCharts!E$2,Sheet2!$A13-1,0)</f>
@@ -38276,15 +38505,15 @@
       </c>
       <c r="B14" s="1">
         <f ca="1">OFFSET(StatCharts!B$2,Sheet2!$A14-1,0)</f>
-        <v>40.4</v>
+        <v>44.4</v>
       </c>
       <c r="C14" s="1">
         <f ca="1">OFFSET(StatCharts!C$2,Sheet2!$A14-1,0)</f>
-        <v>5654.5999999999995</v>
+        <v>5990.5999999999995</v>
       </c>
       <c r="D14" s="1">
         <f ca="1">OFFSET(StatCharts!D$2,Sheet2!$A14-1,0)</f>
-        <v>559</v>
+        <v>569</v>
       </c>
       <c r="E14" s="1">
         <f ca="1">OFFSET(StatCharts!E$2,Sheet2!$A14-1,0)</f>
@@ -38309,15 +38538,15 @@
       </c>
       <c r="B15" s="1">
         <f ca="1">OFFSET(StatCharts!B$2,Sheet2!$A15-1,0)</f>
-        <v>43.050966799187805</v>
+        <v>47.050966799187805</v>
       </c>
       <c r="C15" s="1">
         <f ca="1">OFFSET(StatCharts!C$2,Sheet2!$A15-1,0)</f>
-        <v>6423.6379787260894</v>
+        <v>6787.6379787260894</v>
       </c>
       <c r="D15" s="1">
         <f ca="1">OFFSET(StatCharts!D$2,Sheet2!$A15-1,0)</f>
-        <v>598.00966799187802</v>
+        <v>605.50966799187802</v>
       </c>
       <c r="E15" s="1">
         <f ca="1">OFFSET(StatCharts!E$2,Sheet2!$A15-1,0)</f>
@@ -38342,15 +38571,15 @@
       </c>
       <c r="B16" s="1">
         <f ca="1">OFFSET(StatCharts!B$2,Sheet2!$A16-1,0)</f>
-        <v>46.8</v>
+        <v>50.8</v>
       </c>
       <c r="C16" s="1">
         <f ca="1">OFFSET(StatCharts!C$2,Sheet2!$A16-1,0)</f>
-        <v>7337.4</v>
+        <v>7729.4</v>
       </c>
       <c r="D16" s="1">
         <f ca="1">OFFSET(StatCharts!D$2,Sheet2!$A16-1,0)</f>
-        <v>648</v>
+        <v>653</v>
       </c>
       <c r="E16" s="1">
         <f ca="1">OFFSET(StatCharts!E$2,Sheet2!$A16-1,0)</f>
@@ -38375,15 +38604,15 @@
       </c>
       <c r="B17" s="1">
         <f ca="1">OFFSET(StatCharts!B$2,Sheet2!$A17-1,0)</f>
-        <v>52.101933598375609</v>
+        <v>56.101933598375609</v>
       </c>
       <c r="C17" s="1">
         <f ca="1">OFFSET(StatCharts!C$2,Sheet2!$A17-1,0)</f>
-        <v>8466.7030278294387</v>
+        <v>8886.7030278294387</v>
       </c>
       <c r="D17" s="1">
         <f ca="1">OFFSET(StatCharts!D$2,Sheet2!$A17-1,0)</f>
-        <v>713.51933598375604</v>
+        <v>716.01933598375604</v>
       </c>
       <c r="E17" s="1">
         <f ca="1">OFFSET(StatCharts!E$2,Sheet2!$A17-1,0)</f>
@@ -38408,11 +38637,11 @@
       </c>
       <c r="B18" s="1">
         <f ca="1">OFFSET(StatCharts!B$2,Sheet2!$A18-1,0)</f>
-        <v>73.599999999999994</v>
+        <v>77.599999999999994</v>
       </c>
       <c r="C18" s="1">
         <f ca="1">OFFSET(StatCharts!C$2,Sheet2!$A18-1,0)</f>
-        <v>11484.199999999999</v>
+        <v>11932.199999999999</v>
       </c>
       <c r="D18" s="1">
         <f ca="1">OFFSET(StatCharts!D$2,Sheet2!$A18-1,0)</f>
@@ -38441,15 +38670,15 @@
       </c>
       <c r="B19" s="1">
         <f ca="1">OFFSET(StatCharts!B$2,Sheet2!$A19-1,0)</f>
-        <v>84.203867196751233</v>
+        <v>88.203867196751233</v>
       </c>
       <c r="C19" s="1">
         <f ca="1">OFFSET(StatCharts!C$2,Sheet2!$A19-1,0)</f>
-        <v>13506.260196413396</v>
+        <v>13982.260196413396</v>
       </c>
       <c r="D19" s="1">
         <f ca="1">OFFSET(StatCharts!D$2,Sheet2!$A19-1,0)</f>
-        <v>1059.5386719675123</v>
+        <v>1057.0386719675123</v>
       </c>
       <c r="E19" s="1">
         <f ca="1">OFFSET(StatCharts!E$2,Sheet2!$A19-1,0)</f>
@@ -38474,15 +38703,15 @@
       </c>
       <c r="B20" s="1">
         <f ca="1">OFFSET(StatCharts!B$2,Sheet2!$A20-1,0)</f>
-        <v>119.2</v>
+        <v>128.19999999999999</v>
       </c>
       <c r="C20" s="1">
         <f ca="1">OFFSET(StatCharts!C$2,Sheet2!$A20-1,0)</f>
-        <v>18750.199999999997</v>
+        <v>19884.199999999997</v>
       </c>
       <c r="D20" s="1">
         <f ca="1">OFFSET(StatCharts!D$2,Sheet2!$A20-1,0)</f>
-        <v>1422</v>
+        <v>1467</v>
       </c>
       <c r="E20" s="1">
         <f ca="1">OFFSET(StatCharts!E$2,Sheet2!$A20-1,0)</f>
@@ -38507,15 +38736,15 @@
       </c>
       <c r="B21" s="1">
         <f ca="1">OFFSET(StatCharts!B$2,Sheet2!$A21-1,0)</f>
-        <v>140.40773439350247</v>
+        <v>149.40773439350247</v>
       </c>
       <c r="C21" s="1">
         <f ca="1">OFFSET(StatCharts!C$2,Sheet2!$A21-1,0)</f>
-        <v>22650.228674335827</v>
+        <v>23847.228674335824</v>
       </c>
       <c r="D21" s="1">
         <f ca="1">OFFSET(StatCharts!D$2,Sheet2!$A21-1,0)</f>
-        <v>1646.5773439350246</v>
+        <v>1689.0773439350246</v>
       </c>
       <c r="E21" s="1">
         <f ca="1">OFFSET(StatCharts!E$2,Sheet2!$A21-1,0)</f>
@@ -38540,15 +38769,15 @@
       </c>
       <c r="B22" s="1">
         <f ca="1">OFFSET(StatCharts!B$2,Sheet2!$A22-1,0)</f>
-        <v>163.54257833336908</v>
+        <v>172.54257833336908</v>
       </c>
       <c r="C22" s="1">
         <f ca="1">OFFSET(StatCharts!C$2,Sheet2!$A22-1,0)</f>
-        <v>26839.001357004952</v>
+        <v>28086.401357004954</v>
       </c>
       <c r="D22" s="1">
         <f ca="1">OFFSET(StatCharts!D$2,Sheet2!$A22-1,0)</f>
-        <v>1887.9257833336908</v>
+        <v>1928.4257833336908</v>
       </c>
       <c r="E22" s="1">
         <f ca="1">OFFSET(StatCharts!E$2,Sheet2!$A22-1,0)</f>
@@ -38577,7 +38806,7 @@
   <dimension ref="A1:N25"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <pane ySplit="1" topLeftCell="A5" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="L20" sqref="L20"/>
     </sheetView>
   </sheetViews>
@@ -41863,10 +42092,10 @@
   <dimension ref="A1:N100"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="B8" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="F23" sqref="F23"/>
+      <selection pane="bottomRight" activeCell="D21" sqref="D21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
@@ -41918,7 +42147,7 @@
         <v>1</v>
       </c>
       <c r="B2" s="1">
-        <f>FLOOR(A2/20,1)*FLOOR(A2/20,1)*2+FLOOR(A2/30,1)*FLOOR(A2/30,1)*4+POWER(2,A2/10)/10</f>
+        <f>FLOOR(A2/20,1)*FLOOR(A2/20,1)*MIN(2,A2/30)+FLOOR(A2/30,1)*FLOOR(A2/30,1)*5+POWER(2,A2/10)/10</f>
         <v>0.10717734625362932</v>
       </c>
       <c r="C2" s="1">
@@ -41926,8 +42155,8 @@
         <v>35.15004828475508</v>
       </c>
       <c r="D2" s="1">
-        <f>(5+A2*2.5+10*B2)*MIN(1,0.8+A2*0.015)</f>
-        <v>6.9859953719670784</v>
+        <f>(5+A2*2+10*B2)*MIN(1,0.8+A2*0.015)</f>
+        <v>6.5784953719670787</v>
       </c>
       <c r="E2" s="1">
         <f>(1-POWER(1-((A2+1)/100),2))*20+MAX(0,(A2-10)/3)*N2</f>
@@ -41967,7 +42196,7 @@
         <v>2</v>
       </c>
       <c r="B3" s="1">
-        <f t="shared" ref="B3:B66" si="0">FLOOR(A3/20,1)*FLOOR(A3/20,1)*2+FLOOR(A3/30,1)*FLOOR(A3/30,1)*4+POWER(2,A3/10)/10</f>
+        <f t="shared" ref="B3:B66" si="0">FLOOR(A3/20,1)*FLOOR(A3/20,1)*MIN(2,A3/30)+FLOOR(A3/30,1)*FLOOR(A3/30,1)*5+POWER(2,A3/10)/10</f>
         <v>0.1148698354997035</v>
       </c>
       <c r="C3" s="1">
@@ -41975,8 +42204,8 @@
         <v>49.321635539399168</v>
       </c>
       <c r="D3" s="1">
-        <f t="shared" ref="D3:D28" si="2">(5+A3*2.5+10*B3)*MIN(1,0.8+A3*0.015)</f>
-        <v>9.2534196346475408</v>
+        <f t="shared" ref="D3:D23" si="2">(5+A3*2+10*B3)*MIN(1,0.8+A3*0.015)</f>
+        <v>8.4234196346475407</v>
       </c>
       <c r="E3" s="1">
         <f t="shared" ref="E3:E66" si="3">(1-POWER(1-((A3+1)/100),2))*20+MAX(0,(A3-10)/3)</f>
@@ -42025,7 +42254,7 @@
       </c>
       <c r="D4" s="1">
         <f t="shared" si="2"/>
-        <v>11.602817029276455</v>
+        <v>10.335317029276455</v>
       </c>
       <c r="E4" s="1">
         <f t="shared" si="3"/>
@@ -42074,7 +42303,7 @@
       </c>
       <c r="D5" s="1">
         <f t="shared" si="2"/>
-        <v>14.034776803264691</v>
+        <v>12.31477680326469</v>
       </c>
       <c r="E5" s="1">
         <f t="shared" si="3"/>
@@ -42123,7 +42352,7 @@
       </c>
       <c r="D6" s="1">
         <f t="shared" si="2"/>
-        <v>16.549936867076458</v>
+        <v>14.362436867076459</v>
       </c>
       <c r="E6" s="1">
         <f t="shared" si="3"/>
@@ -42172,7 +42401,7 @@
       </c>
       <c r="D7" s="1">
         <f t="shared" si="2"/>
-        <v>19.148987744194255</v>
+        <v>16.478987744194256</v>
       </c>
       <c r="E7" s="1">
         <f t="shared" si="3"/>
@@ -42221,7 +42450,7 @@
       </c>
       <c r="D8" s="1">
         <f t="shared" si="2"/>
-        <v>21.832676837404787</v>
+        <v>18.665176837404786</v>
       </c>
       <c r="E8" s="1">
         <f t="shared" si="3"/>
@@ -42270,7 +42499,7 @@
       </c>
       <c r="D9" s="1">
         <f t="shared" si="2"/>
-        <v>24.601813036464868</v>
+        <v>20.921813036464869</v>
       </c>
       <c r="E9" s="1">
         <f t="shared" si="3"/>
@@ -42319,7 +42548,7 @@
       </c>
       <c r="D10" s="1">
         <f t="shared" si="2"/>
-        <v>27.45727169417383</v>
+        <v>23.24977169417383</v>
       </c>
       <c r="E10" s="1">
         <f t="shared" si="3"/>
@@ -42368,7 +42597,7 @@
       </c>
       <c r="D11" s="1">
         <f t="shared" si="2"/>
-        <v>30.400000000000002</v>
+        <v>25.650000000000002</v>
       </c>
       <c r="E11" s="1">
         <f t="shared" si="3"/>
@@ -42417,7 +42646,7 @@
       </c>
       <c r="D12" s="1">
         <f t="shared" si="2"/>
-        <v>33.431022782695045</v>
+        <v>28.123522782695048</v>
       </c>
       <c r="E12" s="1">
         <f t="shared" si="3"/>
@@ -42466,7 +42695,7 @@
       </c>
       <c r="D13" s="1">
         <f t="shared" si="2"/>
-        <v>36.551448775794185</v>
+        <v>30.67144877579419</v>
       </c>
       <c r="E13" s="1">
         <f t="shared" si="3"/>
@@ -42515,7 +42744,7 @@
       </c>
       <c r="D14" s="1">
         <f t="shared" si="2"/>
-        <v>39.762477382556391</v>
+        <v>33.29497738255639</v>
       </c>
       <c r="E14" s="1">
         <f t="shared" si="3"/>
@@ -42564,7 +42793,7 @@
       </c>
       <c r="D15" s="1">
         <f t="shared" si="2"/>
-        <v>42.63901582154579</v>
+        <v>35.63901582154579</v>
       </c>
       <c r="E15" s="1">
         <f t="shared" si="3"/>
@@ -42613,7 +42842,7 @@
       </c>
       <c r="D16" s="1">
         <f t="shared" si="2"/>
-        <v>45.328427124746192</v>
+        <v>37.828427124746192</v>
       </c>
       <c r="E16" s="1">
         <f t="shared" si="3"/>
@@ -42662,7 +42891,7 @@
       </c>
       <c r="D17" s="1">
         <f t="shared" si="2"/>
-        <v>48.031433133020798</v>
+        <v>40.031433133020798</v>
       </c>
       <c r="E17" s="1">
         <f t="shared" si="3"/>
@@ -42710,8 +42939,8 @@
         <v>266.73264281331137</v>
       </c>
       <c r="D18" s="1">
-        <f t="shared" si="2"/>
-        <v>50.749009585424943</v>
+        <f>(5+A18*2+10*B18)*MIN(1,0.8+A18*0.015)</f>
+        <v>42.249009585424943</v>
       </c>
       <c r="E18" s="1">
         <f t="shared" si="3"/>
@@ -42760,7 +42989,7 @@
       </c>
       <c r="D19" s="1">
         <f t="shared" si="2"/>
-        <v>53.482202253184496</v>
+        <v>44.482202253184496</v>
       </c>
       <c r="E19" s="1">
         <f t="shared" si="3"/>
@@ -42809,7 +43038,7 @@
       </c>
       <c r="D20" s="1">
         <f t="shared" si="2"/>
-        <v>56.232131966147229</v>
+        <v>46.732131966147229</v>
       </c>
       <c r="E20" s="1">
         <f t="shared" si="3"/>
@@ -42850,15 +43079,15 @@
       </c>
       <c r="B21" s="1">
         <f t="shared" si="0"/>
-        <v>2.4</v>
+        <v>1.0666666666666667</v>
       </c>
       <c r="C21" s="1">
         <f t="shared" si="1"/>
-        <v>368.2</v>
+        <v>330.86666666666667</v>
       </c>
       <c r="D21" s="1">
         <f t="shared" si="2"/>
-        <v>79</v>
+        <v>55.666666666666664</v>
       </c>
       <c r="E21" s="1">
         <f t="shared" si="3"/>
@@ -42899,15 +43128,15 @@
       </c>
       <c r="B22" s="1">
         <f t="shared" si="0"/>
-        <v>2.4287093850145172</v>
+        <v>1.1287093850145173</v>
       </c>
       <c r="C22" s="1">
         <f t="shared" si="1"/>
-        <v>421.40405591942681</v>
+        <v>383.18405591942678</v>
       </c>
       <c r="D22" s="1">
         <f t="shared" si="2"/>
-        <v>81.787093850145169</v>
+        <v>58.287093850145169</v>
       </c>
       <c r="E22" s="1">
         <f t="shared" si="3"/>
@@ -42947,16 +43176,16 @@
         <v>22</v>
       </c>
       <c r="B23" s="1">
-        <f>FLOOR(A23/20,1)*FLOOR(A23/20,1)*2+FLOOR(A23/30,1)*FLOOR(A23/30,1)*4+POWER(2,A23/10)/10</f>
-        <v>2.4594793419988141</v>
+        <f t="shared" si="0"/>
+        <v>1.1928126753321473</v>
       </c>
       <c r="C23" s="1">
         <f t="shared" si="1"/>
-        <v>474.75196373356346</v>
+        <v>435.73863040023014</v>
       </c>
       <c r="D23" s="1">
         <f t="shared" si="2"/>
-        <v>84.59479341998815</v>
+        <v>60.928126753321472</v>
       </c>
       <c r="E23" s="1">
         <f t="shared" si="3"/>
@@ -42997,15 +43226,15 @@
       </c>
       <c r="B24" s="1">
         <f t="shared" si="0"/>
-        <v>2.4924577653379663</v>
+        <v>1.2591244320046331</v>
       </c>
       <c r="C24" s="1">
         <f t="shared" si="1"/>
-        <v>528.25714004388249</v>
+        <v>488.54380671054918</v>
       </c>
       <c r="D24" s="1">
-        <f>(5+A24*2.5+10*B24)*MIN(1,0.8+A24*0.015)</f>
-        <v>87.424577653379657</v>
+        <f t="shared" ref="D3:D66" si="7">(5+A24*2+10*B24)*MIN(1,0.8+A24*0.015)</f>
+        <v>63.591244320046329</v>
       </c>
       <c r="E24" s="1">
         <f t="shared" si="3"/>
@@ -43046,15 +43275,15 @@
       </c>
       <c r="B25" s="1">
         <f t="shared" si="0"/>
-        <v>2.5278031643091579</v>
+        <v>1.3278031643091577</v>
       </c>
       <c r="C25" s="1">
         <f t="shared" si="1"/>
-        <v>581.9341863207876</v>
+        <v>541.61418632078767</v>
       </c>
       <c r="D25" s="1">
-        <f t="shared" si="2"/>
-        <v>90.27803164309158</v>
+        <f t="shared" si="7"/>
+        <v>66.27803164309158</v>
       </c>
       <c r="E25" s="1">
         <f t="shared" si="3"/>
@@ -43095,15 +43324,15 @@
       </c>
       <c r="B26" s="1">
         <f t="shared" si="0"/>
-        <v>2.5656854249492378</v>
+        <v>1.3990187582825713</v>
       </c>
       <c r="C26" s="1">
         <f t="shared" si="1"/>
-        <v>635.79898987322326</v>
+        <v>594.96565653988989</v>
       </c>
       <c r="D26" s="1">
-        <f t="shared" si="2"/>
-        <v>93.156854249492369</v>
+        <f t="shared" si="7"/>
+        <v>68.990187582825712</v>
       </c>
       <c r="E26" s="1">
         <f t="shared" si="3"/>
@@ -43144,15 +43373,15 @@
       </c>
       <c r="B27" s="1">
         <f t="shared" si="0"/>
-        <v>2.6062866266041591</v>
+        <v>1.4729532932708258</v>
       </c>
       <c r="C27" s="1">
         <f t="shared" si="1"/>
-        <v>689.86883320839138</v>
+        <v>648.61549987505805</v>
       </c>
       <c r="D27" s="1">
-        <f t="shared" si="2"/>
-        <v>96.062866266041596</v>
+        <f t="shared" si="7"/>
+        <v>71.729532932708253</v>
       </c>
       <c r="E27" s="1">
         <f t="shared" si="3"/>
@@ -43193,15 +43422,15 @@
       </c>
       <c r="B28" s="1">
         <f t="shared" si="0"/>
-        <v>2.6498019170849885</v>
+        <v>1.5498019170849884</v>
       </c>
       <c r="C28" s="1">
         <f t="shared" si="1"/>
-        <v>744.1625124658126</v>
+        <v>702.58251246581256</v>
       </c>
       <c r="D28" s="1">
-        <f t="shared" si="2"/>
-        <v>98.998019170849886</v>
+        <f t="shared" si="7"/>
+        <v>74.498019170849886</v>
       </c>
       <c r="E28" s="1">
         <f t="shared" si="3"/>
@@ -43242,15 +43471,15 @@
       </c>
       <c r="B29" s="1">
         <f t="shared" si="0"/>
-        <v>2.6964404506368993</v>
+        <v>1.6297737839702324</v>
       </c>
       <c r="C29" s="1">
         <f t="shared" si="1"/>
-        <v>798.70046566496649</v>
+        <v>756.88713233163298</v>
       </c>
       <c r="D29" s="1">
-        <f t="shared" ref="D29:D34" si="7">(5+A29*2.5+10*B29)</f>
-        <v>101.96440450636899</v>
+        <f t="shared" si="7"/>
+        <v>77.297737839702322</v>
       </c>
       <c r="E29" s="1">
         <f t="shared" si="3"/>
@@ -43291,15 +43520,15 @@
       </c>
       <c r="B30" s="1">
         <f t="shared" si="0"/>
-        <v>2.7464263932294459</v>
+        <v>1.7130930598961123</v>
       </c>
       <c r="C30" s="1">
         <f t="shared" si="1"/>
-        <v>853.50491156511544</v>
+        <v>811.55157823178206</v>
       </c>
       <c r="D30" s="1">
         <f t="shared" si="7"/>
-        <v>104.96426393229446</v>
+        <v>80.130930598961129</v>
       </c>
       <c r="E30" s="1">
         <f t="shared" si="3"/>
@@ -43348,7 +43577,7 @@
       </c>
       <c r="D31" s="1">
         <f t="shared" si="7"/>
-        <v>148</v>
+        <v>133</v>
       </c>
       <c r="E31" s="1">
         <f t="shared" si="3"/>
@@ -43389,15 +43618,15 @@
       </c>
       <c r="B32" s="1">
         <f t="shared" si="0"/>
-        <v>6.8574187700290343</v>
+        <v>6.8907521033623675</v>
       </c>
       <c r="C32" s="1">
         <f t="shared" si="1"/>
-        <v>1137.6119746192601</v>
+        <v>1139.0586412859268</v>
       </c>
       <c r="D32" s="1">
         <f t="shared" si="7"/>
-        <v>151.07418770029034</v>
+        <v>135.90752103362368</v>
       </c>
       <c r="E32" s="1">
         <f t="shared" si="3"/>
@@ -43438,15 +43667,15 @@
       </c>
       <c r="B33" s="1">
         <f t="shared" si="0"/>
-        <v>6.9189586839976283</v>
+        <v>6.9856253506642947</v>
       </c>
       <c r="C33" s="1">
         <f t="shared" si="1"/>
-        <v>1198.9693490430936</v>
+        <v>1201.9560157097603</v>
       </c>
       <c r="D33" s="1">
         <f t="shared" si="7"/>
-        <v>154.1895868399763</v>
+        <v>138.85625350664293</v>
       </c>
       <c r="E33" s="1">
         <f t="shared" si="3"/>
@@ -43487,15 +43716,15 @@
       </c>
       <c r="B34" s="1">
         <f t="shared" si="0"/>
-        <v>6.9849155306759325</v>
+        <v>7.0849155306759322</v>
       </c>
       <c r="C34" s="1">
         <f t="shared" si="1"/>
-        <v>1260.7030975172279</v>
+        <v>1265.323097517228</v>
       </c>
       <c r="D34" s="1">
         <f t="shared" si="7"/>
-        <v>157.34915530675931</v>
+        <v>141.84915530675931</v>
       </c>
       <c r="E34" s="1">
         <f t="shared" si="3"/>
@@ -43536,15 +43765,15 @@
       </c>
       <c r="B35" s="1">
         <f t="shared" si="0"/>
-        <v>7.0556063286183157</v>
+        <v>7.1889396619516486</v>
       </c>
       <c r="C35" s="1">
         <f t="shared" si="1"/>
-        <v>1322.8468612422319</v>
+        <v>1329.1935279088984</v>
       </c>
       <c r="D35" s="1">
-        <f t="shared" ref="D35:D66" si="8">(5+A35*2.5+10*B35)*MIN(A35/20*0.4+0.6,1)</f>
-        <v>160.55606328618316</v>
+        <f t="shared" si="7"/>
+        <v>144.8893966195165</v>
       </c>
       <c r="E35" s="1">
         <f t="shared" si="3"/>
@@ -43585,15 +43814,15 @@
       </c>
       <c r="B36" s="1">
         <f t="shared" si="0"/>
-        <v>7.1313708498984756</v>
+        <v>7.2980375165651434</v>
       </c>
       <c r="C36" s="1">
         <f t="shared" si="1"/>
-        <v>1385.4371716450253</v>
+        <v>1393.603838311692</v>
       </c>
       <c r="D36" s="1">
-        <f t="shared" si="8"/>
-        <v>163.81370849898474</v>
+        <f t="shared" si="7"/>
+        <v>147.98037516565142</v>
       </c>
       <c r="E36" s="1">
         <f t="shared" si="3"/>
@@ -43634,15 +43863,15 @@
       </c>
       <c r="B37" s="1">
         <f t="shared" si="0"/>
-        <v>7.2125732532083182</v>
+        <v>7.4125732532083184</v>
       </c>
       <c r="C37" s="1">
         <f t="shared" si="1"/>
-        <v>1448.5136919616991</v>
+        <v>1458.5936919616991</v>
       </c>
       <c r="D37" s="1">
-        <f t="shared" si="8"/>
-        <v>167.12573253208319</v>
+        <f t="shared" si="7"/>
+        <v>151.12573253208319</v>
       </c>
       <c r="E37" s="1">
         <f t="shared" si="3"/>
@@ -43683,15 +43912,15 @@
       </c>
       <c r="B38" s="1">
         <f t="shared" si="0"/>
-        <v>7.2996038341699769</v>
+        <v>7.5329371675033103</v>
       </c>
       <c r="C38" s="1">
         <f t="shared" si="1"/>
-        <v>1512.1194786100048</v>
+        <v>1524.2061452766711</v>
       </c>
       <c r="D38" s="1">
-        <f t="shared" si="8"/>
-        <v>170.49603834169977</v>
+        <f t="shared" si="7"/>
+        <v>154.32937167503309</v>
       </c>
       <c r="E38" s="1">
         <f t="shared" si="3"/>
@@ -43732,15 +43961,15 @@
       </c>
       <c r="B39" s="1">
         <f t="shared" si="0"/>
-        <v>7.3928809012737986</v>
+        <v>7.6595475679404652</v>
       </c>
       <c r="C39" s="1">
         <f t="shared" si="1"/>
-        <v>1576.3012639477661</v>
+        <v>1590.4879306144326</v>
       </c>
       <c r="D39" s="1">
-        <f t="shared" si="8"/>
-        <v>173.92880901273799</v>
+        <f t="shared" si="7"/>
+        <v>157.59547567940467</v>
       </c>
       <c r="E39" s="1">
         <f t="shared" si="3"/>
@@ -43781,15 +44010,15 @@
       </c>
       <c r="B40" s="1">
         <f t="shared" si="0"/>
-        <v>7.4928527864588919</v>
+        <v>7.7928527864588917</v>
       </c>
       <c r="C40" s="1">
         <f t="shared" si="1"/>
-        <v>1641.1097621406554</v>
+        <v>1657.4897621406553</v>
       </c>
       <c r="D40" s="1">
-        <f t="shared" si="8"/>
-        <v>177.42852786458892</v>
+        <f t="shared" si="7"/>
+        <v>160.92852786458892</v>
       </c>
       <c r="E40" s="1">
         <f t="shared" si="3"/>
@@ -43830,15 +44059,15 @@
       </c>
       <c r="B41" s="1">
         <f t="shared" si="0"/>
-        <v>13.6</v>
+        <v>11.933333333333332</v>
       </c>
       <c r="C41" s="1">
         <f t="shared" si="1"/>
-        <v>2042.6</v>
+        <v>1949.2666666666664</v>
       </c>
       <c r="D41" s="1">
-        <f t="shared" si="8"/>
-        <v>241</v>
+        <f t="shared" si="7"/>
+        <v>204.33333333333331</v>
       </c>
       <c r="E41" s="1">
         <f t="shared" si="3"/>
@@ -43879,15 +44108,15 @@
       </c>
       <c r="B42" s="1">
         <f t="shared" si="0"/>
-        <v>13.714837540058069</v>
+        <v>12.181504206724735</v>
       </c>
       <c r="C42" s="1">
         <f t="shared" si="1"/>
-        <v>2117.2316747993327</v>
+        <v>2029.2183414659996</v>
       </c>
       <c r="D42" s="1">
-        <f t="shared" si="8"/>
-        <v>244.64837540058068</v>
+        <f t="shared" si="7"/>
+        <v>208.81504206724736</v>
       </c>
       <c r="E42" s="1">
         <f t="shared" si="3"/>
@@ -43928,15 +44157,15 @@
       </c>
       <c r="B43" s="1">
         <f t="shared" si="0"/>
-        <v>13.837917367995257</v>
+        <v>12.437917367995256</v>
       </c>
       <c r="C43" s="1">
         <f t="shared" si="1"/>
-        <v>2192.6695412381209</v>
+        <v>2110.3495412381208</v>
       </c>
       <c r="D43" s="1">
-        <f t="shared" si="8"/>
-        <v>248.37917367995257</v>
+        <f t="shared" si="7"/>
+        <v>213.37917367995254</v>
       </c>
       <c r="E43" s="1">
         <f t="shared" si="3"/>
@@ -43977,15 +44206,15 @@
       </c>
       <c r="B44" s="1">
         <f t="shared" si="0"/>
-        <v>13.969831061351867</v>
+        <v>12.703164394685201</v>
       </c>
       <c r="C44" s="1">
         <f t="shared" si="1"/>
-        <v>2268.9838298933823</v>
+        <v>2192.7304965600492</v>
       </c>
       <c r="D44" s="1">
-        <f t="shared" si="8"/>
-        <v>252.19831061351866</v>
+        <f t="shared" si="7"/>
+        <v>218.031643946852</v>
       </c>
       <c r="E44" s="1">
         <f t="shared" si="3"/>
@@ -44026,15 +44255,15 @@
       </c>
       <c r="B45" s="1">
         <f t="shared" si="0"/>
-        <v>14.111212657236631</v>
+        <v>12.977879323903299</v>
       </c>
       <c r="C45" s="1">
         <f t="shared" si="1"/>
-        <v>2346.2506996857765</v>
+        <v>2276.437366352443</v>
       </c>
       <c r="D45" s="1">
-        <f t="shared" si="8"/>
-        <v>256.11212657236632</v>
+        <f t="shared" si="7"/>
+        <v>222.77879323903298</v>
       </c>
       <c r="E45" s="1">
         <f t="shared" si="3"/>
@@ -44075,15 +44304,15 @@
       </c>
       <c r="B46" s="1">
         <f t="shared" si="0"/>
-        <v>14.262741699796951</v>
+        <v>13.262741699796951</v>
       </c>
       <c r="C46" s="1">
         <f t="shared" si="1"/>
-        <v>2424.5527270872076</v>
+        <v>2361.5527270872076</v>
       </c>
       <c r="D46" s="1">
-        <f t="shared" si="8"/>
-        <v>260.12741699796948</v>
+        <f t="shared" si="7"/>
+        <v>227.6274169979695</v>
       </c>
       <c r="E46" s="1">
         <f t="shared" si="3"/>
@@ -44124,15 +44353,15 @@
       </c>
       <c r="B47" s="1">
         <f t="shared" si="0"/>
-        <v>14.425146506416635</v>
+        <v>13.558479839749968</v>
       </c>
       <c r="C47" s="1">
         <f t="shared" si="1"/>
-        <v>2503.9794350132311</v>
+        <v>2448.1661016798976</v>
       </c>
       <c r="D47" s="1">
-        <f t="shared" si="8"/>
-        <v>264.25146506416638</v>
+        <f t="shared" si="7"/>
+        <v>232.58479839749967</v>
       </c>
       <c r="E47" s="1">
         <f t="shared" si="3"/>
@@ -44173,15 +44402,15 @@
       </c>
       <c r="B48" s="1">
         <f t="shared" si="0"/>
-        <v>14.599207668339954</v>
+        <v>13.86587433500662</v>
       </c>
       <c r="C48" s="1">
         <f t="shared" si="1"/>
-        <v>2584.6278645767688</v>
+        <v>2536.3745312434353</v>
       </c>
       <c r="D48" s="1">
-        <f t="shared" si="8"/>
-        <v>268.49207668339955</v>
+        <f t="shared" si="7"/>
+        <v>237.6587433500662</v>
       </c>
       <c r="E48" s="1">
         <f t="shared" si="3"/>
@@ -44222,15 +44451,15 @@
       </c>
       <c r="B49" s="1">
         <f t="shared" si="0"/>
-        <v>14.785761802547597</v>
+        <v>14.185761802547598</v>
       </c>
       <c r="C49" s="1">
         <f t="shared" si="1"/>
-        <v>2666.6031931311982</v>
+        <v>2626.2831931311985</v>
       </c>
       <c r="D49" s="1">
-        <f t="shared" si="8"/>
-        <v>272.85761802547597</v>
+        <f t="shared" si="7"/>
+        <v>242.85761802547597</v>
       </c>
       <c r="E49" s="1">
         <f t="shared" si="3"/>
@@ -44271,15 +44500,15 @@
       </c>
       <c r="B50" s="1">
         <f t="shared" si="0"/>
-        <v>14.985705572917784</v>
+        <v>14.519038906251117</v>
       </c>
       <c r="C50" s="1">
         <f t="shared" si="1"/>
-        <v>2750.0194023021595</v>
+        <v>2718.0060689688266</v>
       </c>
       <c r="D50" s="1">
-        <f t="shared" si="8"/>
-        <v>277.35705572917783</v>
+        <f t="shared" si="7"/>
+        <v>248.19038906251117</v>
       </c>
       <c r="E50" s="1">
         <f t="shared" si="3"/>
@@ -44320,15 +44549,15 @@
       </c>
       <c r="B51" s="1">
         <f t="shared" si="0"/>
-        <v>15.2</v>
+        <v>14.866666666666667</v>
       </c>
       <c r="C51" s="1">
         <f t="shared" si="1"/>
-        <v>2835</v>
+        <v>2811.6666666666665</v>
       </c>
       <c r="D51" s="1">
-        <f t="shared" si="8"/>
-        <v>282</v>
+        <f t="shared" si="7"/>
+        <v>253.66666666666669</v>
       </c>
       <c r="E51" s="1">
         <f t="shared" si="3"/>
@@ -44369,15 +44598,15 @@
       </c>
       <c r="B52" s="1">
         <f t="shared" si="0"/>
-        <v>15.429675080116137</v>
+        <v>15.229675080116138</v>
       </c>
       <c r="C52" s="1">
         <f t="shared" si="1"/>
-        <v>2921.6788007202917</v>
+        <v>2907.398800720292</v>
       </c>
       <c r="D52" s="1">
-        <f t="shared" si="8"/>
-        <v>286.79675080116135</v>
+        <f t="shared" si="7"/>
+        <v>259.29675080116135</v>
       </c>
       <c r="E52" s="1">
         <f t="shared" si="3"/>
@@ -44418,15 +44647,15 @@
       </c>
       <c r="B53" s="1">
         <f t="shared" si="0"/>
-        <v>15.675834735990513</v>
+        <v>15.609168069323847</v>
       </c>
       <c r="C53" s="1">
         <f t="shared" si="1"/>
-        <v>3010.2007687801092</v>
+        <v>3005.3474354467758</v>
       </c>
       <c r="D53" s="1">
-        <f t="shared" si="8"/>
-        <v>291.75834735990514</v>
+        <f t="shared" si="7"/>
+        <v>265.09168069323846</v>
       </c>
       <c r="E53" s="1">
         <f t="shared" si="3"/>
@@ -44467,15 +44696,15 @@
       </c>
       <c r="B54" s="1">
         <f t="shared" si="0"/>
-        <v>15.93966212270373</v>
+        <v>16.006328789370396</v>
       </c>
       <c r="C54" s="1">
         <f t="shared" si="1"/>
-        <v>3100.7229295046168</v>
+        <v>3105.669596171283</v>
       </c>
       <c r="D54" s="1">
-        <f t="shared" si="8"/>
-        <v>296.89662122703731</v>
+        <f t="shared" si="7"/>
+        <v>271.063287893704</v>
       </c>
       <c r="E54" s="1">
         <f t="shared" si="3"/>
@@ -44516,15 +44745,15 @@
       </c>
       <c r="B55" s="1">
         <f t="shared" si="0"/>
-        <v>16.222425314473263</v>
+        <v>16.422425314473259</v>
       </c>
       <c r="C55" s="1">
         <f t="shared" si="1"/>
-        <v>3193.4153537741781</v>
+        <v>3208.535353774178</v>
       </c>
       <c r="D55" s="1">
-        <f t="shared" si="8"/>
-        <v>302.22425314473264</v>
+        <f t="shared" si="7"/>
+        <v>277.22425314473259</v>
       </c>
       <c r="E55" s="1">
         <f t="shared" si="3"/>
@@ -44565,15 +44794,15 @@
       </c>
       <c r="B56" s="1">
         <f t="shared" si="0"/>
-        <v>16.525483399593902</v>
+        <v>16.858816732927238</v>
       </c>
       <c r="C56" s="1">
         <f t="shared" si="1"/>
-        <v>3288.4622217687302</v>
+        <v>3314.1288884353971</v>
       </c>
       <c r="D56" s="1">
-        <f t="shared" si="8"/>
-        <v>307.75483399593901</v>
+        <f t="shared" si="7"/>
+        <v>283.58816732927238</v>
       </c>
       <c r="E56" s="1">
         <f t="shared" si="3"/>
@@ -44614,15 +44843,15 @@
       </c>
       <c r="B57" s="1">
         <f t="shared" si="0"/>
-        <v>16.850293012833273</v>
+        <v>17.316959679499938</v>
       </c>
       <c r="C57" s="1">
         <f t="shared" si="1"/>
-        <v>3386.0629722061285</v>
+        <v>3422.6496388727951</v>
       </c>
       <c r="D57" s="1">
-        <f t="shared" si="8"/>
-        <v>313.50293012833276</v>
+        <f t="shared" si="7"/>
+        <v>290.16959679499939</v>
       </c>
       <c r="E57" s="1">
         <f t="shared" si="3"/>
@@ -44663,15 +44892,15 @@
       </c>
       <c r="B58" s="1">
         <f t="shared" si="0"/>
-        <v>17.198415336679908</v>
+        <v>17.798415336679909</v>
       </c>
       <c r="C58" s="1">
         <f t="shared" si="1"/>
-        <v>3486.4335438670564</v>
+        <v>3534.3135438670561</v>
       </c>
       <c r="D58" s="1">
-        <f t="shared" si="8"/>
-        <v>319.48415336679909</v>
+        <f t="shared" si="7"/>
+        <v>296.98415336679909</v>
       </c>
       <c r="E58" s="1">
         <f t="shared" si="3"/>
@@ -44712,15 +44941,15 @@
       </c>
       <c r="B59" s="1">
         <f t="shared" si="0"/>
-        <v>17.571523605095194</v>
+        <v>18.304856938428529</v>
       </c>
       <c r="C59" s="1">
         <f t="shared" si="1"/>
-        <v>3589.8077167337292</v>
+        <v>3649.3543834003963</v>
       </c>
       <c r="D59" s="1">
-        <f t="shared" si="8"/>
-        <v>325.71523605095194</v>
+        <f t="shared" si="7"/>
+        <v>304.04856938428532</v>
       </c>
       <c r="E59" s="1">
         <f t="shared" si="3"/>
@@ -44761,15 +44990,15 @@
       </c>
       <c r="B60" s="1">
         <f t="shared" si="0"/>
-        <v>17.971411145835571</v>
+        <v>18.838077812502238</v>
       </c>
       <c r="C60" s="1">
         <f t="shared" si="1"/>
-        <v>3696.4385606460182</v>
+        <v>3768.0252273126848</v>
       </c>
       <c r="D60" s="1">
-        <f t="shared" si="8"/>
-        <v>332.21411145835572</v>
+        <f t="shared" si="7"/>
+        <v>311.3807781250224</v>
       </c>
       <c r="E60" s="1">
         <f t="shared" si="3"/>
@@ -44810,15 +45039,15 @@
       </c>
       <c r="B61" s="1">
         <f t="shared" si="0"/>
-        <v>40.4</v>
+        <v>44.4</v>
       </c>
       <c r="C61" s="1">
         <f t="shared" si="1"/>
-        <v>5654.5999999999995</v>
+        <v>5990.5999999999995</v>
       </c>
       <c r="D61" s="1">
-        <f t="shared" si="8"/>
-        <v>559</v>
+        <f t="shared" si="7"/>
+        <v>569</v>
       </c>
       <c r="E61" s="1">
         <f t="shared" si="3"/>
@@ -44859,15 +45088,15 @@
       </c>
       <c r="B62" s="1">
         <f t="shared" si="0"/>
-        <v>40.859350160232275</v>
+        <v>44.859350160232275</v>
       </c>
       <c r="C62" s="1">
         <f t="shared" si="1"/>
-        <v>5799.3885036838365</v>
+        <v>6140.9885036838359</v>
       </c>
       <c r="D62" s="1">
-        <f t="shared" si="8"/>
-        <v>566.0935016023227</v>
+        <f t="shared" si="7"/>
+        <v>575.5935016023227</v>
       </c>
       <c r="E62" s="1">
         <f t="shared" si="3"/>
@@ -44908,15 +45137,15 @@
       </c>
       <c r="B63" s="1">
         <f t="shared" si="0"/>
-        <v>41.351669471981019</v>
+        <v>45.351669471981019</v>
       </c>
       <c r="C63" s="1">
         <f t="shared" si="1"/>
-        <v>5948.3249101679512</v>
+        <v>6295.524910167951</v>
       </c>
       <c r="D63" s="1">
-        <f t="shared" si="8"/>
-        <v>573.51669471981018</v>
+        <f t="shared" si="7"/>
+        <v>582.51669471981018</v>
       </c>
       <c r="E63" s="1">
         <f t="shared" si="3"/>
@@ -44957,15 +45186,15 @@
       </c>
       <c r="B64" s="1">
         <f t="shared" si="0"/>
-        <v>41.87932424540746</v>
+        <v>45.87932424540746</v>
       </c>
       <c r="C64" s="1">
         <f t="shared" si="1"/>
-        <v>6101.7563984449371</v>
+        <v>6454.5563984449373</v>
       </c>
       <c r="D64" s="1">
-        <f t="shared" si="8"/>
-        <v>581.29324245407463</v>
+        <f t="shared" si="7"/>
+        <v>589.79324245407463</v>
       </c>
       <c r="E64" s="1">
         <f t="shared" si="3"/>
@@ -45006,15 +45235,15 @@
       </c>
       <c r="B65" s="1">
         <f t="shared" si="0"/>
-        <v>42.444850628946519</v>
+        <v>46.444850628946519</v>
       </c>
       <c r="C65" s="1">
         <f t="shared" si="1"/>
-        <v>6260.0586163536072</v>
+        <v>6618.4586163536069</v>
       </c>
       <c r="D65" s="1">
-        <f t="shared" si="8"/>
-        <v>589.44850628946517</v>
+        <f t="shared" si="7"/>
+        <v>597.44850628946517</v>
       </c>
       <c r="E65" s="1">
         <f t="shared" si="3"/>
@@ -45055,15 +45284,15 @@
       </c>
       <c r="B66" s="1">
         <f t="shared" si="0"/>
-        <v>43.050966799187805</v>
+        <v>47.050966799187805</v>
       </c>
       <c r="C66" s="1">
         <f t="shared" si="1"/>
-        <v>6423.6379787260894</v>
+        <v>6787.6379787260894</v>
       </c>
       <c r="D66" s="1">
-        <f t="shared" si="8"/>
-        <v>598.00966799187802</v>
+        <f t="shared" si="7"/>
+        <v>605.50966799187802</v>
       </c>
       <c r="E66" s="1">
         <f t="shared" si="3"/>
@@ -45103,19 +45332,19 @@
         <v>66</v>
       </c>
       <c r="B67" s="1">
-        <f t="shared" ref="B67:B100" si="9">FLOOR(A67/20,1)*FLOOR(A67/20,1)*2+FLOOR(A67/30,1)*FLOOR(A67/30,1)*4+POWER(2,A67/10)/10</f>
-        <v>43.700586025666546</v>
+        <f t="shared" ref="B67:B100" si="8">FLOOR(A67/20,1)*FLOOR(A67/20,1)*MIN(2,A67/30)+FLOOR(A67/30,1)*FLOOR(A67/30,1)*5+POWER(2,A67/10)/10</f>
+        <v>47.700586025666546</v>
       </c>
       <c r="C67" s="1">
-        <f t="shared" ref="C67:C100" si="10">(A67*20+A67*B67*2+30+(MAX(0,A67-20)*50))*0.7</f>
-        <v>6592.9341487715883</v>
+        <f t="shared" ref="C67:C100" si="9">(A67*20+A67*B67*2+30+(MAX(0,A67-20)*50))*0.7</f>
+        <v>6962.5341487715887</v>
       </c>
       <c r="D67" s="1">
-        <f t="shared" ref="D67:D100" si="11">(5+A67*2.5+10*B67)*MIN(A67/20*0.4+0.6,1)</f>
-        <v>607.00586025666553</v>
+        <f t="shared" ref="D67:D100" si="10">(5+A67*2+10*B67)*MIN(1,0.8+A67*0.015)</f>
+        <v>614.00586025666553</v>
       </c>
       <c r="E67" s="1">
-        <f t="shared" ref="E67:E100" si="12">(1-POWER(1-((A67+1)/100),2))*20+MAX(0,(A67-10)/3)</f>
+        <f t="shared" ref="E67:E100" si="11">(1-POWER(1-((A67+1)/100),2))*20+MAX(0,(A67-10)/3)</f>
         <v>36.488666666666667</v>
       </c>
       <c r="F67" s="1">
@@ -45123,11 +45352,11 @@
         <v>7237.9734346737796</v>
       </c>
       <c r="G67">
-        <f t="shared" ref="G67:G100" si="13">FLOOR(A67*0.8,1)+1</f>
+        <f t="shared" ref="G67:G100" si="12">FLOOR(A67*0.8,1)+1</f>
         <v>53</v>
       </c>
       <c r="H67">
-        <f t="shared" ref="H67:H100" si="14">FLOOR(A67/3,1)+1</f>
+        <f t="shared" ref="H67:H100" si="13">FLOOR(A67/3,1)+1</f>
         <v>23</v>
       </c>
       <c r="J67" s="1">
@@ -45143,7 +45372,7 @@
         <v>4449.340424768975</v>
       </c>
       <c r="N67">
-        <f t="shared" ref="N67:N100" si="15">MAX(1,1+(1-POWER(1-(A67-10)/200,3)))</f>
+        <f t="shared" ref="N67:N100" si="14">MAX(1,1+(1-POWER(1-(A67-10)/200,3)))</f>
         <v>1.626752</v>
       </c>
     </row>
@@ -45152,19 +45381,19 @@
         <v>67</v>
       </c>
       <c r="B68" s="1">
+        <f t="shared" si="8"/>
+        <v>48.396830673359815</v>
+      </c>
+      <c r="C68" s="1">
         <f t="shared" si="9"/>
-        <v>44.396830673359815</v>
-      </c>
-      <c r="C68" s="1">
+        <v>7143.6227171611508</v>
+      </c>
+      <c r="D68" s="1">
         <f t="shared" si="10"/>
-        <v>6768.4227171611501</v>
-      </c>
-      <c r="D68" s="1">
+        <v>622.96830673359818</v>
+      </c>
+      <c r="E68" s="1">
         <f t="shared" si="11"/>
-        <v>616.46830673359818</v>
-      </c>
-      <c r="E68" s="1">
-        <f t="shared" si="12"/>
         <v>36.951999999999998</v>
       </c>
       <c r="F68" s="1">
@@ -45172,11 +45401,11 @@
         <v>7549.7943277765753</v>
       </c>
       <c r="G68">
+        <f t="shared" si="12"/>
+        <v>54</v>
+      </c>
+      <c r="H68">
         <f t="shared" si="13"/>
-        <v>54</v>
-      </c>
-      <c r="H68">
-        <f t="shared" si="14"/>
         <v>23</v>
       </c>
       <c r="J68" s="1">
@@ -45192,7 +45421,7 @@
         <v>4619.096877888217</v>
       </c>
       <c r="N68">
-        <f t="shared" si="15"/>
+        <f t="shared" si="14"/>
         <v>1.6344741249999999</v>
       </c>
     </row>
@@ -45201,19 +45430,19 @@
         <v>68</v>
       </c>
       <c r="B69" s="1">
+        <f t="shared" si="8"/>
+        <v>49.143047210190389</v>
+      </c>
+      <c r="C69" s="1">
         <f t="shared" si="9"/>
-        <v>45.143047210190389</v>
-      </c>
-      <c r="C69" s="1">
+        <v>7331.4180944101245</v>
+      </c>
+      <c r="D69" s="1">
         <f t="shared" si="10"/>
-        <v>6950.6180944101243</v>
-      </c>
-      <c r="D69" s="1">
+        <v>632.43047210190389</v>
+      </c>
+      <c r="E69" s="1">
         <f t="shared" si="11"/>
-        <v>626.43047210190389</v>
-      </c>
-      <c r="E69" s="1">
-        <f t="shared" si="12"/>
         <v>37.411333333333332</v>
       </c>
       <c r="F69" s="1">
@@ -45221,11 +45450,11 @@
         <v>8186.9041466935159</v>
       </c>
       <c r="G69">
+        <f t="shared" si="12"/>
+        <v>55</v>
+      </c>
+      <c r="H69">
         <f t="shared" si="13"/>
-        <v>55</v>
-      </c>
-      <c r="H69">
-        <f t="shared" si="14"/>
         <v>23</v>
       </c>
       <c r="J69" s="1">
@@ -45241,7 +45470,7 @@
         <v>4985.6640819672475</v>
       </c>
       <c r="N69">
-        <f t="shared" si="15"/>
+        <f t="shared" si="14"/>
         <v>1.6420889999999999</v>
       </c>
     </row>
@@ -45250,19 +45479,19 @@
         <v>69</v>
       </c>
       <c r="B70" s="1">
+        <f t="shared" si="8"/>
+        <v>49.942822291671135</v>
+      </c>
+      <c r="C70" s="1">
         <f t="shared" si="9"/>
-        <v>45.942822291671135</v>
-      </c>
-      <c r="C70" s="1">
+        <v>7526.4766333754305</v>
+      </c>
+      <c r="D70" s="1">
         <f t="shared" si="10"/>
-        <v>7140.0766333754309</v>
-      </c>
-      <c r="D70" s="1">
+        <v>642.42822291671132</v>
+      </c>
+      <c r="E70" s="1">
         <f t="shared" si="11"/>
-        <v>636.92822291671132</v>
-      </c>
-      <c r="E70" s="1">
-        <f t="shared" si="12"/>
         <v>37.866666666666667</v>
       </c>
       <c r="F70" s="1">
@@ -45270,11 +45499,11 @@
         <v>8530.6690140845076</v>
       </c>
       <c r="G70">
+        <f t="shared" si="12"/>
+        <v>56</v>
+      </c>
+      <c r="H70">
         <f t="shared" si="13"/>
-        <v>56</v>
-      </c>
-      <c r="H70">
-        <f t="shared" si="14"/>
         <v>24</v>
       </c>
       <c r="J70" s="1">
@@ -45290,7 +45519,7 @@
         <v>5171.3643240275569</v>
       </c>
       <c r="N70">
-        <f t="shared" si="15"/>
+        <f t="shared" si="14"/>
         <v>1.6495973749999999</v>
       </c>
     </row>
@@ -45299,19 +45528,19 @@
         <v>70</v>
       </c>
       <c r="B71" s="1">
+        <f t="shared" si="8"/>
+        <v>50.8</v>
+      </c>
+      <c r="C71" s="1">
         <f t="shared" si="9"/>
-        <v>46.8</v>
-      </c>
-      <c r="C71" s="1">
+        <v>7729.4</v>
+      </c>
+      <c r="D71" s="1">
         <f t="shared" si="10"/>
-        <v>7337.4</v>
-      </c>
-      <c r="D71" s="1">
+        <v>653</v>
+      </c>
+      <c r="E71" s="1">
         <f t="shared" si="11"/>
-        <v>648</v>
-      </c>
-      <c r="E71" s="1">
-        <f t="shared" si="12"/>
         <v>38.317999999999998</v>
       </c>
       <c r="F71" s="1">
@@ -45319,11 +45548,11 @@
         <v>9466.8302103450078</v>
       </c>
       <c r="G71">
+        <f t="shared" si="12"/>
+        <v>57</v>
+      </c>
+      <c r="H71">
         <f t="shared" si="13"/>
-        <v>57</v>
-      </c>
-      <c r="H71">
-        <f t="shared" si="14"/>
         <v>24</v>
       </c>
       <c r="J71" s="1">
@@ -45339,7 +45568,7 @@
         <v>5713.2348885606571</v>
       </c>
       <c r="N71">
-        <f t="shared" si="15"/>
+        <f t="shared" si="14"/>
         <v>1.657</v>
       </c>
     </row>
@@ -45348,19 +45577,19 @@
         <v>71</v>
       </c>
       <c r="B72" s="1">
+        <f t="shared" si="8"/>
+        <v>51.718700320464549</v>
+      </c>
+      <c r="C72" s="1">
         <f t="shared" si="9"/>
-        <v>47.718700320464549</v>
-      </c>
-      <c r="C72" s="1">
+        <v>7940.8388118541761</v>
+      </c>
+      <c r="D72" s="1">
         <f t="shared" si="10"/>
-        <v>7543.2388118541758</v>
-      </c>
-      <c r="D72" s="1">
+        <v>664.18700320464552</v>
+      </c>
+      <c r="E72" s="1">
         <f t="shared" si="11"/>
-        <v>659.68700320464552</v>
-      </c>
-      <c r="E72" s="1">
-        <f t="shared" si="12"/>
         <v>38.765333333333331</v>
       </c>
       <c r="F72" s="1">
@@ -45368,11 +45597,11 @@
         <v>9851.9467565522464</v>
       </c>
       <c r="G72">
+        <f t="shared" si="12"/>
+        <v>57</v>
+      </c>
+      <c r="H72">
         <f t="shared" si="13"/>
-        <v>57</v>
-      </c>
-      <c r="H72">
-        <f t="shared" si="14"/>
         <v>24</v>
       </c>
       <c r="J72" s="1">
@@ -45388,7 +45617,7 @@
         <v>5919.5822961967197</v>
       </c>
       <c r="N72">
-        <f t="shared" si="15"/>
+        <f t="shared" si="14"/>
         <v>1.6642976249999999</v>
       </c>
     </row>
@@ -45397,19 +45626,19 @@
         <v>72</v>
       </c>
       <c r="B73" s="1">
+        <f t="shared" si="8"/>
+        <v>52.703338943962045</v>
+      </c>
+      <c r="C73" s="1">
         <f t="shared" si="9"/>
-        <v>48.703338943962045</v>
-      </c>
-      <c r="C73" s="1">
+        <v>8161.4965655513734</v>
+      </c>
+      <c r="D73" s="1">
         <f t="shared" si="10"/>
-        <v>7758.2965655513735</v>
-      </c>
-      <c r="D73" s="1">
+        <v>676.03338943962046</v>
+      </c>
+      <c r="E73" s="1">
         <f t="shared" si="11"/>
-        <v>672.03338943962046</v>
-      </c>
-      <c r="E73" s="1">
-        <f t="shared" si="12"/>
         <v>39.208666666666673</v>
       </c>
       <c r="F73" s="1">
@@ -45417,11 +45646,11 @@
         <v>10549.198306496861</v>
       </c>
       <c r="G73">
+        <f t="shared" si="12"/>
+        <v>58</v>
+      </c>
+      <c r="H73">
         <f t="shared" si="13"/>
-        <v>58</v>
-      </c>
-      <c r="H73">
-        <f t="shared" si="14"/>
         <v>25</v>
       </c>
       <c r="J73" s="1">
@@ -45437,7 +45666,7 @@
         <v>6311.2504383791847</v>
       </c>
       <c r="N73">
-        <f t="shared" si="15"/>
+        <f t="shared" si="14"/>
         <v>1.6714910000000001</v>
       </c>
     </row>
@@ -45446,19 +45675,19 @@
         <v>73</v>
       </c>
       <c r="B74" s="1">
+        <f t="shared" si="8"/>
+        <v>53.758648490814927</v>
+      </c>
+      <c r="C74" s="1">
         <f t="shared" si="9"/>
-        <v>49.758648490814927</v>
-      </c>
-      <c r="C74" s="1">
+        <v>8392.1338757612848</v>
+      </c>
+      <c r="D74" s="1">
         <f t="shared" si="10"/>
-        <v>7983.3338757612846</v>
-      </c>
-      <c r="D74" s="1">
+        <v>688.58648490814926</v>
+      </c>
+      <c r="E74" s="1">
         <f t="shared" si="11"/>
-        <v>685.08648490814926</v>
-      </c>
-      <c r="E74" s="1">
-        <f t="shared" si="12"/>
         <v>39.647999999999996</v>
       </c>
       <c r="F74" s="1">
@@ -45466,11 +45695,11 @@
         <v>10968.724778046813</v>
       </c>
       <c r="G74">
+        <f t="shared" si="12"/>
+        <v>59</v>
+      </c>
+      <c r="H74">
         <f t="shared" si="13"/>
-        <v>59</v>
-      </c>
-      <c r="H74">
-        <f t="shared" si="14"/>
         <v>25</v>
       </c>
       <c r="J74" s="1">
@@ -45486,7 +45715,7 @@
         <v>6534.5226681715967</v>
       </c>
       <c r="N74">
-        <f t="shared" si="15"/>
+        <f t="shared" si="14"/>
         <v>1.678580875</v>
       </c>
     </row>
@@ -45495,19 +45724,19 @@
         <v>74</v>
       </c>
       <c r="B75" s="1">
+        <f t="shared" si="8"/>
+        <v>54.889701257893044</v>
+      </c>
+      <c r="C75" s="1">
         <f t="shared" si="9"/>
-        <v>50.889701257893044</v>
-      </c>
-      <c r="C75" s="1">
+        <v>8633.5730503177183</v>
+      </c>
+      <c r="D75" s="1">
         <f t="shared" si="10"/>
-        <v>8219.1730503177187</v>
-      </c>
-      <c r="D75" s="1">
+        <v>701.89701257893046</v>
+      </c>
+      <c r="E75" s="1">
         <f t="shared" si="11"/>
-        <v>698.89701257893046</v>
-      </c>
-      <c r="E75" s="1">
-        <f t="shared" si="12"/>
         <v>40.083333333333329</v>
       </c>
       <c r="F75" s="1">
@@ -45515,11 +45744,11 @@
         <v>11956.365904365906</v>
       </c>
       <c r="G75">
+        <f t="shared" si="12"/>
+        <v>60</v>
+      </c>
+      <c r="H75">
         <f t="shared" si="13"/>
-        <v>60</v>
-      </c>
-      <c r="H75">
-        <f t="shared" si="14"/>
         <v>25</v>
       </c>
       <c r="J75" s="1">
@@ -45535,7 +45764,7 @@
         <v>7093.3749954709074</v>
       </c>
       <c r="N75">
-        <f t="shared" si="15"/>
+        <f t="shared" si="14"/>
         <v>1.685568</v>
       </c>
     </row>
@@ -45544,19 +45773,19 @@
         <v>75</v>
       </c>
       <c r="B76" s="1">
+        <f t="shared" si="8"/>
+        <v>56.101933598375609</v>
+      </c>
+      <c r="C76" s="1">
         <f t="shared" si="9"/>
-        <v>52.101933598375609</v>
-      </c>
-      <c r="C76" s="1">
+        <v>8886.7030278294387</v>
+      </c>
+      <c r="D76" s="1">
         <f t="shared" si="10"/>
-        <v>8466.7030278294387</v>
-      </c>
-      <c r="D76" s="1">
+        <v>716.01933598375604</v>
+      </c>
+      <c r="E76" s="1">
         <f t="shared" si="11"/>
-        <v>713.51933598375604</v>
-      </c>
-      <c r="E76" s="1">
-        <f t="shared" si="12"/>
         <v>40.51466666666667</v>
       </c>
       <c r="F76" s="1">
@@ -45564,11 +45793,11 @@
         <v>12419.675179358914</v>
       </c>
       <c r="G76">
+        <f t="shared" si="12"/>
+        <v>61</v>
+      </c>
+      <c r="H76">
         <f t="shared" si="13"/>
-        <v>61</v>
-      </c>
-      <c r="H76">
-        <f t="shared" si="14"/>
         <v>26</v>
       </c>
       <c r="J76" s="1">
@@ -45584,7 +45813,7 @@
         <v>7338.2683371859503</v>
       </c>
       <c r="N76">
-        <f t="shared" si="15"/>
+        <f t="shared" si="14"/>
         <v>1.6924531249999999</v>
       </c>
     </row>
@@ -45593,19 +45822,19 @@
         <v>76</v>
       </c>
       <c r="B77" s="1">
+        <f t="shared" si="8"/>
+        <v>57.401172051333091</v>
+      </c>
+      <c r="C77" s="1">
         <f t="shared" si="9"/>
-        <v>53.401172051333091</v>
-      </c>
-      <c r="C77" s="1">
+        <v>9152.484706261841</v>
+      </c>
+      <c r="D77" s="1">
         <f t="shared" si="10"/>
-        <v>8726.8847062618406</v>
-      </c>
-      <c r="D77" s="1">
+        <v>731.01172051333094</v>
+      </c>
+      <c r="E77" s="1">
         <f t="shared" si="11"/>
-        <v>729.01172051333094</v>
-      </c>
-      <c r="E77" s="1">
-        <f t="shared" si="12"/>
         <v>40.942</v>
       </c>
       <c r="F77" s="1">
@@ -45613,11 +45842,11 @@
         <v>13183.674466318205</v>
       </c>
       <c r="G77">
+        <f t="shared" si="12"/>
+        <v>61</v>
+      </c>
+      <c r="H77">
         <f t="shared" si="13"/>
-        <v>61</v>
-      </c>
-      <c r="H77">
-        <f t="shared" si="14"/>
         <v>26</v>
       </c>
       <c r="J77" s="1">
@@ -45633,7 +45862,7 @@
         <v>7758.5848626873158</v>
       </c>
       <c r="N77">
-        <f t="shared" si="15"/>
+        <f t="shared" si="14"/>
         <v>1.6992370000000001</v>
       </c>
     </row>
@@ -45642,19 +45871,19 @@
         <v>77</v>
       </c>
       <c r="B78" s="1">
+        <f t="shared" si="8"/>
+        <v>58.793661346719624</v>
+      </c>
+      <c r="C78" s="1">
         <f t="shared" si="9"/>
-        <v>54.793661346719624</v>
-      </c>
-      <c r="C78" s="1">
+        <v>9431.9566931763748</v>
+      </c>
+      <c r="D78" s="1">
         <f t="shared" si="10"/>
-        <v>9000.756693176374</v>
-      </c>
-      <c r="D78" s="1">
+        <v>746.93661346719625</v>
+      </c>
+      <c r="E78" s="1">
         <f t="shared" si="11"/>
-        <v>745.43661346719625</v>
-      </c>
-      <c r="E78" s="1">
-        <f t="shared" si="12"/>
         <v>41.365333333333332</v>
       </c>
       <c r="F78" s="1">
@@ -45662,11 +45891,11 @@
         <v>13684.018824136154</v>
       </c>
       <c r="G78">
+        <f t="shared" si="12"/>
+        <v>62</v>
+      </c>
+      <c r="H78">
         <f t="shared" si="13"/>
-        <v>62</v>
-      </c>
-      <c r="H78">
-        <f t="shared" si="14"/>
         <v>26</v>
       </c>
       <c r="J78" s="1">
@@ -45682,7 +45911,7 @@
         <v>8021.4874179787857</v>
       </c>
       <c r="N78">
-        <f t="shared" si="15"/>
+        <f t="shared" si="14"/>
         <v>1.705920375</v>
       </c>
     </row>
@@ -45691,19 +45920,19 @@
         <v>78</v>
       </c>
       <c r="B79" s="1">
+        <f t="shared" si="8"/>
+        <v>60.286094420380778</v>
+      </c>
+      <c r="C79" s="1">
         <f t="shared" si="9"/>
-        <v>56.286094420380778</v>
-      </c>
-      <c r="C79" s="1">
+        <v>9726.2415107055804</v>
+      </c>
+      <c r="D79" s="1">
         <f t="shared" si="10"/>
-        <v>9289.4415107055811</v>
-      </c>
-      <c r="D79" s="1">
+        <v>763.86094420380778</v>
+      </c>
+      <c r="E79" s="1">
         <f t="shared" si="11"/>
-        <v>762.86094420380778</v>
-      </c>
-      <c r="E79" s="1">
-        <f t="shared" si="12"/>
         <v>41.784666666666666</v>
       </c>
       <c r="F79" s="1">
@@ -45711,11 +45940,11 @@
         <v>14731.121464013913</v>
       </c>
       <c r="G79">
+        <f t="shared" si="12"/>
+        <v>63</v>
+      </c>
+      <c r="H79">
         <f t="shared" si="13"/>
-        <v>63</v>
-      </c>
-      <c r="H79">
-        <f t="shared" si="14"/>
         <v>27</v>
       </c>
       <c r="J79" s="1">
@@ -45731,7 +45960,7 @@
         <v>8602.0946310279633</v>
       </c>
       <c r="N79">
-        <f t="shared" si="15"/>
+        <f t="shared" si="14"/>
         <v>1.712504</v>
       </c>
     </row>
@@ -45740,19 +45969,19 @@
         <v>79</v>
       </c>
       <c r="B80" s="1">
+        <f t="shared" si="8"/>
+        <v>61.885644583342263</v>
+      </c>
+      <c r="C80" s="1">
         <f t="shared" si="9"/>
-        <v>57.885644583342263</v>
-      </c>
-      <c r="C80" s="1">
+        <v>10036.552290917652</v>
+      </c>
+      <c r="D80" s="1">
         <f t="shared" si="10"/>
-        <v>9594.1522909176529</v>
-      </c>
-      <c r="D80" s="1">
+        <v>781.85644583342264</v>
+      </c>
+      <c r="E80" s="1">
         <f t="shared" si="11"/>
-        <v>781.35644583342264</v>
-      </c>
-      <c r="E80" s="1">
-        <f t="shared" si="12"/>
         <v>42.2</v>
       </c>
       <c r="F80" s="1">
@@ -45760,11 +45989,11 @@
         <v>15277.654028436018</v>
       </c>
       <c r="G80">
+        <f t="shared" si="12"/>
+        <v>64</v>
+      </c>
+      <c r="H80">
         <f t="shared" si="13"/>
-        <v>64</v>
-      </c>
-      <c r="H80">
-        <f t="shared" si="14"/>
         <v>27</v>
       </c>
       <c r="J80" s="1">
@@ -45780,7 +46009,7 @@
         <v>8887.5829695708526</v>
       </c>
       <c r="N80">
-        <f t="shared" si="15"/>
+        <f t="shared" si="14"/>
         <v>1.7189886249999999</v>
       </c>
     </row>
@@ -45789,19 +46018,19 @@
         <v>80</v>
       </c>
       <c r="B81" s="1">
+        <f t="shared" si="8"/>
+        <v>77.599999999999994</v>
+      </c>
+      <c r="C81" s="1">
         <f t="shared" si="9"/>
-        <v>73.599999999999994</v>
-      </c>
-      <c r="C81" s="1">
+        <v>11932.199999999999</v>
+      </c>
+      <c r="D81" s="1">
         <f t="shared" si="10"/>
-        <v>11484.199999999999</v>
-      </c>
-      <c r="D81" s="1">
+        <v>941</v>
+      </c>
+      <c r="E81" s="1">
         <f t="shared" si="11"/>
-        <v>941</v>
-      </c>
-      <c r="E81" s="1">
-        <f t="shared" si="12"/>
         <v>42.611333333333334</v>
       </c>
       <c r="F81" s="1">
@@ -45809,11 +46038,11 @@
         <v>16749.393745013065</v>
       </c>
       <c r="G81">
+        <f t="shared" si="12"/>
+        <v>65</v>
+      </c>
+      <c r="H81">
         <f t="shared" si="13"/>
-        <v>65</v>
-      </c>
-      <c r="H81">
-        <f t="shared" si="14"/>
         <v>27</v>
       </c>
       <c r="J81" s="1">
@@ -45829,7 +46058,7 @@
         <v>9707.6831094765275</v>
       </c>
       <c r="N81">
-        <f t="shared" si="15"/>
+        <f t="shared" si="14"/>
         <v>1.7253749999999999</v>
       </c>
     </row>
@@ -45838,19 +46067,19 @@
         <v>81</v>
       </c>
       <c r="B82" s="1">
+        <f t="shared" si="8"/>
+        <v>79.437400640929098</v>
+      </c>
+      <c r="C82" s="1">
         <f t="shared" si="9"/>
-        <v>75.437400640929098</v>
-      </c>
-      <c r="C82" s="1">
+        <v>12298.20123268136</v>
+      </c>
+      <c r="D82" s="1">
         <f t="shared" si="10"/>
-        <v>11844.60123268136</v>
-      </c>
-      <c r="D82" s="1">
+        <v>961.37400640929104</v>
+      </c>
+      <c r="E82" s="1">
         <f t="shared" si="11"/>
-        <v>961.87400640929104</v>
-      </c>
-      <c r="E82" s="1">
-        <f t="shared" si="12"/>
         <v>43.018666666666668</v>
       </c>
       <c r="F82" s="1">
@@ -45858,11 +46087,11 @@
         <v>17774.35376890652</v>
       </c>
       <c r="G82">
+        <f t="shared" si="12"/>
+        <v>65</v>
+      </c>
+      <c r="H82">
         <f t="shared" si="13"/>
-        <v>65</v>
-      </c>
-      <c r="H82">
-        <f t="shared" si="14"/>
         <v>28</v>
       </c>
       <c r="J82" s="1">
@@ -45878,7 +46107,7 @@
         <v>10264.320937518271</v>
       </c>
       <c r="N82">
-        <f t="shared" si="15"/>
+        <f t="shared" si="14"/>
         <v>1.731663875</v>
       </c>
     </row>
@@ -45887,19 +46116,19 @@
         <v>82</v>
       </c>
       <c r="B83" s="1">
+        <f t="shared" si="8"/>
+        <v>81.406677887924062</v>
+      </c>
+      <c r="C83" s="1">
         <f t="shared" si="9"/>
-        <v>77.406677887924062</v>
-      </c>
-      <c r="C83" s="1">
+        <v>12684.486621533682</v>
+      </c>
+      <c r="D83" s="1">
         <f t="shared" si="10"/>
-        <v>12225.286621533684</v>
-      </c>
-      <c r="D83" s="1">
+        <v>983.06677887924059</v>
+      </c>
+      <c r="E83" s="1">
         <f t="shared" si="11"/>
-        <v>984.06677887924059</v>
-      </c>
-      <c r="E83" s="1">
-        <f t="shared" si="12"/>
         <v>43.421999999999997</v>
       </c>
       <c r="F83" s="1">
@@ -45907,11 +46136,11 @@
         <v>19351.227488369954</v>
       </c>
       <c r="G83">
+        <f t="shared" si="12"/>
+        <v>66</v>
+      </c>
+      <c r="H83">
         <f t="shared" si="13"/>
-        <v>66</v>
-      </c>
-      <c r="H83">
-        <f t="shared" si="14"/>
         <v>28</v>
       </c>
       <c r="J83" s="1">
@@ -45927,7 +46156,7 @@
         <v>11135.11561853799</v>
       </c>
       <c r="N83">
-        <f t="shared" si="15"/>
+        <f t="shared" si="14"/>
         <v>1.7378559999999998</v>
       </c>
     </row>
@@ -45936,19 +46165,19 @@
         <v>83</v>
       </c>
       <c r="B84" s="1">
+        <f t="shared" si="8"/>
+        <v>83.517296981629883</v>
+      </c>
+      <c r="C84" s="1">
         <f t="shared" si="9"/>
-        <v>79.517296981629883</v>
-      </c>
-      <c r="C84" s="1">
+        <v>13092.70990926539</v>
+      </c>
+      <c r="D84" s="1">
         <f t="shared" si="10"/>
-        <v>12627.909909265391</v>
-      </c>
-      <c r="D84" s="1">
+        <v>1006.1729698162989</v>
+      </c>
+      <c r="E84" s="1">
         <f t="shared" si="11"/>
-        <v>1007.6729698162989</v>
-      </c>
-      <c r="E84" s="1">
-        <f t="shared" si="12"/>
         <v>43.821333333333328</v>
       </c>
       <c r="F84" s="1">
@@ -45956,11 +46185,11 @@
         <v>20472.950769792493</v>
       </c>
       <c r="G84">
+        <f t="shared" si="12"/>
+        <v>67</v>
+      </c>
+      <c r="H84">
         <f t="shared" si="13"/>
-        <v>67</v>
-      </c>
-      <c r="H84">
-        <f t="shared" si="14"/>
         <v>28</v>
       </c>
       <c r="J84" s="1">
@@ -45976,7 +46205,7 @@
         <v>11739.399537583346</v>
       </c>
       <c r="N84">
-        <f t="shared" si="15"/>
+        <f t="shared" si="14"/>
         <v>1.7439521250000001</v>
       </c>
     </row>
@@ -45985,19 +46214,19 @@
         <v>84</v>
       </c>
       <c r="B85" s="1">
+        <f t="shared" si="8"/>
+        <v>85.779402515786089</v>
+      </c>
+      <c r="C85" s="1">
         <f t="shared" si="9"/>
-        <v>81.779402515786089</v>
-      </c>
-      <c r="C85" s="1">
+        <v>13524.657735856443</v>
+      </c>
+      <c r="D85" s="1">
         <f t="shared" si="10"/>
-        <v>13054.257735856443</v>
-      </c>
-      <c r="D85" s="1">
+        <v>1030.7940251578609</v>
+      </c>
+      <c r="E85" s="1">
         <f t="shared" si="11"/>
-        <v>1032.7940251578609</v>
-      </c>
-      <c r="E85" s="1">
-        <f t="shared" si="12"/>
         <v>44.216666666666669</v>
       </c>
       <c r="F85" s="1">
@@ -46005,11 +46234,11 @@
         <v>22513.185073501696</v>
       </c>
       <c r="G85">
+        <f t="shared" si="12"/>
+        <v>68</v>
+      </c>
+      <c r="H85">
         <f t="shared" si="13"/>
-        <v>68</v>
-      </c>
-      <c r="H85">
-        <f t="shared" si="14"/>
         <v>29</v>
       </c>
       <c r="J85" s="1">
@@ -46025,7 +46254,7 @@
         <v>12865.022702610695</v>
       </c>
       <c r="N85">
-        <f t="shared" si="15"/>
+        <f t="shared" si="14"/>
         <v>1.7499530000000001</v>
       </c>
     </row>
@@ -46034,19 +46263,19 @@
         <v>85</v>
       </c>
       <c r="B86" s="1">
+        <f t="shared" si="8"/>
+        <v>88.203867196751233</v>
+      </c>
+      <c r="C86" s="1">
         <f t="shared" si="9"/>
-        <v>84.203867196751233</v>
-      </c>
-      <c r="C86" s="1">
+        <v>13982.260196413396</v>
+      </c>
+      <c r="D86" s="1">
         <f t="shared" si="10"/>
-        <v>13506.260196413396</v>
-      </c>
-      <c r="D86" s="1">
+        <v>1057.0386719675123</v>
+      </c>
+      <c r="E86" s="1">
         <f t="shared" si="11"/>
-        <v>1059.5386719675123</v>
-      </c>
-      <c r="E86" s="1">
-        <f t="shared" si="12"/>
         <v>44.608000000000004</v>
       </c>
       <c r="F86" s="1">
@@ -46054,11 +46283,11 @@
         <v>24151.093974175034</v>
       </c>
       <c r="G86">
+        <f t="shared" si="12"/>
+        <v>69</v>
+      </c>
+      <c r="H86">
         <f t="shared" si="13"/>
-        <v>69</v>
-      </c>
-      <c r="H86">
-        <f t="shared" si="14"/>
         <v>29</v>
       </c>
       <c r="J86" s="1">
@@ -46074,7 +46303,7 @@
         <v>13754.571874057416</v>
       </c>
       <c r="N86">
-        <f t="shared" si="15"/>
+        <f t="shared" si="14"/>
         <v>1.755859375</v>
       </c>
     </row>
@@ -46083,19 +46312,19 @@
         <v>86</v>
       </c>
       <c r="B87" s="1">
+        <f t="shared" si="8"/>
+        <v>90.802344102666183</v>
+      </c>
+      <c r="C87" s="1">
         <f t="shared" si="9"/>
-        <v>86.802344102666183</v>
-      </c>
-      <c r="C87" s="1">
+        <v>14467.602229961009</v>
+      </c>
+      <c r="D87" s="1">
         <f t="shared" si="10"/>
-        <v>13986.002229961008</v>
-      </c>
-      <c r="D87" s="1">
+        <v>1085.0234410266619</v>
+      </c>
+      <c r="E87" s="1">
         <f t="shared" si="11"/>
-        <v>1088.0234410266619</v>
-      </c>
-      <c r="E87" s="1">
-        <f t="shared" si="12"/>
         <v>44.995333333333335</v>
       </c>
       <c r="F87" s="1">
@@ -46103,11 +46332,11 @@
         <v>26350.15483087135</v>
       </c>
       <c r="G87">
+        <f t="shared" si="12"/>
+        <v>69</v>
+      </c>
+      <c r="H87">
         <f t="shared" si="13"/>
-        <v>69</v>
-      </c>
-      <c r="H87">
-        <f t="shared" si="14"/>
         <v>29</v>
       </c>
       <c r="J87" s="1">
@@ -46123,7 +46352,7 @@
         <v>14957.469285355817</v>
       </c>
       <c r="N87">
-        <f t="shared" si="15"/>
+        <f t="shared" si="14"/>
         <v>1.7616719999999999</v>
       </c>
     </row>
@@ -46132,19 +46361,19 @@
         <v>87</v>
       </c>
       <c r="B88" s="1">
+        <f t="shared" si="8"/>
+        <v>93.587322693439219</v>
+      </c>
+      <c r="C88" s="1">
         <f t="shared" si="9"/>
-        <v>89.587322693439219</v>
-      </c>
-      <c r="C88" s="1">
+        <v>14982.935904060896</v>
+      </c>
+      <c r="D88" s="1">
         <f t="shared" si="10"/>
-        <v>14495.735904060897</v>
-      </c>
-      <c r="D88" s="1">
+        <v>1114.8732269343923</v>
+      </c>
+      <c r="E88" s="1">
         <f t="shared" si="11"/>
-        <v>1118.3732269343923</v>
-      </c>
-      <c r="E88" s="1">
-        <f t="shared" si="12"/>
         <v>45.378666666666668</v>
       </c>
       <c r="F88" s="1">
@@ -46152,11 +46381,11 @@
         <v>28139.654463183873</v>
       </c>
       <c r="G88">
+        <f t="shared" si="12"/>
+        <v>70</v>
+      </c>
+      <c r="H88">
         <f t="shared" si="13"/>
-        <v>70</v>
-      </c>
-      <c r="H88">
-        <f t="shared" si="14"/>
         <v>30</v>
       </c>
       <c r="J88" s="1">
@@ -46172,7 +46401,7 @@
         <v>15921.572822426311</v>
       </c>
       <c r="N88">
-        <f t="shared" si="15"/>
+        <f t="shared" si="14"/>
         <v>1.7673916250000001</v>
       </c>
     </row>
@@ -46181,19 +46410,19 @@
         <v>88</v>
       </c>
       <c r="B89" s="1">
+        <f t="shared" si="8"/>
+        <v>96.572188840761555</v>
+      </c>
+      <c r="C89" s="1">
         <f t="shared" si="9"/>
-        <v>92.572188840761555</v>
-      </c>
-      <c r="C89" s="1">
+        <v>15530.693665181823</v>
+      </c>
+      <c r="D89" s="1">
         <f t="shared" si="10"/>
-        <v>15037.893665181822</v>
-      </c>
-      <c r="D89" s="1">
+        <v>1146.7218884076156</v>
+      </c>
+      <c r="E89" s="1">
         <f t="shared" si="11"/>
-        <v>1150.7218884076156</v>
-      </c>
-      <c r="E89" s="1">
-        <f t="shared" si="12"/>
         <v>45.757999999999996</v>
       </c>
       <c r="F89" s="1">
@@ -46201,11 +46430,11 @@
         <v>30846.474933344991</v>
       </c>
       <c r="G89">
+        <f t="shared" si="12"/>
+        <v>71</v>
+      </c>
+      <c r="H89">
         <f t="shared" si="13"/>
-        <v>71</v>
-      </c>
-      <c r="H89">
-        <f t="shared" si="14"/>
         <v>30</v>
       </c>
       <c r="J89" s="1">
@@ -46221,7 +46450,7 @@
         <v>17397.712564470541</v>
       </c>
       <c r="N89">
-        <f t="shared" si="15"/>
+        <f t="shared" si="14"/>
         <v>1.7730190000000001</v>
       </c>
     </row>
@@ -46230,19 +46459,19 @@
         <v>89</v>
       </c>
       <c r="B90" s="1">
+        <f t="shared" si="8"/>
+        <v>99.771289166684539</v>
+      </c>
+      <c r="C90" s="1">
         <f t="shared" si="9"/>
-        <v>95.771289166684539</v>
-      </c>
-      <c r="C90" s="1">
+        <v>16113.502630168892</v>
+      </c>
+      <c r="D90" s="1">
         <f t="shared" si="10"/>
-        <v>15615.102630168891</v>
-      </c>
-      <c r="D90" s="1">
+        <v>1180.7128916668453</v>
+      </c>
+      <c r="E90" s="1">
         <f t="shared" si="11"/>
-        <v>1185.2128916668453</v>
-      </c>
-      <c r="E90" s="1">
-        <f t="shared" si="12"/>
         <v>46.133333333333333</v>
       </c>
       <c r="F90" s="1">
@@ -46250,11 +46479,11 @@
         <v>33195.780346820808</v>
       </c>
       <c r="G90">
+        <f t="shared" si="12"/>
+        <v>72</v>
+      </c>
+      <c r="H90">
         <f t="shared" si="13"/>
-        <v>72</v>
-      </c>
-      <c r="H90">
-        <f t="shared" si="14"/>
         <v>30</v>
       </c>
       <c r="J90" s="1">
@@ -46270,7 +46499,7 @@
         <v>18664.467885378464</v>
       </c>
       <c r="N90">
-        <f t="shared" si="15"/>
+        <f t="shared" si="14"/>
         <v>1.778554875</v>
       </c>
     </row>
@@ -46279,19 +46508,19 @@
         <v>90</v>
       </c>
       <c r="B91" s="1">
+        <f t="shared" si="8"/>
+        <v>128.19999999999999</v>
+      </c>
+      <c r="C91" s="1">
         <f t="shared" si="9"/>
-        <v>119.2</v>
-      </c>
-      <c r="C91" s="1">
+        <v>19884.199999999997</v>
+      </c>
+      <c r="D91" s="1">
         <f t="shared" si="10"/>
-        <v>18750.199999999997</v>
-      </c>
-      <c r="D91" s="1">
+        <v>1467</v>
+      </c>
+      <c r="E91" s="1">
         <f t="shared" si="11"/>
-        <v>1422</v>
-      </c>
-      <c r="E91" s="1">
-        <f t="shared" si="12"/>
         <v>46.504666666666665</v>
       </c>
       <c r="F91" s="1">
@@ -46299,11 +46528,11 @@
         <v>37890.54145103717</v>
       </c>
       <c r="G91">
+        <f t="shared" si="12"/>
+        <v>73</v>
+      </c>
+      <c r="H91">
         <f t="shared" si="13"/>
-        <v>73</v>
-      </c>
-      <c r="H91">
-        <f t="shared" si="14"/>
         <v>31</v>
       </c>
       <c r="J91" s="1">
@@ -46319,7 +46548,7 @@
         <v>21239.092741612763</v>
       </c>
       <c r="N91">
-        <f t="shared" si="15"/>
+        <f t="shared" si="14"/>
         <v>1.784</v>
       </c>
     </row>
@@ -46328,19 +46557,19 @@
         <v>91</v>
       </c>
       <c r="B92" s="1">
+        <f t="shared" si="8"/>
+        <v>131.8748012818582</v>
+      </c>
+      <c r="C92" s="1">
         <f t="shared" si="9"/>
-        <v>122.87480128185821</v>
-      </c>
-      <c r="C92" s="1">
+        <v>20580.849683308734</v>
+      </c>
+      <c r="D92" s="1">
         <f t="shared" si="10"/>
-        <v>19434.249683308735</v>
-      </c>
-      <c r="D92" s="1">
+        <v>1505.7480128185821</v>
+      </c>
+      <c r="E92" s="1">
         <f t="shared" si="11"/>
-        <v>1461.2480128185821</v>
-      </c>
-      <c r="E92" s="1">
-        <f t="shared" si="12"/>
         <v>46.872</v>
       </c>
       <c r="F92" s="1">
@@ -46348,11 +46577,11 @@
         <v>40589.84041645332</v>
       </c>
       <c r="G92">
+        <f t="shared" si="12"/>
+        <v>73</v>
+      </c>
+      <c r="H92">
         <f t="shared" si="13"/>
-        <v>73</v>
-      </c>
-      <c r="H92">
-        <f t="shared" si="14"/>
         <v>31</v>
       </c>
       <c r="J92" s="1">
@@ -46368,7 +46597,7 @@
         <v>22684.060782206838</v>
       </c>
       <c r="N92">
-        <f t="shared" si="15"/>
+        <f t="shared" si="14"/>
         <v>1.7893551250000002</v>
       </c>
     </row>
@@ -46377,19 +46606,19 @@
         <v>92</v>
       </c>
       <c r="B93" s="1">
+        <f t="shared" si="8"/>
+        <v>135.81335577584815</v>
+      </c>
+      <c r="C93" s="1">
         <f t="shared" si="9"/>
-        <v>126.81335577584814</v>
-      </c>
-      <c r="C93" s="1">
+        <v>21321.760223929239</v>
+      </c>
+      <c r="D93" s="1">
         <f t="shared" si="10"/>
-        <v>20162.560223929238</v>
-      </c>
-      <c r="D93" s="1">
+        <v>1547.1335577584814</v>
+      </c>
+      <c r="E93" s="1">
         <f t="shared" si="11"/>
-        <v>1503.1335577584814</v>
-      </c>
-      <c r="E93" s="1">
-        <f t="shared" si="12"/>
         <v>47.23533333333333</v>
       </c>
       <c r="F93" s="1">
@@ -46397,11 +46626,11 @@
         <v>44216.412854783848</v>
       </c>
       <c r="G93">
+        <f t="shared" si="12"/>
+        <v>74</v>
+      </c>
+      <c r="H93">
         <f t="shared" si="13"/>
-        <v>74</v>
-      </c>
-      <c r="H93">
-        <f t="shared" si="14"/>
         <v>31</v>
       </c>
       <c r="J93" s="1">
@@ -46417,7 +46646,7 @@
         <v>24638.30126516064</v>
       </c>
       <c r="N93">
-        <f t="shared" si="15"/>
+        <f t="shared" si="14"/>
         <v>1.7946209999999998</v>
       </c>
     </row>
@@ -46426,19 +46655,19 @@
         <v>93</v>
       </c>
       <c r="B94" s="1">
+        <f t="shared" si="8"/>
+        <v>140.03459396325971</v>
+      </c>
+      <c r="C94" s="1">
         <f t="shared" si="9"/>
-        <v>131.03459396325971</v>
-      </c>
-      <c r="C94" s="1">
+        <v>22110.504134016413</v>
+      </c>
+      <c r="D94" s="1">
         <f t="shared" si="10"/>
-        <v>20938.704134016414</v>
-      </c>
-      <c r="D94" s="1">
+        <v>1591.345939632597</v>
+      </c>
+      <c r="E94" s="1">
         <f t="shared" si="11"/>
-        <v>1547.845939632597</v>
-      </c>
-      <c r="E94" s="1">
-        <f t="shared" si="12"/>
         <v>47.594666666666669</v>
       </c>
       <c r="F94" s="1">
@@ -46446,11 +46675,11 @@
         <v>47537.006947557151</v>
       </c>
       <c r="G94">
+        <f t="shared" si="12"/>
+        <v>75</v>
+      </c>
+      <c r="H94">
         <f t="shared" si="13"/>
-        <v>75</v>
-      </c>
-      <c r="H94">
-        <f t="shared" si="14"/>
         <v>32</v>
       </c>
       <c r="J94" s="1">
@@ -46466,7 +46695,7 @@
         <v>26412.406860605788</v>
       </c>
       <c r="N94">
-        <f t="shared" si="15"/>
+        <f t="shared" si="14"/>
         <v>1.799798375</v>
       </c>
     </row>
@@ -46475,19 +46704,19 @@
         <v>94</v>
       </c>
       <c r="B95" s="1">
+        <f t="shared" si="8"/>
+        <v>144.55880503157218</v>
+      </c>
+      <c r="C95" s="1">
         <f t="shared" si="9"/>
-        <v>135.55880503157218</v>
-      </c>
-      <c r="C95" s="1">
+        <v>22950.9387421549</v>
+      </c>
+      <c r="D95" s="1">
         <f t="shared" si="10"/>
-        <v>21766.538742154899</v>
-      </c>
-      <c r="D95" s="1">
+        <v>1638.5880503157218</v>
+      </c>
+      <c r="E95" s="1">
         <f t="shared" si="11"/>
-        <v>1595.5880503157218</v>
-      </c>
-      <c r="E95" s="1">
-        <f t="shared" si="12"/>
         <v>47.95</v>
       </c>
       <c r="F95" s="1">
@@ -46495,11 +46724,11 @@
         <v>53172.888425443169</v>
       </c>
       <c r="G95">
+        <f t="shared" si="12"/>
+        <v>76</v>
+      </c>
+      <c r="H95">
         <f t="shared" si="13"/>
-        <v>76</v>
-      </c>
-      <c r="H95">
-        <f t="shared" si="14"/>
         <v>32</v>
       </c>
       <c r="J95" s="1">
@@ -46515,7 +46744,7 @@
         <v>29460.491967060094</v>
       </c>
       <c r="N95">
-        <f t="shared" si="15"/>
+        <f t="shared" si="14"/>
         <v>1.804888</v>
       </c>
     </row>
@@ -46524,19 +46753,19 @@
         <v>95</v>
       </c>
       <c r="B96" s="1">
+        <f t="shared" si="8"/>
+        <v>149.40773439350247</v>
+      </c>
+      <c r="C96" s="1">
         <f t="shared" si="9"/>
-        <v>140.40773439350247</v>
-      </c>
-      <c r="C96" s="1">
+        <v>23847.228674335824</v>
+      </c>
+      <c r="D96" s="1">
         <f t="shared" si="10"/>
-        <v>22650.228674335827</v>
-      </c>
-      <c r="D96" s="1">
+        <v>1689.0773439350246</v>
+      </c>
+      <c r="E96" s="1">
         <f t="shared" si="11"/>
-        <v>1646.5773439350246</v>
-      </c>
-      <c r="E96" s="1">
-        <f t="shared" si="12"/>
         <v>48.301333333333332</v>
       </c>
       <c r="F96" s="1">
@@ -46544,11 +46773,11 @@
         <v>56916.461933417988</v>
       </c>
       <c r="G96">
+        <f t="shared" si="12"/>
+        <v>77</v>
+      </c>
+      <c r="H96">
         <f t="shared" si="13"/>
-        <v>77</v>
-      </c>
-      <c r="H96">
-        <f t="shared" si="14"/>
         <v>32</v>
       </c>
       <c r="J96" s="1">
@@ -46564,7 +46793,7 @@
         <v>31447.459391872362</v>
       </c>
       <c r="N96">
-        <f t="shared" si="15"/>
+        <f t="shared" si="14"/>
         <v>1.809890625</v>
       </c>
     </row>
@@ -46573,19 +46802,19 @@
         <v>96</v>
       </c>
       <c r="B97" s="1">
+        <f t="shared" si="8"/>
+        <v>154.60468820533237</v>
+      </c>
+      <c r="C97" s="1">
         <f t="shared" si="9"/>
-        <v>145.60468820533237</v>
-      </c>
-      <c r="C97" s="1">
+        <v>24803.870094796664</v>
+      </c>
+      <c r="D97" s="1">
         <f t="shared" si="10"/>
-        <v>23594.270094796666</v>
-      </c>
-      <c r="D97" s="1">
+        <v>1743.0468820533238</v>
+      </c>
+      <c r="E97" s="1">
         <f t="shared" si="11"/>
-        <v>1701.0468820533238</v>
-      </c>
-      <c r="E97" s="1">
-        <f t="shared" si="12"/>
         <v>48.648666666666671</v>
       </c>
       <c r="F97" s="1">
@@ -46593,11 +46822,11 @@
         <v>61603.024406287252</v>
       </c>
       <c r="G97">
+        <f t="shared" si="12"/>
+        <v>77</v>
+      </c>
+      <c r="H97">
         <f t="shared" si="13"/>
-        <v>77</v>
-      </c>
-      <c r="H97">
-        <f t="shared" si="14"/>
         <v>33</v>
       </c>
       <c r="J97" s="1">
@@ -46613,7 +46842,7 @@
         <v>33944.66982234874</v>
       </c>
       <c r="N97">
-        <f t="shared" si="15"/>
+        <f t="shared" si="14"/>
         <v>1.8148070000000001</v>
       </c>
     </row>
@@ -46622,19 +46851,19 @@
         <v>97</v>
       </c>
       <c r="B98" s="1">
+        <f t="shared" si="8"/>
+        <v>160.17464538687844</v>
+      </c>
+      <c r="C98" s="1">
         <f t="shared" si="9"/>
-        <v>151.17464538687844</v>
-      </c>
-      <c r="C98" s="1">
+        <v>25825.716843538095</v>
+      </c>
+      <c r="D98" s="1">
         <f t="shared" si="10"/>
-        <v>24603.516843538095</v>
-      </c>
-      <c r="D98" s="1">
+        <v>1800.7464538687843</v>
+      </c>
+      <c r="E98" s="1">
         <f t="shared" si="11"/>
-        <v>1759.2464538687843</v>
-      </c>
-      <c r="E98" s="1">
-        <f t="shared" si="12"/>
         <v>48.992000000000004</v>
       </c>
       <c r="F98" s="1">
@@ -46642,11 +46871,11 @@
         <v>66036.475342913123</v>
       </c>
       <c r="G98">
+        <f t="shared" si="12"/>
+        <v>78</v>
+      </c>
+      <c r="H98">
         <f t="shared" si="13"/>
-        <v>78</v>
-      </c>
-      <c r="H98">
-        <f t="shared" si="14"/>
         <v>33</v>
       </c>
       <c r="J98" s="1">
@@ -46662,7 +46891,7 @@
         <v>36290.998472931387</v>
       </c>
       <c r="N98">
-        <f t="shared" si="15"/>
+        <f t="shared" si="14"/>
         <v>1.8196378750000002</v>
       </c>
     </row>
@@ -46671,19 +46900,19 @@
         <v>98</v>
       </c>
       <c r="B99" s="1">
+        <f t="shared" si="8"/>
+        <v>166.14437768152311</v>
+      </c>
+      <c r="C99" s="1">
         <f t="shared" si="9"/>
-        <v>157.14437768152311</v>
-      </c>
-      <c r="C99" s="1">
+        <v>26918.008617904969</v>
+      </c>
+      <c r="D99" s="1">
         <f t="shared" si="10"/>
-        <v>25683.208617904969</v>
-      </c>
-      <c r="D99" s="1">
+        <v>1862.4437768152311</v>
+      </c>
+      <c r="E99" s="1">
         <f t="shared" si="11"/>
-        <v>1821.4437768152311</v>
-      </c>
-      <c r="E99" s="1">
-        <f t="shared" si="12"/>
         <v>49.331333333333333</v>
       </c>
       <c r="F99" s="1">
@@ -46691,11 +46920,11 @@
         <v>72765.132370231222</v>
       </c>
       <c r="G99">
+        <f t="shared" si="12"/>
+        <v>79</v>
+      </c>
+      <c r="H99">
         <f t="shared" si="13"/>
-        <v>79</v>
-      </c>
-      <c r="H99">
-        <f t="shared" si="14"/>
         <v>33</v>
       </c>
       <c r="J99" s="1">
@@ -46711,7 +46940,7 @@
         <v>39884.767883423243</v>
       </c>
       <c r="N99">
-        <f t="shared" si="15"/>
+        <f t="shared" si="14"/>
         <v>1.824384</v>
       </c>
     </row>
@@ -46720,19 +46949,19 @@
         <v>99</v>
       </c>
       <c r="B100" s="1">
+        <f t="shared" si="8"/>
+        <v>172.54257833336908</v>
+      </c>
+      <c r="C100" s="1">
         <f t="shared" si="9"/>
-        <v>163.54257833336908</v>
-      </c>
-      <c r="C100" s="1">
+        <v>28086.401357004954</v>
+      </c>
+      <c r="D100" s="1">
         <f t="shared" si="10"/>
-        <v>26839.001357004952</v>
-      </c>
-      <c r="D100" s="1">
+        <v>1928.4257833336908</v>
+      </c>
+      <c r="E100" s="1">
         <f t="shared" si="11"/>
-        <v>1887.9257833336908</v>
-      </c>
-      <c r="E100" s="1">
-        <f t="shared" si="12"/>
         <v>49.666666666666671</v>
       </c>
       <c r="F100" s="1">
@@ -46740,11 +46969,11 @@
         <v>77701.288590604017</v>
       </c>
       <c r="G100">
+        <f t="shared" si="12"/>
+        <v>80</v>
+      </c>
+      <c r="H100">
         <f t="shared" si="13"/>
-        <v>80</v>
-      </c>
-      <c r="H100">
-        <f t="shared" si="14"/>
         <v>34</v>
       </c>
       <c r="J100" s="1">
@@ -46760,7 +46989,7 @@
         <v>42481.863922706711</v>
       </c>
       <c r="N100">
-        <f t="shared" si="15"/>
+        <f t="shared" si="14"/>
         <v>1.8290461250000001</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Finished character creation, cleaned up item db a bit.
</commit_message>
<xml_diff>
--- a/Other/RoStatProcessing.xlsx
+++ b/Other/RoStatProcessing.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\ProjectsSSD\RagnarokRebuildTcp\Other\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A099BD5A-BDE1-43FB-9610-C7C24588F3DE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B167A517-D173-499F-BD72-803F5841CBE1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="883" yWindow="2889" windowWidth="29220" windowHeight="11442" xr2:uid="{1C41742B-2950-4FF8-AA39-6557869B44EA}"/>
   </bookViews>
@@ -51,7 +51,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3026" uniqueCount="1135">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3026" uniqueCount="1136">
   <si>
     <t>Id</t>
   </si>
@@ -3456,6 +3456,9 @@
   </si>
   <si>
     <t>Raptice</t>
+  </si>
+  <si>
+    <t>raptice.spr</t>
   </si>
 </sst>
 </file>
@@ -3898,10 +3901,10 @@
   <dimension ref="A1:AJ306"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <pane xSplit="4" ySplit="1" topLeftCell="E284" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="4" ySplit="1" topLeftCell="E280" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="E1" sqref="E1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="U295" sqref="U295"/>
+      <selection pane="bottomRight" activeCell="A306" sqref="A306"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
@@ -36686,7 +36689,7 @@
         <v>324</v>
       </c>
       <c r="AF306" t="s">
-        <v>340</v>
+        <v>1135</v>
       </c>
       <c r="AG306">
         <v>0</v>

</xml_diff>

<commit_message>
Implementing item weight, plus some balance adjustments and new mobs.
</commit_message>
<xml_diff>
--- a/Other/RoStatProcessing.xlsx
+++ b/Other/RoStatProcessing.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\ProjectsSSD\RagnarokRebuildTcp\Other\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6A636066-4C20-4140-922A-81A1A0DD21EE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C19BA483-3DB5-4B0F-9DBF-2C7B3247BF3C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="2331" yWindow="2983" windowWidth="28346" windowHeight="14786" xr2:uid="{1C41742B-2950-4FF8-AA39-6557869B44EA}"/>
   </bookViews>
@@ -51,7 +51,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3042" uniqueCount="1141">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3124" uniqueCount="1169">
   <si>
     <t>Id</t>
   </si>
@@ -3474,6 +3474,90 @@
   </si>
   <si>
     <t>Stitch</t>
+  </si>
+  <si>
+    <t>SOLDIER_ANDRE</t>
+  </si>
+  <si>
+    <t>SOLDIER_DENIRO</t>
+  </si>
+  <si>
+    <t>SOLDIER_PIERE</t>
+  </si>
+  <si>
+    <t>Soldier Andre</t>
+  </si>
+  <si>
+    <t>Soldier Deniro</t>
+  </si>
+  <si>
+    <t>Soldier Piere</t>
+  </si>
+  <si>
+    <t>soldier_andre.spr</t>
+  </si>
+  <si>
+    <t>soldier_deniro.spr</t>
+  </si>
+  <si>
+    <t>soldier_piere.spr</t>
+  </si>
+  <si>
+    <t>ANDRE_LARVA</t>
+  </si>
+  <si>
+    <t>DENIRO_LARVA</t>
+  </si>
+  <si>
+    <t>PIERE_LARVA</t>
+  </si>
+  <si>
+    <t>Andre Larva</t>
+  </si>
+  <si>
+    <t>Deniro Larva</t>
+  </si>
+  <si>
+    <t>Piere Larva</t>
+  </si>
+  <si>
+    <t>ANT_EGG2</t>
+  </si>
+  <si>
+    <t>Mature Ant Egg</t>
+  </si>
+  <si>
+    <t>andre_larva.spr</t>
+  </si>
+  <si>
+    <t>deniro_larva.spr</t>
+  </si>
+  <si>
+    <t>piere_larva.spr</t>
+  </si>
+  <si>
+    <t>fungus.spr</t>
+  </si>
+  <si>
+    <t>deathspore.spr</t>
+  </si>
+  <si>
+    <t>FUNGUS</t>
+  </si>
+  <si>
+    <t>DEATHSPORE</t>
+  </si>
+  <si>
+    <t>Fungus</t>
+  </si>
+  <si>
+    <t>Deathspore</t>
+  </si>
+  <si>
+    <t>Stationary,Plant</t>
+  </si>
+  <si>
+    <t>Stationary</t>
   </si>
 </sst>
 </file>
@@ -3542,7 +3626,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
@@ -3555,6 +3639,7 @@
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -3914,13 +3999,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{811A97A5-94A7-4FFA-A162-65D076B52481}">
-  <dimension ref="A1:AJ307"/>
+  <dimension ref="A1:AJ316"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <pane xSplit="4" ySplit="1" topLeftCell="E268" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="4" ySplit="1" topLeftCell="E290" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="E1" sqref="E1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="O305" sqref="O305"/>
+      <selection pane="bottomRight" activeCell="B312" sqref="B312"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
@@ -10730,16 +10815,16 @@
         <v>100</v>
       </c>
       <c r="I64">
-        <v>100</v>
+        <v>130</v>
       </c>
       <c r="J64">
-        <v>100</v>
+        <v>50</v>
       </c>
       <c r="K64">
         <v>100</v>
       </c>
       <c r="L64">
-        <v>100</v>
+        <v>130</v>
       </c>
       <c r="M64">
         <v>10</v>
@@ -11360,7 +11445,7 @@
         <v>39</v>
       </c>
       <c r="E70">
-        <v>300</v>
+        <v>200</v>
       </c>
       <c r="F70">
         <v>100</v>
@@ -12213,7 +12298,7 @@
         <v>314</v>
       </c>
       <c r="D78">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="E78">
         <v>130</v>
@@ -12222,7 +12307,7 @@
         <v>60</v>
       </c>
       <c r="G78">
-        <v>140</v>
+        <v>200</v>
       </c>
       <c r="H78">
         <v>110</v>
@@ -12252,7 +12337,7 @@
         <v>110</v>
       </c>
       <c r="Q78">
-        <v>95</v>
+        <v>110</v>
       </c>
       <c r="R78">
         <v>100</v>
@@ -12427,10 +12512,10 @@
         <v>320</v>
       </c>
       <c r="D80">
-        <v>61</v>
+        <v>48</v>
       </c>
       <c r="E80">
-        <v>100</v>
+        <v>150</v>
       </c>
       <c r="F80">
         <v>100</v>
@@ -12451,7 +12536,7 @@
         <v>100</v>
       </c>
       <c r="L80">
-        <v>100</v>
+        <v>120</v>
       </c>
       <c r="M80">
         <v>10</v>
@@ -12534,7 +12619,7 @@
         <v>324</v>
       </c>
       <c r="D81">
-        <v>41</v>
+        <v>34</v>
       </c>
       <c r="E81">
         <v>100</v>
@@ -12558,7 +12643,7 @@
         <v>100</v>
       </c>
       <c r="L81">
-        <v>100</v>
+        <v>110</v>
       </c>
       <c r="M81">
         <v>10</v>
@@ -14749,7 +14834,7 @@
         <v>41</v>
       </c>
       <c r="AC101" t="s">
-        <v>39</v>
+        <v>1167</v>
       </c>
       <c r="AD101" t="s">
         <v>115</v>
@@ -36178,7 +36263,7 @@
     </row>
     <row r="302" spans="1:36" x14ac:dyDescent="0.4">
       <c r="A302">
-        <v>4298</v>
+        <v>6000</v>
       </c>
       <c r="B302" t="s">
         <v>1096</v>
@@ -36288,7 +36373,7 @@
     </row>
     <row r="303" spans="1:36" x14ac:dyDescent="0.4">
       <c r="A303">
-        <v>4299</v>
+        <v>6001</v>
       </c>
       <c r="B303" t="s">
         <v>1105</v>
@@ -36395,7 +36480,7 @@
     </row>
     <row r="304" spans="1:36" x14ac:dyDescent="0.4">
       <c r="A304">
-        <v>4300</v>
+        <v>6002</v>
       </c>
       <c r="B304" t="s">
         <v>1106</v>
@@ -36505,7 +36590,7 @@
     </row>
     <row r="305" spans="1:36" x14ac:dyDescent="0.4">
       <c r="A305">
-        <v>4301</v>
+        <v>6003</v>
       </c>
       <c r="B305" t="s">
         <v>1126</v>
@@ -36547,10 +36632,10 @@
         <v>1</v>
       </c>
       <c r="O305">
-        <v>400</v>
+        <v>800</v>
       </c>
       <c r="P305">
-        <v>400</v>
+        <v>800</v>
       </c>
       <c r="Q305">
         <v>100</v>
@@ -36612,7 +36697,7 @@
     </row>
     <row r="306" spans="1:36" x14ac:dyDescent="0.4">
       <c r="A306">
-        <v>4302</v>
+        <v>6004</v>
       </c>
       <c r="B306" t="s">
         <v>1129</v>
@@ -36684,7 +36769,7 @@
         <v>1540</v>
       </c>
       <c r="Y306">
-        <v>432</v>
+        <v>576</v>
       </c>
       <c r="Z306">
         <v>720</v>
@@ -36719,7 +36804,7 @@
     </row>
     <row r="307" spans="1:36" x14ac:dyDescent="0.4">
       <c r="A307">
-        <v>4303</v>
+        <v>6005</v>
       </c>
       <c r="B307" t="s">
         <v>1139</v>
@@ -36728,7 +36813,7 @@
         <v>1140</v>
       </c>
       <c r="D307">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="E307">
         <v>100</v>
@@ -36825,6 +36910,969 @@
       </c>
       <c r="AJ307" t="s">
         <v>1138</v>
+      </c>
+    </row>
+    <row r="308" spans="1:36" x14ac:dyDescent="0.4">
+      <c r="A308">
+        <v>6006</v>
+      </c>
+      <c r="B308" t="s">
+        <v>1141</v>
+      </c>
+      <c r="C308" t="s">
+        <v>1144</v>
+      </c>
+      <c r="D308">
+        <v>31</v>
+      </c>
+      <c r="E308">
+        <v>100</v>
+      </c>
+      <c r="F308">
+        <v>100</v>
+      </c>
+      <c r="G308">
+        <v>100</v>
+      </c>
+      <c r="H308">
+        <v>100</v>
+      </c>
+      <c r="I308">
+        <v>100</v>
+      </c>
+      <c r="J308">
+        <v>100</v>
+      </c>
+      <c r="K308">
+        <v>100</v>
+      </c>
+      <c r="L308">
+        <v>100</v>
+      </c>
+      <c r="M308">
+        <v>10</v>
+      </c>
+      <c r="N308">
+        <v>1</v>
+      </c>
+      <c r="O308">
+        <v>100</v>
+      </c>
+      <c r="P308">
+        <v>100</v>
+      </c>
+      <c r="Q308">
+        <v>100</v>
+      </c>
+      <c r="R308">
+        <v>100</v>
+      </c>
+      <c r="S308">
+        <v>10</v>
+      </c>
+      <c r="T308">
+        <v>12</v>
+      </c>
+      <c r="U308" t="s">
+        <v>47</v>
+      </c>
+      <c r="V308" t="s">
+        <v>48</v>
+      </c>
+      <c r="W308" t="s">
+        <v>113</v>
+      </c>
+      <c r="X308">
+        <v>916</v>
+      </c>
+      <c r="Y308">
+        <v>576</v>
+      </c>
+      <c r="Z308">
+        <v>648</v>
+      </c>
+      <c r="AA308">
+        <v>250</v>
+      </c>
+      <c r="AB308" t="s">
+        <v>41</v>
+      </c>
+      <c r="AC308" t="s">
+        <v>48</v>
+      </c>
+      <c r="AD308" t="s">
+        <v>1123</v>
+      </c>
+      <c r="AE308">
+        <v>180</v>
+      </c>
+      <c r="AF308" t="s">
+        <v>1147</v>
+      </c>
+      <c r="AG308">
+        <v>0</v>
+      </c>
+      <c r="AH308">
+        <v>0.5</v>
+      </c>
+      <c r="AI308">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="309" spans="1:36" x14ac:dyDescent="0.4">
+      <c r="A309">
+        <v>6007</v>
+      </c>
+      <c r="B309" s="10" t="s">
+        <v>1142</v>
+      </c>
+      <c r="C309" t="s">
+        <v>1145</v>
+      </c>
+      <c r="D309">
+        <v>33</v>
+      </c>
+      <c r="E309">
+        <v>100</v>
+      </c>
+      <c r="F309">
+        <v>100</v>
+      </c>
+      <c r="G309">
+        <v>100</v>
+      </c>
+      <c r="H309">
+        <v>100</v>
+      </c>
+      <c r="I309">
+        <v>100</v>
+      </c>
+      <c r="J309">
+        <v>100</v>
+      </c>
+      <c r="K309">
+        <v>100</v>
+      </c>
+      <c r="L309">
+        <v>130</v>
+      </c>
+      <c r="M309">
+        <v>10</v>
+      </c>
+      <c r="N309">
+        <v>1</v>
+      </c>
+      <c r="O309">
+        <v>100</v>
+      </c>
+      <c r="P309">
+        <v>100</v>
+      </c>
+      <c r="Q309">
+        <v>100</v>
+      </c>
+      <c r="R309">
+        <v>100</v>
+      </c>
+      <c r="S309">
+        <v>10</v>
+      </c>
+      <c r="T309">
+        <v>12</v>
+      </c>
+      <c r="U309" t="s">
+        <v>47</v>
+      </c>
+      <c r="V309" t="s">
+        <v>48</v>
+      </c>
+      <c r="W309" t="s">
+        <v>113</v>
+      </c>
+      <c r="X309">
+        <v>1200</v>
+      </c>
+      <c r="Y309">
+        <v>576</v>
+      </c>
+      <c r="Z309">
+        <v>648</v>
+      </c>
+      <c r="AA309">
+        <v>160</v>
+      </c>
+      <c r="AB309" t="s">
+        <v>41</v>
+      </c>
+      <c r="AC309" t="s">
+        <v>48</v>
+      </c>
+      <c r="AD309" t="s">
+        <v>1123</v>
+      </c>
+      <c r="AE309">
+        <v>144</v>
+      </c>
+      <c r="AF309" t="s">
+        <v>1148</v>
+      </c>
+      <c r="AG309">
+        <v>0</v>
+      </c>
+      <c r="AH309">
+        <v>0.5</v>
+      </c>
+      <c r="AI309">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="310" spans="1:36" x14ac:dyDescent="0.4">
+      <c r="A310">
+        <v>6008</v>
+      </c>
+      <c r="B310" s="10" t="s">
+        <v>1143</v>
+      </c>
+      <c r="C310" t="s">
+        <v>1146</v>
+      </c>
+      <c r="D310">
+        <v>36</v>
+      </c>
+      <c r="E310">
+        <v>100</v>
+      </c>
+      <c r="F310">
+        <v>100</v>
+      </c>
+      <c r="G310">
+        <v>100</v>
+      </c>
+      <c r="H310">
+        <v>100</v>
+      </c>
+      <c r="I310">
+        <v>100</v>
+      </c>
+      <c r="J310">
+        <v>100</v>
+      </c>
+      <c r="K310">
+        <v>100</v>
+      </c>
+      <c r="L310">
+        <v>100</v>
+      </c>
+      <c r="M310">
+        <v>10</v>
+      </c>
+      <c r="N310">
+        <v>1</v>
+      </c>
+      <c r="O310">
+        <v>100</v>
+      </c>
+      <c r="P310">
+        <v>100</v>
+      </c>
+      <c r="Q310">
+        <v>110</v>
+      </c>
+      <c r="R310">
+        <v>100</v>
+      </c>
+      <c r="S310">
+        <v>10</v>
+      </c>
+      <c r="T310">
+        <v>12</v>
+      </c>
+      <c r="U310" t="s">
+        <v>47</v>
+      </c>
+      <c r="V310" t="s">
+        <v>48</v>
+      </c>
+      <c r="W310" t="s">
+        <v>113</v>
+      </c>
+      <c r="X310">
+        <v>800</v>
+      </c>
+      <c r="Y310">
+        <v>576</v>
+      </c>
+      <c r="Z310">
+        <v>648</v>
+      </c>
+      <c r="AA310">
+        <v>200</v>
+      </c>
+      <c r="AB310" t="s">
+        <v>41</v>
+      </c>
+      <c r="AC310" t="s">
+        <v>48</v>
+      </c>
+      <c r="AD310" t="s">
+        <v>1123</v>
+      </c>
+      <c r="AE310">
+        <v>144</v>
+      </c>
+      <c r="AF310" t="s">
+        <v>1149</v>
+      </c>
+      <c r="AG310">
+        <v>0</v>
+      </c>
+      <c r="AH310">
+        <v>0.5</v>
+      </c>
+      <c r="AI310">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="311" spans="1:36" x14ac:dyDescent="0.4">
+      <c r="A311">
+        <v>6009</v>
+      </c>
+      <c r="B311" t="s">
+        <v>1150</v>
+      </c>
+      <c r="C311" t="s">
+        <v>1153</v>
+      </c>
+      <c r="D311">
+        <v>18</v>
+      </c>
+      <c r="E311">
+        <v>100</v>
+      </c>
+      <c r="F311">
+        <v>100</v>
+      </c>
+      <c r="G311">
+        <v>100</v>
+      </c>
+      <c r="H311">
+        <v>100</v>
+      </c>
+      <c r="I311">
+        <v>100</v>
+      </c>
+      <c r="J311">
+        <v>100</v>
+      </c>
+      <c r="K311">
+        <v>100</v>
+      </c>
+      <c r="L311">
+        <v>150</v>
+      </c>
+      <c r="M311">
+        <v>10</v>
+      </c>
+      <c r="N311">
+        <v>1</v>
+      </c>
+      <c r="O311">
+        <v>100</v>
+      </c>
+      <c r="P311">
+        <v>100</v>
+      </c>
+      <c r="Q311">
+        <v>170</v>
+      </c>
+      <c r="R311">
+        <v>170</v>
+      </c>
+      <c r="S311">
+        <v>10</v>
+      </c>
+      <c r="T311">
+        <v>12</v>
+      </c>
+      <c r="U311" t="s">
+        <v>47</v>
+      </c>
+      <c r="V311" t="s">
+        <v>48</v>
+      </c>
+      <c r="W311" t="s">
+        <v>49</v>
+      </c>
+      <c r="X311">
+        <v>600</v>
+      </c>
+      <c r="Y311">
+        <v>384</v>
+      </c>
+      <c r="Z311">
+        <v>288</v>
+      </c>
+      <c r="AA311">
+        <v>160</v>
+      </c>
+      <c r="AB311" t="s">
+        <v>41</v>
+      </c>
+      <c r="AC311" t="s">
+        <v>48</v>
+      </c>
+      <c r="AD311" t="s">
+        <v>1121</v>
+      </c>
+      <c r="AE311">
+        <v>180</v>
+      </c>
+      <c r="AF311" t="s">
+        <v>1158</v>
+      </c>
+      <c r="AG311">
+        <v>0</v>
+      </c>
+      <c r="AH311">
+        <v>0.25</v>
+      </c>
+      <c r="AI311">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="312" spans="1:36" x14ac:dyDescent="0.4">
+      <c r="A312">
+        <v>6010</v>
+      </c>
+      <c r="B312" t="s">
+        <v>1151</v>
+      </c>
+      <c r="C312" t="s">
+        <v>1154</v>
+      </c>
+      <c r="D312">
+        <v>20</v>
+      </c>
+      <c r="E312">
+        <v>100</v>
+      </c>
+      <c r="F312">
+        <v>100</v>
+      </c>
+      <c r="G312">
+        <v>100</v>
+      </c>
+      <c r="H312">
+        <v>100</v>
+      </c>
+      <c r="I312">
+        <v>100</v>
+      </c>
+      <c r="J312">
+        <v>100</v>
+      </c>
+      <c r="K312">
+        <v>100</v>
+      </c>
+      <c r="L312">
+        <v>150</v>
+      </c>
+      <c r="M312">
+        <v>10</v>
+      </c>
+      <c r="N312">
+        <v>1</v>
+      </c>
+      <c r="O312">
+        <v>100</v>
+      </c>
+      <c r="P312">
+        <v>100</v>
+      </c>
+      <c r="Q312">
+        <v>170</v>
+      </c>
+      <c r="R312">
+        <v>170</v>
+      </c>
+      <c r="S312">
+        <v>10</v>
+      </c>
+      <c r="T312">
+        <v>12</v>
+      </c>
+      <c r="U312" t="s">
+        <v>47</v>
+      </c>
+      <c r="V312" t="s">
+        <v>48</v>
+      </c>
+      <c r="W312" t="s">
+        <v>49</v>
+      </c>
+      <c r="X312">
+        <v>600</v>
+      </c>
+      <c r="Y312">
+        <v>576</v>
+      </c>
+      <c r="Z312">
+        <v>288</v>
+      </c>
+      <c r="AA312">
+        <v>80</v>
+      </c>
+      <c r="AB312" t="s">
+        <v>41</v>
+      </c>
+      <c r="AC312" t="s">
+        <v>48</v>
+      </c>
+      <c r="AD312" t="s">
+        <v>1121</v>
+      </c>
+      <c r="AE312">
+        <v>144</v>
+      </c>
+      <c r="AF312" t="s">
+        <v>1159</v>
+      </c>
+      <c r="AG312">
+        <v>0</v>
+      </c>
+      <c r="AH312">
+        <v>0.25</v>
+      </c>
+      <c r="AI312">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="313" spans="1:36" x14ac:dyDescent="0.4">
+      <c r="A313">
+        <v>6011</v>
+      </c>
+      <c r="B313" t="s">
+        <v>1152</v>
+      </c>
+      <c r="C313" t="s">
+        <v>1155</v>
+      </c>
+      <c r="D313">
+        <v>22</v>
+      </c>
+      <c r="E313">
+        <v>100</v>
+      </c>
+      <c r="F313">
+        <v>100</v>
+      </c>
+      <c r="G313">
+        <v>100</v>
+      </c>
+      <c r="H313">
+        <v>100</v>
+      </c>
+      <c r="I313">
+        <v>100</v>
+      </c>
+      <c r="J313">
+        <v>100</v>
+      </c>
+      <c r="K313">
+        <v>100</v>
+      </c>
+      <c r="L313">
+        <v>150</v>
+      </c>
+      <c r="M313">
+        <v>10</v>
+      </c>
+      <c r="N313">
+        <v>1</v>
+      </c>
+      <c r="O313">
+        <v>100</v>
+      </c>
+      <c r="P313">
+        <v>100</v>
+      </c>
+      <c r="Q313">
+        <v>170</v>
+      </c>
+      <c r="R313">
+        <v>170</v>
+      </c>
+      <c r="S313">
+        <v>10</v>
+      </c>
+      <c r="T313">
+        <v>12</v>
+      </c>
+      <c r="U313" t="s">
+        <v>47</v>
+      </c>
+      <c r="V313" t="s">
+        <v>48</v>
+      </c>
+      <c r="W313" t="s">
+        <v>49</v>
+      </c>
+      <c r="X313">
+        <v>600</v>
+      </c>
+      <c r="Y313">
+        <v>576</v>
+      </c>
+      <c r="Z313">
+        <v>288</v>
+      </c>
+      <c r="AA313">
+        <v>140</v>
+      </c>
+      <c r="AB313" t="s">
+        <v>41</v>
+      </c>
+      <c r="AC313" t="s">
+        <v>48</v>
+      </c>
+      <c r="AD313" t="s">
+        <v>1121</v>
+      </c>
+      <c r="AE313">
+        <v>144</v>
+      </c>
+      <c r="AF313" t="s">
+        <v>1160</v>
+      </c>
+      <c r="AG313">
+        <v>0</v>
+      </c>
+      <c r="AH313">
+        <v>0.25</v>
+      </c>
+      <c r="AI313">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="314" spans="1:36" x14ac:dyDescent="0.4">
+      <c r="A314">
+        <v>6012</v>
+      </c>
+      <c r="B314" t="s">
+        <v>1156</v>
+      </c>
+      <c r="C314" t="s">
+        <v>1157</v>
+      </c>
+      <c r="D314">
+        <v>20</v>
+      </c>
+      <c r="E314">
+        <v>100</v>
+      </c>
+      <c r="F314">
+        <v>100</v>
+      </c>
+      <c r="G314">
+        <v>100</v>
+      </c>
+      <c r="H314">
+        <v>100</v>
+      </c>
+      <c r="I314">
+        <v>100</v>
+      </c>
+      <c r="J314">
+        <v>100</v>
+      </c>
+      <c r="K314">
+        <v>100</v>
+      </c>
+      <c r="L314">
+        <v>100</v>
+      </c>
+      <c r="M314">
+        <v>10</v>
+      </c>
+      <c r="N314">
+        <v>0</v>
+      </c>
+      <c r="O314">
+        <v>100</v>
+      </c>
+      <c r="P314">
+        <v>100</v>
+      </c>
+      <c r="Q314">
+        <v>170</v>
+      </c>
+      <c r="R314">
+        <v>170</v>
+      </c>
+      <c r="S314">
+        <v>10</v>
+      </c>
+      <c r="T314">
+        <v>12</v>
+      </c>
+      <c r="U314" t="s">
+        <v>47</v>
+      </c>
+      <c r="V314" t="s">
+        <v>140</v>
+      </c>
+      <c r="W314" t="s">
+        <v>54</v>
+      </c>
+      <c r="X314">
+        <v>1001</v>
+      </c>
+      <c r="Y314">
+        <v>1</v>
+      </c>
+      <c r="Z314">
+        <v>1</v>
+      </c>
+      <c r="AA314">
+        <v>1000</v>
+      </c>
+      <c r="AB314" t="s">
+        <v>41</v>
+      </c>
+      <c r="AC314" t="s">
+        <v>58</v>
+      </c>
+      <c r="AD314" t="s">
+        <v>59</v>
+      </c>
+      <c r="AE314">
+        <v>672</v>
+      </c>
+      <c r="AF314" t="s">
+        <v>334</v>
+      </c>
+      <c r="AG314">
+        <v>0</v>
+      </c>
+      <c r="AH314">
+        <v>-1</v>
+      </c>
+      <c r="AI314">
+        <v>1.05</v>
+      </c>
+    </row>
+    <row r="315" spans="1:36" x14ac:dyDescent="0.4">
+      <c r="A315">
+        <v>6013</v>
+      </c>
+      <c r="B315" t="s">
+        <v>1163</v>
+      </c>
+      <c r="C315" t="s">
+        <v>1165</v>
+      </c>
+      <c r="D315">
+        <v>36</v>
+      </c>
+      <c r="E315">
+        <v>100</v>
+      </c>
+      <c r="F315">
+        <v>100</v>
+      </c>
+      <c r="G315">
+        <v>100</v>
+      </c>
+      <c r="H315">
+        <v>80</v>
+      </c>
+      <c r="I315">
+        <v>110</v>
+      </c>
+      <c r="J315">
+        <v>110</v>
+      </c>
+      <c r="K315">
+        <v>100</v>
+      </c>
+      <c r="L315">
+        <v>100</v>
+      </c>
+      <c r="M315">
+        <v>10</v>
+      </c>
+      <c r="N315">
+        <v>1</v>
+      </c>
+      <c r="O315">
+        <v>70</v>
+      </c>
+      <c r="P315">
+        <v>70</v>
+      </c>
+      <c r="Q315">
+        <v>100</v>
+      </c>
+      <c r="R315">
+        <v>100</v>
+      </c>
+      <c r="S315">
+        <v>10</v>
+      </c>
+      <c r="T315">
+        <v>12</v>
+      </c>
+      <c r="U315" t="s">
+        <v>38</v>
+      </c>
+      <c r="V315" t="s">
+        <v>39</v>
+      </c>
+      <c r="W315" t="s">
+        <v>437</v>
+      </c>
+      <c r="X315">
+        <v>1472</v>
+      </c>
+      <c r="Y315">
+        <v>288</v>
+      </c>
+      <c r="Z315">
+        <v>672</v>
+      </c>
+      <c r="AA315">
+        <v>180</v>
+      </c>
+      <c r="AB315" t="s">
+        <v>41</v>
+      </c>
+      <c r="AC315" t="s">
+        <v>39</v>
+      </c>
+      <c r="AD315" t="s">
+        <v>99</v>
+      </c>
+      <c r="AE315">
+        <v>528</v>
+      </c>
+      <c r="AF315" t="s">
+        <v>1161</v>
+      </c>
+      <c r="AG315">
+        <v>0</v>
+      </c>
+      <c r="AH315">
+        <v>0.5</v>
+      </c>
+      <c r="AI315">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="316" spans="1:36" x14ac:dyDescent="0.4">
+      <c r="A316">
+        <v>6014</v>
+      </c>
+      <c r="B316" t="s">
+        <v>1164</v>
+      </c>
+      <c r="C316" t="s">
+        <v>1166</v>
+      </c>
+      <c r="D316">
+        <v>42</v>
+      </c>
+      <c r="E316">
+        <v>90</v>
+      </c>
+      <c r="F316">
+        <v>100</v>
+      </c>
+      <c r="G316">
+        <v>100</v>
+      </c>
+      <c r="H316">
+        <v>80</v>
+      </c>
+      <c r="I316">
+        <v>110</v>
+      </c>
+      <c r="J316">
+        <v>110</v>
+      </c>
+      <c r="K316">
+        <v>100</v>
+      </c>
+      <c r="L316">
+        <v>200</v>
+      </c>
+      <c r="M316">
+        <v>10</v>
+      </c>
+      <c r="N316">
+        <v>1</v>
+      </c>
+      <c r="O316">
+        <v>70</v>
+      </c>
+      <c r="P316">
+        <v>70</v>
+      </c>
+      <c r="Q316">
+        <v>125</v>
+      </c>
+      <c r="R316">
+        <v>125</v>
+      </c>
+      <c r="S316">
+        <v>10</v>
+      </c>
+      <c r="T316">
+        <v>12</v>
+      </c>
+      <c r="U316" t="s">
+        <v>38</v>
+      </c>
+      <c r="V316" t="s">
+        <v>39</v>
+      </c>
+      <c r="W316" t="s">
+        <v>1029</v>
+      </c>
+      <c r="X316">
+        <v>1272</v>
+      </c>
+      <c r="Y316">
+        <v>288</v>
+      </c>
+      <c r="Z316">
+        <v>672</v>
+      </c>
+      <c r="AA316">
+        <v>170</v>
+      </c>
+      <c r="AB316" t="s">
+        <v>41</v>
+      </c>
+      <c r="AC316" t="s">
+        <v>225</v>
+      </c>
+      <c r="AD316" t="s">
+        <v>99</v>
+      </c>
+      <c r="AE316">
+        <v>528</v>
+      </c>
+      <c r="AF316" t="s">
+        <v>1162</v>
+      </c>
+      <c r="AG316">
+        <v>0</v>
+      </c>
+      <c r="AH316">
+        <v>0.5</v>
+      </c>
+      <c r="AI316">
+        <v>1</v>
       </c>
     </row>
   </sheetData>
@@ -38932,11 +39980,11 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0E19C42E-4D03-4797-B846-FB5E09BB39D3}">
-  <dimension ref="A1:N27"/>
+  <dimension ref="A1:N28"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C26" sqref="C26"/>
+      <selection pane="bottomLeft" activeCell="F9" sqref="F9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
@@ -39298,43 +40346,43 @@
     </row>
     <row r="9" spans="1:14" x14ac:dyDescent="0.4">
       <c r="A9" t="s">
-        <v>176</v>
+        <v>1168</v>
       </c>
       <c r="B9">
-        <v>80</v>
+        <v>100</v>
       </c>
       <c r="C9">
-        <v>80</v>
+        <v>130</v>
       </c>
       <c r="D9">
-        <v>95</v>
+        <v>100</v>
       </c>
       <c r="E9">
         <v>80</v>
       </c>
       <c r="F9">
-        <v>100</v>
+        <v>110</v>
       </c>
       <c r="G9">
-        <v>100</v>
+        <v>110</v>
       </c>
       <c r="H9">
-        <v>120</v>
+        <v>90</v>
       </c>
       <c r="I9">
         <v>100</v>
       </c>
       <c r="J9">
-        <v>90</v>
+        <v>100</v>
       </c>
       <c r="K9">
-        <v>90</v>
+        <v>100</v>
       </c>
       <c r="L9">
-        <v>85</v>
+        <v>100</v>
       </c>
       <c r="M9">
-        <v>85</v>
+        <v>100</v>
       </c>
       <c r="N9">
         <v>1</v>
@@ -39342,25 +40390,25 @@
     </row>
     <row r="10" spans="1:14" x14ac:dyDescent="0.4">
       <c r="A10" t="s">
-        <v>1111</v>
+        <v>176</v>
       </c>
       <c r="B10">
-        <v>100</v>
+        <v>80</v>
       </c>
       <c r="C10">
-        <v>100</v>
+        <v>80</v>
       </c>
       <c r="D10">
-        <v>70</v>
+        <v>95</v>
       </c>
       <c r="E10">
         <v>80</v>
       </c>
       <c r="F10">
-        <v>90</v>
+        <v>100</v>
       </c>
       <c r="G10">
-        <v>150</v>
+        <v>100</v>
       </c>
       <c r="H10">
         <v>120</v>
@@ -39369,16 +40417,16 @@
         <v>100</v>
       </c>
       <c r="J10">
-        <v>80</v>
+        <v>90</v>
       </c>
       <c r="K10">
-        <v>200</v>
+        <v>90</v>
       </c>
       <c r="L10">
-        <v>105</v>
+        <v>85</v>
       </c>
       <c r="M10">
-        <v>115</v>
+        <v>85</v>
       </c>
       <c r="N10">
         <v>1</v>
@@ -39386,13 +40434,13 @@
     </row>
     <row r="11" spans="1:14" x14ac:dyDescent="0.4">
       <c r="A11" t="s">
-        <v>39</v>
+        <v>1111</v>
       </c>
       <c r="B11">
-        <v>110</v>
+        <v>100</v>
       </c>
       <c r="C11">
-        <v>90</v>
+        <v>100</v>
       </c>
       <c r="D11">
         <v>70</v>
@@ -39401,28 +40449,28 @@
         <v>80</v>
       </c>
       <c r="F11">
-        <v>112</v>
+        <v>90</v>
       </c>
       <c r="G11">
-        <v>100</v>
+        <v>150</v>
       </c>
       <c r="H11">
+        <v>120</v>
+      </c>
+      <c r="I11">
+        <v>100</v>
+      </c>
+      <c r="J11">
         <v>80</v>
       </c>
-      <c r="I11">
-        <v>100</v>
-      </c>
-      <c r="J11">
-        <v>120</v>
-      </c>
       <c r="K11">
-        <v>120</v>
+        <v>200</v>
       </c>
       <c r="L11">
-        <v>92</v>
+        <v>105</v>
       </c>
       <c r="M11">
-        <v>90</v>
+        <v>115</v>
       </c>
       <c r="N11">
         <v>1</v>
@@ -39430,43 +40478,43 @@
     </row>
     <row r="12" spans="1:14" x14ac:dyDescent="0.4">
       <c r="A12" t="s">
-        <v>48</v>
+        <v>39</v>
       </c>
       <c r="B12">
+        <v>110</v>
+      </c>
+      <c r="C12">
+        <v>90</v>
+      </c>
+      <c r="D12">
+        <v>70</v>
+      </c>
+      <c r="E12">
         <v>80</v>
       </c>
-      <c r="C12">
-        <v>105</v>
-      </c>
-      <c r="D12">
+      <c r="F12">
+        <v>112</v>
+      </c>
+      <c r="G12">
+        <v>100</v>
+      </c>
+      <c r="H12">
         <v>80</v>
       </c>
-      <c r="E12">
-        <v>130</v>
-      </c>
-      <c r="F12">
-        <v>85</v>
-      </c>
-      <c r="G12">
-        <v>85</v>
-      </c>
-      <c r="H12">
+      <c r="I12">
+        <v>100</v>
+      </c>
+      <c r="J12">
         <v>120</v>
       </c>
-      <c r="I12">
-        <v>72</v>
-      </c>
-      <c r="J12">
-        <v>110</v>
-      </c>
       <c r="K12">
+        <v>120</v>
+      </c>
+      <c r="L12">
+        <v>92</v>
+      </c>
+      <c r="M12">
         <v>90</v>
-      </c>
-      <c r="L12">
-        <v>94</v>
-      </c>
-      <c r="M12">
-        <v>106</v>
       </c>
       <c r="N12">
         <v>1</v>
@@ -39474,43 +40522,43 @@
     </row>
     <row r="13" spans="1:14" x14ac:dyDescent="0.4">
       <c r="A13" t="s">
-        <v>219</v>
+        <v>48</v>
       </c>
       <c r="B13">
-        <v>92</v>
+        <v>80</v>
       </c>
       <c r="C13">
+        <v>105</v>
+      </c>
+      <c r="D13">
+        <v>80</v>
+      </c>
+      <c r="E13">
+        <v>130</v>
+      </c>
+      <c r="F13">
+        <v>85</v>
+      </c>
+      <c r="G13">
+        <v>85</v>
+      </c>
+      <c r="H13">
+        <v>120</v>
+      </c>
+      <c r="I13">
+        <v>72</v>
+      </c>
+      <c r="J13">
         <v>110</v>
       </c>
-      <c r="D13">
-        <v>110</v>
-      </c>
-      <c r="E13">
-        <v>98</v>
-      </c>
-      <c r="F13">
+      <c r="K13">
         <v>90</v>
       </c>
-      <c r="G13">
-        <v>120</v>
-      </c>
-      <c r="H13">
-        <v>102</v>
-      </c>
-      <c r="I13">
-        <v>95</v>
-      </c>
-      <c r="J13">
-        <v>95</v>
-      </c>
-      <c r="K13">
-        <v>95</v>
-      </c>
       <c r="L13">
-        <v>105</v>
+        <v>94</v>
       </c>
       <c r="M13">
-        <v>95</v>
+        <v>106</v>
       </c>
       <c r="N13">
         <v>1</v>
@@ -39518,43 +40566,43 @@
     </row>
     <row r="14" spans="1:14" x14ac:dyDescent="0.4">
       <c r="A14" t="s">
-        <v>547</v>
+        <v>219</v>
       </c>
       <c r="B14">
-        <v>60</v>
+        <v>92</v>
       </c>
       <c r="C14">
-        <v>100</v>
+        <v>110</v>
       </c>
       <c r="D14">
-        <v>60</v>
+        <v>110</v>
       </c>
       <c r="E14">
+        <v>98</v>
+      </c>
+      <c r="F14">
+        <v>90</v>
+      </c>
+      <c r="G14">
         <v>120</v>
       </c>
-      <c r="F14">
-        <v>50</v>
-      </c>
-      <c r="G14">
-        <v>150</v>
-      </c>
       <c r="H14">
-        <v>130</v>
+        <v>102</v>
       </c>
       <c r="I14">
-        <v>60</v>
+        <v>95</v>
       </c>
       <c r="J14">
-        <v>50</v>
+        <v>95</v>
       </c>
       <c r="K14">
-        <v>130</v>
+        <v>95</v>
       </c>
       <c r="L14">
-        <v>100</v>
+        <v>105</v>
       </c>
       <c r="M14">
-        <v>100</v>
+        <v>95</v>
       </c>
       <c r="N14">
         <v>1</v>
@@ -39562,43 +40610,43 @@
     </row>
     <row r="15" spans="1:14" x14ac:dyDescent="0.4">
       <c r="A15" t="s">
-        <v>469</v>
+        <v>547</v>
       </c>
       <c r="B15">
-        <v>115</v>
+        <v>60</v>
       </c>
       <c r="C15">
-        <v>90</v>
+        <v>100</v>
       </c>
       <c r="D15">
-        <v>70</v>
+        <v>60</v>
       </c>
       <c r="E15">
-        <v>90</v>
+        <v>120</v>
       </c>
       <c r="F15">
+        <v>50</v>
+      </c>
+      <c r="G15">
+        <v>150</v>
+      </c>
+      <c r="H15">
+        <v>130</v>
+      </c>
+      <c r="I15">
         <v>60</v>
       </c>
-      <c r="G15">
-        <v>90</v>
-      </c>
-      <c r="H15">
-        <v>100</v>
-      </c>
-      <c r="I15">
-        <v>0</v>
-      </c>
       <c r="J15">
-        <v>70</v>
+        <v>50</v>
       </c>
       <c r="K15">
-        <v>110</v>
+        <v>130</v>
       </c>
       <c r="L15">
-        <v>90</v>
+        <v>100</v>
       </c>
       <c r="M15">
-        <v>85</v>
+        <v>100</v>
       </c>
       <c r="N15">
         <v>1</v>
@@ -39606,43 +40654,43 @@
     </row>
     <row r="16" spans="1:14" x14ac:dyDescent="0.4">
       <c r="A16" t="s">
-        <v>229</v>
+        <v>469</v>
       </c>
       <c r="B16">
-        <v>105</v>
+        <v>115</v>
       </c>
       <c r="C16">
-        <v>120</v>
+        <v>90</v>
       </c>
       <c r="D16">
+        <v>70</v>
+      </c>
+      <c r="E16">
         <v>90</v>
       </c>
-      <c r="E16">
-        <v>100</v>
-      </c>
       <c r="F16">
-        <v>110</v>
+        <v>60</v>
       </c>
       <c r="G16">
-        <v>130</v>
+        <v>90</v>
       </c>
       <c r="H16">
-        <v>110</v>
+        <v>100</v>
       </c>
       <c r="I16">
-        <v>130</v>
+        <v>0</v>
       </c>
       <c r="J16">
-        <v>90</v>
+        <v>70</v>
       </c>
       <c r="K16">
         <v>110</v>
       </c>
       <c r="L16">
-        <v>105</v>
+        <v>90</v>
       </c>
       <c r="M16">
-        <v>110</v>
+        <v>85</v>
       </c>
       <c r="N16">
         <v>1</v>
@@ -39650,43 +40698,43 @@
     </row>
     <row r="17" spans="1:14" x14ac:dyDescent="0.4">
       <c r="A17" t="s">
-        <v>275</v>
+        <v>229</v>
       </c>
       <c r="B17">
         <v>105</v>
       </c>
       <c r="C17">
+        <v>120</v>
+      </c>
+      <c r="D17">
+        <v>90</v>
+      </c>
+      <c r="E17">
+        <v>100</v>
+      </c>
+      <c r="F17">
         <v>110</v>
       </c>
-      <c r="D17">
+      <c r="G17">
         <v>130</v>
       </c>
-      <c r="E17">
-        <v>100</v>
-      </c>
-      <c r="F17">
-        <v>120</v>
-      </c>
-      <c r="G17">
-        <v>70</v>
-      </c>
       <c r="H17">
+        <v>110</v>
+      </c>
+      <c r="I17">
+        <v>130</v>
+      </c>
+      <c r="J17">
         <v>90</v>
       </c>
-      <c r="I17">
-        <v>80</v>
-      </c>
-      <c r="J17">
-        <v>80</v>
-      </c>
       <c r="K17">
-        <v>80</v>
+        <v>110</v>
       </c>
       <c r="L17">
         <v>105</v>
       </c>
       <c r="M17">
-        <v>95</v>
+        <v>110</v>
       </c>
       <c r="N17">
         <v>1</v>
@@ -39694,43 +40742,43 @@
     </row>
     <row r="18" spans="1:14" x14ac:dyDescent="0.4">
       <c r="A18" t="s">
-        <v>379</v>
+        <v>275</v>
       </c>
       <c r="B18">
         <v>105</v>
       </c>
       <c r="C18">
+        <v>110</v>
+      </c>
+      <c r="D18">
+        <v>130</v>
+      </c>
+      <c r="E18">
+        <v>100</v>
+      </c>
+      <c r="F18">
         <v>120</v>
       </c>
-      <c r="D18">
-        <v>120</v>
-      </c>
-      <c r="E18">
-        <v>110</v>
-      </c>
-      <c r="F18">
-        <v>110</v>
-      </c>
       <c r="G18">
+        <v>70</v>
+      </c>
+      <c r="H18">
         <v>90</v>
       </c>
-      <c r="H18">
-        <v>100</v>
-      </c>
       <c r="I18">
-        <v>100</v>
+        <v>80</v>
       </c>
       <c r="J18">
-        <v>100</v>
+        <v>80</v>
       </c>
       <c r="K18">
-        <v>100</v>
+        <v>80</v>
       </c>
       <c r="L18">
-        <v>110</v>
+        <v>105</v>
       </c>
       <c r="M18">
-        <v>105</v>
+        <v>95</v>
       </c>
       <c r="N18">
         <v>1</v>
@@ -39738,43 +40786,43 @@
     </row>
     <row r="19" spans="1:14" x14ac:dyDescent="0.4">
       <c r="A19" t="s">
-        <v>828</v>
+        <v>379</v>
       </c>
       <c r="B19">
-        <v>110</v>
+        <v>105</v>
       </c>
       <c r="C19">
         <v>120</v>
       </c>
       <c r="D19">
+        <v>120</v>
+      </c>
+      <c r="E19">
         <v>110</v>
       </c>
-      <c r="E19">
-        <v>70</v>
-      </c>
       <c r="F19">
-        <v>130</v>
+        <v>110</v>
       </c>
       <c r="G19">
         <v>90</v>
       </c>
       <c r="H19">
-        <v>90</v>
+        <v>100</v>
       </c>
       <c r="I19">
-        <v>90</v>
+        <v>100</v>
       </c>
       <c r="J19">
-        <v>150</v>
+        <v>100</v>
       </c>
       <c r="K19">
-        <v>110</v>
+        <v>100</v>
       </c>
       <c r="L19">
         <v>110</v>
       </c>
       <c r="M19">
-        <v>110</v>
+        <v>105</v>
       </c>
       <c r="N19">
         <v>1</v>
@@ -39782,25 +40830,25 @@
     </row>
     <row r="20" spans="1:14" x14ac:dyDescent="0.4">
       <c r="A20" t="s">
-        <v>327</v>
+        <v>828</v>
       </c>
       <c r="B20">
+        <v>110</v>
+      </c>
+      <c r="C20">
+        <v>120</v>
+      </c>
+      <c r="D20">
+        <v>110</v>
+      </c>
+      <c r="E20">
+        <v>70</v>
+      </c>
+      <c r="F20">
         <v>130</v>
       </c>
-      <c r="C20">
-        <v>110</v>
-      </c>
-      <c r="D20">
-        <v>120</v>
-      </c>
-      <c r="E20">
-        <v>60</v>
-      </c>
-      <c r="F20">
-        <v>150</v>
-      </c>
       <c r="G20">
-        <v>80</v>
+        <v>90</v>
       </c>
       <c r="H20">
         <v>90</v>
@@ -39812,13 +40860,13 @@
         <v>150</v>
       </c>
       <c r="K20">
-        <v>105</v>
+        <v>110</v>
       </c>
       <c r="L20">
         <v>110</v>
       </c>
       <c r="M20">
-        <v>120</v>
+        <v>110</v>
       </c>
       <c r="N20">
         <v>1</v>
@@ -39826,43 +40874,43 @@
     </row>
     <row r="21" spans="1:14" x14ac:dyDescent="0.4">
       <c r="A21" t="s">
-        <v>286</v>
+        <v>327</v>
       </c>
       <c r="B21">
         <v>130</v>
       </c>
       <c r="C21">
-        <v>130</v>
+        <v>110</v>
       </c>
       <c r="D21">
-        <v>110</v>
+        <v>120</v>
       </c>
       <c r="E21">
-        <v>100</v>
+        <v>60</v>
       </c>
       <c r="F21">
-        <v>110</v>
+        <v>150</v>
       </c>
       <c r="G21">
-        <v>95</v>
+        <v>80</v>
       </c>
       <c r="H21">
-        <v>100</v>
+        <v>90</v>
       </c>
       <c r="I21">
-        <v>100</v>
+        <v>90</v>
       </c>
       <c r="J21">
+        <v>150</v>
+      </c>
+      <c r="K21">
         <v>105</v>
-      </c>
-      <c r="K21">
-        <v>95</v>
       </c>
       <c r="L21">
         <v>110</v>
       </c>
       <c r="M21">
-        <v>110</v>
+        <v>120</v>
       </c>
       <c r="N21">
         <v>1</v>
@@ -39870,10 +40918,10 @@
     </row>
     <row r="22" spans="1:14" x14ac:dyDescent="0.4">
       <c r="A22" t="s">
-        <v>456</v>
+        <v>286</v>
       </c>
       <c r="B22">
-        <v>150</v>
+        <v>130</v>
       </c>
       <c r="C22">
         <v>130</v>
@@ -39882,75 +40930,75 @@
         <v>110</v>
       </c>
       <c r="E22">
-        <v>110</v>
+        <v>100</v>
       </c>
       <c r="F22">
         <v>110</v>
       </c>
       <c r="G22">
+        <v>95</v>
+      </c>
+      <c r="H22">
+        <v>100</v>
+      </c>
+      <c r="I22">
+        <v>100</v>
+      </c>
+      <c r="J22">
+        <v>105</v>
+      </c>
+      <c r="K22">
+        <v>95</v>
+      </c>
+      <c r="L22">
         <v>110</v>
       </c>
-      <c r="H22">
+      <c r="M22">
         <v>110</v>
       </c>
-      <c r="I22">
-        <v>110</v>
-      </c>
-      <c r="J22">
-        <v>110</v>
-      </c>
-      <c r="K22">
-        <v>110</v>
-      </c>
-      <c r="L22">
-        <v>120</v>
-      </c>
-      <c r="M22">
-        <v>135</v>
-      </c>
       <c r="N22">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="23" spans="1:14" x14ac:dyDescent="0.4">
       <c r="A23" t="s">
-        <v>181</v>
+        <v>456</v>
       </c>
       <c r="B23">
-        <v>200</v>
+        <v>150</v>
       </c>
       <c r="C23">
-        <v>150</v>
+        <v>130</v>
       </c>
       <c r="D23">
+        <v>110</v>
+      </c>
+      <c r="E23">
+        <v>110</v>
+      </c>
+      <c r="F23">
+        <v>110</v>
+      </c>
+      <c r="G23">
+        <v>110</v>
+      </c>
+      <c r="H23">
+        <v>110</v>
+      </c>
+      <c r="I23">
+        <v>110</v>
+      </c>
+      <c r="J23">
+        <v>110</v>
+      </c>
+      <c r="K23">
+        <v>110</v>
+      </c>
+      <c r="L23">
         <v>120</v>
       </c>
-      <c r="E23">
-        <v>120</v>
-      </c>
-      <c r="F23">
-        <v>120</v>
-      </c>
-      <c r="G23">
-        <v>120</v>
-      </c>
-      <c r="H23">
-        <v>120</v>
-      </c>
-      <c r="I23">
-        <v>120</v>
-      </c>
-      <c r="J23">
-        <v>120</v>
-      </c>
-      <c r="K23">
-        <v>120</v>
-      </c>
-      <c r="L23">
-        <v>140</v>
-      </c>
       <c r="M23">
-        <v>50</v>
+        <v>135</v>
       </c>
       <c r="N23">
         <v>2</v>
@@ -39958,75 +41006,75 @@
     </row>
     <row r="24" spans="1:14" x14ac:dyDescent="0.4">
       <c r="A24" t="s">
-        <v>753</v>
+        <v>181</v>
       </c>
       <c r="B24">
-        <v>240</v>
+        <v>200</v>
       </c>
       <c r="C24">
-        <v>170</v>
+        <v>150</v>
       </c>
       <c r="D24">
-        <v>130</v>
+        <v>120</v>
       </c>
       <c r="E24">
-        <v>130</v>
+        <v>120</v>
       </c>
       <c r="F24">
-        <v>130</v>
+        <v>120</v>
       </c>
       <c r="G24">
-        <v>130</v>
+        <v>120</v>
       </c>
       <c r="H24">
-        <v>130</v>
+        <v>120</v>
       </c>
       <c r="I24">
-        <v>130</v>
+        <v>120</v>
       </c>
       <c r="J24">
-        <v>130</v>
+        <v>120</v>
       </c>
       <c r="K24">
-        <v>130</v>
+        <v>120</v>
       </c>
       <c r="L24">
-        <v>160</v>
+        <v>140</v>
       </c>
       <c r="M24">
-        <v>150</v>
+        <v>50</v>
       </c>
       <c r="N24">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="25" spans="1:14" x14ac:dyDescent="0.4">
       <c r="A25" t="s">
-        <v>192</v>
+        <v>753</v>
       </c>
       <c r="B25">
-        <v>600</v>
+        <v>240</v>
       </c>
       <c r="C25">
-        <v>180</v>
+        <v>170</v>
       </c>
       <c r="D25">
-        <v>140</v>
+        <v>130</v>
       </c>
       <c r="E25">
-        <v>140</v>
+        <v>130</v>
       </c>
       <c r="F25">
-        <v>140</v>
+        <v>130</v>
       </c>
       <c r="G25">
-        <v>140</v>
+        <v>130</v>
       </c>
       <c r="H25">
-        <v>140</v>
+        <v>130</v>
       </c>
       <c r="I25">
-        <v>140</v>
+        <v>130</v>
       </c>
       <c r="J25">
         <v>130</v>
@@ -40035,65 +41083,65 @@
         <v>130</v>
       </c>
       <c r="L25">
-        <v>300</v>
+        <v>160</v>
       </c>
       <c r="M25">
-        <v>300</v>
+        <v>150</v>
       </c>
       <c r="N25">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="26" spans="1:14" x14ac:dyDescent="0.4">
       <c r="A26" t="s">
-        <v>681</v>
+        <v>192</v>
       </c>
       <c r="B26">
-        <v>1400</v>
+        <v>600</v>
       </c>
       <c r="C26">
-        <v>200</v>
+        <v>180</v>
       </c>
       <c r="D26">
-        <v>180</v>
+        <v>140</v>
       </c>
       <c r="E26">
-        <v>180</v>
+        <v>140</v>
       </c>
       <c r="F26">
-        <v>180</v>
+        <v>140</v>
       </c>
       <c r="G26">
-        <v>180</v>
+        <v>140</v>
       </c>
       <c r="H26">
-        <v>180</v>
+        <v>140</v>
       </c>
       <c r="I26">
-        <v>180</v>
+        <v>140</v>
       </c>
       <c r="J26">
-        <v>140</v>
+        <v>130</v>
       </c>
       <c r="K26">
-        <v>140</v>
+        <v>130</v>
       </c>
       <c r="L26">
-        <v>600</v>
+        <v>300</v>
       </c>
       <c r="M26">
-        <v>800</v>
+        <v>300</v>
       </c>
       <c r="N26">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="27" spans="1:14" x14ac:dyDescent="0.4">
       <c r="A27" t="s">
-        <v>1134</v>
+        <v>681</v>
       </c>
       <c r="B27">
-        <v>3200</v>
+        <v>1400</v>
       </c>
       <c r="C27">
         <v>200</v>
@@ -40123,12 +41171,56 @@
         <v>140</v>
       </c>
       <c r="L27">
+        <v>600</v>
+      </c>
+      <c r="M27">
+        <v>800</v>
+      </c>
+      <c r="N27">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="28" spans="1:14" x14ac:dyDescent="0.4">
+      <c r="A28" t="s">
+        <v>1134</v>
+      </c>
+      <c r="B28">
+        <v>3200</v>
+      </c>
+      <c r="C28">
+        <v>200</v>
+      </c>
+      <c r="D28">
+        <v>180</v>
+      </c>
+      <c r="E28">
+        <v>180</v>
+      </c>
+      <c r="F28">
+        <v>180</v>
+      </c>
+      <c r="G28">
+        <v>180</v>
+      </c>
+      <c r="H28">
+        <v>180</v>
+      </c>
+      <c r="I28">
+        <v>180</v>
+      </c>
+      <c r="J28">
+        <v>140</v>
+      </c>
+      <c r="K28">
+        <v>140</v>
+      </c>
+      <c r="L28">
         <v>1000</v>
       </c>
-      <c r="M27">
+      <c r="M28">
         <v>120</v>
       </c>
-      <c r="N27">
+      <c r="N28">
         <v>5</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Updating project setup to create temporary sprites for custom mobs. Plus sprite sorting fix and some balance adjustments.
</commit_message>
<xml_diff>
--- a/Other/RoStatProcessing.xlsx
+++ b/Other/RoStatProcessing.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\ProjectsSSD\RagnarokRebuildTcp\Other\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0E69EE0D-C875-4046-8939-54A83C8138F4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5951A205-3029-4AC8-97F3-B0B6ABA187BE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="2606" yWindow="2606" windowWidth="28345" windowHeight="14785" xr2:uid="{1C41742B-2950-4FF8-AA39-6557869B44EA}"/>
   </bookViews>
@@ -4017,10 +4017,10 @@
   <dimension ref="A1:AJ316"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <pane xSplit="4" ySplit="1" topLeftCell="E283" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="4" ySplit="1" topLeftCell="E41" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="E1" sqref="E1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="D303" sqref="D303"/>
+      <selection pane="bottomRight" activeCell="O62" sqref="O62"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
@@ -10506,34 +10506,34 @@
         <v>100</v>
       </c>
       <c r="H61">
-        <v>100</v>
+        <v>150</v>
       </c>
       <c r="I61">
-        <v>100</v>
+        <v>80</v>
       </c>
       <c r="J61">
-        <v>100</v>
+        <v>80</v>
       </c>
       <c r="K61">
         <v>100</v>
       </c>
       <c r="L61">
-        <v>100</v>
+        <v>150</v>
       </c>
       <c r="M61">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="N61">
         <v>1</v>
       </c>
       <c r="O61">
-        <v>100</v>
+        <v>130</v>
       </c>
       <c r="P61">
-        <v>100</v>
+        <v>30</v>
       </c>
       <c r="Q61">
-        <v>100</v>
+        <v>130</v>
       </c>
       <c r="R61">
         <v>100</v>
@@ -11163,7 +11163,7 @@
         <v>100</v>
       </c>
       <c r="M67">
-        <v>10</v>
+        <v>15</v>
       </c>
       <c r="N67">
         <v>1</v>
@@ -12551,10 +12551,10 @@
         <v>100</v>
       </c>
       <c r="L80">
-        <v>100</v>
+        <v>110</v>
       </c>
       <c r="M80">
-        <v>10</v>
+        <v>18</v>
       </c>
       <c r="N80">
         <v>1</v>
@@ -12661,7 +12661,7 @@
         <v>110</v>
       </c>
       <c r="M81">
-        <v>10</v>
+        <v>15</v>
       </c>
       <c r="N81">
         <v>2</v>
@@ -20365,7 +20365,7 @@
         <v>100</v>
       </c>
       <c r="M153">
-        <v>10</v>
+        <v>15</v>
       </c>
       <c r="N153">
         <v>1</v>
@@ -20472,7 +20472,7 @@
         <v>80</v>
       </c>
       <c r="M154">
-        <v>10</v>
+        <v>20</v>
       </c>
       <c r="N154">
         <v>1</v>
@@ -22291,7 +22291,7 @@
         <v>100</v>
       </c>
       <c r="M171">
-        <v>10</v>
+        <v>15</v>
       </c>
       <c r="N171">
         <v>2</v>
@@ -22398,7 +22398,7 @@
         <v>100</v>
       </c>
       <c r="M172">
-        <v>10</v>
+        <v>15</v>
       </c>
       <c r="N172">
         <v>1</v>
@@ -24538,7 +24538,7 @@
         <v>100</v>
       </c>
       <c r="M192">
-        <v>10</v>
+        <v>20</v>
       </c>
       <c r="N192">
         <v>1</v>
@@ -24645,7 +24645,7 @@
         <v>100</v>
       </c>
       <c r="M193">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="N193">
         <v>1</v>
@@ -24752,7 +24752,7 @@
         <v>100</v>
       </c>
       <c r="M194">
-        <v>5</v>
+        <v>14</v>
       </c>
       <c r="N194">
         <v>1</v>
@@ -24859,7 +24859,7 @@
         <v>100</v>
       </c>
       <c r="M195">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="N195">
         <v>1</v>
@@ -24966,7 +24966,7 @@
         <v>100</v>
       </c>
       <c r="M196">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="N196">
         <v>1</v>
@@ -25073,7 +25073,7 @@
         <v>100</v>
       </c>
       <c r="M197">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="N197">
         <v>1</v>
@@ -25180,7 +25180,7 @@
         <v>100</v>
       </c>
       <c r="M198">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="N198">
         <v>1</v>
@@ -25287,7 +25287,7 @@
         <v>100</v>
       </c>
       <c r="M199">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="N199">
         <v>1</v>
@@ -25394,7 +25394,7 @@
         <v>100</v>
       </c>
       <c r="M200">
-        <v>5</v>
+        <v>15</v>
       </c>
       <c r="N200">
         <v>2</v>
@@ -25501,7 +25501,7 @@
         <v>100</v>
       </c>
       <c r="M201">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="N201">
         <v>1</v>
@@ -25715,7 +25715,7 @@
         <v>100</v>
       </c>
       <c r="M203">
-        <v>5</v>
+        <v>15</v>
       </c>
       <c r="N203">
         <v>1</v>
@@ -25822,7 +25822,7 @@
         <v>100</v>
       </c>
       <c r="M204">
-        <v>5</v>
+        <v>15</v>
       </c>
       <c r="N204">
         <v>1</v>
@@ -25929,7 +25929,7 @@
         <v>100</v>
       </c>
       <c r="M205">
-        <v>5</v>
+        <v>15</v>
       </c>
       <c r="N205">
         <v>1</v>
@@ -26036,7 +26036,7 @@
         <v>100</v>
       </c>
       <c r="M206">
-        <v>5</v>
+        <v>15</v>
       </c>
       <c r="N206">
         <v>1</v>
@@ -26143,7 +26143,7 @@
         <v>80</v>
       </c>
       <c r="M207">
-        <v>5</v>
+        <v>15</v>
       </c>
       <c r="N207">
         <v>1</v>
@@ -26250,7 +26250,7 @@
         <v>100</v>
       </c>
       <c r="M208">
-        <v>5</v>
+        <v>15</v>
       </c>
       <c r="N208">
         <v>1</v>
@@ -26357,7 +26357,7 @@
         <v>120</v>
       </c>
       <c r="M209">
-        <v>5</v>
+        <v>15</v>
       </c>
       <c r="N209">
         <v>1</v>
@@ -26464,7 +26464,7 @@
         <v>70</v>
       </c>
       <c r="M210">
-        <v>5</v>
+        <v>15</v>
       </c>
       <c r="N210">
         <v>1</v>
@@ -26571,7 +26571,7 @@
         <v>100</v>
       </c>
       <c r="M211">
-        <v>5</v>
+        <v>15</v>
       </c>
       <c r="N211">
         <v>1</v>
@@ -26678,7 +26678,7 @@
         <v>100</v>
       </c>
       <c r="M212">
-        <v>5</v>
+        <v>15</v>
       </c>
       <c r="N212">
         <v>9</v>
@@ -26785,7 +26785,7 @@
         <v>100</v>
       </c>
       <c r="M213">
-        <v>5</v>
+        <v>15</v>
       </c>
       <c r="N213">
         <v>1</v>
@@ -26892,7 +26892,7 @@
         <v>100</v>
       </c>
       <c r="M214">
-        <v>5</v>
+        <v>15</v>
       </c>
       <c r="N214">
         <v>1</v>
@@ -26999,7 +26999,7 @@
         <v>100</v>
       </c>
       <c r="M215">
-        <v>5</v>
+        <v>20</v>
       </c>
       <c r="N215">
         <v>1</v>
@@ -27106,7 +27106,7 @@
         <v>100</v>
       </c>
       <c r="M216">
-        <v>5</v>
+        <v>15</v>
       </c>
       <c r="N216">
         <v>1</v>
@@ -27213,7 +27213,7 @@
         <v>100</v>
       </c>
       <c r="M217">
-        <v>5</v>
+        <v>15</v>
       </c>
       <c r="N217">
         <v>1</v>
@@ -27320,7 +27320,7 @@
         <v>100</v>
       </c>
       <c r="M218">
-        <v>5</v>
+        <v>20</v>
       </c>
       <c r="N218">
         <v>2</v>
@@ -27427,7 +27427,7 @@
         <v>110</v>
       </c>
       <c r="M219">
-        <v>10</v>
+        <v>20</v>
       </c>
       <c r="N219">
         <v>2</v>
@@ -27534,7 +27534,7 @@
         <v>120</v>
       </c>
       <c r="M220">
-        <v>5</v>
+        <v>15</v>
       </c>
       <c r="N220">
         <v>1</v>
@@ -27641,7 +27641,7 @@
         <v>100</v>
       </c>
       <c r="M221">
-        <v>5</v>
+        <v>15</v>
       </c>
       <c r="N221">
         <v>1</v>
@@ -27748,7 +27748,7 @@
         <v>110</v>
       </c>
       <c r="M222">
-        <v>5</v>
+        <v>15</v>
       </c>
       <c r="N222">
         <v>1</v>
@@ -27855,7 +27855,7 @@
         <v>100</v>
       </c>
       <c r="M223">
-        <v>5</v>
+        <v>15</v>
       </c>
       <c r="N223">
         <v>1</v>
@@ -27962,7 +27962,7 @@
         <v>100</v>
       </c>
       <c r="M224">
-        <v>5</v>
+        <v>15</v>
       </c>
       <c r="N224">
         <v>9</v>
@@ -28069,7 +28069,7 @@
         <v>100</v>
       </c>
       <c r="M225">
-        <v>5</v>
+        <v>15</v>
       </c>
       <c r="N225">
         <v>3</v>
@@ -28176,7 +28176,7 @@
         <v>110</v>
       </c>
       <c r="M226">
-        <v>10</v>
+        <v>15</v>
       </c>
       <c r="N226">
         <v>1</v>
@@ -28283,7 +28283,7 @@
         <v>105</v>
       </c>
       <c r="M227">
-        <v>10</v>
+        <v>15</v>
       </c>
       <c r="N227">
         <v>1</v>
@@ -28390,7 +28390,7 @@
         <v>100</v>
       </c>
       <c r="M228">
-        <v>10</v>
+        <v>20</v>
       </c>
       <c r="N228">
         <v>1</v>
@@ -28604,7 +28604,7 @@
         <v>100</v>
       </c>
       <c r="M230">
-        <v>5</v>
+        <v>15</v>
       </c>
       <c r="N230">
         <v>1</v>
@@ -28711,7 +28711,7 @@
         <v>100</v>
       </c>
       <c r="M231">
-        <v>5</v>
+        <v>15</v>
       </c>
       <c r="N231">
         <v>2</v>
@@ -28818,7 +28818,7 @@
         <v>110</v>
       </c>
       <c r="M232">
-        <v>5</v>
+        <v>15</v>
       </c>
       <c r="N232">
         <v>1</v>
@@ -28925,7 +28925,7 @@
         <v>100</v>
       </c>
       <c r="M233">
-        <v>5</v>
+        <v>15</v>
       </c>
       <c r="N233">
         <v>1</v>
@@ -29032,7 +29032,7 @@
         <v>115</v>
       </c>
       <c r="M234">
-        <v>5</v>
+        <v>15</v>
       </c>
       <c r="N234">
         <v>1</v>
@@ -29139,7 +29139,7 @@
         <v>100</v>
       </c>
       <c r="M235">
-        <v>5</v>
+        <v>15</v>
       </c>
       <c r="N235">
         <v>1</v>
@@ -29246,7 +29246,7 @@
         <v>100</v>
       </c>
       <c r="M236">
-        <v>5</v>
+        <v>15</v>
       </c>
       <c r="N236">
         <v>1</v>
@@ -29353,7 +29353,7 @@
         <v>100</v>
       </c>
       <c r="M237">
-        <v>5</v>
+        <v>15</v>
       </c>
       <c r="N237">
         <v>1</v>
@@ -29460,7 +29460,7 @@
         <v>80</v>
       </c>
       <c r="M238">
-        <v>5</v>
+        <v>15</v>
       </c>
       <c r="N238">
         <v>2</v>
@@ -29567,7 +29567,7 @@
         <v>100</v>
       </c>
       <c r="M239">
-        <v>5</v>
+        <v>15</v>
       </c>
       <c r="N239">
         <v>2</v>
@@ -29674,7 +29674,7 @@
         <v>100</v>
       </c>
       <c r="M240">
-        <v>5</v>
+        <v>15</v>
       </c>
       <c r="N240">
         <v>2</v>
@@ -29781,7 +29781,7 @@
         <v>100</v>
       </c>
       <c r="M241">
-        <v>5</v>
+        <v>15</v>
       </c>
       <c r="N241">
         <v>2</v>
@@ -29888,7 +29888,7 @@
         <v>120</v>
       </c>
       <c r="M242">
-        <v>5</v>
+        <v>15</v>
       </c>
       <c r="N242">
         <v>2</v>
@@ -29995,7 +29995,7 @@
         <v>100</v>
       </c>
       <c r="M243">
-        <v>5</v>
+        <v>20</v>
       </c>
       <c r="N243">
         <v>2</v>
@@ -36314,7 +36314,7 @@
         <v>66</v>
       </c>
       <c r="M302">
-        <v>10</v>
+        <v>15</v>
       </c>
       <c r="N302">
         <v>1</v>
@@ -36641,7 +36641,7 @@
         <v>100</v>
       </c>
       <c r="M305">
-        <v>10</v>
+        <v>15</v>
       </c>
       <c r="N305">
         <v>1</v>
@@ -39999,7 +39999,7 @@
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C18" sqref="C18"/>
+      <selection pane="bottomLeft" activeCell="C22" sqref="C22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>

</xml_diff>

<commit_message>
Arrow fixes, shop script cleanup, sunken ship npc, and some minor adjustments.
</commit_message>
<xml_diff>
--- a/Other/RoStatProcessing.xlsx
+++ b/Other/RoStatProcessing.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\ProjectsSSD\RagnarokRebuildTcp\Other\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DE167560-1B83-48D0-ADCB-6C13C49648B1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C15F8C2C-3EA3-47B3-80FA-E04490B354CE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3634" yWindow="2914" windowWidth="26932" windowHeight="13937" activeTab="1" xr2:uid="{1C41742B-2950-4FF8-AA39-6557869B44EA}"/>
+    <workbookView xWindow="3634" yWindow="2914" windowWidth="26932" windowHeight="13937" xr2:uid="{1C41742B-2950-4FF8-AA39-6557869B44EA}"/>
   </bookViews>
   <sheets>
     <sheet name="StatDef" sheetId="3" r:id="rId1"/>
@@ -4022,11 +4022,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{811A97A5-94A7-4FFA-A162-65D076B52481}">
   <dimension ref="A1:AJ316"/>
   <sheetViews>
-    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <pane xSplit="4" ySplit="1" topLeftCell="E198" activePane="bottomRight" state="frozen"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <pane xSplit="4" ySplit="1" topLeftCell="E102" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="E1" sqref="E1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="P213" sqref="P213"/>
+      <selection pane="bottomRight" activeCell="D105" sqref="D105"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
@@ -6434,7 +6434,7 @@
         <v>123</v>
       </c>
       <c r="D23">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="E23">
         <v>100</v>
@@ -6541,7 +6541,7 @@
         <v>126</v>
       </c>
       <c r="D24">
-        <v>26</v>
+        <v>21</v>
       </c>
       <c r="E24">
         <v>100</v>
@@ -9041,10 +9041,10 @@
         <v>70</v>
       </c>
       <c r="Q47">
-        <v>100</v>
+        <v>110</v>
       </c>
       <c r="R47">
-        <v>100</v>
+        <v>110</v>
       </c>
       <c r="S47">
         <v>10</v>
@@ -9965,10 +9965,10 @@
         <v>242</v>
       </c>
       <c r="D56">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="E56">
-        <v>100</v>
+        <v>90</v>
       </c>
       <c r="F56">
         <v>100</v>
@@ -10179,7 +10179,7 @@
         <v>248</v>
       </c>
       <c r="D58">
-        <v>25</v>
+        <v>20</v>
       </c>
       <c r="E58">
         <v>100</v>
@@ -15211,7 +15211,7 @@
         <v>402</v>
       </c>
       <c r="D105">
-        <v>28</v>
+        <v>15</v>
       </c>
       <c r="E105">
         <v>100</v>
@@ -15532,7 +15532,7 @@
         <v>411</v>
       </c>
       <c r="D108">
-        <v>26</v>
+        <v>20</v>
       </c>
       <c r="E108">
         <v>100</v>
@@ -16709,7 +16709,7 @@
         <v>446</v>
       </c>
       <c r="D119">
-        <v>33</v>
+        <v>28</v>
       </c>
       <c r="E119">
         <v>100</v>
@@ -16923,7 +16923,7 @@
         <v>452</v>
       </c>
       <c r="D121">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="E121">
         <v>100</v>
@@ -17458,7 +17458,7 @@
         <v>468</v>
       </c>
       <c r="D126">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="E126">
         <v>110</v>
@@ -17497,10 +17497,10 @@
         <v>30</v>
       </c>
       <c r="Q126">
-        <v>99</v>
+        <v>105</v>
       </c>
       <c r="R126">
-        <v>98</v>
+        <v>100</v>
       </c>
       <c r="S126">
         <v>10</v>
@@ -17565,7 +17565,7 @@
         <v>473</v>
       </c>
       <c r="D127">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="E127">
         <v>100</v>
@@ -17604,7 +17604,7 @@
         <v>70</v>
       </c>
       <c r="Q127">
-        <v>96</v>
+        <v>92</v>
       </c>
       <c r="R127">
         <v>94</v>
@@ -17672,7 +17672,7 @@
         <v>476</v>
       </c>
       <c r="D128">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="E128">
         <v>130</v>
@@ -40007,7 +40007,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0E19C42E-4D03-4797-B846-FB5E09BB39D3}">
   <dimension ref="A1:N29"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="K11" sqref="K11"/>
     </sheetView>

</xml_diff>

<commit_message>
A bazillion fixes and changes to prepare for testing.
</commit_message>
<xml_diff>
--- a/Other/RoStatProcessing.xlsx
+++ b/Other/RoStatProcessing.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\ProjectsSSD\RagnarokRebuildTcp\Other\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4D795A50-C69B-4EE7-B61F-1F66F8E60E36}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F0A419BA-3480-429F-B2AD-4F490FF96816}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="463" yWindow="3137" windowWidth="26931" windowHeight="13937" xr2:uid="{1C41742B-2950-4FF8-AA39-6557869B44EA}"/>
+    <workbookView xWindow="1543" yWindow="2931" windowWidth="29974" windowHeight="13938" xr2:uid="{1C41742B-2950-4FF8-AA39-6557869B44EA}"/>
   </bookViews>
   <sheets>
     <sheet name="StatDef" sheetId="3" r:id="rId1"/>
@@ -4038,17 +4038,17 @@
   <dimension ref="A1:AJ317"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <pane xSplit="4" ySplit="1" topLeftCell="E284" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="4" ySplit="1" topLeftCell="E38" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="E1" sqref="E1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="W302" sqref="W302"/>
+      <selection pane="bottomRight" activeCell="L56" sqref="L56"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
   <cols>
     <col min="1" max="1" width="5.07421875" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="22.61328125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="15.921875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="20.15234375" customWidth="1"/>
     <col min="4" max="4" width="7.61328125" bestFit="1" customWidth="1"/>
     <col min="5" max="8" width="5.765625" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="6.61328125" bestFit="1" customWidth="1"/>
@@ -10004,7 +10004,7 @@
         <v>110</v>
       </c>
       <c r="L56">
-        <v>120</v>
+        <v>125</v>
       </c>
       <c r="M56">
         <v>10</v>
@@ -10019,10 +10019,10 @@
         <v>70</v>
       </c>
       <c r="Q56">
-        <v>100</v>
+        <v>95</v>
       </c>
       <c r="R56">
-        <v>100</v>
+        <v>95</v>
       </c>
       <c r="S56">
         <v>10</v>
@@ -17277,7 +17277,7 @@
         <v>110</v>
       </c>
       <c r="I124">
-        <v>110</v>
+        <v>130</v>
       </c>
       <c r="J124">
         <v>100</v>
@@ -17337,7 +17337,7 @@
         <v>41</v>
       </c>
       <c r="AC124" t="s">
-        <v>188</v>
+        <v>1114</v>
       </c>
       <c r="AD124" t="s">
         <v>1120</v>
@@ -20154,7 +20154,7 @@
         <v>33</v>
       </c>
       <c r="E151">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="F151">
         <v>130</v>
@@ -20163,19 +20163,19 @@
         <v>100</v>
       </c>
       <c r="H151">
-        <v>100</v>
+        <v>130</v>
       </c>
       <c r="I151">
-        <v>100</v>
+        <v>110</v>
       </c>
       <c r="J151">
-        <v>100</v>
+        <v>110</v>
       </c>
       <c r="K151">
-        <v>100</v>
+        <v>130</v>
       </c>
       <c r="L151">
-        <v>100</v>
+        <v>110</v>
       </c>
       <c r="M151">
         <v>10</v>
@@ -20184,13 +20184,13 @@
         <v>1</v>
       </c>
       <c r="O151">
-        <v>100</v>
+        <v>20</v>
       </c>
       <c r="P151">
-        <v>100</v>
+        <v>70</v>
       </c>
       <c r="Q151">
-        <v>100</v>
+        <v>105</v>
       </c>
       <c r="R151">
         <v>100</v>
@@ -20368,7 +20368,7 @@
         <v>69</v>
       </c>
       <c r="E153">
-        <v>90</v>
+        <v>100</v>
       </c>
       <c r="F153">
         <v>100</v>
@@ -20380,34 +20380,34 @@
         <v>100</v>
       </c>
       <c r="I153">
-        <v>100</v>
+        <v>110</v>
       </c>
       <c r="J153">
         <v>100</v>
       </c>
       <c r="K153">
-        <v>130</v>
+        <v>170</v>
       </c>
       <c r="L153">
         <v>80</v>
       </c>
       <c r="M153">
-        <v>20</v>
+        <v>8</v>
       </c>
       <c r="N153">
         <v>1</v>
       </c>
       <c r="O153">
-        <v>100</v>
+        <v>140</v>
       </c>
       <c r="P153">
-        <v>100</v>
+        <v>140</v>
       </c>
       <c r="Q153">
-        <v>104</v>
+        <v>115</v>
       </c>
       <c r="R153">
-        <v>96</v>
+        <v>110</v>
       </c>
       <c r="S153">
         <v>10</v>
@@ -20493,7 +20493,7 @@
         <v>100</v>
       </c>
       <c r="K154">
-        <v>130</v>
+        <v>170</v>
       </c>
       <c r="L154">
         <v>80</v>
@@ -20505,10 +20505,10 @@
         <v>1</v>
       </c>
       <c r="O154">
-        <v>100</v>
+        <v>40</v>
       </c>
       <c r="P154">
-        <v>100</v>
+        <v>110</v>
       </c>
       <c r="Q154">
         <v>104</v>
@@ -20805,19 +20805,19 @@
         <v>100</v>
       </c>
       <c r="H157">
-        <v>100</v>
+        <v>60</v>
       </c>
       <c r="I157">
-        <v>120</v>
+        <v>130</v>
       </c>
       <c r="J157">
         <v>420</v>
       </c>
       <c r="K157">
-        <v>100</v>
+        <v>90</v>
       </c>
       <c r="L157">
-        <v>100</v>
+        <v>110</v>
       </c>
       <c r="M157">
         <v>10</v>
@@ -20826,10 +20826,10 @@
         <v>1</v>
       </c>
       <c r="O157">
-        <v>100</v>
+        <v>0</v>
       </c>
       <c r="P157">
-        <v>100</v>
+        <v>190</v>
       </c>
       <c r="Q157">
         <v>100</v>
@@ -20903,7 +20903,7 @@
         <v>59</v>
       </c>
       <c r="E158">
-        <v>85</v>
+        <v>110</v>
       </c>
       <c r="F158">
         <v>100</v>
@@ -20915,7 +20915,7 @@
         <v>80</v>
       </c>
       <c r="I158">
-        <v>140</v>
+        <v>200</v>
       </c>
       <c r="J158">
         <v>100</v>
@@ -20924,7 +20924,7 @@
         <v>110</v>
       </c>
       <c r="L158">
-        <v>105</v>
+        <v>110</v>
       </c>
       <c r="M158">
         <v>10</v>
@@ -20933,16 +20933,16 @@
         <v>1</v>
       </c>
       <c r="O158">
-        <v>90</v>
+        <v>50</v>
       </c>
       <c r="P158">
-        <v>90</v>
+        <v>140</v>
       </c>
       <c r="Q158">
         <v>105</v>
       </c>
       <c r="R158">
-        <v>110</v>
+        <v>115</v>
       </c>
       <c r="S158">
         <v>10</v>
@@ -21016,10 +21016,10 @@
         <v>100</v>
       </c>
       <c r="G159">
-        <v>110</v>
+        <v>60</v>
       </c>
       <c r="H159">
-        <v>80</v>
+        <v>40</v>
       </c>
       <c r="I159">
         <v>100</v>
@@ -21028,7 +21028,7 @@
         <v>100</v>
       </c>
       <c r="K159">
-        <v>110</v>
+        <v>90</v>
       </c>
       <c r="L159">
         <v>100</v>
@@ -21120,13 +21120,13 @@
         <v>100</v>
       </c>
       <c r="F160">
-        <v>100</v>
+        <v>90</v>
       </c>
       <c r="G160">
         <v>100</v>
       </c>
       <c r="H160">
-        <v>100</v>
+        <v>60</v>
       </c>
       <c r="I160">
         <v>100</v>
@@ -21135,10 +21135,10 @@
         <v>100</v>
       </c>
       <c r="K160">
-        <v>100</v>
+        <v>120</v>
       </c>
       <c r="L160">
-        <v>100</v>
+        <v>120</v>
       </c>
       <c r="M160">
         <v>10</v>
@@ -21153,7 +21153,7 @@
         <v>100</v>
       </c>
       <c r="Q160">
-        <v>100</v>
+        <v>110</v>
       </c>
       <c r="R160">
         <v>100</v>
@@ -21230,22 +21230,22 @@
         <v>100</v>
       </c>
       <c r="G161">
-        <v>150</v>
+        <v>170</v>
       </c>
       <c r="H161">
         <v>90</v>
       </c>
       <c r="I161">
-        <v>110</v>
+        <v>95</v>
       </c>
       <c r="J161">
-        <v>80</v>
+        <v>100</v>
       </c>
       <c r="K161">
-        <v>100</v>
+        <v>130</v>
       </c>
       <c r="L161">
-        <v>90</v>
+        <v>70</v>
       </c>
       <c r="M161">
         <v>10</v>
@@ -21254,13 +21254,13 @@
         <v>3</v>
       </c>
       <c r="O161">
-        <v>90</v>
+        <v>110</v>
       </c>
       <c r="P161">
-        <v>110</v>
+        <v>170</v>
       </c>
       <c r="Q161">
-        <v>110</v>
+        <v>120</v>
       </c>
       <c r="R161">
         <v>120</v>
@@ -36457,10 +36457,10 @@
         <v>1</v>
       </c>
       <c r="O303">
-        <v>100</v>
+        <v>60</v>
       </c>
       <c r="P303">
-        <v>100</v>
+        <v>110</v>
       </c>
       <c r="Q303">
         <v>0</v>
@@ -40137,12 +40137,12 @@
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A13" sqref="A13"/>
+      <selection pane="bottomLeft" activeCell="A20" sqref="A20:N20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
   <cols>
-    <col min="1" max="1" width="11.3828125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="16.53515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:14" x14ac:dyDescent="0.4">
@@ -41431,8 +41431,8 @@
   <dimension ref="A1:M41"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A17" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="K33" sqref="K33"/>
+      <pane ySplit="1" topLeftCell="A11" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="K30" sqref="K30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
@@ -43129,7 +43129,7 @@
   <dimension ref="A1:M11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C16" sqref="C16"/>
+      <selection activeCell="K10" sqref="K10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
@@ -43207,10 +43207,10 @@
         <v>100</v>
       </c>
       <c r="J2">
-        <v>100</v>
+        <v>102</v>
       </c>
       <c r="K2">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="L2">
         <v>100</v>
@@ -43289,10 +43289,10 @@
         <v>100</v>
       </c>
       <c r="J4">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="K4">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="L4">
         <v>100</v>
@@ -43330,10 +43330,10 @@
         <v>100</v>
       </c>
       <c r="J5">
-        <v>103</v>
+        <v>99</v>
       </c>
       <c r="K5">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="L5">
         <v>100</v>
@@ -43371,10 +43371,10 @@
         <v>100</v>
       </c>
       <c r="J6">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="K6">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="L6">
         <v>100</v>
@@ -43412,10 +43412,10 @@
         <v>100</v>
       </c>
       <c r="J7">
-        <v>97</v>
+        <v>98</v>
       </c>
       <c r="K7">
-        <v>97</v>
+        <v>98</v>
       </c>
       <c r="L7">
         <v>100</v>
@@ -43494,10 +43494,10 @@
         <v>100</v>
       </c>
       <c r="J9">
-        <v>100</v>
+        <v>102</v>
       </c>
       <c r="K9">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="L9">
         <v>102</v>
@@ -43538,7 +43538,7 @@
         <v>100</v>
       </c>
       <c r="K10">
-        <v>100</v>
+        <v>103</v>
       </c>
       <c r="L10">
         <v>103</v>
@@ -43576,10 +43576,10 @@
         <v>100</v>
       </c>
       <c r="J11">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="K11">
-        <v>100</v>
+        <v>102</v>
       </c>
       <c r="L11">
         <v>105</v>

</xml_diff>

<commit_message>
Revamping database inventory storage, better alive/dead handling, server config scripts, and more.
</commit_message>
<xml_diff>
--- a/Other/RoStatProcessing.xlsx
+++ b/Other/RoStatProcessing.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28227"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28324"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\ProjectsSSD\RagnarokRebuildTcp\Other\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F0A419BA-3480-429F-B2AD-4F490FF96816}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8F360CC4-C867-41C3-9254-5F9FAAEC098F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1543" yWindow="2931" windowWidth="29974" windowHeight="13938" xr2:uid="{1C41742B-2950-4FF8-AA39-6557869B44EA}"/>
+    <workbookView xWindow="2091" yWindow="2091" windowWidth="26932" windowHeight="14323" xr2:uid="{1C41742B-2950-4FF8-AA39-6557869B44EA}"/>
   </bookViews>
   <sheets>
     <sheet name="StatDef" sheetId="3" r:id="rId1"/>
@@ -4038,10 +4038,10 @@
   <dimension ref="A1:AJ317"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <pane xSplit="4" ySplit="1" topLeftCell="E38" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="4" ySplit="1" topLeftCell="E284" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="E1" sqref="E1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="L56" sqref="L56"/>
+      <selection pane="bottomRight" activeCell="K310" sqref="K310"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
@@ -11374,7 +11374,7 @@
         <v>289</v>
       </c>
       <c r="D69">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="E69">
         <v>160</v>
@@ -36534,7 +36534,7 @@
         <v>77</v>
       </c>
       <c r="D304">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="E304">
         <v>100</v>
@@ -36546,7 +36546,7 @@
         <v>100</v>
       </c>
       <c r="H304">
-        <v>100</v>
+        <v>80</v>
       </c>
       <c r="I304">
         <v>100</v>
@@ -36641,10 +36641,10 @@
         <v>1105</v>
       </c>
       <c r="D305">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="E305">
-        <v>100</v>
+        <v>90</v>
       </c>
       <c r="F305">
         <v>100</v>
@@ -36665,7 +36665,7 @@
         <v>100</v>
       </c>
       <c r="L305">
-        <v>100</v>
+        <v>105</v>
       </c>
       <c r="M305">
         <v>10</v>
@@ -37078,7 +37078,7 @@
         <v>31</v>
       </c>
       <c r="E309">
-        <v>100</v>
+        <v>130</v>
       </c>
       <c r="F309">
         <v>100</v>
@@ -37087,7 +37087,7 @@
         <v>100</v>
       </c>
       <c r="H309">
-        <v>100</v>
+        <v>130</v>
       </c>
       <c r="I309">
         <v>100</v>
@@ -37096,7 +37096,7 @@
         <v>100</v>
       </c>
       <c r="K309">
-        <v>100</v>
+        <v>80</v>
       </c>
       <c r="L309">
         <v>100</v>
@@ -37108,13 +37108,13 @@
         <v>1</v>
       </c>
       <c r="O309">
-        <v>100</v>
+        <v>130</v>
       </c>
       <c r="P309">
         <v>100</v>
       </c>
       <c r="Q309">
-        <v>100</v>
+        <v>105</v>
       </c>
       <c r="R309">
         <v>100</v>
@@ -37197,10 +37197,10 @@
         <v>100</v>
       </c>
       <c r="I310">
-        <v>100</v>
+        <v>130</v>
       </c>
       <c r="J310">
-        <v>100</v>
+        <v>85</v>
       </c>
       <c r="K310">
         <v>100</v>
@@ -37221,10 +37221,10 @@
         <v>100</v>
       </c>
       <c r="Q310">
-        <v>100</v>
+        <v>105</v>
       </c>
       <c r="R310">
-        <v>100</v>
+        <v>105</v>
       </c>
       <c r="S310">
         <v>10</v>
@@ -37292,25 +37292,25 @@
         <v>36</v>
       </c>
       <c r="E311">
-        <v>100</v>
+        <v>95</v>
       </c>
       <c r="F311">
         <v>100</v>
       </c>
       <c r="G311">
-        <v>100</v>
+        <v>130</v>
       </c>
       <c r="H311">
         <v>100</v>
       </c>
       <c r="I311">
-        <v>100</v>
+        <v>90</v>
       </c>
       <c r="J311">
-        <v>100</v>
+        <v>130</v>
       </c>
       <c r="K311">
-        <v>100</v>
+        <v>110</v>
       </c>
       <c r="L311">
         <v>100</v>
@@ -37325,13 +37325,13 @@
         <v>100</v>
       </c>
       <c r="P311">
-        <v>100</v>
+        <v>130</v>
       </c>
       <c r="Q311">
-        <v>110</v>
+        <v>112</v>
       </c>
       <c r="R311">
-        <v>100</v>
+        <v>105</v>
       </c>
       <c r="S311">
         <v>10</v>
@@ -40137,7 +40137,7 @@
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A20" sqref="A20:N20"/>
+      <selection pane="bottomLeft" activeCell="E3" sqref="E3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>

</xml_diff>

<commit_message>
Huge number of skills and effects, including warp portal, safety wall, soul strike, teleport, etc.
</commit_message>
<xml_diff>
--- a/Other/RoStatProcessing.xlsx
+++ b/Other/RoStatProcessing.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\ProjectsSSD\RagnarokRebuildTcp\Other\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BC33B416-8C2A-4943-847A-9E85BFE7F95E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B3E88BB5-AACD-4E9E-81DF-EDD3D56C3277}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="3626" yWindow="2931" windowWidth="26931" windowHeight="13938" xr2:uid="{1C41742B-2950-4FF8-AA39-6557869B44EA}"/>
   </bookViews>
@@ -4060,10 +4060,10 @@
   <dimension ref="A1:AK317"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <pane xSplit="4" ySplit="1" topLeftCell="Y265" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="4" ySplit="1" topLeftCell="E246" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="E1" sqref="E1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="AE286" sqref="AE286"/>
+      <selection pane="bottomRight" activeCell="O262" sqref="O262"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
@@ -9472,7 +9472,7 @@
         <v>39</v>
       </c>
       <c r="AD50" t="s">
-        <v>42</v>
+        <v>1118</v>
       </c>
       <c r="AF50">
         <v>288</v>
@@ -32165,7 +32165,7 @@
         <v>100</v>
       </c>
       <c r="G262">
-        <v>100</v>
+        <v>250</v>
       </c>
       <c r="H262">
         <v>100</v>

</xml_diff>

<commit_message>
Added a license, a whole bunch of skills/effects, and AI adjustments.
</commit_message>
<xml_diff>
--- a/Other/RoStatProcessing.xlsx
+++ b/Other/RoStatProcessing.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\ProjectsSSD\RagnarokRebuildTcp\Other\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B3E88BB5-AACD-4E9E-81DF-EDD3D56C3277}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2E08F2DE-A8CD-46FB-8966-770148FD26B5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="3626" yWindow="2931" windowWidth="26931" windowHeight="13938" xr2:uid="{1C41742B-2950-4FF8-AA39-6557869B44EA}"/>
   </bookViews>
@@ -4060,10 +4060,10 @@
   <dimension ref="A1:AK317"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <pane xSplit="4" ySplit="1" topLeftCell="E246" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="4" ySplit="1" topLeftCell="E143" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="E1" sqref="E1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="O262" sqref="O262"/>
+      <selection pane="bottomRight" activeCell="G161" sqref="G161"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
@@ -21358,7 +21358,7 @@
         <v>100</v>
       </c>
       <c r="G161">
-        <v>170</v>
+        <v>160</v>
       </c>
       <c r="H161">
         <v>90</v>

</xml_diff>

<commit_message>
Sleep, curse, freeze, and blind statuses, frost diver, blood drain, agi up, call minion and status attack skills.
</commit_message>
<xml_diff>
--- a/Other/RoStatProcessing.xlsx
+++ b/Other/RoStatProcessing.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\ProjectsSSD\RagnarokRebuildTcp\Other\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2E08F2DE-A8CD-46FB-8966-770148FD26B5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F8433FAE-C8C6-4DC0-8383-0B4E6D10F8B9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="3626" yWindow="2931" windowWidth="26931" windowHeight="13938" xr2:uid="{1C41742B-2950-4FF8-AA39-6557869B44EA}"/>
   </bookViews>
@@ -51,7 +51,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3186" uniqueCount="1187">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3195" uniqueCount="1190">
   <si>
     <t>Id</t>
   </si>
@@ -3612,6 +3612,15 @@
   </si>
   <si>
     <t>TotalBase</t>
+  </si>
+  <si>
+    <t>GIANT_HONET</t>
+  </si>
+  <si>
+    <t>giant_honet.spr</t>
+  </si>
+  <si>
+    <t>Giant Hornet</t>
   </si>
 </sst>
 </file>
@@ -3712,10 +3721,10 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{5AE4419D-5DB5-4D1B-9713-9E17C7E1903B}" name="Table1" displayName="Table1" ref="A1:AK413" totalsRowShown="0">
-  <autoFilter ref="A1:AK413" xr:uid="{5AE4419D-5DB5-4D1B-9713-9E17C7E1903B}"/>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:AK317">
-    <sortCondition ref="A1:A413"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{5AE4419D-5DB5-4D1B-9713-9E17C7E1903B}" name="Table1" displayName="Table1" ref="A1:AK414" totalsRowShown="0">
+  <autoFilter ref="A1:AK414" xr:uid="{5AE4419D-5DB5-4D1B-9713-9E17C7E1903B}"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:AK318">
+    <sortCondition ref="A1:A414"/>
   </sortState>
   <tableColumns count="37">
     <tableColumn id="1" xr3:uid="{B859DFBF-EB68-4198-9FF0-FEBC6A5D6D92}" name="Id"/>
@@ -4057,13 +4066,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{811A97A5-94A7-4FFA-A162-65D076B52481}">
-  <dimension ref="A1:AK317"/>
+  <dimension ref="A1:AK318"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <pane xSplit="4" ySplit="1" topLeftCell="E143" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="4" ySplit="1" topLeftCell="L281" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="E1" sqref="E1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="G161" sqref="G161"/>
+      <selection pane="bottomRight" activeCell="AB302" sqref="AB302"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
@@ -15003,7 +15012,7 @@
         <v>100</v>
       </c>
       <c r="J102">
-        <v>100</v>
+        <v>90</v>
       </c>
       <c r="K102">
         <v>100</v>
@@ -15110,13 +15119,13 @@
         <v>100</v>
       </c>
       <c r="J103">
-        <v>100</v>
+        <v>80</v>
       </c>
       <c r="K103">
         <v>100</v>
       </c>
       <c r="L103">
-        <v>110</v>
+        <v>115</v>
       </c>
       <c r="M103">
         <v>10</v>
@@ -15125,13 +15134,13 @@
         <v>1</v>
       </c>
       <c r="O103">
-        <v>100</v>
+        <v>125</v>
       </c>
       <c r="P103">
-        <v>100</v>
+        <v>0</v>
       </c>
       <c r="Q103">
-        <v>105</v>
+        <v>108</v>
       </c>
       <c r="R103">
         <v>95</v>
@@ -19224,7 +19233,7 @@
         <v>110</v>
       </c>
       <c r="J141">
-        <v>75</v>
+        <v>70</v>
       </c>
       <c r="K141">
         <v>100</v>
@@ -36445,52 +36454,52 @@
     </row>
     <row r="302" spans="1:37" x14ac:dyDescent="0.4">
       <c r="A302">
-        <v>5000</v>
+        <v>4299</v>
       </c>
       <c r="B302" t="s">
-        <v>44</v>
+        <v>1187</v>
       </c>
       <c r="C302" t="s">
-        <v>37</v>
+        <v>1189</v>
       </c>
       <c r="D302">
-        <v>50</v>
+        <v>56</v>
       </c>
       <c r="E302">
-        <v>80</v>
+        <v>100</v>
       </c>
       <c r="F302">
-        <v>80</v>
+        <v>100</v>
       </c>
       <c r="G302">
-        <v>80</v>
+        <v>100</v>
       </c>
       <c r="H302">
-        <v>80</v>
+        <v>100</v>
       </c>
       <c r="I302">
-        <v>80</v>
+        <v>100</v>
       </c>
       <c r="J302">
-        <v>80</v>
+        <v>100</v>
       </c>
       <c r="K302">
-        <v>80</v>
+        <v>100</v>
       </c>
       <c r="L302">
         <v>100</v>
       </c>
       <c r="M302">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="N302">
         <v>1</v>
       </c>
       <c r="O302">
-        <v>50</v>
+        <v>100</v>
       </c>
       <c r="P302">
-        <v>50</v>
+        <v>100</v>
       </c>
       <c r="Q302">
         <v>100</v>
@@ -36505,40 +36514,40 @@
         <v>12</v>
       </c>
       <c r="U302" t="s">
-        <v>38</v>
+        <v>47</v>
       </c>
       <c r="V302" t="s">
-        <v>39</v>
+        <v>48</v>
       </c>
       <c r="W302" t="s">
-        <v>40</v>
+        <v>63</v>
       </c>
       <c r="X302">
-        <v>1872</v>
+        <v>1292</v>
       </c>
       <c r="Y302">
-        <v>480</v>
+        <v>340</v>
       </c>
       <c r="Z302">
-        <v>672</v>
+        <v>792</v>
       </c>
       <c r="AA302">
-        <v>400</v>
+        <v>155</v>
       </c>
       <c r="AB302" t="s">
+        <v>181</v>
+      </c>
+      <c r="AC302" t="s">
         <v>41</v>
       </c>
-      <c r="AC302" t="s">
-        <v>39</v>
-      </c>
       <c r="AD302" t="s">
-        <v>1118</v>
+        <v>42</v>
       </c>
       <c r="AF302">
-        <v>288</v>
+        <v>825</v>
       </c>
       <c r="AG302" t="s">
-        <v>43</v>
+        <v>1188</v>
       </c>
       <c r="AH302">
         <v>0</v>
@@ -36547,63 +36556,63 @@
         <v>0.5</v>
       </c>
       <c r="AJ302">
-        <v>1.1000000000000001</v>
+        <v>1</v>
       </c>
     </row>
     <row r="303" spans="1:37" x14ac:dyDescent="0.4">
       <c r="A303">
-        <v>6000</v>
+        <v>5000</v>
       </c>
       <c r="B303" t="s">
-        <v>1094</v>
+        <v>44</v>
       </c>
       <c r="C303" t="s">
-        <v>565</v>
+        <v>37</v>
       </c>
       <c r="D303">
-        <v>65</v>
+        <v>50</v>
       </c>
       <c r="E303">
-        <v>15</v>
+        <v>80</v>
       </c>
       <c r="F303">
-        <v>100</v>
+        <v>80</v>
       </c>
       <c r="G303">
-        <v>100</v>
+        <v>80</v>
       </c>
       <c r="H303">
-        <v>100</v>
+        <v>80</v>
       </c>
       <c r="I303">
-        <v>100</v>
+        <v>80</v>
       </c>
       <c r="J303">
-        <v>100</v>
+        <v>80</v>
       </c>
       <c r="K303">
-        <v>130</v>
+        <v>80</v>
       </c>
       <c r="L303">
-        <v>66</v>
+        <v>100</v>
       </c>
       <c r="M303">
-        <v>15</v>
+        <v>5</v>
       </c>
       <c r="N303">
         <v>1</v>
       </c>
       <c r="O303">
-        <v>60</v>
+        <v>50</v>
       </c>
       <c r="P303">
-        <v>110</v>
+        <v>50</v>
       </c>
       <c r="Q303">
-        <v>0</v>
+        <v>100</v>
       </c>
       <c r="R303">
-        <v>0</v>
+        <v>100</v>
       </c>
       <c r="S303">
         <v>10</v>
@@ -36615,37 +36624,37 @@
         <v>38</v>
       </c>
       <c r="V303" t="s">
-        <v>219</v>
+        <v>39</v>
       </c>
       <c r="W303" t="s">
-        <v>274</v>
+        <v>40</v>
       </c>
       <c r="X303">
-        <v>1276</v>
+        <v>1872</v>
       </c>
       <c r="Y303">
+        <v>480</v>
+      </c>
+      <c r="Z303">
+        <v>672</v>
+      </c>
+      <c r="AA303">
+        <v>400</v>
+      </c>
+      <c r="AB303" t="s">
+        <v>41</v>
+      </c>
+      <c r="AC303" t="s">
+        <v>39</v>
+      </c>
+      <c r="AD303" t="s">
+        <v>1118</v>
+      </c>
+      <c r="AF303">
         <v>288</v>
       </c>
-      <c r="Z303">
-        <v>576</v>
-      </c>
-      <c r="AA303">
-        <v>150</v>
-      </c>
-      <c r="AB303" t="s">
-        <v>119</v>
-      </c>
-      <c r="AC303" t="s">
-        <v>566</v>
-      </c>
-      <c r="AD303" t="s">
-        <v>1121</v>
-      </c>
-      <c r="AF303">
-        <v>180</v>
-      </c>
       <c r="AG303" t="s">
-        <v>567</v>
+        <v>43</v>
       </c>
       <c r="AH303">
         <v>0</v>
@@ -36654,27 +36663,24 @@
         <v>0.5</v>
       </c>
       <c r="AJ303">
-        <v>1</v>
-      </c>
-      <c r="AK303" t="s">
-        <v>1095</v>
+        <v>1.1000000000000001</v>
       </c>
     </row>
     <row r="304" spans="1:37" x14ac:dyDescent="0.4">
       <c r="A304">
-        <v>6001</v>
+        <v>6000</v>
       </c>
       <c r="B304" t="s">
-        <v>1103</v>
+        <v>1094</v>
       </c>
       <c r="C304" t="s">
-        <v>77</v>
+        <v>565</v>
       </c>
       <c r="D304">
-        <v>13</v>
+        <v>65</v>
       </c>
       <c r="E304">
-        <v>100</v>
+        <v>15</v>
       </c>
       <c r="F304">
         <v>100</v>
@@ -36683,7 +36689,7 @@
         <v>100</v>
       </c>
       <c r="H304">
-        <v>80</v>
+        <v>100</v>
       </c>
       <c r="I304">
         <v>100</v>
@@ -36692,22 +36698,22 @@
         <v>100</v>
       </c>
       <c r="K304">
-        <v>100</v>
+        <v>130</v>
       </c>
       <c r="L304">
-        <v>100</v>
+        <v>66</v>
       </c>
       <c r="M304">
-        <v>10</v>
+        <v>15</v>
       </c>
       <c r="N304">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="O304">
-        <v>100</v>
+        <v>60</v>
       </c>
       <c r="P304">
-        <v>100</v>
+        <v>110</v>
       </c>
       <c r="Q304">
         <v>0</v>
@@ -36716,72 +36722,75 @@
         <v>0</v>
       </c>
       <c r="S304">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="T304">
-        <v>1</v>
+        <v>12</v>
       </c>
       <c r="U304" t="s">
-        <v>47</v>
+        <v>38</v>
       </c>
       <c r="V304" t="s">
-        <v>48</v>
+        <v>219</v>
       </c>
       <c r="W304" t="s">
-        <v>619</v>
+        <v>274</v>
       </c>
       <c r="X304">
-        <v>701</v>
+        <v>1276</v>
       </c>
       <c r="Y304">
-        <v>1</v>
+        <v>288</v>
       </c>
       <c r="Z304">
-        <v>1</v>
+        <v>576</v>
       </c>
       <c r="AA304">
-        <v>-1</v>
+        <v>150</v>
       </c>
       <c r="AB304" t="s">
-        <v>41</v>
+        <v>119</v>
       </c>
       <c r="AC304" t="s">
-        <v>1090</v>
+        <v>566</v>
       </c>
       <c r="AD304" t="s">
-        <v>59</v>
+        <v>1121</v>
       </c>
       <c r="AF304">
-        <v>288</v>
+        <v>180</v>
       </c>
       <c r="AG304" t="s">
-        <v>79</v>
+        <v>567</v>
       </c>
       <c r="AH304">
         <v>0</v>
       </c>
       <c r="AI304">
-        <v>-1</v>
+        <v>0.5</v>
       </c>
       <c r="AJ304">
-        <v>1.2</v>
+        <v>1</v>
+      </c>
+      <c r="AK304" t="s">
+        <v>1095</v>
       </c>
     </row>
     <row r="305" spans="1:37" x14ac:dyDescent="0.4">
       <c r="A305">
-        <v>6002</v>
+        <v>6001</v>
       </c>
       <c r="B305" t="s">
-        <v>1104</v>
+        <v>1103</v>
       </c>
       <c r="C305" t="s">
-        <v>1105</v>
+        <v>77</v>
       </c>
       <c r="D305">
-        <v>24</v>
+        <v>13</v>
       </c>
       <c r="E305">
-        <v>90</v>
+        <v>100</v>
       </c>
       <c r="F305">
         <v>100</v>
@@ -36790,7 +36799,7 @@
         <v>100</v>
       </c>
       <c r="H305">
-        <v>100</v>
+        <v>80</v>
       </c>
       <c r="I305">
         <v>100</v>
@@ -36802,13 +36811,13 @@
         <v>100</v>
       </c>
       <c r="L305">
-        <v>105</v>
+        <v>100</v>
       </c>
       <c r="M305">
         <v>10</v>
       </c>
       <c r="N305">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="O305">
         <v>100</v>
@@ -36823,13 +36832,13 @@
         <v>0</v>
       </c>
       <c r="S305">
-        <v>12</v>
+        <v>1</v>
       </c>
       <c r="T305">
-        <v>12</v>
+        <v>1</v>
       </c>
       <c r="U305" t="s">
-        <v>38</v>
+        <v>47</v>
       </c>
       <c r="V305" t="s">
         <v>48</v>
@@ -36838,60 +36847,57 @@
         <v>619</v>
       </c>
       <c r="X305">
-        <v>500</v>
+        <v>701</v>
       </c>
       <c r="Y305">
-        <v>288</v>
+        <v>1</v>
       </c>
       <c r="Z305">
-        <v>288</v>
+        <v>1</v>
       </c>
       <c r="AA305">
-        <v>120</v>
+        <v>-1</v>
       </c>
       <c r="AB305" t="s">
         <v>41</v>
       </c>
       <c r="AC305" t="s">
-        <v>1089</v>
+        <v>1090</v>
       </c>
       <c r="AD305" t="s">
-        <v>1121</v>
+        <v>59</v>
       </c>
       <c r="AF305">
-        <v>504</v>
+        <v>288</v>
       </c>
       <c r="AG305" t="s">
-        <v>283</v>
+        <v>79</v>
       </c>
       <c r="AH305">
         <v>0</v>
       </c>
       <c r="AI305">
-        <v>0.5</v>
+        <v>-1</v>
       </c>
       <c r="AJ305">
-        <v>0.7</v>
-      </c>
-      <c r="AK305" t="s">
-        <v>1106</v>
+        <v>1.2</v>
       </c>
     </row>
     <row r="306" spans="1:37" x14ac:dyDescent="0.4">
       <c r="A306">
-        <v>6003</v>
+        <v>6002</v>
       </c>
       <c r="B306" t="s">
-        <v>1123</v>
+        <v>1104</v>
       </c>
       <c r="C306" t="s">
-        <v>1124</v>
+        <v>1105</v>
       </c>
       <c r="D306">
-        <v>48</v>
+        <v>24</v>
       </c>
       <c r="E306">
-        <v>40</v>
+        <v>90</v>
       </c>
       <c r="F306">
         <v>100</v>
@@ -36912,28 +36918,28 @@
         <v>100</v>
       </c>
       <c r="L306">
-        <v>100</v>
+        <v>105</v>
       </c>
       <c r="M306">
-        <v>15</v>
+        <v>10</v>
       </c>
       <c r="N306">
         <v>1</v>
       </c>
       <c r="O306">
-        <v>350</v>
+        <v>100</v>
       </c>
       <c r="P306">
-        <v>350</v>
+        <v>100</v>
       </c>
       <c r="Q306">
-        <v>100</v>
+        <v>0</v>
       </c>
       <c r="R306">
-        <v>100</v>
+        <v>0</v>
       </c>
       <c r="S306">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="T306">
         <v>12</v>
@@ -36942,37 +36948,37 @@
         <v>38</v>
       </c>
       <c r="V306" t="s">
-        <v>53</v>
+        <v>48</v>
       </c>
       <c r="W306" t="s">
         <v>619</v>
       </c>
       <c r="X306">
-        <v>902</v>
+        <v>500</v>
       </c>
       <c r="Y306">
-        <v>432</v>
+        <v>288</v>
       </c>
       <c r="Z306">
-        <v>648</v>
+        <v>288</v>
       </c>
       <c r="AA306">
-        <v>150</v>
+        <v>120</v>
       </c>
       <c r="AB306" t="s">
-        <v>119</v>
+        <v>41</v>
       </c>
       <c r="AC306" t="s">
-        <v>120</v>
+        <v>1089</v>
       </c>
       <c r="AD306" t="s">
         <v>1121</v>
       </c>
       <c r="AF306">
-        <v>216</v>
+        <v>504</v>
       </c>
       <c r="AG306" t="s">
-        <v>1125</v>
+        <v>283</v>
       </c>
       <c r="AH306">
         <v>0</v>
@@ -36981,24 +36987,27 @@
         <v>0.5</v>
       </c>
       <c r="AJ306">
-        <v>1</v>
+        <v>0.7</v>
+      </c>
+      <c r="AK306" t="s">
+        <v>1106</v>
       </c>
     </row>
     <row r="307" spans="1:37" x14ac:dyDescent="0.4">
       <c r="A307">
-        <v>6004</v>
+        <v>6003</v>
       </c>
       <c r="B307" t="s">
-        <v>1126</v>
+        <v>1123</v>
       </c>
       <c r="C307" t="s">
-        <v>1127</v>
+        <v>1124</v>
       </c>
       <c r="D307">
-        <v>38</v>
+        <v>48</v>
       </c>
       <c r="E307">
-        <v>100</v>
+        <v>40</v>
       </c>
       <c r="F307">
         <v>100</v>
@@ -37022,16 +37031,16 @@
         <v>100</v>
       </c>
       <c r="M307">
-        <v>10</v>
+        <v>15</v>
       </c>
       <c r="N307">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="O307">
-        <v>100</v>
+        <v>350</v>
       </c>
       <c r="P307">
-        <v>100</v>
+        <v>350</v>
       </c>
       <c r="Q307">
         <v>100</v>
@@ -37052,34 +37061,34 @@
         <v>53</v>
       </c>
       <c r="W307" t="s">
-        <v>40</v>
+        <v>619</v>
       </c>
       <c r="X307">
-        <v>1540</v>
+        <v>902</v>
       </c>
       <c r="Y307">
-        <v>576</v>
+        <v>432</v>
       </c>
       <c r="Z307">
-        <v>720</v>
+        <v>648</v>
       </c>
       <c r="AA307">
-        <v>300</v>
+        <v>150</v>
       </c>
       <c r="AB307" t="s">
-        <v>41</v>
+        <v>119</v>
       </c>
       <c r="AC307" t="s">
-        <v>41</v>
+        <v>120</v>
       </c>
       <c r="AD307" t="s">
-        <v>1120</v>
+        <v>1121</v>
       </c>
       <c r="AF307">
-        <v>324</v>
+        <v>216</v>
       </c>
       <c r="AG307" t="s">
-        <v>1128</v>
+        <v>1125</v>
       </c>
       <c r="AH307">
         <v>0</v>
@@ -37093,16 +37102,16 @@
     </row>
     <row r="308" spans="1:37" x14ac:dyDescent="0.4">
       <c r="A308">
-        <v>6005</v>
+        <v>6004</v>
       </c>
       <c r="B308" t="s">
-        <v>1134</v>
+        <v>1126</v>
       </c>
       <c r="C308" t="s">
-        <v>1135</v>
+        <v>1127</v>
       </c>
       <c r="D308">
-        <v>34</v>
+        <v>38</v>
       </c>
       <c r="E308">
         <v>100</v>
@@ -37132,7 +37141,7 @@
         <v>10</v>
       </c>
       <c r="N308">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="O308">
         <v>100</v>
@@ -37153,40 +37162,40 @@
         <v>12</v>
       </c>
       <c r="U308" t="s">
-        <v>47</v>
+        <v>38</v>
       </c>
       <c r="V308" t="s">
         <v>53</v>
       </c>
       <c r="W308" t="s">
-        <v>49</v>
+        <v>40</v>
       </c>
       <c r="X308">
-        <v>1000</v>
+        <v>1540</v>
       </c>
       <c r="Y308">
-        <v>1000</v>
+        <v>576</v>
       </c>
       <c r="Z308">
-        <v>500</v>
+        <v>720</v>
       </c>
       <c r="AA308">
-        <v>140</v>
+        <v>300</v>
       </c>
       <c r="AB308" t="s">
         <v>41</v>
       </c>
       <c r="AC308" t="s">
-        <v>275</v>
+        <v>41</v>
       </c>
       <c r="AD308" t="s">
         <v>1120</v>
       </c>
       <c r="AF308">
-        <v>620</v>
+        <v>324</v>
       </c>
       <c r="AG308" t="s">
-        <v>103</v>
+        <v>1128</v>
       </c>
       <c r="AH308">
         <v>0</v>
@@ -37197,25 +37206,22 @@
       <c r="AJ308">
         <v>1</v>
       </c>
-      <c r="AK308" t="s">
-        <v>1133</v>
-      </c>
     </row>
     <row r="309" spans="1:37" x14ac:dyDescent="0.4">
       <c r="A309">
-        <v>6006</v>
+        <v>6005</v>
       </c>
       <c r="B309" t="s">
-        <v>1136</v>
+        <v>1134</v>
       </c>
       <c r="C309" t="s">
-        <v>1139</v>
+        <v>1135</v>
       </c>
       <c r="D309">
-        <v>31</v>
+        <v>34</v>
       </c>
       <c r="E309">
-        <v>130</v>
+        <v>100</v>
       </c>
       <c r="F309">
         <v>100</v>
@@ -37224,7 +37230,7 @@
         <v>100</v>
       </c>
       <c r="H309">
-        <v>130</v>
+        <v>100</v>
       </c>
       <c r="I309">
         <v>100</v>
@@ -37233,7 +37239,7 @@
         <v>100</v>
       </c>
       <c r="K309">
-        <v>80</v>
+        <v>100</v>
       </c>
       <c r="L309">
         <v>100</v>
@@ -37245,13 +37251,13 @@
         <v>1</v>
       </c>
       <c r="O309">
-        <v>130</v>
+        <v>100</v>
       </c>
       <c r="P309">
         <v>100</v>
       </c>
       <c r="Q309">
-        <v>105</v>
+        <v>100</v>
       </c>
       <c r="R309">
         <v>100</v>
@@ -37266,40 +37272,37 @@
         <v>47</v>
       </c>
       <c r="V309" t="s">
-        <v>48</v>
+        <v>53</v>
       </c>
       <c r="W309" t="s">
-        <v>113</v>
+        <v>49</v>
       </c>
       <c r="X309">
-        <v>916</v>
+        <v>1000</v>
       </c>
       <c r="Y309">
-        <v>576</v>
+        <v>1000</v>
       </c>
       <c r="Z309">
-        <v>648</v>
+        <v>500</v>
       </c>
       <c r="AA309">
-        <v>250</v>
+        <v>140</v>
       </c>
       <c r="AB309" t="s">
         <v>41</v>
       </c>
       <c r="AC309" t="s">
-        <v>48</v>
+        <v>275</v>
       </c>
       <c r="AD309" t="s">
         <v>1120</v>
       </c>
-      <c r="AE309" t="s">
-        <v>1184</v>
-      </c>
       <c r="AF309">
-        <v>180</v>
+        <v>620</v>
       </c>
       <c r="AG309" t="s">
-        <v>1142</v>
+        <v>103</v>
       </c>
       <c r="AH309">
         <v>0</v>
@@ -37310,22 +37313,25 @@
       <c r="AJ309">
         <v>1</v>
       </c>
+      <c r="AK309" t="s">
+        <v>1133</v>
+      </c>
     </row>
     <row r="310" spans="1:37" x14ac:dyDescent="0.4">
       <c r="A310">
-        <v>6007</v>
-      </c>
-      <c r="B310" s="9" t="s">
-        <v>1137</v>
+        <v>6006</v>
+      </c>
+      <c r="B310" t="s">
+        <v>1136</v>
       </c>
       <c r="C310" t="s">
-        <v>1140</v>
+        <v>1139</v>
       </c>
       <c r="D310">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="E310">
-        <v>100</v>
+        <v>130</v>
       </c>
       <c r="F310">
         <v>100</v>
@@ -37334,19 +37340,19 @@
         <v>100</v>
       </c>
       <c r="H310">
-        <v>100</v>
+        <v>130</v>
       </c>
       <c r="I310">
-        <v>130</v>
+        <v>100</v>
       </c>
       <c r="J310">
-        <v>85</v>
+        <v>100</v>
       </c>
       <c r="K310">
-        <v>100</v>
+        <v>80</v>
       </c>
       <c r="L310">
-        <v>130</v>
+        <v>100</v>
       </c>
       <c r="M310">
         <v>10</v>
@@ -37355,7 +37361,7 @@
         <v>1</v>
       </c>
       <c r="O310">
-        <v>100</v>
+        <v>130</v>
       </c>
       <c r="P310">
         <v>100</v>
@@ -37364,7 +37370,7 @@
         <v>105</v>
       </c>
       <c r="R310">
-        <v>105</v>
+        <v>100</v>
       </c>
       <c r="S310">
         <v>10</v>
@@ -37382,7 +37388,7 @@
         <v>113</v>
       </c>
       <c r="X310">
-        <v>1200</v>
+        <v>916</v>
       </c>
       <c r="Y310">
         <v>576</v>
@@ -37391,7 +37397,7 @@
         <v>648</v>
       </c>
       <c r="AA310">
-        <v>160</v>
+        <v>250</v>
       </c>
       <c r="AB310" t="s">
         <v>41</v>
@@ -37406,10 +37412,10 @@
         <v>1184</v>
       </c>
       <c r="AF310">
-        <v>144</v>
+        <v>180</v>
       </c>
       <c r="AG310" t="s">
-        <v>1143</v>
+        <v>1142</v>
       </c>
       <c r="AH310">
         <v>0</v>
@@ -37423,40 +37429,40 @@
     </row>
     <row r="311" spans="1:37" x14ac:dyDescent="0.4">
       <c r="A311">
-        <v>6008</v>
+        <v>6007</v>
       </c>
       <c r="B311" s="9" t="s">
-        <v>1138</v>
+        <v>1137</v>
       </c>
       <c r="C311" t="s">
-        <v>1141</v>
+        <v>1140</v>
       </c>
       <c r="D311">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="E311">
-        <v>95</v>
+        <v>100</v>
       </c>
       <c r="F311">
         <v>100</v>
       </c>
       <c r="G311">
+        <v>100</v>
+      </c>
+      <c r="H311">
+        <v>100</v>
+      </c>
+      <c r="I311">
         <v>130</v>
       </c>
-      <c r="H311">
-        <v>100</v>
-      </c>
-      <c r="I311">
-        <v>90</v>
-      </c>
       <c r="J311">
+        <v>85</v>
+      </c>
+      <c r="K311">
+        <v>100</v>
+      </c>
+      <c r="L311">
         <v>130</v>
-      </c>
-      <c r="K311">
-        <v>110</v>
-      </c>
-      <c r="L311">
-        <v>100</v>
       </c>
       <c r="M311">
         <v>10</v>
@@ -37468,10 +37474,10 @@
         <v>100</v>
       </c>
       <c r="P311">
-        <v>130</v>
+        <v>100</v>
       </c>
       <c r="Q311">
-        <v>112</v>
+        <v>105</v>
       </c>
       <c r="R311">
         <v>105</v>
@@ -37492,7 +37498,7 @@
         <v>113</v>
       </c>
       <c r="X311">
-        <v>800</v>
+        <v>1200</v>
       </c>
       <c r="Y311">
         <v>576</v>
@@ -37501,7 +37507,7 @@
         <v>648</v>
       </c>
       <c r="AA311">
-        <v>200</v>
+        <v>160</v>
       </c>
       <c r="AB311" t="s">
         <v>41</v>
@@ -37519,7 +37525,7 @@
         <v>144</v>
       </c>
       <c r="AG311" t="s">
-        <v>1144</v>
+        <v>1143</v>
       </c>
       <c r="AH311">
         <v>0</v>
@@ -37533,40 +37539,40 @@
     </row>
     <row r="312" spans="1:37" x14ac:dyDescent="0.4">
       <c r="A312">
-        <v>6009</v>
-      </c>
-      <c r="B312" t="s">
-        <v>1145</v>
+        <v>6008</v>
+      </c>
+      <c r="B312" s="9" t="s">
+        <v>1138</v>
       </c>
       <c r="C312" t="s">
-        <v>1148</v>
+        <v>1141</v>
       </c>
       <c r="D312">
-        <v>18</v>
+        <v>36</v>
       </c>
       <c r="E312">
-        <v>100</v>
+        <v>95</v>
       </c>
       <c r="F312">
         <v>100</v>
       </c>
       <c r="G312">
-        <v>100</v>
+        <v>130</v>
       </c>
       <c r="H312">
         <v>100</v>
       </c>
       <c r="I312">
-        <v>100</v>
+        <v>90</v>
       </c>
       <c r="J312">
-        <v>100</v>
+        <v>130</v>
       </c>
       <c r="K312">
-        <v>100</v>
+        <v>110</v>
       </c>
       <c r="L312">
-        <v>150</v>
+        <v>100</v>
       </c>
       <c r="M312">
         <v>10</v>
@@ -37578,13 +37584,13 @@
         <v>100</v>
       </c>
       <c r="P312">
-        <v>100</v>
+        <v>130</v>
       </c>
       <c r="Q312">
-        <v>170</v>
+        <v>112</v>
       </c>
       <c r="R312">
-        <v>170</v>
+        <v>105</v>
       </c>
       <c r="S312">
         <v>10</v>
@@ -37599,19 +37605,19 @@
         <v>48</v>
       </c>
       <c r="W312" t="s">
-        <v>49</v>
+        <v>113</v>
       </c>
       <c r="X312">
-        <v>600</v>
+        <v>800</v>
       </c>
       <c r="Y312">
-        <v>384</v>
+        <v>576</v>
       </c>
       <c r="Z312">
-        <v>288</v>
+        <v>648</v>
       </c>
       <c r="AA312">
-        <v>160</v>
+        <v>200</v>
       </c>
       <c r="AB312" t="s">
         <v>41</v>
@@ -37620,22 +37626,22 @@
         <v>48</v>
       </c>
       <c r="AD312" t="s">
-        <v>1119</v>
+        <v>1120</v>
       </c>
       <c r="AE312" t="s">
         <v>1184</v>
       </c>
       <c r="AF312">
-        <v>180</v>
+        <v>144</v>
       </c>
       <c r="AG312" t="s">
-        <v>1153</v>
+        <v>1144</v>
       </c>
       <c r="AH312">
         <v>0</v>
       </c>
       <c r="AI312">
-        <v>0.25</v>
+        <v>0.5</v>
       </c>
       <c r="AJ312">
         <v>1</v>
@@ -37643,16 +37649,16 @@
     </row>
     <row r="313" spans="1:37" x14ac:dyDescent="0.4">
       <c r="A313">
-        <v>6010</v>
+        <v>6009</v>
       </c>
       <c r="B313" t="s">
-        <v>1146</v>
+        <v>1145</v>
       </c>
       <c r="C313" t="s">
-        <v>1149</v>
+        <v>1148</v>
       </c>
       <c r="D313">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="E313">
         <v>100</v>
@@ -37715,13 +37721,13 @@
         <v>600</v>
       </c>
       <c r="Y313">
-        <v>576</v>
+        <v>384</v>
       </c>
       <c r="Z313">
         <v>288</v>
       </c>
       <c r="AA313">
-        <v>80</v>
+        <v>160</v>
       </c>
       <c r="AB313" t="s">
         <v>41</v>
@@ -37736,10 +37742,10 @@
         <v>1184</v>
       </c>
       <c r="AF313">
-        <v>144</v>
+        <v>180</v>
       </c>
       <c r="AG313" t="s">
-        <v>1154</v>
+        <v>1153</v>
       </c>
       <c r="AH313">
         <v>0</v>
@@ -37753,16 +37759,16 @@
     </row>
     <row r="314" spans="1:37" x14ac:dyDescent="0.4">
       <c r="A314">
-        <v>6011</v>
+        <v>6010</v>
       </c>
       <c r="B314" t="s">
-        <v>1147</v>
+        <v>1146</v>
       </c>
       <c r="C314" t="s">
-        <v>1150</v>
+        <v>1149</v>
       </c>
       <c r="D314">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="E314">
         <v>100</v>
@@ -37831,7 +37837,7 @@
         <v>288</v>
       </c>
       <c r="AA314">
-        <v>140</v>
+        <v>80</v>
       </c>
       <c r="AB314" t="s">
         <v>41</v>
@@ -37849,7 +37855,7 @@
         <v>144</v>
       </c>
       <c r="AG314" t="s">
-        <v>1155</v>
+        <v>1154</v>
       </c>
       <c r="AH314">
         <v>0</v>
@@ -37863,16 +37869,16 @@
     </row>
     <row r="315" spans="1:37" x14ac:dyDescent="0.4">
       <c r="A315">
-        <v>6012</v>
+        <v>6011</v>
       </c>
       <c r="B315" t="s">
-        <v>1151</v>
+        <v>1147</v>
       </c>
       <c r="C315" t="s">
-        <v>1152</v>
+        <v>1150</v>
       </c>
       <c r="D315">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="E315">
         <v>100</v>
@@ -37896,13 +37902,13 @@
         <v>100</v>
       </c>
       <c r="L315">
-        <v>100</v>
+        <v>150</v>
       </c>
       <c r="M315">
         <v>10</v>
       </c>
       <c r="N315">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="O315">
         <v>100</v>
@@ -37926,63 +37932,63 @@
         <v>47</v>
       </c>
       <c r="V315" t="s">
+        <v>48</v>
+      </c>
+      <c r="W315" t="s">
+        <v>49</v>
+      </c>
+      <c r="X315">
+        <v>600</v>
+      </c>
+      <c r="Y315">
+        <v>576</v>
+      </c>
+      <c r="Z315">
+        <v>288</v>
+      </c>
+      <c r="AA315">
         <v>140</v>
-      </c>
-      <c r="W315" t="s">
-        <v>54</v>
-      </c>
-      <c r="X315">
-        <v>1001</v>
-      </c>
-      <c r="Y315">
-        <v>1</v>
-      </c>
-      <c r="Z315">
-        <v>1</v>
-      </c>
-      <c r="AA315">
-        <v>1000</v>
       </c>
       <c r="AB315" t="s">
         <v>41</v>
       </c>
       <c r="AC315" t="s">
-        <v>58</v>
+        <v>48</v>
       </c>
       <c r="AD315" t="s">
-        <v>59</v>
+        <v>1119</v>
       </c>
       <c r="AE315" t="s">
         <v>1184</v>
       </c>
       <c r="AF315">
-        <v>672</v>
+        <v>144</v>
       </c>
       <c r="AG315" t="s">
-        <v>334</v>
+        <v>1155</v>
       </c>
       <c r="AH315">
         <v>0</v>
       </c>
       <c r="AI315">
-        <v>-1</v>
+        <v>0.25</v>
       </c>
       <c r="AJ315">
-        <v>1.05</v>
+        <v>1</v>
       </c>
     </row>
     <row r="316" spans="1:37" x14ac:dyDescent="0.4">
       <c r="A316">
-        <v>6013</v>
+        <v>6012</v>
       </c>
       <c r="B316" t="s">
-        <v>1158</v>
+        <v>1151</v>
       </c>
       <c r="C316" t="s">
-        <v>1160</v>
+        <v>1152</v>
       </c>
       <c r="D316">
-        <v>36</v>
+        <v>20</v>
       </c>
       <c r="E316">
         <v>100</v>
@@ -37994,13 +38000,13 @@
         <v>100</v>
       </c>
       <c r="H316">
-        <v>80</v>
+        <v>100</v>
       </c>
       <c r="I316">
-        <v>110</v>
+        <v>100</v>
       </c>
       <c r="J316">
-        <v>110</v>
+        <v>100</v>
       </c>
       <c r="K316">
         <v>100</v>
@@ -38012,19 +38018,19 @@
         <v>10</v>
       </c>
       <c r="N316">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="O316">
-        <v>70</v>
+        <v>100</v>
       </c>
       <c r="P316">
-        <v>70</v>
+        <v>100</v>
       </c>
       <c r="Q316">
-        <v>100</v>
+        <v>170</v>
       </c>
       <c r="R316">
-        <v>100</v>
+        <v>170</v>
       </c>
       <c r="S316">
         <v>10</v>
@@ -38033,66 +38039,69 @@
         <v>12</v>
       </c>
       <c r="U316" t="s">
-        <v>38</v>
+        <v>47</v>
       </c>
       <c r="V316" t="s">
-        <v>39</v>
+        <v>140</v>
       </c>
       <c r="W316" t="s">
-        <v>437</v>
+        <v>54</v>
       </c>
       <c r="X316">
-        <v>1472</v>
+        <v>1001</v>
       </c>
       <c r="Y316">
-        <v>288</v>
+        <v>1</v>
       </c>
       <c r="Z316">
-        <v>672</v>
+        <v>1</v>
       </c>
       <c r="AA316">
-        <v>180</v>
+        <v>1000</v>
       </c>
       <c r="AB316" t="s">
         <v>41</v>
       </c>
       <c r="AC316" t="s">
-        <v>39</v>
+        <v>58</v>
       </c>
       <c r="AD316" t="s">
-        <v>99</v>
+        <v>59</v>
+      </c>
+      <c r="AE316" t="s">
+        <v>1184</v>
       </c>
       <c r="AF316">
-        <v>528</v>
+        <v>672</v>
       </c>
       <c r="AG316" t="s">
-        <v>1156</v>
+        <v>334</v>
       </c>
       <c r="AH316">
         <v>0</v>
       </c>
       <c r="AI316">
-        <v>0.5</v>
+        <v>-1</v>
       </c>
       <c r="AJ316">
-        <v>1</v>
+        <v>1.05</v>
       </c>
     </row>
     <row r="317" spans="1:37" x14ac:dyDescent="0.4">
       <c r="A317">
-        <v>6014</v>
+        <v>6013</v>
       </c>
       <c r="B317" t="s">
-        <v>1159</v>
+        <v>1158</v>
       </c>
       <c r="C317" t="s">
-        <v>1161</v>
+        <v>1160</v>
       </c>
       <c r="D317">
-        <v>42</v>
+        <v>36</v>
       </c>
       <c r="E317">
-        <v>85</v>
+        <v>100</v>
       </c>
       <c r="F317">
         <v>100</v>
@@ -38113,7 +38122,7 @@
         <v>100</v>
       </c>
       <c r="L317">
-        <v>170</v>
+        <v>100</v>
       </c>
       <c r="M317">
         <v>10</v>
@@ -38128,10 +38137,10 @@
         <v>70</v>
       </c>
       <c r="Q317">
-        <v>125</v>
+        <v>100</v>
       </c>
       <c r="R317">
-        <v>125</v>
+        <v>100</v>
       </c>
       <c r="S317">
         <v>10</v>
@@ -38146,10 +38155,10 @@
         <v>39</v>
       </c>
       <c r="W317" t="s">
-        <v>1027</v>
+        <v>437</v>
       </c>
       <c r="X317">
-        <v>1272</v>
+        <v>1472</v>
       </c>
       <c r="Y317">
         <v>288</v>
@@ -38158,13 +38167,13 @@
         <v>672</v>
       </c>
       <c r="AA317">
-        <v>170</v>
+        <v>180</v>
       </c>
       <c r="AB317" t="s">
         <v>41</v>
       </c>
       <c r="AC317" t="s">
-        <v>225</v>
+        <v>39</v>
       </c>
       <c r="AD317" t="s">
         <v>99</v>
@@ -38173,7 +38182,7 @@
         <v>528</v>
       </c>
       <c r="AG317" t="s">
-        <v>1157</v>
+        <v>1156</v>
       </c>
       <c r="AH317">
         <v>0</v>
@@ -38182,6 +38191,113 @@
         <v>0.5</v>
       </c>
       <c r="AJ317">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="318" spans="1:37" x14ac:dyDescent="0.4">
+      <c r="A318">
+        <v>6014</v>
+      </c>
+      <c r="B318" t="s">
+        <v>1159</v>
+      </c>
+      <c r="C318" t="s">
+        <v>1161</v>
+      </c>
+      <c r="D318">
+        <v>42</v>
+      </c>
+      <c r="E318">
+        <v>85</v>
+      </c>
+      <c r="F318">
+        <v>100</v>
+      </c>
+      <c r="G318">
+        <v>100</v>
+      </c>
+      <c r="H318">
+        <v>80</v>
+      </c>
+      <c r="I318">
+        <v>110</v>
+      </c>
+      <c r="J318">
+        <v>110</v>
+      </c>
+      <c r="K318">
+        <v>100</v>
+      </c>
+      <c r="L318">
+        <v>170</v>
+      </c>
+      <c r="M318">
+        <v>10</v>
+      </c>
+      <c r="N318">
+        <v>1</v>
+      </c>
+      <c r="O318">
+        <v>70</v>
+      </c>
+      <c r="P318">
+        <v>70</v>
+      </c>
+      <c r="Q318">
+        <v>125</v>
+      </c>
+      <c r="R318">
+        <v>125</v>
+      </c>
+      <c r="S318">
+        <v>10</v>
+      </c>
+      <c r="T318">
+        <v>12</v>
+      </c>
+      <c r="U318" t="s">
+        <v>38</v>
+      </c>
+      <c r="V318" t="s">
+        <v>39</v>
+      </c>
+      <c r="W318" t="s">
+        <v>1027</v>
+      </c>
+      <c r="X318">
+        <v>1272</v>
+      </c>
+      <c r="Y318">
+        <v>288</v>
+      </c>
+      <c r="Z318">
+        <v>672</v>
+      </c>
+      <c r="AA318">
+        <v>170</v>
+      </c>
+      <c r="AB318" t="s">
+        <v>41</v>
+      </c>
+      <c r="AC318" t="s">
+        <v>225</v>
+      </c>
+      <c r="AD318" t="s">
+        <v>99</v>
+      </c>
+      <c r="AF318">
+        <v>528</v>
+      </c>
+      <c r="AG318" t="s">
+        <v>1157</v>
+      </c>
+      <c r="AH318">
+        <v>0</v>
+      </c>
+      <c r="AI318">
+        <v>0.5</v>
+      </c>
+      <c r="AJ318">
         <v>1</v>
       </c>
     </row>
@@ -40295,7 +40411,7 @@
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C16" sqref="C16"/>
+      <selection pane="bottomLeft" activeCell="E25" sqref="E25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
@@ -41285,7 +41401,7 @@
         <v>110</v>
       </c>
       <c r="E23">
-        <v>110</v>
+        <v>105</v>
       </c>
       <c r="F23">
         <v>110</v>
@@ -41329,7 +41445,7 @@
         <v>120</v>
       </c>
       <c r="E24">
-        <v>115</v>
+        <v>105</v>
       </c>
       <c r="F24">
         <v>115</v>
@@ -41373,7 +41489,7 @@
         <v>130</v>
       </c>
       <c r="E25">
-        <v>120</v>
+        <v>110</v>
       </c>
       <c r="F25">
         <v>120</v>
@@ -41417,7 +41533,7 @@
         <v>140</v>
       </c>
       <c r="E26">
-        <v>125</v>
+        <v>110</v>
       </c>
       <c r="F26">
         <v>125</v>
@@ -41461,7 +41577,7 @@
         <v>150</v>
       </c>
       <c r="E27">
-        <v>130</v>
+        <v>115</v>
       </c>
       <c r="F27">
         <v>130</v>
@@ -41505,7 +41621,7 @@
         <v>160</v>
       </c>
       <c r="E28">
-        <v>135</v>
+        <v>120</v>
       </c>
       <c r="F28">
         <v>150</v>
@@ -41549,7 +41665,7 @@
         <v>180</v>
       </c>
       <c r="E29">
-        <v>140</v>
+        <v>125</v>
       </c>
       <c r="F29">
         <v>160</v>

</xml_diff>

<commit_message>
Party UI added, more skill changes, other small fixes.
</commit_message>
<xml_diff>
--- a/Other/RoStatProcessing.xlsx
+++ b/Other/RoStatProcessing.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28526"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28623"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\ProjectsSSD\RagnarokRebuildTcp\Other\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{90F342A3-C737-4DF0-A42D-267EF6965D63}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A91276FA-6ADA-4C40-A423-16AD8EE97A73}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3634" yWindow="2914" windowWidth="26932" windowHeight="13937" xr2:uid="{1C41742B-2950-4FF8-AA39-6557869B44EA}"/>
+    <workbookView xWindow="2477" yWindow="1106" windowWidth="28612" windowHeight="13457" xr2:uid="{1C41742B-2950-4FF8-AA39-6557869B44EA}"/>
   </bookViews>
   <sheets>
     <sheet name="StatDef" sheetId="3" r:id="rId1"/>
@@ -10821,7 +10821,7 @@
         <v>100</v>
       </c>
       <c r="G63">
-        <v>100</v>
+        <v>160</v>
       </c>
       <c r="H63">
         <v>100</v>
@@ -17298,7 +17298,7 @@
         <v>120</v>
       </c>
       <c r="G123">
-        <v>130</v>
+        <v>120</v>
       </c>
       <c r="H123">
         <v>120</v>
@@ -18270,7 +18270,7 @@
         <v>490</v>
       </c>
       <c r="D132">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="E132">
         <v>100</v>
@@ -23837,7 +23837,7 @@
         <v>659</v>
       </c>
       <c r="D184">
-        <v>46</v>
+        <v>51</v>
       </c>
       <c r="E184">
         <v>100</v>
@@ -23861,7 +23861,7 @@
         <v>120</v>
       </c>
       <c r="L184">
-        <v>135</v>
+        <v>130</v>
       </c>
       <c r="M184">
         <v>10</v>
@@ -23876,10 +23876,10 @@
         <v>120</v>
       </c>
       <c r="Q184">
-        <v>130</v>
+        <v>120</v>
       </c>
       <c r="R184">
-        <v>115</v>
+        <v>110</v>
       </c>
       <c r="S184">
         <v>10</v>

</xml_diff>

<commit_message>
Skill and monster ai adjustments. Added Angry monster AI type.
</commit_message>
<xml_diff>
--- a/Other/RoStatProcessing.xlsx
+++ b/Other/RoStatProcessing.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\ProjectsSSD\RagnarokRebuildTcp\Other\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A91276FA-6ADA-4C40-A423-16AD8EE97A73}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2E4545A7-6C05-4C64-AF2F-9B9EC572F0A2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2477" yWindow="1106" windowWidth="28612" windowHeight="13457" xr2:uid="{1C41742B-2950-4FF8-AA39-6557869B44EA}"/>
+    <workbookView xWindow="2820" yWindow="1449" windowWidth="28611" windowHeight="13457" xr2:uid="{1C41742B-2950-4FF8-AA39-6557869B44EA}"/>
   </bookViews>
   <sheets>
     <sheet name="StatDef" sheetId="3" r:id="rId1"/>
@@ -51,7 +51,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3197" uniqueCount="1196">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3197" uniqueCount="1197">
   <si>
     <t>Id</t>
   </si>
@@ -3639,6 +3639,9 @@
   </si>
   <si>
     <t>Golem,Buff</t>
+  </si>
+  <si>
+    <t>AiAngry</t>
   </si>
 </sst>
 </file>
@@ -4087,10 +4090,10 @@
   <dimension ref="A1:AK318"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <pane xSplit="4" ySplit="1" topLeftCell="E106" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="4" ySplit="1" topLeftCell="E214" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="E1" sqref="E1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="G123" sqref="G123"/>
+      <selection pane="bottomRight" activeCell="AD232" sqref="AD232"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
@@ -13271,7 +13274,7 @@
         <v>41</v>
       </c>
       <c r="AD85" t="s">
-        <v>99</v>
+        <v>1196</v>
       </c>
       <c r="AF85">
         <v>324</v>
@@ -13806,7 +13809,7 @@
         <v>41</v>
       </c>
       <c r="AD90" t="s">
-        <v>99</v>
+        <v>1196</v>
       </c>
       <c r="AF90">
         <v>432</v>
@@ -18134,7 +18137,7 @@
         <v>1107</v>
       </c>
       <c r="AD130" t="s">
-        <v>99</v>
+        <v>1196</v>
       </c>
       <c r="AF130">
         <v>288</v>
@@ -24346,7 +24349,7 @@
         <v>41</v>
       </c>
       <c r="AD188" t="s">
-        <v>99</v>
+        <v>1196</v>
       </c>
       <c r="AF188">
         <v>720</v>
@@ -24560,7 +24563,7 @@
         <v>286</v>
       </c>
       <c r="AD190" t="s">
-        <v>1119</v>
+        <v>1196</v>
       </c>
       <c r="AF190">
         <v>432</v>
@@ -28947,7 +28950,7 @@
         <v>1085</v>
       </c>
       <c r="AD231" t="s">
-        <v>99</v>
+        <v>1196</v>
       </c>
       <c r="AF231">
         <v>432</v>

</xml_diff>

<commit_message>
A variety of skill and monster skill AI adjustments.
</commit_message>
<xml_diff>
--- a/Other/RoStatProcessing.xlsx
+++ b/Other/RoStatProcessing.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28623"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28827"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\ProjectsSSD\RagnarokRebuildTcp\Other\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2E4545A7-6C05-4C64-AF2F-9B9EC572F0A2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{26987204-6271-4772-B1C4-8292D0123673}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2820" yWindow="1449" windowWidth="28611" windowHeight="13457" xr2:uid="{1C41742B-2950-4FF8-AA39-6557869B44EA}"/>
+    <workbookView xWindow="1620" yWindow="2734" windowWidth="27746" windowHeight="13406" xr2:uid="{1C41742B-2950-4FF8-AA39-6557869B44EA}"/>
   </bookViews>
   <sheets>
     <sheet name="StatDef" sheetId="3" r:id="rId1"/>
@@ -4090,10 +4090,10 @@
   <dimension ref="A1:AK318"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <pane xSplit="4" ySplit="1" topLeftCell="E214" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="4" ySplit="1" topLeftCell="G110" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="E1" sqref="E1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="AD232" sqref="AD232"/>
+      <selection pane="bottomRight" activeCell="AD142" sqref="AD142"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
@@ -19421,7 +19421,7 @@
         <v>469</v>
       </c>
       <c r="AD142" t="s">
-        <v>99</v>
+        <v>1196</v>
       </c>
       <c r="AF142">
         <v>816</v>
@@ -25847,7 +25847,7 @@
         <v>41</v>
       </c>
       <c r="AD202" t="s">
-        <v>99</v>
+        <v>1196</v>
       </c>
       <c r="AF202">
         <v>216</v>
@@ -25954,7 +25954,7 @@
         <v>41</v>
       </c>
       <c r="AD203" t="s">
-        <v>99</v>
+        <v>1196</v>
       </c>
       <c r="AF203">
         <v>192</v>
@@ -26061,7 +26061,7 @@
         <v>456</v>
       </c>
       <c r="AD204" t="s">
-        <v>99</v>
+        <v>1196</v>
       </c>
       <c r="AF204">
         <v>108</v>

</xml_diff>

<commit_message>
Added damage vs tag, wiki adjustments, and otehr small changes.
</commit_message>
<xml_diff>
--- a/Other/RoStatProcessing.xlsx
+++ b/Other/RoStatProcessing.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\ProjectsSSD\RagnarokRebuildTcp\Other\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{26987204-6271-4772-B1C4-8292D0123673}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5EB727D5-0349-45C3-9FEA-419B76C18E6D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1620" yWindow="2734" windowWidth="27746" windowHeight="13406" xr2:uid="{1C41742B-2950-4FF8-AA39-6557869B44EA}"/>
+    <workbookView xWindow="2443" yWindow="2211" windowWidth="27746" windowHeight="13406" xr2:uid="{1C41742B-2950-4FF8-AA39-6557869B44EA}"/>
   </bookViews>
   <sheets>
     <sheet name="StatDef" sheetId="3" r:id="rId1"/>
@@ -4090,10 +4090,10 @@
   <dimension ref="A1:AK318"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <pane xSplit="4" ySplit="1" topLeftCell="G110" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="4" ySplit="1" topLeftCell="E63" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="E1" sqref="E1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="AD142" sqref="AD142"/>
+      <selection pane="bottomRight" activeCell="L79" sqref="L79"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
@@ -12542,16 +12542,16 @@
         <v>320</v>
       </c>
       <c r="D79">
-        <v>52</v>
+        <v>56</v>
       </c>
       <c r="E79">
-        <v>140</v>
+        <v>130</v>
       </c>
       <c r="F79">
         <v>100</v>
       </c>
       <c r="G79">
-        <v>180</v>
+        <v>175</v>
       </c>
       <c r="H79">
         <v>85</v>
@@ -12560,13 +12560,13 @@
         <v>100</v>
       </c>
       <c r="J79">
-        <v>130</v>
+        <v>125</v>
       </c>
       <c r="K79">
         <v>140</v>
       </c>
       <c r="L79">
-        <v>110</v>
+        <v>105</v>
       </c>
       <c r="M79">
         <v>18</v>
@@ -12575,10 +12575,10 @@
         <v>1</v>
       </c>
       <c r="O79">
-        <v>150</v>
+        <v>145</v>
       </c>
       <c r="P79">
-        <v>120</v>
+        <v>115</v>
       </c>
       <c r="Q79">
         <v>100</v>
@@ -12652,16 +12652,16 @@
         <v>324</v>
       </c>
       <c r="D80">
-        <v>38</v>
+        <v>42</v>
       </c>
       <c r="E80">
-        <v>140</v>
+        <v>130</v>
       </c>
       <c r="F80">
         <v>100</v>
       </c>
       <c r="G80">
-        <v>180</v>
+        <v>175</v>
       </c>
       <c r="H80">
         <v>85</v>
@@ -12670,13 +12670,13 @@
         <v>100</v>
       </c>
       <c r="J80">
-        <v>130</v>
+        <v>125</v>
       </c>
       <c r="K80">
-        <v>100</v>
+        <v>140</v>
       </c>
       <c r="L80">
-        <v>130</v>
+        <v>115</v>
       </c>
       <c r="M80">
         <v>15</v>
@@ -12685,10 +12685,10 @@
         <v>2</v>
       </c>
       <c r="O80">
-        <v>150</v>
+        <v>145</v>
       </c>
       <c r="P80">
-        <v>120</v>
+        <v>115</v>
       </c>
       <c r="Q80">
         <v>100</v>

</xml_diff>

<commit_message>
Combo items, damage formula adjustments, juno field spawns, wiki changes, bug fixes, and more.
</commit_message>
<xml_diff>
--- a/Other/RoStatProcessing.xlsx
+++ b/Other/RoStatProcessing.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\ProjectsSSD\RagnarokRebuildTcp\Other\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5EB727D5-0349-45C3-9FEA-419B76C18E6D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{99907911-030C-4B7F-B0B8-5644504E60A4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="2443" yWindow="2211" windowWidth="27746" windowHeight="13406" xr2:uid="{1C41742B-2950-4FF8-AA39-6557869B44EA}"/>
   </bookViews>
@@ -51,7 +51,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3197" uniqueCount="1197">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3198" uniqueCount="1198">
   <si>
     <t>Id</t>
   </si>
@@ -3642,6 +3642,9 @@
   </si>
   <si>
     <t>AiAngry</t>
+  </si>
+  <si>
+    <t>WeakVsSilver</t>
   </si>
 </sst>
 </file>
@@ -4090,10 +4093,10 @@
   <dimension ref="A1:AK318"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <pane xSplit="4" ySplit="1" topLeftCell="E63" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="4" ySplit="1" topLeftCell="E197" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="E1" sqref="E1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="L79" sqref="L79"/>
+      <selection pane="bottomRight" activeCell="I214" sqref="I214"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
@@ -16965,7 +16968,7 @@
         <v>74</v>
       </c>
       <c r="E120">
-        <v>100</v>
+        <v>110</v>
       </c>
       <c r="F120">
         <v>120</v>
@@ -27068,7 +27071,7 @@
         <v>95</v>
       </c>
       <c r="I214">
-        <v>130</v>
+        <v>115</v>
       </c>
       <c r="J214">
         <v>80</v>
@@ -37031,7 +37034,7 @@
         <v>48</v>
       </c>
       <c r="E307">
-        <v>40</v>
+        <v>70</v>
       </c>
       <c r="F307">
         <v>100</v>
@@ -37052,7 +37055,7 @@
         <v>100</v>
       </c>
       <c r="L307">
-        <v>110</v>
+        <v>125</v>
       </c>
       <c r="M307">
         <v>15</v>
@@ -37061,7 +37064,7 @@
         <v>1</v>
       </c>
       <c r="O307">
-        <v>350</v>
+        <v>300</v>
       </c>
       <c r="P307">
         <v>350</v>
@@ -37085,7 +37088,7 @@
         <v>53</v>
       </c>
       <c r="W307" t="s">
-        <v>619</v>
+        <v>49</v>
       </c>
       <c r="X307">
         <v>902</v>
@@ -37107,6 +37110,9 @@
       </c>
       <c r="AD307" t="s">
         <v>1120</v>
+      </c>
+      <c r="AE307" t="s">
+        <v>1197</v>
       </c>
       <c r="AF307">
         <v>216</v>

</xml_diff>

<commit_message>
Ankle snare, enchant poison, charge attack, kicking and promoting party members, plus other skill/card/status effect fixes and changes.
</commit_message>
<xml_diff>
--- a/Other/RoStatProcessing.xlsx
+++ b/Other/RoStatProcessing.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\ProjectsSSD\RagnarokRebuildTcp\Other\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9C80D109-6F6A-4AAB-A371-B9D8DAF86523}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D811D747-237D-4816-8B05-64381433CC19}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="7637" yWindow="2314" windowWidth="23152" windowHeight="14829" xr2:uid="{1C41742B-2950-4FF8-AA39-6557869B44EA}"/>
+    <workbookView xWindow="4971" yWindow="2117" windowWidth="23606" windowHeight="14829" xr2:uid="{1C41742B-2950-4FF8-AA39-6557869B44EA}"/>
   </bookViews>
   <sheets>
     <sheet name="StatDef" sheetId="3" r:id="rId1"/>
@@ -52,7 +52,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3228" uniqueCount="1210">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3270" uniqueCount="1213">
   <si>
     <t>Id</t>
   </si>
@@ -3682,6 +3682,15 @@
   </si>
   <si>
     <t>poring_.spr</t>
+  </si>
+  <si>
+    <t>Flying</t>
+  </si>
+  <si>
+    <t>Goblin,Flying</t>
+  </si>
+  <si>
+    <t>Fungus,Flying</t>
   </si>
 </sst>
 </file>
@@ -4135,10 +4144,10 @@
   <dimension ref="A1:AK319"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <pane xSplit="4" ySplit="1" topLeftCell="E280" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="4" ySplit="1" topLeftCell="E138" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="E1" sqref="E1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="E307" sqref="E307"/>
+      <selection pane="bottomRight" activeCell="Q158" sqref="Q158"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
@@ -4918,6 +4927,9 @@
       <c r="AD7" t="s">
         <v>42</v>
       </c>
+      <c r="AE7" t="s">
+        <v>1210</v>
+      </c>
       <c r="AF7">
         <v>432</v>
       </c>
@@ -5453,6 +5465,9 @@
       <c r="AD12" t="s">
         <v>74</v>
       </c>
+      <c r="AE12" t="s">
+        <v>1210</v>
+      </c>
       <c r="AF12">
         <v>576</v>
       </c>
@@ -5991,6 +6006,9 @@
       <c r="AD17" t="s">
         <v>99</v>
       </c>
+      <c r="AE17" t="s">
+        <v>1210</v>
+      </c>
       <c r="AF17">
         <v>360</v>
       </c>
@@ -7382,6 +7400,9 @@
       <c r="AD30" t="s">
         <v>74</v>
       </c>
+      <c r="AE30" t="s">
+        <v>1210</v>
+      </c>
       <c r="AF30">
         <v>360</v>
       </c>
@@ -8474,7 +8495,7 @@
         <v>1120</v>
       </c>
       <c r="AE40" t="s">
-        <v>1180</v>
+        <v>1211</v>
       </c>
       <c r="AF40">
         <v>324</v>
@@ -8584,7 +8605,7 @@
         <v>1112</v>
       </c>
       <c r="AE41" t="s">
-        <v>1180</v>
+        <v>1211</v>
       </c>
       <c r="AF41">
         <v>324</v>
@@ -8694,7 +8715,7 @@
         <v>99</v>
       </c>
       <c r="AE42" t="s">
-        <v>1180</v>
+        <v>1211</v>
       </c>
       <c r="AF42">
         <v>1008</v>
@@ -9665,6 +9686,9 @@
       <c r="AD51" t="s">
         <v>1120</v>
       </c>
+      <c r="AE51" t="s">
+        <v>1210</v>
+      </c>
       <c r="AF51">
         <v>336</v>
       </c>
@@ -10093,6 +10117,9 @@
       <c r="AD55" t="s">
         <v>1120</v>
       </c>
+      <c r="AE55" t="s">
+        <v>1210</v>
+      </c>
       <c r="AF55">
         <v>360</v>
       </c>
@@ -10738,6 +10765,9 @@
       <c r="AD61" t="s">
         <v>1112</v>
       </c>
+      <c r="AE61" t="s">
+        <v>1210</v>
+      </c>
       <c r="AF61">
         <v>324</v>
       </c>
@@ -11059,6 +11089,9 @@
       <c r="AD64" t="s">
         <v>1097</v>
       </c>
+      <c r="AE64" t="s">
+        <v>1210</v>
+      </c>
       <c r="AF64">
         <v>552</v>
       </c>
@@ -13975,6 +14008,9 @@
       <c r="AD91" t="s">
         <v>1118</v>
       </c>
+      <c r="AE91" t="s">
+        <v>1210</v>
+      </c>
       <c r="AF91">
         <v>288</v>
       </c>
@@ -14082,6 +14118,9 @@
       <c r="AD92" t="s">
         <v>1120</v>
       </c>
+      <c r="AE92" t="s">
+        <v>1210</v>
+      </c>
       <c r="AF92">
         <v>288</v>
       </c>
@@ -14189,6 +14228,9 @@
       <c r="AD93" t="s">
         <v>99</v>
       </c>
+      <c r="AE93" t="s">
+        <v>1210</v>
+      </c>
       <c r="AF93">
         <v>288</v>
       </c>
@@ -14296,6 +14338,9 @@
       <c r="AD94" t="s">
         <v>42</v>
       </c>
+      <c r="AE94" t="s">
+        <v>1210</v>
+      </c>
       <c r="AF94">
         <v>288</v>
       </c>
@@ -14831,6 +14876,9 @@
       <c r="AD99" t="s">
         <v>1119</v>
       </c>
+      <c r="AE99" t="s">
+        <v>1210</v>
+      </c>
       <c r="AF99">
         <v>336</v>
       </c>
@@ -15366,6 +15414,9 @@
       <c r="AD104" t="s">
         <v>1120</v>
       </c>
+      <c r="AE104" t="s">
+        <v>1210</v>
+      </c>
       <c r="AF104">
         <v>288</v>
       </c>
@@ -15690,6 +15741,9 @@
       <c r="AD107" t="s">
         <v>1112</v>
       </c>
+      <c r="AE107" t="s">
+        <v>1210</v>
+      </c>
       <c r="AF107">
         <v>252</v>
       </c>
@@ -18089,6 +18143,9 @@
       <c r="AD129" t="s">
         <v>1119</v>
       </c>
+      <c r="AE129" t="s">
+        <v>1210</v>
+      </c>
       <c r="AF129">
         <v>288</v>
       </c>
@@ -20125,6 +20182,9 @@
       <c r="AD148" t="s">
         <v>1119</v>
       </c>
+      <c r="AE148" t="s">
+        <v>1210</v>
+      </c>
       <c r="AF148">
         <v>720</v>
       </c>
@@ -20232,6 +20292,9 @@
       <c r="AD149" t="s">
         <v>59</v>
       </c>
+      <c r="AE149" t="s">
+        <v>1210</v>
+      </c>
       <c r="AF149">
         <v>720</v>
       </c>
@@ -20339,6 +20402,9 @@
       <c r="AD150" t="s">
         <v>1120</v>
       </c>
+      <c r="AE150" t="s">
+        <v>1210</v>
+      </c>
       <c r="AF150">
         <v>1152</v>
       </c>
@@ -21089,7 +21155,7 @@
         <v>1119</v>
       </c>
       <c r="AE157" t="s">
-        <v>1159</v>
+        <v>1212</v>
       </c>
       <c r="AF157">
         <v>900</v>
@@ -21136,7 +21202,7 @@
         <v>200</v>
       </c>
       <c r="J158">
-        <v>140</v>
+        <v>170</v>
       </c>
       <c r="K158">
         <v>110</v>
@@ -21197,6 +21263,9 @@
       </c>
       <c r="AD158" t="s">
         <v>1120</v>
+      </c>
+      <c r="AE158" t="s">
+        <v>1210</v>
       </c>
       <c r="AF158">
         <v>468</v>
@@ -21305,6 +21374,9 @@
       <c r="AD159" t="s">
         <v>1120</v>
       </c>
+      <c r="AE159" t="s">
+        <v>1210</v>
+      </c>
       <c r="AF159">
         <v>288</v>
       </c>
@@ -21412,6 +21484,9 @@
       <c r="AD160" t="s">
         <v>1112</v>
       </c>
+      <c r="AE160" t="s">
+        <v>1210</v>
+      </c>
       <c r="AF160">
         <v>384</v>
       </c>
@@ -22054,6 +22129,9 @@
       <c r="AD166" t="s">
         <v>1112</v>
       </c>
+      <c r="AE166" t="s">
+        <v>1210</v>
+      </c>
       <c r="AF166">
         <v>432</v>
       </c>
@@ -22524,19 +22602,19 @@
         <v>100</v>
       </c>
       <c r="I171">
-        <v>100</v>
+        <v>140</v>
       </c>
       <c r="J171">
-        <v>100</v>
+        <v>140</v>
       </c>
       <c r="K171">
         <v>100</v>
       </c>
       <c r="L171">
-        <v>100</v>
+        <v>105</v>
       </c>
       <c r="M171">
-        <v>15</v>
+        <v>8</v>
       </c>
       <c r="N171">
         <v>1</v>
@@ -23698,19 +23776,19 @@
         <v>100</v>
       </c>
       <c r="H182">
-        <v>100</v>
+        <v>140</v>
       </c>
       <c r="I182">
         <v>115</v>
       </c>
       <c r="J182">
+        <v>175</v>
+      </c>
+      <c r="K182">
+        <v>100</v>
+      </c>
+      <c r="L182">
         <v>125</v>
-      </c>
-      <c r="K182">
-        <v>100</v>
-      </c>
-      <c r="L182">
-        <v>112</v>
       </c>
       <c r="M182">
         <v>30</v>
@@ -23725,10 +23803,10 @@
         <v>200</v>
       </c>
       <c r="Q182">
-        <v>100</v>
+        <v>105</v>
       </c>
       <c r="R182">
-        <v>100</v>
+        <v>115</v>
       </c>
       <c r="S182">
         <v>10</v>
@@ -23765,6 +23843,9 @@
       </c>
       <c r="AD182" t="s">
         <v>99</v>
+      </c>
+      <c r="AE182" t="s">
+        <v>1210</v>
       </c>
       <c r="AF182">
         <v>780</v>
@@ -23873,6 +23954,9 @@
       <c r="AD183" t="s">
         <v>1119</v>
       </c>
+      <c r="AE183" t="s">
+        <v>1210</v>
+      </c>
       <c r="AF183">
         <v>240</v>
       </c>
@@ -26016,6 +26100,9 @@
       <c r="AD203" t="s">
         <v>1196</v>
       </c>
+      <c r="AE203" t="s">
+        <v>1210</v>
+      </c>
       <c r="AF203">
         <v>192</v>
       </c>
@@ -26230,6 +26317,9 @@
       <c r="AD205" t="s">
         <v>1112</v>
       </c>
+      <c r="AE205" t="s">
+        <v>1210</v>
+      </c>
       <c r="AF205">
         <v>288</v>
       </c>
@@ -26551,6 +26641,9 @@
       <c r="AD208" t="s">
         <v>1120</v>
       </c>
+      <c r="AE208" t="s">
+        <v>1210</v>
+      </c>
       <c r="AF208">
         <v>360</v>
       </c>
@@ -27086,6 +27179,9 @@
       <c r="AD213" t="s">
         <v>1120</v>
       </c>
+      <c r="AE213" t="s">
+        <v>1210</v>
+      </c>
       <c r="AF213">
         <v>168</v>
       </c>
@@ -27407,6 +27503,9 @@
       <c r="AD216" t="s">
         <v>1120</v>
       </c>
+      <c r="AE216" t="s">
+        <v>1210</v>
+      </c>
       <c r="AF216">
         <v>384</v>
       </c>
@@ -27514,6 +27613,9 @@
       <c r="AD217" t="s">
         <v>1120</v>
       </c>
+      <c r="AE217" t="s">
+        <v>1210</v>
+      </c>
       <c r="AF217">
         <v>269</v>
       </c>
@@ -27621,6 +27723,9 @@
       <c r="AD218" t="s">
         <v>1120</v>
       </c>
+      <c r="AE218" t="s">
+        <v>1210</v>
+      </c>
       <c r="AF218">
         <v>408</v>
       </c>
@@ -28156,6 +28261,9 @@
       <c r="AD223" t="s">
         <v>99</v>
       </c>
+      <c r="AE223" t="s">
+        <v>1210</v>
+      </c>
       <c r="AF223">
         <v>600</v>
       </c>
@@ -28905,6 +29013,9 @@
       <c r="AD230" t="s">
         <v>1120</v>
       </c>
+      <c r="AE230" t="s">
+        <v>1210</v>
+      </c>
       <c r="AF230">
         <v>720</v>
       </c>
@@ -30510,6 +30621,9 @@
       <c r="AD245" t="s">
         <v>1097</v>
       </c>
+      <c r="AE245" t="s">
+        <v>1210</v>
+      </c>
       <c r="AF245">
         <v>336</v>
       </c>
@@ -31476,6 +31590,9 @@
       <c r="AD254" t="s">
         <v>1196</v>
       </c>
+      <c r="AE254" t="s">
+        <v>1210</v>
+      </c>
       <c r="AF254">
         <v>384</v>
       </c>
@@ -32977,6 +33094,9 @@
       <c r="AD268" t="s">
         <v>1120</v>
       </c>
+      <c r="AE268" t="s">
+        <v>1210</v>
+      </c>
       <c r="AF268">
         <v>720</v>
       </c>
@@ -34154,6 +34274,9 @@
       <c r="AD279" t="s">
         <v>1120</v>
       </c>
+      <c r="AE279" t="s">
+        <v>1210</v>
+      </c>
       <c r="AF279">
         <v>288</v>
       </c>
@@ -35129,6 +35252,9 @@
       <c r="AD288" t="s">
         <v>984</v>
       </c>
+      <c r="AE288" t="s">
+        <v>1210</v>
+      </c>
       <c r="AF288">
         <v>216</v>
       </c>
@@ -35239,6 +35365,9 @@
       <c r="AD289" t="s">
         <v>99</v>
       </c>
+      <c r="AE289" t="s">
+        <v>1210</v>
+      </c>
       <c r="AF289">
         <v>504</v>
       </c>
@@ -36309,6 +36438,9 @@
       <c r="AD299" t="s">
         <v>99</v>
       </c>
+      <c r="AE299" t="s">
+        <v>1210</v>
+      </c>
       <c r="AF299">
         <v>540</v>
       </c>
@@ -36632,6 +36764,9 @@
       </c>
       <c r="AD302" t="s">
         <v>42</v>
+      </c>
+      <c r="AE302" t="s">
+        <v>1210</v>
       </c>
       <c r="AF302">
         <v>825</v>

</xml_diff>

<commit_message>
Gigantic update to prepare for test server.
</commit_message>
<xml_diff>
--- a/Other/RoStatProcessing.xlsx
+++ b/Other/RoStatProcessing.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\ProjectsSSD\RagnarokRebuildTcp\Other\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D811D747-237D-4816-8B05-64381433CC19}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{669005F6-E4C4-4B0D-A4AB-EC62CB34D1D3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4971" yWindow="2117" windowWidth="23606" windowHeight="14829" xr2:uid="{1C41742B-2950-4FF8-AA39-6557869B44EA}"/>
+    <workbookView xWindow="1063" yWindow="1749" windowWidth="31080" windowHeight="14828" xr2:uid="{1C41742B-2950-4FF8-AA39-6557869B44EA}"/>
   </bookViews>
   <sheets>
     <sheet name="StatDef" sheetId="3" r:id="rId1"/>
@@ -52,7 +52,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3270" uniqueCount="1213">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3324" uniqueCount="1233">
   <si>
     <t>Id</t>
   </si>
@@ -3691,6 +3691,66 @@
   </si>
   <si>
     <t>Fungus,Flying</t>
+  </si>
+  <si>
+    <t>SUCCUBUS</t>
+  </si>
+  <si>
+    <t>succubus.spr</t>
+  </si>
+  <si>
+    <t>INCUBUS</t>
+  </si>
+  <si>
+    <t>incubus.spr</t>
+  </si>
+  <si>
+    <t>OBSERVATION</t>
+  </si>
+  <si>
+    <t>observation.spr</t>
+  </si>
+  <si>
+    <t>RETRIBUTION</t>
+  </si>
+  <si>
+    <t>retribution.spr</t>
+  </si>
+  <si>
+    <t>SOLACE</t>
+  </si>
+  <si>
+    <t>solace.spr</t>
+  </si>
+  <si>
+    <t>SHELTER</t>
+  </si>
+  <si>
+    <t>shelter.spr</t>
+  </si>
+  <si>
+    <t>Succubus</t>
+  </si>
+  <si>
+    <t>Incubus</t>
+  </si>
+  <si>
+    <t>Buff,Angel</t>
+  </si>
+  <si>
+    <t>Strong,Angel</t>
+  </si>
+  <si>
+    <t>Elite,Angel</t>
+  </si>
+  <si>
+    <t>Baroness of Retribution</t>
+  </si>
+  <si>
+    <t>Dame of Sentinel</t>
+  </si>
+  <si>
+    <t>Mistress of Shelter</t>
   </si>
 </sst>
 </file>
@@ -4141,13 +4201,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{811A97A5-94A7-4FFA-A162-65D076B52481}">
-  <dimension ref="A1:AK319"/>
+  <dimension ref="A1:AK325"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <pane xSplit="4" ySplit="1" topLeftCell="E138" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="4" ySplit="1" topLeftCell="E289" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="E1" sqref="E1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="Q158" sqref="Q158"/>
+      <selection pane="bottomRight" activeCell="AD296" sqref="AD296"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
@@ -35288,7 +35348,7 @@
         <v>99</v>
       </c>
       <c r="E289">
-        <v>150</v>
+        <v>100</v>
       </c>
       <c r="F289">
         <v>100</v>
@@ -35300,16 +35360,16 @@
         <v>70</v>
       </c>
       <c r="I289">
-        <v>100</v>
+        <v>70</v>
       </c>
       <c r="J289">
-        <v>100</v>
+        <v>30</v>
       </c>
       <c r="K289">
-        <v>170</v>
+        <v>100</v>
       </c>
       <c r="L289">
-        <v>100</v>
+        <v>40</v>
       </c>
       <c r="M289">
         <v>10</v>
@@ -35330,10 +35390,10 @@
         <v>100</v>
       </c>
       <c r="S289">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="T289">
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="U289" t="s">
         <v>144</v>
@@ -35342,7 +35402,7 @@
         <v>229</v>
       </c>
       <c r="W289" t="s">
-        <v>230</v>
+        <v>109</v>
       </c>
       <c r="X289">
         <v>576</v>
@@ -35381,7 +35441,7 @@
         <v>0.5</v>
       </c>
       <c r="AJ289">
-        <v>1</v>
+        <v>1.4</v>
       </c>
     </row>
     <row r="290" spans="1:37" x14ac:dyDescent="0.4">
@@ -35398,7 +35458,7 @@
         <v>99</v>
       </c>
       <c r="E290">
-        <v>100</v>
+        <v>75</v>
       </c>
       <c r="F290">
         <v>100</v>
@@ -35407,19 +35467,19 @@
         <v>100</v>
       </c>
       <c r="H290">
-        <v>100</v>
+        <v>70</v>
       </c>
       <c r="I290">
-        <v>100</v>
+        <v>70</v>
       </c>
       <c r="J290">
-        <v>100</v>
+        <v>30</v>
       </c>
       <c r="K290">
         <v>100</v>
       </c>
       <c r="L290">
-        <v>50</v>
+        <v>45</v>
       </c>
       <c r="M290">
         <v>10</v>
@@ -35428,10 +35488,10 @@
         <v>3</v>
       </c>
       <c r="O290">
-        <v>100</v>
+        <v>60</v>
       </c>
       <c r="P290">
-        <v>100</v>
+        <v>70</v>
       </c>
       <c r="Q290">
         <v>100</v>
@@ -35440,10 +35500,10 @@
         <v>100</v>
       </c>
       <c r="S290">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="T290">
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="U290" t="s">
         <v>144</v>
@@ -35452,7 +35512,7 @@
         <v>229</v>
       </c>
       <c r="W290" t="s">
-        <v>230</v>
+        <v>109</v>
       </c>
       <c r="X290">
         <v>576</v>
@@ -36008,7 +36068,7 @@
         <v>41</v>
       </c>
       <c r="AD295" t="s">
-        <v>99</v>
+        <v>1196</v>
       </c>
       <c r="AF295">
         <v>624</v>
@@ -36436,7 +36496,7 @@
         <v>456</v>
       </c>
       <c r="AD299" t="s">
-        <v>99</v>
+        <v>1196</v>
       </c>
       <c r="AE299" t="s">
         <v>1210</v>
@@ -38639,6 +38699,648 @@
         <v>0.5</v>
       </c>
       <c r="AJ319">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="320" spans="1:37" x14ac:dyDescent="0.4">
+      <c r="A320">
+        <v>6016</v>
+      </c>
+      <c r="B320" t="s">
+        <v>1213</v>
+      </c>
+      <c r="C320" t="s">
+        <v>1225</v>
+      </c>
+      <c r="D320">
+        <v>85</v>
+      </c>
+      <c r="E320">
+        <v>100</v>
+      </c>
+      <c r="F320">
+        <v>100</v>
+      </c>
+      <c r="G320">
+        <v>100</v>
+      </c>
+      <c r="H320">
+        <v>100</v>
+      </c>
+      <c r="I320">
+        <v>100</v>
+      </c>
+      <c r="J320">
+        <v>100</v>
+      </c>
+      <c r="K320">
+        <v>100</v>
+      </c>
+      <c r="L320">
+        <v>100</v>
+      </c>
+      <c r="M320">
+        <v>10</v>
+      </c>
+      <c r="N320">
+        <v>2</v>
+      </c>
+      <c r="O320">
+        <v>100</v>
+      </c>
+      <c r="P320">
+        <v>100</v>
+      </c>
+      <c r="Q320">
+        <v>100</v>
+      </c>
+      <c r="R320">
+        <v>100</v>
+      </c>
+      <c r="S320">
+        <v>10</v>
+      </c>
+      <c r="T320">
+        <v>12</v>
+      </c>
+      <c r="U320" t="s">
+        <v>38</v>
+      </c>
+      <c r="V320" t="s">
+        <v>219</v>
+      </c>
+      <c r="W320" t="s">
+        <v>619</v>
+      </c>
+      <c r="X320">
+        <v>1306</v>
+      </c>
+      <c r="Y320">
+        <v>288</v>
+      </c>
+      <c r="Z320">
+        <v>1056</v>
+      </c>
+      <c r="AA320">
+        <v>155</v>
+      </c>
+      <c r="AB320" t="s">
+        <v>41</v>
+      </c>
+      <c r="AC320" t="s">
+        <v>1115</v>
+      </c>
+      <c r="AD320" t="s">
+        <v>1120</v>
+      </c>
+      <c r="AF320">
+        <v>576</v>
+      </c>
+      <c r="AG320" t="s">
+        <v>1214</v>
+      </c>
+      <c r="AH320">
+        <v>0</v>
+      </c>
+      <c r="AI320">
+        <v>0.5</v>
+      </c>
+      <c r="AJ320">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="321" spans="1:36" x14ac:dyDescent="0.4">
+      <c r="A321">
+        <v>6017</v>
+      </c>
+      <c r="B321" t="s">
+        <v>1215</v>
+      </c>
+      <c r="C321" t="s">
+        <v>1226</v>
+      </c>
+      <c r="D321">
+        <v>75</v>
+      </c>
+      <c r="E321">
+        <v>100</v>
+      </c>
+      <c r="F321">
+        <v>100</v>
+      </c>
+      <c r="G321">
+        <v>100</v>
+      </c>
+      <c r="H321">
+        <v>100</v>
+      </c>
+      <c r="I321">
+        <v>100</v>
+      </c>
+      <c r="J321">
+        <v>100</v>
+      </c>
+      <c r="K321">
+        <v>100</v>
+      </c>
+      <c r="L321">
+        <v>100</v>
+      </c>
+      <c r="M321">
+        <v>10</v>
+      </c>
+      <c r="N321">
+        <v>2</v>
+      </c>
+      <c r="O321">
+        <v>100</v>
+      </c>
+      <c r="P321">
+        <v>100</v>
+      </c>
+      <c r="Q321">
+        <v>100</v>
+      </c>
+      <c r="R321">
+        <v>100</v>
+      </c>
+      <c r="S321">
+        <v>10</v>
+      </c>
+      <c r="T321">
+        <v>12</v>
+      </c>
+      <c r="U321" t="s">
+        <v>38</v>
+      </c>
+      <c r="V321" t="s">
+        <v>219</v>
+      </c>
+      <c r="W321" t="s">
+        <v>619</v>
+      </c>
+      <c r="X321">
+        <v>850</v>
+      </c>
+      <c r="Y321">
+        <v>336</v>
+      </c>
+      <c r="Z321">
+        <v>600</v>
+      </c>
+      <c r="AA321">
+        <v>165</v>
+      </c>
+      <c r="AB321" t="s">
+        <v>41</v>
+      </c>
+      <c r="AC321" t="s">
+        <v>1115</v>
+      </c>
+      <c r="AD321" t="s">
+        <v>1120</v>
+      </c>
+      <c r="AF321">
+        <v>420</v>
+      </c>
+      <c r="AG321" t="s">
+        <v>1216</v>
+      </c>
+      <c r="AH321">
+        <v>0</v>
+      </c>
+      <c r="AI321">
+        <v>0.5</v>
+      </c>
+      <c r="AJ321">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="322" spans="1:36" x14ac:dyDescent="0.4">
+      <c r="A322">
+        <v>6018</v>
+      </c>
+      <c r="B322" t="s">
+        <v>1217</v>
+      </c>
+      <c r="C322" t="s">
+        <v>1231</v>
+      </c>
+      <c r="D322">
+        <v>81</v>
+      </c>
+      <c r="E322">
+        <v>100</v>
+      </c>
+      <c r="F322">
+        <v>100</v>
+      </c>
+      <c r="G322">
+        <v>100</v>
+      </c>
+      <c r="H322">
+        <v>100</v>
+      </c>
+      <c r="I322">
+        <v>100</v>
+      </c>
+      <c r="J322">
+        <v>100</v>
+      </c>
+      <c r="K322">
+        <v>100</v>
+      </c>
+      <c r="L322">
+        <v>100</v>
+      </c>
+      <c r="M322">
+        <v>10</v>
+      </c>
+      <c r="N322">
+        <v>2</v>
+      </c>
+      <c r="O322">
+        <v>100</v>
+      </c>
+      <c r="P322">
+        <v>100</v>
+      </c>
+      <c r="Q322">
+        <v>100</v>
+      </c>
+      <c r="R322">
+        <v>100</v>
+      </c>
+      <c r="S322">
+        <v>10</v>
+      </c>
+      <c r="T322">
+        <v>12</v>
+      </c>
+      <c r="U322" t="s">
+        <v>38</v>
+      </c>
+      <c r="V322" t="s">
+        <v>229</v>
+      </c>
+      <c r="W322" t="s">
+        <v>585</v>
+      </c>
+      <c r="X322">
+        <v>432</v>
+      </c>
+      <c r="Y322">
+        <v>360</v>
+      </c>
+      <c r="Z322">
+        <v>480</v>
+      </c>
+      <c r="AA322">
+        <v>100</v>
+      </c>
+      <c r="AB322" t="s">
+        <v>119</v>
+      </c>
+      <c r="AC322" t="s">
+        <v>1228</v>
+      </c>
+      <c r="AD322" t="s">
+        <v>1120</v>
+      </c>
+      <c r="AF322">
+        <v>300</v>
+      </c>
+      <c r="AG322" t="s">
+        <v>1218</v>
+      </c>
+      <c r="AH322">
+        <v>0</v>
+      </c>
+      <c r="AI322">
+        <v>0.5</v>
+      </c>
+      <c r="AJ322">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="323" spans="1:36" x14ac:dyDescent="0.4">
+      <c r="A323">
+        <v>6019</v>
+      </c>
+      <c r="B323" t="s">
+        <v>1219</v>
+      </c>
+      <c r="C323" t="s">
+        <v>1230</v>
+      </c>
+      <c r="D323">
+        <v>79</v>
+      </c>
+      <c r="E323">
+        <v>100</v>
+      </c>
+      <c r="F323">
+        <v>100</v>
+      </c>
+      <c r="G323">
+        <v>100</v>
+      </c>
+      <c r="H323">
+        <v>100</v>
+      </c>
+      <c r="I323">
+        <v>100</v>
+      </c>
+      <c r="J323">
+        <v>100</v>
+      </c>
+      <c r="K323">
+        <v>100</v>
+      </c>
+      <c r="L323">
+        <v>100</v>
+      </c>
+      <c r="M323">
+        <v>10</v>
+      </c>
+      <c r="N323">
+        <v>2</v>
+      </c>
+      <c r="O323">
+        <v>100</v>
+      </c>
+      <c r="P323">
+        <v>100</v>
+      </c>
+      <c r="Q323">
+        <v>100</v>
+      </c>
+      <c r="R323">
+        <v>100</v>
+      </c>
+      <c r="S323">
+        <v>10</v>
+      </c>
+      <c r="T323">
+        <v>12</v>
+      </c>
+      <c r="U323" t="s">
+        <v>38</v>
+      </c>
+      <c r="V323" t="s">
+        <v>229</v>
+      </c>
+      <c r="W323" t="s">
+        <v>619</v>
+      </c>
+      <c r="X323">
+        <v>360</v>
+      </c>
+      <c r="Y323">
+        <v>360</v>
+      </c>
+      <c r="Z323">
+        <v>480</v>
+      </c>
+      <c r="AA323">
+        <v>120</v>
+      </c>
+      <c r="AB323" t="s">
+        <v>119</v>
+      </c>
+      <c r="AC323" t="s">
+        <v>1228</v>
+      </c>
+      <c r="AD323" t="s">
+        <v>1120</v>
+      </c>
+      <c r="AF323">
+        <v>240</v>
+      </c>
+      <c r="AG323" t="s">
+        <v>1220</v>
+      </c>
+      <c r="AH323">
+        <v>0</v>
+      </c>
+      <c r="AI323">
+        <v>0.5</v>
+      </c>
+      <c r="AJ323">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="324" spans="1:36" x14ac:dyDescent="0.4">
+      <c r="A324">
+        <v>6020</v>
+      </c>
+      <c r="B324" t="s">
+        <v>1221</v>
+      </c>
+      <c r="C324" t="s">
+        <v>1231</v>
+      </c>
+      <c r="D324">
+        <v>77</v>
+      </c>
+      <c r="E324">
+        <v>100</v>
+      </c>
+      <c r="F324">
+        <v>100</v>
+      </c>
+      <c r="G324">
+        <v>100</v>
+      </c>
+      <c r="H324">
+        <v>100</v>
+      </c>
+      <c r="I324">
+        <v>100</v>
+      </c>
+      <c r="J324">
+        <v>100</v>
+      </c>
+      <c r="K324">
+        <v>100</v>
+      </c>
+      <c r="L324">
+        <v>100</v>
+      </c>
+      <c r="M324">
+        <v>10</v>
+      </c>
+      <c r="N324">
+        <v>2</v>
+      </c>
+      <c r="O324">
+        <v>100</v>
+      </c>
+      <c r="P324">
+        <v>100</v>
+      </c>
+      <c r="Q324">
+        <v>100</v>
+      </c>
+      <c r="R324">
+        <v>100</v>
+      </c>
+      <c r="S324">
+        <v>10</v>
+      </c>
+      <c r="T324">
+        <v>12</v>
+      </c>
+      <c r="U324" t="s">
+        <v>38</v>
+      </c>
+      <c r="V324" t="s">
+        <v>229</v>
+      </c>
+      <c r="W324" t="s">
+        <v>866</v>
+      </c>
+      <c r="X324">
+        <v>576</v>
+      </c>
+      <c r="Y324">
+        <v>360</v>
+      </c>
+      <c r="Z324">
+        <v>420</v>
+      </c>
+      <c r="AA324">
+        <v>180</v>
+      </c>
+      <c r="AB324" t="s">
+        <v>119</v>
+      </c>
+      <c r="AC324" t="s">
+        <v>1227</v>
+      </c>
+      <c r="AD324" t="s">
+        <v>1120</v>
+      </c>
+      <c r="AF324">
+        <v>384</v>
+      </c>
+      <c r="AG324" t="s">
+        <v>1222</v>
+      </c>
+      <c r="AH324">
+        <v>0</v>
+      </c>
+      <c r="AI324">
+        <v>0.5</v>
+      </c>
+      <c r="AJ324">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="325" spans="1:36" x14ac:dyDescent="0.4">
+      <c r="A325">
+        <v>6021</v>
+      </c>
+      <c r="B325" t="s">
+        <v>1223</v>
+      </c>
+      <c r="C325" t="s">
+        <v>1232</v>
+      </c>
+      <c r="D325">
+        <v>80</v>
+      </c>
+      <c r="E325">
+        <v>100</v>
+      </c>
+      <c r="F325">
+        <v>100</v>
+      </c>
+      <c r="G325">
+        <v>100</v>
+      </c>
+      <c r="H325">
+        <v>100</v>
+      </c>
+      <c r="I325">
+        <v>100</v>
+      </c>
+      <c r="J325">
+        <v>100</v>
+      </c>
+      <c r="K325">
+        <v>100</v>
+      </c>
+      <c r="L325">
+        <v>100</v>
+      </c>
+      <c r="M325">
+        <v>10</v>
+      </c>
+      <c r="N325">
+        <v>2</v>
+      </c>
+      <c r="O325">
+        <v>100</v>
+      </c>
+      <c r="P325">
+        <v>100</v>
+      </c>
+      <c r="Q325">
+        <v>100</v>
+      </c>
+      <c r="R325">
+        <v>100</v>
+      </c>
+      <c r="S325">
+        <v>10</v>
+      </c>
+      <c r="T325">
+        <v>12</v>
+      </c>
+      <c r="U325" t="s">
+        <v>38</v>
+      </c>
+      <c r="V325" t="s">
+        <v>229</v>
+      </c>
+      <c r="W325" t="s">
+        <v>866</v>
+      </c>
+      <c r="X325">
+        <v>432</v>
+      </c>
+      <c r="Y325">
+        <v>360</v>
+      </c>
+      <c r="Z325">
+        <v>420</v>
+      </c>
+      <c r="AA325">
+        <v>160</v>
+      </c>
+      <c r="AB325" t="s">
+        <v>119</v>
+      </c>
+      <c r="AC325" t="s">
+        <v>1229</v>
+      </c>
+      <c r="AD325" t="s">
+        <v>1120</v>
+      </c>
+      <c r="AF325">
+        <v>240</v>
+      </c>
+      <c r="AG325" t="s">
+        <v>1224</v>
+      </c>
+      <c r="AH325">
+        <v>0</v>
+      </c>
+      <c r="AI325">
+        <v>0.5</v>
+      </c>
+      <c r="AJ325">
         <v>1</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Fixing party panel targeting, options for sprite filtering/damage numbers, more monster skills, and more.
</commit_message>
<xml_diff>
--- a/Other/RoStatProcessing.xlsx
+++ b/Other/RoStatProcessing.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\ProjectsSSD\RagnarokRebuildTcp\Other\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{669005F6-E4C4-4B0D-A4AB-EC62CB34D1D3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{82D4CF96-70C0-4FD0-978C-FB8F0CE7B1B4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1063" yWindow="1749" windowWidth="31080" windowHeight="14828" xr2:uid="{1C41742B-2950-4FF8-AA39-6557869B44EA}"/>
   </bookViews>
@@ -4204,10 +4204,10 @@
   <dimension ref="A1:AK325"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <pane xSplit="4" ySplit="1" topLeftCell="E289" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="4" ySplit="1" topLeftCell="E273" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="E1" sqref="E1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="AD296" sqref="AD296"/>
+      <selection pane="bottomRight" activeCell="AD294" sqref="AD294"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
@@ -17871,7 +17871,7 @@
         <v>469</v>
       </c>
       <c r="AD126" t="s">
-        <v>99</v>
+        <v>1196</v>
       </c>
       <c r="AE126" t="s">
         <v>1182</v>
@@ -17981,7 +17981,7 @@
         <v>469</v>
       </c>
       <c r="AD127" t="s">
-        <v>99</v>
+        <v>1196</v>
       </c>
       <c r="AE127" t="s">
         <v>1182</v>
@@ -35854,7 +35854,7 @@
         <v>41</v>
       </c>
       <c r="AD293" t="s">
-        <v>99</v>
+        <v>1196</v>
       </c>
       <c r="AF293">
         <v>576</v>

</xml_diff>

<commit_message>
Variety of server and client fixes for the test.
</commit_message>
<xml_diff>
--- a/Other/RoStatProcessing.xlsx
+++ b/Other/RoStatProcessing.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\ProjectsSSD\RagnarokRebuildTcp\Other\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D13EDDEA-BB71-4266-A116-EE45F99E5DDD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B4447C75-CC58-449B-A2C1-46804C81C5BC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="814" yWindow="1569" windowWidth="31080" windowHeight="14828" xr2:uid="{1C41742B-2950-4FF8-AA39-6557869B44EA}"/>
+    <workbookView xWindow="369" yWindow="2006" windowWidth="31080" windowHeight="14828" xr2:uid="{1C41742B-2950-4FF8-AA39-6557869B44EA}"/>
   </bookViews>
   <sheets>
     <sheet name="StatDef" sheetId="3" r:id="rId1"/>
@@ -4204,10 +4204,10 @@
   <dimension ref="A1:AK325"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <pane xSplit="4" ySplit="1" topLeftCell="E221" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="4" ySplit="1" topLeftCell="E269" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="E1" sqref="E1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="E238" sqref="E238"/>
+      <selection pane="bottomRight" activeCell="E290" sqref="E290"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
@@ -32828,7 +32828,7 @@
         <v>41</v>
       </c>
       <c r="AC265" t="s">
-        <v>456</v>
+        <v>181</v>
       </c>
       <c r="AD265" t="s">
         <v>99</v>
@@ -35348,7 +35348,7 @@
         <v>99</v>
       </c>
       <c r="E289">
-        <v>170</v>
+        <v>280</v>
       </c>
       <c r="F289">
         <v>100</v>
@@ -35381,7 +35381,7 @@
         <v>50</v>
       </c>
       <c r="P289">
-        <v>30</v>
+        <v>10</v>
       </c>
       <c r="Q289">
         <v>100</v>
@@ -35491,7 +35491,7 @@
         <v>60</v>
       </c>
       <c r="P290">
-        <v>40</v>
+        <v>10</v>
       </c>
       <c r="Q290">
         <v>100</v>
@@ -41585,7 +41585,7 @@
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="N1" sqref="N1"/>
+      <selection pane="bottomLeft" activeCell="B31" sqref="B31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
@@ -42874,7 +42874,7 @@
         <v>1163</v>
       </c>
       <c r="B30">
-        <v>3200</v>
+        <v>4000</v>
       </c>
       <c r="C30">
         <v>190</v>

</xml_diff>